<commit_message>
Atualização automática: Mon Jan 19 03:32:43 UTC 2026
</commit_message>
<xml_diff>
--- a/vagas_apinfo.xlsx
+++ b/vagas_apinfo.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I279"/>
+  <dimension ref="A1:I368"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13378,6 +13378,4117 @@
         <v>20</v>
       </c>
     </row>
+    <row r="280">
+      <c r="A280" t="inlineStr">
+        <is>
+          <t>19/01/2026</t>
+        </is>
+      </c>
+      <c r="B280" t="inlineStr">
+        <is>
+          <t>82018</t>
+        </is>
+      </c>
+      <c r="C280" t="inlineStr">
+        <is>
+          <t>Dev PHP Pleno – PJ – Híbrido (Guarulhos)</t>
+        </is>
+      </c>
+      <c r="D280" t="inlineStr">
+        <is>
+          <t>Pleno</t>
+        </is>
+      </c>
+      <c r="E280" t="inlineStr">
+        <is>
+          <t>Híbrido</t>
+        </is>
+      </c>
+      <c r="F280" t="inlineStr">
+        <is>
+          <t>Guarulhos - SP - 19/01/26</t>
+        </is>
+      </c>
+      <c r="G280" t="inlineStr">
+        <is>
+          <t>Buscamos um(a) Dev PHP Pleno com perfil colaborativo, comprometido e em constante aprendizado. Atuará no desenvolvimento de sistemas em PHP (Laravel), com foco em GraphQL, PostgreSQL, Redis, Elasticsearch, Firebase e Vue.js.  É essencial ter experiência prática com PHP, Laravel, GraphQL e GIT, além de interesse em evoluir tecnicamente e contribuir com o time.  Requisitos: - PHP + Laravel / MVC - GraphQL (principal) e REST - PostgreSQL, Redis, Elasticsearch - Firebase, Vue.js - GIT e boas práticas  Modelo híbrido – Guarulhos/SP  Diferenciais: - Formação em áreas de TI e boa capacidade de comunicação em equipe.  Regime: PJ  Faixa: R$ 5.000 – R$ 8.000 / mês Ambiente colaborativo, com autonomia, inovação e aprendizado constante.
+Empresa .....:  Bomvalor</t>
+        </is>
+      </c>
+      <c r="H280" t="inlineStr">
+        <is>
+          <t>Guarulhos - SP - 19/01/26 || Dev PHP Pleno – PJ – Híbrido (Guarulhos) || Buscamos um(a) Dev PHP Pleno com perfil colaborativo, comprometido e em constante aprendizado. Atuará no desenvolvimento de sistemas em PHP (Laravel), com foco em GraphQL, PostgreSQL, Redis, Elasticsearch, Firebase e Vue.js.  É essencial ter experiência prática com PHP, Laravel, GraphQL e GIT, além de interesse em evoluir tecnicamente e contribuir com o time.  Requisitos: - PHP + Laravel / MVC - GraphQL (principal) e REST - PostgreSQL, Redis, Elasticsearch - Firebase, Vue.js - GIT e boas práticas  Modelo híbrido – Guarulhos/SP  Diferenciais: - Formação em áreas de TI e boa capacidade de comunicação em equipe.  Regime: PJ  Faixa: R$ 5.000 – R$ 8.000 / mês Ambiente colaborativo, com autonomia, inovação e aprendizado constante. || Empresa .....:  Bomvalor</t>
+        </is>
+      </c>
+      <c r="I280" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" t="inlineStr">
+        <is>
+          <t>19/01/2026</t>
+        </is>
+      </c>
+      <c r="B281" t="inlineStr">
+        <is>
+          <t>82072</t>
+        </is>
+      </c>
+      <c r="C281" t="inlineStr">
+        <is>
+          <t>Analista de Dados Pleno</t>
+        </is>
+      </c>
+      <c r="D281" t="inlineStr">
+        <is>
+          <t>Pleno</t>
+        </is>
+      </c>
+      <c r="E281" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F281" t="inlineStr">
+        <is>
+          <t>Holambra - SP - 19/01/26</t>
+        </is>
+      </c>
+      <c r="G281" t="inlineStr">
+        <is>
+          <t>Responsabilidades: Desenvolver a lógica de cálculo da remuneração variável do time produtivo Automatizar os indicadores já existentes Estruturar e organizar os dados disponíveis na empresa Criar e manter planilhas automatizadas com fórmulas e dashboards no Excel Garantir a integridade das informações e apoiar na transição para as áreas responsáveis após a implantação.  Requisitos: Excel intermediário a avançado (fórmulas, tabelas dinâmicas, PROCX, SOMASES, etc.) Ensino superior completo em Dados, Ciências da Computação, Engenharia, Administração, Matemática, Físca ou áreas correlatas Capacidade analítica, atenção aos detalhes e organização Desejável Conhecimento em Power BI ou ferramentas similares.  Modelo: CLT, Presencial em Holambra - SP  Benefícios: Vale Alimentação Refeição no local Ajuda de custo para deslocamento Plano Odontológico - Uniodonto Totalpass Seguro de vida.
+Empresa .....:  IVO SERVICES TECH RECRUIT</t>
+        </is>
+      </c>
+      <c r="H281" t="inlineStr">
+        <is>
+          <t>Holambra - SP - 19/01/26 || Analista de Dados Pleno || Responsabilidades: Desenvolver a lógica de cálculo da remuneração variável do time produtivo Automatizar os indicadores já existentes Estruturar e organizar os dados disponíveis na empresa Criar e manter planilhas automatizadas com fórmulas e dashboards no Excel Garantir a integridade das informações e apoiar na transição para as áreas responsáveis após a implantação.  Requisitos: Excel intermediário a avançado (fórmulas, tabelas dinâmicas, PROCX, SOMASES, etc.) Ensino superior completo em Dados, Ciências da Computação, Engenharia, Administração, Matemática, Físca ou áreas correlatas Capacidade analítica, atenção aos detalhes e organização Desejável Conhecimento em Power BI ou ferramentas similares.  Modelo: CLT, Presencial em Holambra - SP  Benefícios: Vale Alimentação Refeição no local Ajuda de custo para deslocamento Plano Odontológico - Uniodonto Totalpass Seguro de vida. || Empresa .....:  IVO SERVICES TECH RECRUIT</t>
+        </is>
+      </c>
+      <c r="I281" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" t="inlineStr">
+        <is>
+          <t>19/01/2026</t>
+        </is>
+      </c>
+      <c r="B282" t="inlineStr">
+        <is>
+          <t>82948</t>
+        </is>
+      </c>
+      <c r="C282" t="inlineStr">
+        <is>
+          <t>analista de TI pleno</t>
+        </is>
+      </c>
+      <c r="D282" t="inlineStr">
+        <is>
+          <t>Pleno</t>
+        </is>
+      </c>
+      <c r="E282" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F282" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 19/01/26</t>
+        </is>
+      </c>
+      <c r="G282" t="inlineStr">
+        <is>
+          <t>Objetivo: Atuação em projetos estratégicos, com foco em soluções para o setor de Telecomunicações, especialmente em Sistemas de Mediação. Regime: Totalmente Remoto Horário: Comercial  Experiência Necessária Vivência comprovada em projetos de Telecom, especialmente em Sistemas de Mediação. Sólido conhecimento em Linux. Programação em Python e Shell Script em ambientes produtivos. Atuação com integrações entre sistemas complexos e alto volume de dados.  Desejável Experiência em linguagens como CGDC, Java, C e JavaScript. Conhecimento em ferramentas de versionamento (Git) e pipelines de CI/CD. Experiência em metodologias ágeis (Scrum, Kanban). Vivência em ambientes de alta disponibilidade e monitoramento de aplicações.
+Empresa .....:  ITShare Soluções em Tecnologia</t>
+        </is>
+      </c>
+      <c r="H282" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 19/01/26 || analista de TI pleno || Objetivo: Atuação em projetos estratégicos, com foco em soluções para o setor de Telecomunicações, especialmente em Sistemas de Mediação. Regime: Totalmente Remoto Horário: Comercial  Experiência Necessária Vivência comprovada em projetos de Telecom, especialmente em Sistemas de Mediação. Sólido conhecimento em Linux. Programação em Python e Shell Script em ambientes produtivos. Atuação com integrações entre sistemas complexos e alto volume de dados.  Desejável Experiência em linguagens como CGDC, Java, C e JavaScript. Conhecimento em ferramentas de versionamento (Git) e pipelines de CI/CD. Experiência em metodologias ágeis (Scrum, Kanban). Vivência em ambientes de alta disponibilidade e monitoramento de aplicações. || Empresa .....:  ITShare Soluções em Tecnologia</t>
+        </is>
+      </c>
+      <c r="I282" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" t="inlineStr">
+        <is>
+          <t>19/01/2026</t>
+        </is>
+      </c>
+      <c r="B283" t="inlineStr">
+        <is>
+          <t>82872</t>
+        </is>
+      </c>
+      <c r="C283" t="inlineStr">
+        <is>
+          <t>Analista Desenvolvedor Sênior – PJ – Part-time</t>
+        </is>
+      </c>
+      <c r="D283" t="inlineStr">
+        <is>
+          <t>Sênior</t>
+        </is>
+      </c>
+      <c r="E283" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F283" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 19/01/26</t>
+        </is>
+      </c>
+      <c r="G283" t="inlineStr">
+        <is>
+          <t>Buscamos um dev para o desenvolvimento da plataforma SaaS HPY Assessment. Responsabilidades: backend + frontend, criação de módulos administrativos, área do cliente/fornecedor, questionários dinâmicos, anexos seguros, pontuação automática, dashboards, APIs, MFA, criptografia avançada, logs de auditoria completos e arquitetura multi-tenant com isolamento. Requisitos: domínio em Node.js/NestJS (ou Django/FastAPI/Rails), React/Next.js, PostgreSQL, Docker, S3/MinIO, MFA, hashing seguro, OWASP Top 10, testes e código limpo.  Diferenciais: experiência com SaaS escalável, LGPD/ISO 27001/NIST, workflows e automações. Envio: portfólio + GitHub + arquitetura proposta + pretensão  Diferenciais (fortemente desejáveis) Experiência prévia com SaaS multi-tenant Experiência com plataformas de questionários e workflows  PJ – Part-time (20h/semana) Projeto inicial de 60 a 90 dias (MVP) Possibilidade de extensão e participação em evolução
+Empresa .....:  HPY Consulting</t>
+        </is>
+      </c>
+      <c r="H283" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 19/01/26 || Analista Desenvolvedor Sênior – PJ – Part-time || Buscamos um dev para o desenvolvimento da plataforma SaaS HPY Assessment. Responsabilidades: backend + frontend, criação de módulos administrativos, área do cliente/fornecedor, questionários dinâmicos, anexos seguros, pontuação automática, dashboards, APIs, MFA, criptografia avançada, logs de auditoria completos e arquitetura multi-tenant com isolamento. Requisitos: domínio em Node.js/NestJS (ou Django/FastAPI/Rails), React/Next.js, PostgreSQL, Docker, S3/MinIO, MFA, hashing seguro, OWASP Top 10, testes e código limpo.  Diferenciais: experiência com SaaS escalável, LGPD/ISO 27001/NIST, workflows e automações. Envio: portfólio + GitHub + arquitetura proposta + pretensão  Diferenciais (fortemente desejáveis) Experiência prévia com SaaS multi-tenant Experiência com plataformas de questionários e workflows  PJ – Part-time (20h/semana) Projeto inicial de 60 a 90 dias (MVP) Possibilidade de extensão e participação em evolução || Empresa .....:  HPY Consulting</t>
+        </is>
+      </c>
+      <c r="I283" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" t="inlineStr">
+        <is>
+          <t>19/01/2026</t>
+        </is>
+      </c>
+      <c r="B284" t="inlineStr">
+        <is>
+          <t>82750</t>
+        </is>
+      </c>
+      <c r="C284" t="inlineStr">
+        <is>
+          <t>Cientista de Dados - Sênior</t>
+        </is>
+      </c>
+      <c r="D284" t="inlineStr">
+        <is>
+          <t>Sênior</t>
+        </is>
+      </c>
+      <c r="E284" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F284" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 19/01/26</t>
+        </is>
+      </c>
+      <c r="G284" t="inlineStr">
+        <is>
+          <t>Vaga: Cientista de Dados - Sênior  Requisitos: Formação em ciência da computação, estatística ou área relacionada  Experiência comprovada em ciência de dados: Ter um histórico sólido na área de análise de dados e aprendizado de máquina. Proficiência em linguagens de programação: Saber programar em Python, R, SQL, entre outras. Conhecimento em ferramentas de análise de dados: Familiaridade com ferramentas como TensorFlow, Keras, PyTorch, Spacy, Transformers e outras. Habilidades analíticas e de resolução de problemas: Capacidade de identificar e resolver problemas complexos de dados. Pensamento crítico para explorar padrões e tendencias nos dados. Capacidade de trabalhar em equipe: Trabalho em equipe colaborando com engenheiros de dados, analistas e outros perfis de áreas de atividades fim da organização assim como as administrativas, consultorias e outras tecnoestruturas.  Atuação: Remota
+Empresa .....:  GTCON Tecnologia  Serviços</t>
+        </is>
+      </c>
+      <c r="H284" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 19/01/26 || Cientista de Dados - Sênior || Vaga: Cientista de Dados - Sênior  Requisitos: Formação em ciência da computação, estatística ou área relacionada  Experiência comprovada em ciência de dados: Ter um histórico sólido na área de análise de dados e aprendizado de máquina. Proficiência em linguagens de programação: Saber programar em Python, R, SQL, entre outras. Conhecimento em ferramentas de análise de dados: Familiaridade com ferramentas como TensorFlow, Keras, PyTorch, Spacy, Transformers e outras. Habilidades analíticas e de resolução de problemas: Capacidade de identificar e resolver problemas complexos de dados. Pensamento crítico para explorar padrões e tendencias nos dados. Capacidade de trabalhar em equipe: Trabalho em equipe colaborando com engenheiros de dados, analistas e outros perfis de áreas de atividades fim da organização assim como as administrativas, consultorias e outras tecnoestruturas.  Atuação: Remota || Empresa .....:  GTCON Tecnologia  Serviços</t>
+        </is>
+      </c>
+      <c r="I284" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" t="inlineStr">
+        <is>
+          <t>19/01/2026</t>
+        </is>
+      </c>
+      <c r="B285" t="inlineStr">
+        <is>
+          <t>82033</t>
+        </is>
+      </c>
+      <c r="C285" t="inlineStr">
+        <is>
+          <t>Data Steward (IDMC)</t>
+        </is>
+      </c>
+      <c r="D285" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E285" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F285" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 19/01/26</t>
+        </is>
+      </c>
+      <c r="G285" t="inlineStr">
+        <is>
+          <t>Data Steward (IDMC)  - Experiência mandatória com IDMC (Intelligent Data Management Cloud). - Levantamento das regras com as áreas de negócio e mapeamento dos dados. - Documentação técnica completa da solução, processos na ferramenta, técnica e funcional da solução implementada. - Experiência com gestão de dados corporativos, garantia de qualidade, segurança e conformidade LGPD, governança de dados, curadoria de dados - Conhecimento em bancos de dados e ferramentas de ETL (Extract, Transform, Load). - Especialização em governança de dados, data management ou compliance são valorizados.  Vaga Hibrida (1x na semana no presencial) e CLT Vaga por tempo determinado - 6 meses  Temos: VA ou VR, VT, Assistência Médica Odontológica, Auxílio creche e WellHub.
+Empresa .....:  PSM COM PROFESSIONAL SERVICES MANAGEMENT</t>
+        </is>
+      </c>
+      <c r="H285" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 19/01/26 || Data Steward (IDMC) || Data Steward (IDMC)  - Experiência mandatória com IDMC (Intelligent Data Management Cloud). - Levantamento das regras com as áreas de negócio e mapeamento dos dados. - Documentação técnica completa da solução, processos na ferramenta, técnica e funcional da solução implementada. - Experiência com gestão de dados corporativos, garantia de qualidade, segurança e conformidade LGPD, governança de dados, curadoria de dados - Conhecimento em bancos de dados e ferramentas de ETL (Extract, Transform, Load). - Especialização em governança de dados, data management ou compliance são valorizados.  Vaga Hibrida (1x na semana no presencial) e CLT Vaga por tempo determinado - 6 meses  Temos: VA ou VR, VT, Assistência Médica Odontológica, Auxílio creche e WellHub. || Empresa .....:  PSM COM PROFESSIONAL SERVICES MANAGEMENT</t>
+        </is>
+      </c>
+      <c r="I285" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" t="inlineStr">
+        <is>
+          <t>19/01/2026</t>
+        </is>
+      </c>
+      <c r="B286" t="inlineStr">
+        <is>
+          <t>83046</t>
+        </is>
+      </c>
+      <c r="C286" t="inlineStr">
+        <is>
+          <t>Desenvolvedor Front-End Sênior</t>
+        </is>
+      </c>
+      <c r="D286" t="inlineStr">
+        <is>
+          <t>Sênior</t>
+        </is>
+      </c>
+      <c r="E286" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F286" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 19/01/26</t>
+        </is>
+      </c>
+      <c r="G286" t="inlineStr">
+        <is>
+          <t>A Pentacom IT Solutions, há mais de 20 anos no mercado, busca Desenvolvedor Front-end Sênior:  Requisitos e Conhecimentos Essenciais: - Linguagens: JavaScript (ES6+), TypeScript (Interfaces, Types, Generics) - Core  Frameworks: React.js (ou Vue.js / Angular), Next.js (ou Nuxt.js) - Estilização: CSS-in-JS - Styled-components ou Emotion, Tailwind CSS, Sass/SCSS - Gerenciamento de Estado  API: Context API, TanStack Query (React Query), Axios ou Fetch API, Zod ou Yup - Qualidade  Testes: TDD, React Testing Library - Ferramentas de Build  Documentação: Webpack, Git (CLI), Storybook, Docker (Desejável: básico para rodar ambiente)  Período: Indeterminado Início: Imediato Contratação: CLT Atuação: Home Office  Profissionais interessados, enviar currículo informando disponibilidade para início
+Empresa .....:  Pentacom IT Solutions</t>
+        </is>
+      </c>
+      <c r="H286" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 19/01/26 || Desenvolvedor Front-End Sênior || A Pentacom IT Solutions, há mais de 20 anos no mercado, busca Desenvolvedor Front-end Sênior:  Requisitos e Conhecimentos Essenciais: - Linguagens: JavaScript (ES6+), TypeScript (Interfaces, Types, Generics) - Core  Frameworks: React.js (ou Vue.js / Angular), Next.js (ou Nuxt.js) - Estilização: CSS-in-JS - Styled-components ou Emotion, Tailwind CSS, Sass/SCSS - Gerenciamento de Estado  API: Context API, TanStack Query (React Query), Axios ou Fetch API, Zod ou Yup - Qualidade  Testes: TDD, React Testing Library - Ferramentas de Build  Documentação: Webpack, Git (CLI), Storybook, Docker (Desejável: básico para rodar ambiente)  Período: Indeterminado Início: Imediato Contratação: CLT Atuação: Home Office  Profissionais interessados, enviar currículo informando disponibilidade para início || Empresa .....:  Pentacom IT Solutions</t>
+        </is>
+      </c>
+      <c r="I286" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" t="inlineStr">
+        <is>
+          <t>19/01/2026</t>
+        </is>
+      </c>
+      <c r="B287" t="inlineStr">
+        <is>
+          <t>82059</t>
+        </is>
+      </c>
+      <c r="C287" t="inlineStr">
+        <is>
+          <t>Desenvolvedor Power Builder</t>
+        </is>
+      </c>
+      <c r="D287" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E287" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F287" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 19/01/26</t>
+        </is>
+      </c>
+      <c r="G287" t="inlineStr">
+        <is>
+          <t>Responsabilidades: Desenvolver e manter aplicações corporativas em PowerBuilder, integradas a banco de dados Oracle. Criar e otimizar DataWindows, triggers e procedures. Garantir performance, estabilidade e segurança das aplicações. Participar de revisões de código, planejamentos ágeis e definições técnicas. Documentar soluções, versionar entregas e manter backlog atualizado.  Requisitos: Experiência sólida com PowerBuilder (versão 6.5 ou superior). Domínio de Oracle (consultas, procedures, functions, triggers e views). Vivência com Git/Bitbucket e controle de versões. Experiência em metodologias ágeis (Scrum ou Kanban). Boas práticas de Clean Code e manutenção de código legado.  Modelo de atuação: Híbrido ou Remoto.  Informações adicionais: Cliente fica localizado em São Paulo Se residir até 25km de São Paulo - 4 dias presencial e 1 home-office. Se residir mais de 25km (ou fora da grande São Paulo ou demais localizações) será home-office.
+Empresa .....:  Emphasys It Services</t>
+        </is>
+      </c>
+      <c r="H287" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 19/01/26 || Desenvolvedor Power Builder || Responsabilidades: Desenvolver e manter aplicações corporativas em PowerBuilder, integradas a banco de dados Oracle. Criar e otimizar DataWindows, triggers e procedures. Garantir performance, estabilidade e segurança das aplicações. Participar de revisões de código, planejamentos ágeis e definições técnicas. Documentar soluções, versionar entregas e manter backlog atualizado.  Requisitos: Experiência sólida com PowerBuilder (versão 6.5 ou superior). Domínio de Oracle (consultas, procedures, functions, triggers e views). Vivência com Git/Bitbucket e controle de versões. Experiência em metodologias ágeis (Scrum ou Kanban). Boas práticas de Clean Code e manutenção de código legado.  Modelo de atuação: Híbrido ou Remoto.  Informações adicionais: Cliente fica localizado em São Paulo Se residir até 25km de São Paulo - 4 dias presencial e 1 home-office. Se residir mais de 25km (ou fora da grande São Paulo ou demais localizações) será home-office. || Empresa .....:  Emphasys It Services</t>
+        </is>
+      </c>
+      <c r="I287" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" t="inlineStr">
+        <is>
+          <t>19/01/2026</t>
+        </is>
+      </c>
+      <c r="B288" t="inlineStr">
+        <is>
+          <t>83298</t>
+        </is>
+      </c>
+      <c r="C288" t="inlineStr">
+        <is>
+          <t>Engenheiro de Software Java Backend - Sênior</t>
+        </is>
+      </c>
+      <c r="D288" t="inlineStr">
+        <is>
+          <t>Sênior</t>
+        </is>
+      </c>
+      <c r="E288" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F288" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 19/01/26</t>
+        </is>
+      </c>
+      <c r="G288" t="inlineStr">
+        <is>
+          <t>Engenheiro(a) de Software Java Backend Sênior  Sobre a CBDS Somos uma empresa brasileira focada em Squad as a Service, com mais de 16 anos de experiência. Estamos em busca de um(a) Engenheiro(a) de Software Java Backend Sênior para atuar de forma Totalmente remota.  Responsabilidades Desenvolver aplicações Java de alta performance, arquitetar microserviços com Spring Boot, criar APIs RESTful e atuar como referência técnica no time.  Experiência Obrigatória • 7+ anos em Java (11+) • Spring Boot, Spring MVC, Spring Data, Spring Security • Padrões de Projeto (GoF) e SOLID • Arquitetura de microserviços • APIs RESTful e Swagger • Hibernate/JPA e bancos relacionais • Git, Maven/Gradle • Testes: JUnit, Mockito  Diferenciais Kotlin, DDD, Kafka/RabbitMQ, NoSQL, AWS/GCP/Azure, Docker/Kubernetes, CI/CD, Spring WebFlux.  Formação Graduação em Ciência da Computação ou áreas correlatas.  Contratação: PJ, período integral, longo prazo.
+Empresa .....:  CBDS</t>
+        </is>
+      </c>
+      <c r="H288" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 19/01/26 || Engenheiro de Software Java Backend - Sênior || Engenheiro(a) de Software Java Backend Sênior  Sobre a CBDS Somos uma empresa brasileira focada em Squad as a Service, com mais de 16 anos de experiência. Estamos em busca de um(a) Engenheiro(a) de Software Java Backend Sênior para atuar de forma Totalmente remota.  Responsabilidades Desenvolver aplicações Java de alta performance, arquitetar microserviços com Spring Boot, criar APIs RESTful e atuar como referência técnica no time.  Experiência Obrigatória • 7+ anos em Java (11+) • Spring Boot, Spring MVC, Spring Data, Spring Security • Padrões de Projeto (GoF) e SOLID • Arquitetura de microserviços • APIs RESTful e Swagger • Hibernate/JPA e bancos relacionais • Git, Maven/Gradle • Testes: JUnit, Mockito  Diferenciais Kotlin, DDD, Kafka/RabbitMQ, NoSQL, AWS/GCP/Azure, Docker/Kubernetes, CI/CD, Spring WebFlux.  Formação Graduação em Ciência da Computação ou áreas correlatas.  Contratação: PJ, período integral, longo prazo. || Empresa .....:  CBDS</t>
+        </is>
+      </c>
+      <c r="I288" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" t="inlineStr">
+        <is>
+          <t>19/01/2026</t>
+        </is>
+      </c>
+      <c r="B289" t="inlineStr">
+        <is>
+          <t>81889</t>
+        </is>
+      </c>
+      <c r="C289" t="inlineStr">
+        <is>
+          <t>Especialista em Oracle Integration Cloud</t>
+        </is>
+      </c>
+      <c r="D289" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E289" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F289" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 19/01/26</t>
+        </is>
+      </c>
+      <c r="G289" t="inlineStr">
+        <is>
+          <t>Requisitos: Experiência comprovada e sólida no desenvolvimento de integrações usando Oracle Integration Cloud (OIC). Profundo conhecimento em arquiteturas orientadas a serviços (SOA) e padrões de integração. Habilidade para trabalhar com formatos de dados JSON e XML. Conhecimento e experiência prática com serviços REST e SOAP. Capacidade de resolver problemas e depurar falhas em fluxos de integração rapidamente. Familiaridade com conceitos de segurança em APIs e integrações (OAuth, JWT, certificados SSL).  Contratação PJ Remoto
+Empresa .....:  TO Brasil</t>
+        </is>
+      </c>
+      <c r="H289" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 19/01/26 || Especialista em Oracle Integration Cloud || Requisitos: Experiência comprovada e sólida no desenvolvimento de integrações usando Oracle Integration Cloud (OIC). Profundo conhecimento em arquiteturas orientadas a serviços (SOA) e padrões de integração. Habilidade para trabalhar com formatos de dados JSON e XML. Conhecimento e experiência prática com serviços REST e SOAP. Capacidade de resolver problemas e depurar falhas em fluxos de integração rapidamente. Familiaridade com conceitos de segurança em APIs e integrações (OAuth, JWT, certificados SSL).  Contratação PJ Remoto || Empresa .....:  TO Brasil</t>
+        </is>
+      </c>
+      <c r="I289" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" t="inlineStr">
+        <is>
+          <t>19/01/2026</t>
+        </is>
+      </c>
+      <c r="B290" t="inlineStr">
+        <is>
+          <t>82597</t>
+        </is>
+      </c>
+      <c r="C290" t="inlineStr">
+        <is>
+          <t>Analista de Negócios TI Supply  TOTVS Protheus</t>
+        </is>
+      </c>
+      <c r="D290" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E290" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F290" t="inlineStr">
+        <is>
+          <t>Itatiba - SP - 19/01/26</t>
+        </is>
+      </c>
+      <c r="G290" t="inlineStr">
+        <is>
+          <t>CLT + Bônus anual + Todos os Benefícios para indústria em SP (Local de Trabalho em Itatiba ou SP, zona norte) 4 x presencial e 1 x remoto  Esse Analista de Negócios de TI Sr fará atendimento da área de Supply. Imprescindível expertise em TOTVS Protheus e profundidade com sistemas de Logística.
+Empresa .....:  Umbrella Talent</t>
+        </is>
+      </c>
+      <c r="H290" t="inlineStr">
+        <is>
+          <t>Itatiba - SP - 19/01/26 || Analista de Negócios TI Supply  TOTVS Protheus || CLT + Bônus anual + Todos os Benefícios para indústria em SP (Local de Trabalho em Itatiba ou SP, zona norte) 4 x presencial e 1 x remoto  Esse Analista de Negócios de TI Sr fará atendimento da área de Supply. Imprescindível expertise em TOTVS Protheus e profundidade com sistemas de Logística. || Empresa .....:  Umbrella Talent</t>
+        </is>
+      </c>
+      <c r="I290" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" t="inlineStr">
+        <is>
+          <t>19/01/2026</t>
+        </is>
+      </c>
+      <c r="B291" t="inlineStr">
+        <is>
+          <t>82217</t>
+        </is>
+      </c>
+      <c r="C291" t="inlineStr">
+        <is>
+          <t>Arquiteto de Software (.Net)</t>
+        </is>
+      </c>
+      <c r="D291" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E291" t="inlineStr">
+        <is>
+          <t>Híbrido</t>
+        </is>
+      </c>
+      <c r="F291" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro - RJ - 19/01/26</t>
+        </is>
+      </c>
+      <c r="G291" t="inlineStr">
+        <is>
+          <t>Já pensou em trabalhar como Arquiteto de Software em uma empresa referência no desenvolvimento de projetos de rodovias?  Profissional atuará com a definição da arquitetura de referência e roadmap de evolução. Modelar sistemas com boas práticas (DDD, arquitetura hexagonal, modularização, CQRS quando aplicável). Estabelecer padrões de API (REST/GraphQL), contratos e versionamento. Experiência sólida com C#/.NET (Core/7/8) e SQL Server (otimização e tuning). Vivência prática com containers (Docker/Kubernetes), microserviços e mensageria. Experiência em cloud (Azure/AWS/GCP) com serviços gerenciados. Definição de APIs (REST/GraphQL), autenticação/autorização (OAuth2/OIDC). Conhecimentos em observabilidade (logs estruturados, métricas, tracing distribuído). Experiência com pipelines de CI/CD e Infra as Code.  Contratação: CLT Full + Benefícios Atuação no Modelo Híbrido: 3x na semana presencial Local: Rio de Janeiro
+Empresa .....:  TalentGroup</t>
+        </is>
+      </c>
+      <c r="H291" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro - RJ - 19/01/26 || Arquiteto de Software (.Net) || Já pensou em trabalhar como Arquiteto de Software em uma empresa referência no desenvolvimento de projetos de rodovias?  Profissional atuará com a definição da arquitetura de referência e roadmap de evolução. Modelar sistemas com boas práticas (DDD, arquitetura hexagonal, modularização, CQRS quando aplicável). Estabelecer padrões de API (REST/GraphQL), contratos e versionamento. Experiência sólida com C#/.NET (Core/7/8) e SQL Server (otimização e tuning). Vivência prática com containers (Docker/Kubernetes), microserviços e mensageria. Experiência em cloud (Azure/AWS/GCP) com serviços gerenciados. Definição de APIs (REST/GraphQL), autenticação/autorização (OAuth2/OIDC). Conhecimentos em observabilidade (logs estruturados, métricas, tracing distribuído). Experiência com pipelines de CI/CD e Infra as Code.  Contratação: CLT Full + Benefícios Atuação no Modelo Híbrido: 3x na semana presencial Local: Rio de Janeiro || Empresa .....:  TalentGroup</t>
+        </is>
+      </c>
+      <c r="I291" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" t="inlineStr">
+        <is>
+          <t>19/01/2026</t>
+        </is>
+      </c>
+      <c r="B292" t="inlineStr">
+        <is>
+          <t>81959</t>
+        </is>
+      </c>
+      <c r="C292" t="inlineStr">
+        <is>
+          <t>Assistente de Informática</t>
+        </is>
+      </c>
+      <c r="D292" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E292" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F292" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro - RJ - 19/01/26</t>
+        </is>
+      </c>
+      <c r="G292" t="inlineStr">
+        <is>
+          <t>Oferecemos vaga para profissional  de informática com experiência em atendimento ao cliente. Deve possuir características como proatividade, trabalho em equipe, resiliência, criatividade e comunicação.  Formação: Superior completo nas áreas de informática ou cursando a partir do 5º período. Cursos extra curriculares e experiência do cliente serão um diferencial.  Pedimos experiência de pelo menos 2 anos com as seguintes habilidades técnicas: Experiência em pacote Office (avançado em Excel), Design Gráfico (CorelDraw, Adobe PhotoShop, Canva). ERP, Banco de Dados Oracle, linguagem SQL para consultas e atualizações e APIs.  HTML 5 e JavaScript. Será um diferencial conhecimento em suporte computacional e em Redes Físicas/Lógicas.  Descrição da vaga: Atuação no setor de informática e relacionamento com o associado. Trabalho presencial no Centro do Rio de Janeiro. Segunda a sexta, das 09h às 18h. Regime CLT, plano de saúde, VR e  VT.
+Empresa .....:  Sincor RJ</t>
+        </is>
+      </c>
+      <c r="H292" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro - RJ - 19/01/26 || Assistente de Informática || Oferecemos vaga para profissional  de informática com experiência em atendimento ao cliente. Deve possuir características como proatividade, trabalho em equipe, resiliência, criatividade e comunicação.  Formação: Superior completo nas áreas de informática ou cursando a partir do 5º período. Cursos extra curriculares e experiência do cliente serão um diferencial.  Pedimos experiência de pelo menos 2 anos com as seguintes habilidades técnicas: Experiência em pacote Office (avançado em Excel), Design Gráfico (CorelDraw, Adobe PhotoShop, Canva). ERP, Banco de Dados Oracle, linguagem SQL para consultas e atualizações e APIs.  HTML 5 e JavaScript. Será um diferencial conhecimento em suporte computacional e em Redes Físicas/Lógicas.  Descrição da vaga: Atuação no setor de informática e relacionamento com o associado. Trabalho presencial no Centro do Rio de Janeiro. Segunda a sexta, das 09h às 18h. Regime CLT, plano de saúde, VR e  VT. || Empresa .....:  Sincor RJ</t>
+        </is>
+      </c>
+      <c r="I292" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" t="inlineStr">
+        <is>
+          <t>19/01/2026</t>
+        </is>
+      </c>
+      <c r="B293" t="inlineStr">
+        <is>
+          <t>82031</t>
+        </is>
+      </c>
+      <c r="C293" t="inlineStr">
+        <is>
+          <t>PMO  Pleno</t>
+        </is>
+      </c>
+      <c r="D293" t="inlineStr">
+        <is>
+          <t>Pleno</t>
+        </is>
+      </c>
+      <c r="E293" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F293" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro - RJ - 19/01/26</t>
+        </is>
+      </c>
+      <c r="G293" t="inlineStr">
+        <is>
+          <t>PMO Pleno Botafogo  RJ ( Presencial)  Atuar com: Suporte às equipes responsáveis pelos projetos. Gerenciar a execução das atividades e monitorar o andamento usando KPIs. Fazer relatórios de desempenho e monitorar cronogramas, orçamentos e escopos dos projetos.  Requisitos Background de sistemas SAP Conhecer de ferramentas de ITSM será um **diferencial**
+Empresa .....:  Blend IT Consultoria</t>
+        </is>
+      </c>
+      <c r="H293" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro - RJ - 19/01/26 || PMO  Pleno || PMO Pleno Botafogo  RJ ( Presencial)  Atuar com: Suporte às equipes responsáveis pelos projetos. Gerenciar a execução das atividades e monitorar o andamento usando KPIs. Fazer relatórios de desempenho e monitorar cronogramas, orçamentos e escopos dos projetos.  Requisitos Background de sistemas SAP Conhecer de ferramentas de ITSM será um **diferencial** || Empresa .....:  Blend IT Consultoria</t>
+        </is>
+      </c>
+      <c r="I293" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" t="inlineStr">
+        <is>
+          <t>19/01/2026</t>
+        </is>
+      </c>
+      <c r="B294" t="inlineStr">
+        <is>
+          <t>82777</t>
+        </is>
+      </c>
+      <c r="C294" t="inlineStr">
+        <is>
+          <t>Agile Coach Sênior</t>
+        </is>
+      </c>
+      <c r="D294" t="inlineStr">
+        <is>
+          <t>Sênior</t>
+        </is>
+      </c>
+      <c r="E294" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F294" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 19/01/26</t>
+        </is>
+      </c>
+      <c r="G294" t="inlineStr">
+        <is>
+          <t>Estamos em busca de um(a) AGILE COACH SENIOR para atuar em uma das maiores empresas varejista farmacêutica do Brasil.  O profissional será responsável por difundir a mentalidade ágil na organização, apoiando times na adoção e evolução de frameworks como Scrum, Kanban, Lean e SAFe. Atua conduzindo workshops, treinamentos e cerimônias, além de oferecer coaching para Scrum Masters, Product Owners e equipes. Identifica impedimentos organizacionais, avalia a maturidade ágil dos times e direciona planos de melhoria contínua, autonomia e autogestão. Também apoia iniciativas de transformação ágil em escala, garantindo alinhamento entre áreas.  Requisitos: experiência sólida com métodos ágeis, coaching de equipes, transformação organizacional, gestão de mudanças e excelentes habilidades de comunicação e facilitação.  Diferenciais: certificações como CSM, PSM, KMP, ICP-ACC, SAFe Agilist.
+Empresa .....:  3CON Consultoria e Sistemas S/A</t>
+        </is>
+      </c>
+      <c r="H294" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 19/01/26 || Agile Coach Sênior || Estamos em busca de um(a) AGILE COACH SENIOR para atuar em uma das maiores empresas varejista farmacêutica do Brasil.  O profissional será responsável por difundir a mentalidade ágil na organização, apoiando times na adoção e evolução de frameworks como Scrum, Kanban, Lean e SAFe. Atua conduzindo workshops, treinamentos e cerimônias, além de oferecer coaching para Scrum Masters, Product Owners e equipes. Identifica impedimentos organizacionais, avalia a maturidade ágil dos times e direciona planos de melhoria contínua, autonomia e autogestão. Também apoia iniciativas de transformação ágil em escala, garantindo alinhamento entre áreas.  Requisitos: experiência sólida com métodos ágeis, coaching de equipes, transformação organizacional, gestão de mudanças e excelentes habilidades de comunicação e facilitação.  Diferenciais: certificações como CSM, PSM, KMP, ICP-ACC, SAFe Agilist. || Empresa .....:  3CON Consultoria e Sistemas S/A</t>
+        </is>
+      </c>
+      <c r="I294" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" t="inlineStr">
+        <is>
+          <t>19/01/2026</t>
+        </is>
+      </c>
+      <c r="B295" t="inlineStr">
+        <is>
+          <t>81949</t>
+        </is>
+      </c>
+      <c r="C295" t="inlineStr">
+        <is>
+          <t>Analista Automacao</t>
+        </is>
+      </c>
+      <c r="D295" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E295" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F295" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 19/01/26</t>
+        </is>
+      </c>
+      <c r="G295" t="inlineStr">
+        <is>
+          <t>Descrição da vaga Estamos em busca de um Analista de Automação para integrar o time técnico da NNumbers, atuando na criação, otimização e automação de rotinas de infraestrutura, redes, cloud e processos operacionais. O profissional será responsável por desenvolver scripts, pipelines e integrações que aumentem a eficiência, padronização e segurança dos ambientes da empresa e de nossos clientes corporativos.  Requisitos técnicos Experiência comprovada em automação de infraestrutura e/ou DevOps Conhecimento sólido em Python, PowerShell ou Bash Conhecimento em APIs REST e integração entre sistemas  Vivência em ambientes Windows Server
+Empresa .....:  NNumbers</t>
+        </is>
+      </c>
+      <c r="H295" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 19/01/26 || Analista Automacao || Descrição da vaga Estamos em busca de um Analista de Automação para integrar o time técnico da NNumbers, atuando na criação, otimização e automação de rotinas de infraestrutura, redes, cloud e processos operacionais. O profissional será responsável por desenvolver scripts, pipelines e integrações que aumentem a eficiência, padronização e segurança dos ambientes da empresa e de nossos clientes corporativos.  Requisitos técnicos Experiência comprovada em automação de infraestrutura e/ou DevOps Conhecimento sólido em Python, PowerShell ou Bash Conhecimento em APIs REST e integração entre sistemas  Vivência em ambientes Windows Server || Empresa .....:  NNumbers</t>
+        </is>
+      </c>
+      <c r="I295" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" t="inlineStr">
+        <is>
+          <t>19/01/2026</t>
+        </is>
+      </c>
+      <c r="B296" t="inlineStr">
+        <is>
+          <t>82875</t>
+        </is>
+      </c>
+      <c r="C296" t="inlineStr">
+        <is>
+          <t>ANALISTA DE BI JÚNIOR - HÍBRIDO SÃO PAULO/SP</t>
+        </is>
+      </c>
+      <c r="D296" t="inlineStr">
+        <is>
+          <t>Júnior</t>
+        </is>
+      </c>
+      <c r="E296" t="inlineStr">
+        <is>
+          <t>Híbrido</t>
+        </is>
+      </c>
+      <c r="F296" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 19/01/26</t>
+        </is>
+      </c>
+      <c r="G296" t="inlineStr">
+        <is>
+          <t>ATUAÇÃO HÍBRIDA DE 2X A 3X POR SEMANA NO BAIRRO DO MORUMBI, ZONA SUL DE SÃO PAULO/SP Contratação CLT + Benefícios  Perfil: Os analistas BI precisam ter experiência de pelo menos  02 anos com modelagem de DATA WAREHOUSE, TALEND, SQL .  As atividades serão: Desenvolvimento de arquitetura de dados utilizando a Modelagem de Data Warehouse Realizar integrações de dados utilizando Talend Desenvolvimento de dashboards utilizando a ferramenta Power BI Realizar levantamento de requisitos junto ao Key Users Manutenção de estrutura e implementação de novos processos Documentar os processos desenvolvidos.
+Empresa .....:  KLB Group</t>
+        </is>
+      </c>
+      <c r="H296" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 19/01/26 || ANALISTA DE BI JÚNIOR - HÍBRIDO SÃO PAULO/SP || ATUAÇÃO HÍBRIDA DE 2X A 3X POR SEMANA NO BAIRRO DO MORUMBI, ZONA SUL DE SÃO PAULO/SP Contratação CLT + Benefícios  Perfil: Os analistas BI precisam ter experiência de pelo menos  02 anos com modelagem de DATA WAREHOUSE, TALEND, SQL .  As atividades serão: Desenvolvimento de arquitetura de dados utilizando a Modelagem de Data Warehouse Realizar integrações de dados utilizando Talend Desenvolvimento de dashboards utilizando a ferramenta Power BI Realizar levantamento de requisitos junto ao Key Users Manutenção de estrutura e implementação de novos processos Documentar os processos desenvolvidos. || Empresa .....:  KLB Group</t>
+        </is>
+      </c>
+      <c r="I296" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" t="inlineStr">
+        <is>
+          <t>19/01/2026</t>
+        </is>
+      </c>
+      <c r="B297" t="inlineStr">
+        <is>
+          <t>82780</t>
+        </is>
+      </c>
+      <c r="C297" t="inlineStr">
+        <is>
+          <t>Analista de Negócios - Pl (Presencial)</t>
+        </is>
+      </c>
+      <c r="D297" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E297" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F297" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 19/01/26</t>
+        </is>
+      </c>
+      <c r="G297" t="inlineStr">
+        <is>
+          <t>Oportunidade para Analista de Negócios / Product Owner – Projeto Industrial  Líder global no segmento de carne bovina  Estamos em busca de um(a) profissional com forte perfil analítico e visão de negócio para atuar presencialmente no Morumbi, contribuindo na evolução de produtos e processos industriais dentro de uma operação de grande porte.  Requisitos: Experiência com regras de negócio e especificações funcionais. Vivência em ambientes industriais ou áreas de negócio. Conhecimento em BDD, UML, BPMN e Cucumber. Experiência com metodologias ágeis (Scrum/Kanban). Pacote Office avançado. Familiaridade com práticas DevSecOps.  Diferencial: Conhecimento ou certificação BPM CBOK.
+Empresa .....:  Icon</t>
+        </is>
+      </c>
+      <c r="H297" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 19/01/26 || Analista de Negócios - Pl (Presencial) || Oportunidade para Analista de Negócios / Product Owner – Projeto Industrial  Líder global no segmento de carne bovina  Estamos em busca de um(a) profissional com forte perfil analítico e visão de negócio para atuar presencialmente no Morumbi, contribuindo na evolução de produtos e processos industriais dentro de uma operação de grande porte.  Requisitos: Experiência com regras de negócio e especificações funcionais. Vivência em ambientes industriais ou áreas de negócio. Conhecimento em BDD, UML, BPMN e Cucumber. Experiência com metodologias ágeis (Scrum/Kanban). Pacote Office avançado. Familiaridade com práticas DevSecOps.  Diferencial: Conhecimento ou certificação BPM CBOK. || Empresa .....:  Icon</t>
+        </is>
+      </c>
+      <c r="I297" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" t="inlineStr">
+        <is>
+          <t>19/01/2026</t>
+        </is>
+      </c>
+      <c r="B298" t="inlineStr">
+        <is>
+          <t>82865</t>
+        </is>
+      </c>
+      <c r="C298" t="inlineStr">
+        <is>
+          <t>ANALISTA DE SEGURANÇA DA INFORMAÇÃO PL</t>
+        </is>
+      </c>
+      <c r="D298" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E298" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F298" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 19/01/26</t>
+        </is>
+      </c>
+      <c r="G298" t="inlineStr">
+        <is>
+          <t>Analista de Segurança da Informação Pleno  Requisitos e Qualificações Formação : Graduação completa em Redes, Tecnologia da Informação, Cibersegurança ou áreas correlatas.  Idiomas : Inglês  Habilidades Técnicas Diagnosticar e resolver problemas de segurança nos ambientes dos clientes. Realizar análises de logs e identificar padrões para prevenir incidentes. Atuar com equipes internas para implementar upgrades e novas configurações. Acompanhar SLAs, documentar atendimentos e garantir cumprimento dos padrões. Capacidade de realizar treinamentos e capacitações para clientes e parceiros. Forte habilidade em análise de logs, detecção de vulnerabilidades e automação. Experiência com ferramentas como firewalls, IDS/IPS, DLP e antivírus. Sólido conhecimento em infraestrutura: Windows Server, Linux, gestão de acessos, AD, DHCP, DNS, GPO, NAT, file server, terminal server, SQL Server, virtualização e cloud. Conhecimento intermediário em Microsoft SQL Server.
+Empresa .....:  Mazzatech</t>
+        </is>
+      </c>
+      <c r="H298" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 19/01/26 || ANALISTA DE SEGURANÇA DA INFORMAÇÃO PL || Analista de Segurança da Informação Pleno  Requisitos e Qualificações Formação : Graduação completa em Redes, Tecnologia da Informação, Cibersegurança ou áreas correlatas.  Idiomas : Inglês  Habilidades Técnicas Diagnosticar e resolver problemas de segurança nos ambientes dos clientes. Realizar análises de logs e identificar padrões para prevenir incidentes. Atuar com equipes internas para implementar upgrades e novas configurações. Acompanhar SLAs, documentar atendimentos e garantir cumprimento dos padrões. Capacidade de realizar treinamentos e capacitações para clientes e parceiros. Forte habilidade em análise de logs, detecção de vulnerabilidades e automação. Experiência com ferramentas como firewalls, IDS/IPS, DLP e antivírus. Sólido conhecimento em infraestrutura: Windows Server, Linux, gestão de acessos, AD, DHCP, DNS, GPO, NAT, file server, terminal server, SQL Server, virtualização e cloud. Conhecimento intermediário em Microsoft SQL Server. || Empresa .....:  Mazzatech</t>
+        </is>
+      </c>
+      <c r="I298" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" t="inlineStr">
+        <is>
+          <t>19/01/2026</t>
+        </is>
+      </c>
+      <c r="B299" t="inlineStr">
+        <is>
+          <t>82747</t>
+        </is>
+      </c>
+      <c r="C299" t="inlineStr">
+        <is>
+          <t>Analista de Segurança da Informação Sênior</t>
+        </is>
+      </c>
+      <c r="D299" t="inlineStr">
+        <is>
+          <t>Sênior</t>
+        </is>
+      </c>
+      <c r="E299" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F299" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 19/01/26</t>
+        </is>
+      </c>
+      <c r="G299" t="inlineStr">
+        <is>
+          <t>Requisitos Domínio em gestão de riscos, incidentes e vulnerabilidades. Conhecimento avançado de redes, protocolos, arquitetura e modelos de segurança. Experiência com Azure (Microsoft M365) e AWS em contexto de segurança. Vivência com ferramentas SIEM, EDR/XDR e soluções de proteção de endpoint. Entendimento de LGPD e compliance regulatório aplicável. Experiência com IAM, políticas e controles de acesso.  Responsabilidades Liderar iniciativas de segurança, frameworks de mercado (NIST, CIS, LGPD). Conduzir avaliações de risco, análises de vulnerabilidade e propor planos de mitigação eficazes. Realizar Patch Management no Ambiente afim de mitigar vulnerabilidades. Coordenar investigações e resposta a incidentes de segurança de de ponta a ponta. Desenvolver, revisar e reforçar políticas, padrões e procedimentos de SI. Monitorar eventos e ameaças em ferramentas de SIEM/SOC. Realizar hardening de sistemas, aplicações, redes e ambientes cloud. Gerir identidade e acesso (IAM).
+Empresa .....:  TailorIT</t>
+        </is>
+      </c>
+      <c r="H299" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 19/01/26 || Analista de Segurança da Informação Sênior || Requisitos Domínio em gestão de riscos, incidentes e vulnerabilidades. Conhecimento avançado de redes, protocolos, arquitetura e modelos de segurança. Experiência com Azure (Microsoft M365) e AWS em contexto de segurança. Vivência com ferramentas SIEM, EDR/XDR e soluções de proteção de endpoint. Entendimento de LGPD e compliance regulatório aplicável. Experiência com IAM, políticas e controles de acesso.  Responsabilidades Liderar iniciativas de segurança, frameworks de mercado (NIST, CIS, LGPD). Conduzir avaliações de risco, análises de vulnerabilidade e propor planos de mitigação eficazes. Realizar Patch Management no Ambiente afim de mitigar vulnerabilidades. Coordenar investigações e resposta a incidentes de segurança de de ponta a ponta. Desenvolver, revisar e reforçar políticas, padrões e procedimentos de SI. Monitorar eventos e ameaças em ferramentas de SIEM/SOC. Realizar hardening de sistemas, aplicações, redes e ambientes cloud. Gerir identidade e acesso (IAM). || Empresa .....:  TailorIT</t>
+        </is>
+      </c>
+      <c r="I299" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" t="inlineStr">
+        <is>
+          <t>19/01/2026</t>
+        </is>
+      </c>
+      <c r="B300" t="inlineStr">
+        <is>
+          <t>82822</t>
+        </is>
+      </c>
+      <c r="C300" t="inlineStr">
+        <is>
+          <t>Analista de Sistemas Inteligência Artificial p/ BI</t>
+        </is>
+      </c>
+      <c r="D300" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E300" t="inlineStr">
+        <is>
+          <t>Híbrido</t>
+        </is>
+      </c>
+      <c r="F300" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 19/01/26</t>
+        </is>
+      </c>
+      <c r="G300" t="inlineStr">
+        <is>
+          <t>Requisitos:  Atuar no desenvolvimento e integração de soluções de IA (incluindo IA Generativa) aplicadas à área de dados e Business Intelligence, garantindo governança, escalabilidade e alinhamento às diretrizes corporativas. O profissional será responsável por transformar dados em insights estratégicos, automatizar processos analíticos e potencializar a tomada de decisão com tecnologias avançadas.  Contratação CLT Híbrido 1 vz SP
+Empresa .....:  TO Brasil</t>
+        </is>
+      </c>
+      <c r="H300" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 19/01/26 || Analista de Sistemas Inteligência Artificial p/ BI || Requisitos:  Atuar no desenvolvimento e integração de soluções de IA (incluindo IA Generativa) aplicadas à área de dados e Business Intelligence, garantindo governança, escalabilidade e alinhamento às diretrizes corporativas. O profissional será responsável por transformar dados em insights estratégicos, automatizar processos analíticos e potencializar a tomada de decisão com tecnologias avançadas.  Contratação CLT Híbrido 1 vz SP || Empresa .....:  TO Brasil</t>
+        </is>
+      </c>
+      <c r="I300" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" t="inlineStr">
+        <is>
+          <t>19/01/2026</t>
+        </is>
+      </c>
+      <c r="B301" t="inlineStr">
+        <is>
+          <t>83297</t>
+        </is>
+      </c>
+      <c r="C301" t="inlineStr">
+        <is>
+          <t>Assistente de Infraestrutura - Presencial</t>
+        </is>
+      </c>
+      <c r="D301" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E301" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F301" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 19/01/26</t>
+        </is>
+      </c>
+      <c r="G301" t="inlineStr">
+        <is>
+          <t>Procuramos um(a) Assistente de Infraestrutura para atuar em São Paulo, SP, em um cargo presencial e de tempo integral.  Experiência Técnica: - Linux Server - Básico de Telecom (Switches, Roteadores, Vlan, Link de Dados) - Virtualização (Hyper-V / Vmware) - Ferramentas de backup: Veeam - Ferramentas de monitoramento - Telefonia VOIP - Administração de Storage / servidores Blades - Suporte a sistemas operacionais e redes - Manutenção e Instalação de Softwares, Hardwares e Impressoras e - Atendimento Field, Microinformática, infraestrutura básica, gestão de chamados.  Local: Avenida Paulista – SP ( e duas vezes por mês em Alphaville ) Modelo: Totalmente Presencial  Somente Candidatos com Pretensão Salarial CLT serão avaliados.
+Empresa .....:  Endereco Fiscal LTDA</t>
+        </is>
+      </c>
+      <c r="H301" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 19/01/26 || Assistente de Infraestrutura - Presencial || Procuramos um(a) Assistente de Infraestrutura para atuar em São Paulo, SP, em um cargo presencial e de tempo integral.  Experiência Técnica: - Linux Server - Básico de Telecom (Switches, Roteadores, Vlan, Link de Dados) - Virtualização (Hyper-V / Vmware) - Ferramentas de backup: Veeam - Ferramentas de monitoramento - Telefonia VOIP - Administração de Storage / servidores Blades - Suporte a sistemas operacionais e redes - Manutenção e Instalação de Softwares, Hardwares e Impressoras e - Atendimento Field, Microinformática, infraestrutura básica, gestão de chamados.  Local: Avenida Paulista – SP ( e duas vezes por mês em Alphaville ) Modelo: Totalmente Presencial  Somente Candidatos com Pretensão Salarial CLT serão avaliados. || Empresa .....:  Endereco Fiscal LTDA</t>
+        </is>
+      </c>
+      <c r="I301" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>19/01/2026</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>82972</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>Desenvolvedor .NET Core Sr</t>
+        </is>
+      </c>
+      <c r="D302" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E302" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F302" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 19/01/26</t>
+        </is>
+      </c>
+      <c r="G302" t="inlineStr">
+        <is>
+          <t>Somos uma empresa de tecnologia em rápido crescimento, atuando no segmento de soluções corporativas para o setor financeiro.  Responsabilidades Desenvolver e aprimorar serviços em .NET 8 e C#. Projetar e otimizar bancos de dados SQL Server e Azure SQL Participar de revisões de código, testes unitários e integração contínua Colaborar com equipes multifuncionais em metodologias ágeis Documentar soluções e manter boas práticas de desenvolvimento  Requisitos e qualificações Graduação em Ciência da Computação, Engenharia de Software ou áreas afins Experiência com desenvolvimento em .NET Core Domínio de C# e arquitetura de microserviços Experiência comprovada com SQL Server e modelagem de dados Conhecimento em Microsoft Visual Studio e GitHub/ Github actions. Facilidade em propor soluções técnicas e não apenas executá-las.  4x presencial e 1x remoto na semana, modelo CLT
+Empresa .....:  GlobalTI</t>
+        </is>
+      </c>
+      <c r="H302" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 19/01/26 || Desenvolvedor .NET Core Sr || Somos uma empresa de tecnologia em rápido crescimento, atuando no segmento de soluções corporativas para o setor financeiro.  Responsabilidades Desenvolver e aprimorar serviços em .NET 8 e C#. Projetar e otimizar bancos de dados SQL Server e Azure SQL Participar de revisões de código, testes unitários e integração contínua Colaborar com equipes multifuncionais em metodologias ágeis Documentar soluções e manter boas práticas de desenvolvimento  Requisitos e qualificações Graduação em Ciência da Computação, Engenharia de Software ou áreas afins Experiência com desenvolvimento em .NET Core Domínio de C# e arquitetura de microserviços Experiência comprovada com SQL Server e modelagem de dados Conhecimento em Microsoft Visual Studio e GitHub/ Github actions. Facilidade em propor soluções técnicas e não apenas executá-las.  4x presencial e 1x remoto na semana, modelo CLT || Empresa .....:  GlobalTI</t>
+        </is>
+      </c>
+      <c r="I302" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>19/01/2026</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>81764</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>DESENVOLVEDOR JAVA - INGLÊS - HÍBRIDO SP</t>
+        </is>
+      </c>
+      <c r="D303" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E303" t="inlineStr">
+        <is>
+          <t>Híbrido</t>
+        </is>
+      </c>
+      <c r="F303" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 19/01/26</t>
+        </is>
+      </c>
+      <c r="G303" t="inlineStr">
+        <is>
+          <t>ATUAÇÃO HÍBRIDA 3X POR SEMANA NO BAIRRO DO MORUMBI, ZONA SUL DE SÃO PAULO/SP Contratação CLT + Benefícios  Horário de Trabalho: Das 09hs às 18hs  Requisitos: - Superior completo na área de tecnologia - INGLÊS AVANÇADO (MANDATÓRIO, INTERAÇÃO COM TIME GLOBAL) - Experiência em Java versão 21 - Experiência prática em desenvolvimento de aplicações Java, incluindo conhecimento em frameworks como Spring boot, Hibernate - Experiência em banco de dados SQL, MongoDB - Experiência na criação e consumo de APIs RESTful, garantindo a comunicação eficiente entre o front-end e o back-end. - Vivência com Git para controle de versão e colaboração em projetos de desenvolvimento. - Experiência em testes automatizados, utilizando frameworks como JUnit ou Mockito, para garantir a qualidade do código.  Escopo: será detalhado em entrevista técnica
+Empresa .....:  KLB Group</t>
+        </is>
+      </c>
+      <c r="H303" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 19/01/26 || DESENVOLVEDOR JAVA - INGLÊS - HÍBRIDO SP || ATUAÇÃO HÍBRIDA 3X POR SEMANA NO BAIRRO DO MORUMBI, ZONA SUL DE SÃO PAULO/SP Contratação CLT + Benefícios  Horário de Trabalho: Das 09hs às 18hs  Requisitos: - Superior completo na área de tecnologia - INGLÊS AVANÇADO (MANDATÓRIO, INTERAÇÃO COM TIME GLOBAL) - Experiência em Java versão 21 - Experiência prática em desenvolvimento de aplicações Java, incluindo conhecimento em frameworks como Spring boot, Hibernate - Experiência em banco de dados SQL, MongoDB - Experiência na criação e consumo de APIs RESTful, garantindo a comunicação eficiente entre o front-end e o back-end. - Vivência com Git para controle de versão e colaboração em projetos de desenvolvimento. - Experiência em testes automatizados, utilizando frameworks como JUnit ou Mockito, para garantir a qualidade do código.  Escopo: será detalhado em entrevista técnica || Empresa .....:  KLB Group</t>
+        </is>
+      </c>
+      <c r="I303" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>19/01/2026</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>81731</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>Desenvolvedor Python Senior - IA</t>
+        </is>
+      </c>
+      <c r="D304" t="inlineStr">
+        <is>
+          <t>Sênior</t>
+        </is>
+      </c>
+      <c r="E304" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F304" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 19/01/26</t>
+        </is>
+      </c>
+      <c r="G304" t="inlineStr">
+        <is>
+          <t>Atividades: Desenvolver e manter chatbots inteligentes integrados a WhatsApp Projetar, treinar e otimizar modelos de NLP e LLMs Integrar soluções de IA com APIs externas, CRMs e bancos de dados. Implementar arquiteturas como RAG Garantir a escalabilidade, segurança e performance das soluções de IA.  Requisitos: Python Experiência prática com frameworks de IA (LangChain, LangFuse, CrewAI ou similares). Conhecimento em NLP, embeddings e bancos de dados vetoriais. Experiência em consumo e desenvolvimento de APIs RESTful (FastAPI, Flask, etc.). Experiência com chatbots (WhatsApp Cloud API, Z-API, Gupshup, Twilio). Git, testes automatizados, CI/CD, versionamento de código. Bancos de dados relacionais e não relacionais.  Contrato: PJ ou CLT Local de trabalho: Tatuapé, SP (Presencial)
+Empresa .....:  Grupo Qualiconsig</t>
+        </is>
+      </c>
+      <c r="H304" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 19/01/26 || Desenvolvedor Python Senior - IA || Atividades: Desenvolver e manter chatbots inteligentes integrados a WhatsApp Projetar, treinar e otimizar modelos de NLP e LLMs Integrar soluções de IA com APIs externas, CRMs e bancos de dados. Implementar arquiteturas como RAG Garantir a escalabilidade, segurança e performance das soluções de IA.  Requisitos: Python Experiência prática com frameworks de IA (LangChain, LangFuse, CrewAI ou similares). Conhecimento em NLP, embeddings e bancos de dados vetoriais. Experiência em consumo e desenvolvimento de APIs RESTful (FastAPI, Flask, etc.). Experiência com chatbots (WhatsApp Cloud API, Z-API, Gupshup, Twilio). Git, testes automatizados, CI/CD, versionamento de código. Bancos de dados relacionais e não relacionais.  Contrato: PJ ou CLT Local de trabalho: Tatuapé, SP (Presencial) || Empresa .....:  Grupo Qualiconsig</t>
+        </is>
+      </c>
+      <c r="I304" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>19/01/2026</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>81737</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>Desenvolvedor Web Sr - (Prazo determinado)</t>
+        </is>
+      </c>
+      <c r="D305" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E305" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F305" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 19/01/26</t>
+        </is>
+      </c>
+      <c r="G305" t="inlineStr">
+        <is>
+          <t>Estamos procurando um profissional de TI experiente e motivado para se juntar à nossa equipe como Desenvolvedor Web Se você é um especialista em CMS (Drupal, Wordpress e/ou Plone) e está procurando por um desafio que combine desenvolvimento, inovação e tecnologia, essa é a oportunidade certa para você. Atuará no desenvolvimento de novas funcionalidades, integração com sistemas legados, otimização de fluxos de trabalho e suporte técnico avançado.
+Empresa .....:  FUNDASP</t>
+        </is>
+      </c>
+      <c r="H305" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 19/01/26 || Desenvolvedor Web Sr - (Prazo determinado) || Estamos procurando um profissional de TI experiente e motivado para se juntar à nossa equipe como Desenvolvedor Web Se você é um especialista em CMS (Drupal, Wordpress e/ou Plone) e está procurando por um desafio que combine desenvolvimento, inovação e tecnologia, essa é a oportunidade certa para você. Atuará no desenvolvimento de novas funcionalidades, integração com sistemas legados, otimização de fluxos de trabalho e suporte técnico avançado. || Empresa .....:  FUNDASP</t>
+        </is>
+      </c>
+      <c r="I305" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>19/01/2026</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>82146</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>Segurança Cibernética Sr - Presencial SP</t>
+        </is>
+      </c>
+      <c r="D306" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E306" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F306" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 19/01/26</t>
+        </is>
+      </c>
+      <c r="G306" t="inlineStr">
+        <is>
+          <t>Analista de Segurança Cibernética Sênior PRESENCIAL EM SP ( Não negociável) Bairro: Bela Vista - SP Efetivo CLT + Benefícios  Trata-se de uma oportunidade Efetiva, contratação CLT direta do meu cliente  Experiência sólida em modelagem de ameaças e análise de riscos em sistemas complexos Capacidade de entender fluxos de negócio, jornadas de usuário, integrações e perfis de acesso Conhecimento em revisão de código seguro nas linguagens: Python, JavaScript, C#, Java Experiência em análise de segurança de APIs REST e GraphQL Domínio de ferramentas de segurança: SAST, DAST, SCA Vivência com aplicações legadas e modernas Conhecimento em DevOps e integração de segurança nas esteiras: Jenkins, GitLab CI/CD, Azure DevOps, Docker, Kubernetes, Terraform  Familiaridade com frameworks e guias de segurança: OWASP SAMM/ASVS/MASVS, NIST SSDF, CIS Benchmarks, STRIDE, PASTA, MITRE ATTCK (para modelagem de ameaças).
+Empresa .....:  k2 partnering Solutions</t>
+        </is>
+      </c>
+      <c r="H306" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 19/01/26 || Segurança Cibernética Sr - Presencial SP || Analista de Segurança Cibernética Sênior PRESENCIAL EM SP ( Não negociável) Bairro: Bela Vista - SP Efetivo CLT + Benefícios  Trata-se de uma oportunidade Efetiva, contratação CLT direta do meu cliente  Experiência sólida em modelagem de ameaças e análise de riscos em sistemas complexos Capacidade de entender fluxos de negócio, jornadas de usuário, integrações e perfis de acesso Conhecimento em revisão de código seguro nas linguagens: Python, JavaScript, C#, Java Experiência em análise de segurança de APIs REST e GraphQL Domínio de ferramentas de segurança: SAST, DAST, SCA Vivência com aplicações legadas e modernas Conhecimento em DevOps e integração de segurança nas esteiras: Jenkins, GitLab CI/CD, Azure DevOps, Docker, Kubernetes, Terraform  Familiaridade com frameworks e guias de segurança: OWASP SAMM/ASVS/MASVS, NIST SSDF, CIS Benchmarks, STRIDE, PASTA, MITRE ATTCK (para modelagem de ameaças). || Empresa .....:  k2 partnering Solutions</t>
+        </is>
+      </c>
+      <c r="I306" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>19/01/2026</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>82969</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>Técnico de Bancada</t>
+        </is>
+      </c>
+      <c r="D307" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E307" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F307" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 19/01/26</t>
+        </is>
+      </c>
+      <c r="G307" t="inlineStr">
+        <is>
+          <t>Buscamos um Técnico de Bancada organizado, analítico e comprometido com a qualidade técnica para atuar no diagnóstico, manutenção e reparo de equipamentos em bancada. Esse profissional será essencial para garantir o pleno funcionamento dos dispositivos, seguindo padrões técnicos, prazos e boas práticas.  Responsabilidades: Realizar diagnóstico técnico executar manutenções preventivas e corretivas identificar falhas e realizar reparos com precisão testar equipamentos após manutenção registrar ordens de serviço e laudos manter a organização da bancada, ferramentas e ambiente apoiar o time técnico quando necessário Utilizar sistema Salesforce.  Benefícios: VR de R$ 32,50/dia VT creditado em conta Convênio médico e odontológico (após período de experiência) Pix de aniversário Convênio com o SESC  * Presencial (não trabalhamos com home office) * Jornada: 44 horas semanais
+Empresa .....:  Dunker It</t>
+        </is>
+      </c>
+      <c r="H307" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 19/01/26 || Técnico de Bancada || Buscamos um Técnico de Bancada organizado, analítico e comprometido com a qualidade técnica para atuar no diagnóstico, manutenção e reparo de equipamentos em bancada. Esse profissional será essencial para garantir o pleno funcionamento dos dispositivos, seguindo padrões técnicos, prazos e boas práticas.  Responsabilidades: Realizar diagnóstico técnico executar manutenções preventivas e corretivas identificar falhas e realizar reparos com precisão testar equipamentos após manutenção registrar ordens de serviço e laudos manter a organização da bancada, ferramentas e ambiente apoiar o time técnico quando necessário Utilizar sistema Salesforce.  Benefícios: VR de R$ 32,50/dia VT creditado em conta Convênio médico e odontológico (após período de experiência) Pix de aniversário Convênio com o SESC  * Presencial (não trabalhamos com home office) * Jornada: 44 horas semanais || Empresa .....:  Dunker It</t>
+        </is>
+      </c>
+      <c r="I307" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>19/01/2026</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>82928</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>Desenvolvedor .Net Pleno</t>
+        </is>
+      </c>
+      <c r="D308" t="inlineStr">
+        <is>
+          <t>Pleno</t>
+        </is>
+      </c>
+      <c r="E308" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F308" t="inlineStr">
+        <is>
+          <t>Belo Horizonte - MG - 17/01/26</t>
+        </is>
+      </c>
+      <c r="G308" t="inlineStr">
+        <is>
+          <t>Desenvolvedor(a) .NET Pleno – Sustentação e Melhorias  Estamos em busca de uma Desenvolvedor(a) .NET Pleno para atuar em sustentação e evolução de sistemas de um cliente, realizando melhorias contínuas, correções e implementações em aplicações desktop, web e mobile. A atuação será em um ambiente ágil, com foco em qualidade, estabilidade e evolução técnica das soluções existentes.  Principais responsabilidades •	Atuar na sustentação de sistemas, realizando correções e melhorias •	Desenvolver e evoluir aplicações desktop, web e mobile •	Trabalhar com C# e .NET no desenvolvimento de soluções •	Desenvolver interfaces utilizando WPF •	Criar, otimizar e manter consultas e rotinas em SQL •	Atuar em conjunto com o time para análise de demandas e propostas de melhoria •	Utilizar GitHub para versionamento e controle de código •	Participar de cerimônias ágeis e colaborar com boas práticas de desenvolvimento.
+Empresa .....:  Plus It</t>
+        </is>
+      </c>
+      <c r="H308" t="inlineStr">
+        <is>
+          <t>Belo Horizonte - MG - 17/01/26 || Desenvolvedor .Net Pleno || Desenvolvedor(a) .NET Pleno – Sustentação e Melhorias  Estamos em busca de uma Desenvolvedor(a) .NET Pleno para atuar em sustentação e evolução de sistemas de um cliente, realizando melhorias contínuas, correções e implementações em aplicações desktop, web e mobile. A atuação será em um ambiente ágil, com foco em qualidade, estabilidade e evolução técnica das soluções existentes.  Principais responsabilidades •	Atuar na sustentação de sistemas, realizando correções e melhorias •	Desenvolver e evoluir aplicações desktop, web e mobile •	Trabalhar com C# e .NET no desenvolvimento de soluções •	Desenvolver interfaces utilizando WPF •	Criar, otimizar e manter consultas e rotinas em SQL •	Atuar em conjunto com o time para análise de demandas e propostas de melhoria •	Utilizar GitHub para versionamento e controle de código •	Participar de cerimônias ágeis e colaborar com boas práticas de desenvolvimento. || Empresa .....:  Plus It</t>
+        </is>
+      </c>
+      <c r="I308" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>19/01/2026</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>83290</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>Head de Produto  Tecnologia</t>
+        </is>
+      </c>
+      <c r="D309" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E309" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F309" t="inlineStr">
+        <is>
+          <t>Blumenau - SC - 17/01/26</t>
+        </is>
+      </c>
+      <c r="G309" t="inlineStr">
+        <is>
+          <t>O que você irá fazer - Conduzir a estratégia e evolução de produtos digitais com aplicação de IA - Atuar de forma próxima ao cliente, entendendo profundamente a sua jornada - Identificar oportunidades de automação, OCR e redução de esforço operacional - Liderar a priorização do backlog, garantindo foco em valor e impacto - Coordenar o desenvolvimento dos produtos junto ao time técnico - Desenvolver e estruturar o time, identificando gaps e fortalecendo a cultura de produto - Conduzir rituais ágeis, incluindo dailys, alinhamentos estratégicos e acompanhamento de KPIs - Levar insights de mercado, tendências e diferenciais competitivos para o roadmap - Garantir que as soluções entreguem segurança jurídica, confiabilidade e escalabilidade.  Requisitos - Especialização em Gestão de Projetos ou áreas afins. - Experiência sólida em produto digital B2B, preferencialmente em ambientes SaaS ou ERP. - Vivência em escrita, especificação de requisitos e organização do backlog.
+Empresa .....:  KeepTalent</t>
+        </is>
+      </c>
+      <c r="H309" t="inlineStr">
+        <is>
+          <t>Blumenau - SC - 17/01/26 || Head de Produto  Tecnologia || O que você irá fazer - Conduzir a estratégia e evolução de produtos digitais com aplicação de IA - Atuar de forma próxima ao cliente, entendendo profundamente a sua jornada - Identificar oportunidades de automação, OCR e redução de esforço operacional - Liderar a priorização do backlog, garantindo foco em valor e impacto - Coordenar o desenvolvimento dos produtos junto ao time técnico - Desenvolver e estruturar o time, identificando gaps e fortalecendo a cultura de produto - Conduzir rituais ágeis, incluindo dailys, alinhamentos estratégicos e acompanhamento de KPIs - Levar insights de mercado, tendências e diferenciais competitivos para o roadmap - Garantir que as soluções entreguem segurança jurídica, confiabilidade e escalabilidade.  Requisitos - Especialização em Gestão de Projetos ou áreas afins. - Experiência sólida em produto digital B2B, preferencialmente em ambientes SaaS ou ERP. - Vivência em escrita, especificação de requisitos e organização do backlog. || Empresa .....:  KeepTalent</t>
+        </is>
+      </c>
+      <c r="I309" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>19/01/2026</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>83295</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>ANALISTA DE DADOS</t>
+        </is>
+      </c>
+      <c r="D310" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E310" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F310" t="inlineStr">
+        <is>
+          <t>Campinas - SP - 17/01/26</t>
+        </is>
+      </c>
+      <c r="G310" t="inlineStr">
+        <is>
+          <t>Atividades: Cadastro e atta de dados técnicos de veículos projeção da frota circulante no BR análise de perda total e estudos de frota apoio ao time de Mkt com dados técnicos geração de relatórios de vendas e frota análises automotivas internas e externas análise de performance de produtos desenvolvimento de dashboards no Power BI identificação de padrões e oportunidades transformação de dados em insights de negócio apoio na definição de KPIs melhoria e automação de processos de dados.  Requisitos Técnicos: Superior completo ou cursando Power BI avançado Excel com Power Query SQL básico/intermediário noções de Python ou R (diferencial) interpretação de dados com foco em IA supervisionada. Desejável certificações em BI, SQL ou análise de dados.  Condições: Seg–Sex, 8h30 às 17h30, modelo híbrido (2x home office) Local: Vila Industrial – Campinas/SP  Faixa salarial: R$ 6.500 a R$ 7.000 (PJ)  Benefícios: Plano de saúde (reembolso), VT, Wellhub, ass psicológica, etc
+Empresa .....:  SOMNIS CONSULTING</t>
+        </is>
+      </c>
+      <c r="H310" t="inlineStr">
+        <is>
+          <t>Campinas - SP - 17/01/26 || ANALISTA DE DADOS || Atividades: Cadastro e atta de dados técnicos de veículos projeção da frota circulante no BR análise de perda total e estudos de frota apoio ao time de Mkt com dados técnicos geração de relatórios de vendas e frota análises automotivas internas e externas análise de performance de produtos desenvolvimento de dashboards no Power BI identificação de padrões e oportunidades transformação de dados em insights de negócio apoio na definição de KPIs melhoria e automação de processos de dados.  Requisitos Técnicos: Superior completo ou cursando Power BI avançado Excel com Power Query SQL básico/intermediário noções de Python ou R (diferencial) interpretação de dados com foco em IA supervisionada. Desejável certificações em BI, SQL ou análise de dados.  Condições: Seg–Sex, 8h30 às 17h30, modelo híbrido (2x home office) Local: Vila Industrial – Campinas/SP  Faixa salarial: R$ 6.500 a R$ 7.000 (PJ)  Benefícios: Plano de saúde (reembolso), VT, Wellhub, ass psicológica, etc || Empresa .....:  SOMNIS CONSULTING</t>
+        </is>
+      </c>
+      <c r="I310" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>19/01/2026</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>83294</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>DESENVOLVEDOR</t>
+        </is>
+      </c>
+      <c r="D311" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E311" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F311" t="inlineStr">
+        <is>
+          <t>Campinas - SP - 17/01/26</t>
+        </is>
+      </c>
+      <c r="G311" t="inlineStr">
+        <is>
+          <t>Atividades: Desenvolvimento e manutenção de APIs REST e GraphQL participação em decisões arquiteturais modelagem e uso de bancos SQL e NoSQL atuação em ambientes containerizados com Kubernetes integração de sistemas via mensageria code reviews refatorações e melhorias técnicas colaboração com times de Produto, Arquitetura e DevOps apoio técnico ao time.  Requisitos: C#/.NET, APIs REST e GraphQL, padrões de projeto (Factory, Strategy, Repository, Builder), Clean Architecture e SOLID, bancos SQL (PostgreSQL, SQL Server, MySQL) e NoSQL (MongoDB, Redis, DynamoDB), Git, CI/CD e experiência em produção.  Requisitos Comportamentais: Proatividade, aprendizado contínuo, boa comunicação, organização, responsabilidade e foco em qualidade.  Condições: Seg–Sex, 8h30 às 17h30, modelo híbrido (2x home office). Local: Vila Industrial – Campinas/SP. Salário: R$11.000 - R$13.000 (PJ)  Benefícios: Plano de saúde (reembolso), seguro de vida, VT, Wellhub, assistência psicológica.
+Empresa .....:  SOMNIS CONSULTING</t>
+        </is>
+      </c>
+      <c r="H311" t="inlineStr">
+        <is>
+          <t>Campinas - SP - 17/01/26 || DESENVOLVEDOR || Atividades: Desenvolvimento e manutenção de APIs REST e GraphQL participação em decisões arquiteturais modelagem e uso de bancos SQL e NoSQL atuação em ambientes containerizados com Kubernetes integração de sistemas via mensageria code reviews refatorações e melhorias técnicas colaboração com times de Produto, Arquitetura e DevOps apoio técnico ao time.  Requisitos: C#/.NET, APIs REST e GraphQL, padrões de projeto (Factory, Strategy, Repository, Builder), Clean Architecture e SOLID, bancos SQL (PostgreSQL, SQL Server, MySQL) e NoSQL (MongoDB, Redis, DynamoDB), Git, CI/CD e experiência em produção.  Requisitos Comportamentais: Proatividade, aprendizado contínuo, boa comunicação, organização, responsabilidade e foco em qualidade.  Condições: Seg–Sex, 8h30 às 17h30, modelo híbrido (2x home office). Local: Vila Industrial – Campinas/SP. Salário: R$11.000 - R$13.000 (PJ)  Benefícios: Plano de saúde (reembolso), seguro de vida, VT, Wellhub, assistência psicológica. || Empresa .....:  SOMNIS CONSULTING</t>
+        </is>
+      </c>
+      <c r="I311" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>19/01/2026</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>82645</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>Analista de Requisitos Pleno</t>
+        </is>
+      </c>
+      <c r="D312" t="inlineStr">
+        <is>
+          <t>Pleno</t>
+        </is>
+      </c>
+      <c r="E312" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F312" t="inlineStr">
+        <is>
+          <t>Curitiba - PR - 17/01/26</t>
+        </is>
+      </c>
+      <c r="G312" t="inlineStr">
+        <is>
+          <t>Oportunidade: Analista de Requisitos Pleno  Modelo: Presencial Flexível em Curitiba/PR Contratação: PJ + TotalPass + Alura Horário: Comercial  Dia a Dia: • Levantar e detalhar requisitos funcionais e não funcionais com as áreas de negócio • Mapear processos, propor melhorias e apoiar o desenvolvimento de soluções em ERP/CRM • Elaborar user stories, casos de uso, documentos funcionais e fluxogramas • Garantir rastreabilidade dos requisitos e apoiar a validação/homologação do software • Facilitar a comunicação entre equipes técnicas e de negócio  Requisitos • Experiência como Analista de Requisitos (+2 anos) • Imprescindível ter trabalhado em projetos de ERP • Domínio em levantamento e análise de requisitos • Vivência em Scrum/Kanban • Experiência com BPMN ou UML • Experiência com ClickUp, Jira ou Azure DevOps  Você vai se destacar se tiver: • SQL/PLSQL e análise de dados • Certificações (IREB, CPRE, BABOK ou Product Owner) • Ensino superior completo em TI
+Empresa .....:  Code Group</t>
+        </is>
+      </c>
+      <c r="H312" t="inlineStr">
+        <is>
+          <t>Curitiba - PR - 17/01/26 || Analista de Requisitos Pleno || Oportunidade: Analista de Requisitos Pleno  Modelo: Presencial Flexível em Curitiba/PR Contratação: PJ + TotalPass + Alura Horário: Comercial  Dia a Dia: • Levantar e detalhar requisitos funcionais e não funcionais com as áreas de negócio • Mapear processos, propor melhorias e apoiar o desenvolvimento de soluções em ERP/CRM • Elaborar user stories, casos de uso, documentos funcionais e fluxogramas • Garantir rastreabilidade dos requisitos e apoiar a validação/homologação do software • Facilitar a comunicação entre equipes técnicas e de negócio  Requisitos • Experiência como Analista de Requisitos (+2 anos) • Imprescindível ter trabalhado em projetos de ERP • Domínio em levantamento e análise de requisitos • Vivência em Scrum/Kanban • Experiência com BPMN ou UML • Experiência com ClickUp, Jira ou Azure DevOps  Você vai se destacar se tiver: • SQL/PLSQL e análise de dados • Certificações (IREB, CPRE, BABOK ou Product Owner) • Ensino superior completo em TI || Empresa .....:  Code Group</t>
+        </is>
+      </c>
+      <c r="I312" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>19/01/2026</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>81895</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>Desenvolvedor Backend Sr - Curitiba</t>
+        </is>
+      </c>
+      <c r="D313" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E313" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F313" t="inlineStr">
+        <is>
+          <t>Curitiba - PR - 17/01/26</t>
+        </is>
+      </c>
+      <c r="G313" t="inlineStr">
+        <is>
+          <t>Requisitos: Experiência prática com C# e .NET (Core/7/8) em projetos de médio e grande porte Experiência comprovada no desenvolvimento de APIs REST com ASP.NET Core Vivência em arquitetura de software aplicando DDD, SOLID, Clean Architecture e design patterns Atuação com Entity Framework Core e Postgree, incluindo modelagem de dados e performance tuning Experiência com testes automatizados (unitários e integrados) Conhecimento em Docker e integração de pipelines de CI/CD (Azure DevOps, GitHub Actions ou similares) Integração com mensageria (RabbitMQ, Kafka) e serviços externos Vivência em metodologias ágeis (Scrum/Kanban) Experiencia em Microsserviços Noções de front-end (react/Angular) para integração fullstack.
+Empresa .....:  Entrust It</t>
+        </is>
+      </c>
+      <c r="H313" t="inlineStr">
+        <is>
+          <t>Curitiba - PR - 17/01/26 || Desenvolvedor Backend Sr - Curitiba || Requisitos: Experiência prática com C# e .NET (Core/7/8) em projetos de médio e grande porte Experiência comprovada no desenvolvimento de APIs REST com ASP.NET Core Vivência em arquitetura de software aplicando DDD, SOLID, Clean Architecture e design patterns Atuação com Entity Framework Core e Postgree, incluindo modelagem de dados e performance tuning Experiência com testes automatizados (unitários e integrados) Conhecimento em Docker e integração de pipelines de CI/CD (Azure DevOps, GitHub Actions ou similares) Integração com mensageria (RabbitMQ, Kafka) e serviços externos Vivência em metodologias ágeis (Scrum/Kanban) Experiencia em Microsserviços Noções de front-end (react/Angular) para integração fullstack. || Empresa .....:  Entrust It</t>
+        </is>
+      </c>
+      <c r="I313" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>19/01/2026</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>82370</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>Desenvolvedor(a) .NET Pleno</t>
+        </is>
+      </c>
+      <c r="D314" t="inlineStr">
+        <is>
+          <t>Pleno</t>
+        </is>
+      </c>
+      <c r="E314" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F314" t="inlineStr">
+        <is>
+          <t>Curitiba - PR - 17/01/26</t>
+        </is>
+      </c>
+      <c r="G314" t="inlineStr">
+        <is>
+          <t>Buscamos profissional para atuar no desenvolvimento e manutenção de aplicações e serviços em C# / .NET Core e .NET Framework, colaborando com arquitetos e analistas de negócio. Necessário mínimo de 3 anos de experiência, sólidos conhecimentos em POO, SOLID, SQL (SQL Server, PostgreSQL, Oracle ou MySQL), APIs REST e SOAP, Entity Framework, GIT e metodologias ágeis (Scrum/Kanban).  Modelo: Híbrido – 3x remoto e 2x presencial Local: Curitiba – PR Contratação: CLT Horário: Segunda a sexta, horário comercial  Benefícios: Alimentação R$970,00 + Plano de saúde e odontológico + PLR + VT Diferenciais: Docker, DDD, AWS, DevOps, CI/CD, segurança de software, React, Angular, Flutter Vaga também disponível para PcD.
+Empresa .....:  Code Group</t>
+        </is>
+      </c>
+      <c r="H314" t="inlineStr">
+        <is>
+          <t>Curitiba - PR - 17/01/26 || Desenvolvedor(a) .NET Pleno || Buscamos profissional para atuar no desenvolvimento e manutenção de aplicações e serviços em C# / .NET Core e .NET Framework, colaborando com arquitetos e analistas de negócio. Necessário mínimo de 3 anos de experiência, sólidos conhecimentos em POO, SOLID, SQL (SQL Server, PostgreSQL, Oracle ou MySQL), APIs REST e SOAP, Entity Framework, GIT e metodologias ágeis (Scrum/Kanban).  Modelo: Híbrido – 3x remoto e 2x presencial Local: Curitiba – PR Contratação: CLT Horário: Segunda a sexta, horário comercial  Benefícios: Alimentação R$970,00 + Plano de saúde e odontológico + PLR + VT Diferenciais: Docker, DDD, AWS, DevOps, CI/CD, segurança de software, React, Angular, Flutter Vaga também disponível para PcD. || Empresa .....:  Code Group</t>
+        </is>
+      </c>
+      <c r="I314" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>19/01/2026</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>82669</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>Analista Protheus – Nível Pleno</t>
+        </is>
+      </c>
+      <c r="D315" t="inlineStr">
+        <is>
+          <t>Pleno</t>
+        </is>
+      </c>
+      <c r="E315" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F315" t="inlineStr">
+        <is>
+          <t>Guarulhos - SP - 17/01/26</t>
+        </is>
+      </c>
+      <c r="G315" t="inlineStr">
+        <is>
+          <t>Local: Guarulhos (Centro) – SP Modelo: Presencial Salário: Pretensão salarial a combinar  Descrição da Vaga: Buscamos um Analista Protheus Pleno com sólida experiência nos principais módulos do ERP, capaz de atuar em análises, parametrizações, suporte funcional e acompanhamento de rotinas internas. O profissional trabalhará em conjunto com as áreas usuárias, garantindo fluidez nos processos e evolução contínua do sistema.  Responsabilidades: Atuar nos módulos: Compras, Faturamento, Estoque, Financeiro e Contabilidade. Realizar análises funcionais, levantamento de requisitos e suporte aos usuários. Parametrizar, ajustar e acompanhar processos dentro do Protheus. Apoiar em testes, homologações e implementação de melhorias. Conhecimento em rotinas, integrações e parametrizações do Protheus.  Desejável: Conhecimento no módulo Configurador. Conhecimento em comandos SQL. Noções ou experiência em desenvolvimento ADVPL.
+Empresa .....:  Gestão Dinâmica Tecnologia</t>
+        </is>
+      </c>
+      <c r="H315" t="inlineStr">
+        <is>
+          <t>Guarulhos - SP - 17/01/26 || Analista Protheus – Nível Pleno || Local: Guarulhos (Centro) – SP Modelo: Presencial Salário: Pretensão salarial a combinar  Descrição da Vaga: Buscamos um Analista Protheus Pleno com sólida experiência nos principais módulos do ERP, capaz de atuar em análises, parametrizações, suporte funcional e acompanhamento de rotinas internas. O profissional trabalhará em conjunto com as áreas usuárias, garantindo fluidez nos processos e evolução contínua do sistema.  Responsabilidades: Atuar nos módulos: Compras, Faturamento, Estoque, Financeiro e Contabilidade. Realizar análises funcionais, levantamento de requisitos e suporte aos usuários. Parametrizar, ajustar e acompanhar processos dentro do Protheus. Apoiar em testes, homologações e implementação de melhorias. Conhecimento em rotinas, integrações e parametrizações do Protheus.  Desejável: Conhecimento no módulo Configurador. Conhecimento em comandos SQL. Noções ou experiência em desenvolvimento ADVPL. || Empresa .....:  Gestão Dinâmica Tecnologia</t>
+        </is>
+      </c>
+      <c r="I315" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>19/01/2026</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>81897</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>Analista de Estatistica Sênior</t>
+        </is>
+      </c>
+      <c r="D316" t="inlineStr">
+        <is>
+          <t>Sênior</t>
+        </is>
+      </c>
+      <c r="E316" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F316" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 17/01/26</t>
+        </is>
+      </c>
+      <c r="G316" t="inlineStr">
+        <is>
+          <t>Requisitos Indispensáveis:  Graduação em curso de nível superior em Estatística acompanhado de certificado de curso de pós-graduação (especialização, mestrado ou doutorado) na área de estatística, matemática ou correlata de, no mínimo, 360 horas. SAS (SAS Enterprise Guide, SAS Enterprise Miner, SAS Forecast Studio) Mínimo de 5 anos de experiênciaem projetos SAS.  Requisitos Desejáveis: Statistics / SAS Enterprise Guide: ANOVA, Regression, and Logistic Regression Predictive Modeling Using Logistic Regression Applied Analytics Using SAS Enterprise Miner Advanced Predictive Modeling Using SAS Enterprise Miner Forecasting Using SAS Forecast Server Software Using SAS High-Performance Forecasting Software.#8203  Atividades / Responsabilidades: Profissional capacitado para preparar dados, realizar e interpretar análises estatísticas, bem como construir segmentações e modelos através das ferramentas analíticas do SAS
+Empresa .....:  TO Brasil Ltda</t>
+        </is>
+      </c>
+      <c r="H316" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 17/01/26 || Analista de Estatistica Sênior || Requisitos Indispensáveis:  Graduação em curso de nível superior em Estatística acompanhado de certificado de curso de pós-graduação (especialização, mestrado ou doutorado) na área de estatística, matemática ou correlata de, no mínimo, 360 horas. SAS (SAS Enterprise Guide, SAS Enterprise Miner, SAS Forecast Studio) Mínimo de 5 anos de experiênciaem projetos SAS.  Requisitos Desejáveis: Statistics / SAS Enterprise Guide: ANOVA, Regression, and Logistic Regression Predictive Modeling Using Logistic Regression Applied Analytics Using SAS Enterprise Miner Advanced Predictive Modeling Using SAS Enterprise Miner Forecasting Using SAS Forecast Server Software Using SAS High-Performance Forecasting Software.#8203  Atividades / Responsabilidades: Profissional capacitado para preparar dados, realizar e interpretar análises estatísticas, bem como construir segmentações e modelos através das ferramentas analíticas do SAS || Empresa .....:  TO Brasil Ltda</t>
+        </is>
+      </c>
+      <c r="I316" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>19/01/2026</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>82046</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>Analista Programador Dynamics Sênior</t>
+        </is>
+      </c>
+      <c r="D317" t="inlineStr">
+        <is>
+          <t>Sênior</t>
+        </is>
+      </c>
+      <c r="E317" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F317" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 17/01/26</t>
+        </is>
+      </c>
+      <c r="G317" t="inlineStr">
+        <is>
+          <t>Descrição - Desenvolvimento de plugins em C# para Dynamics. - Criação e manutenção de Azure Functions para integração com OData do Dynamics. - Integração com Kafka e Service Bus. - Monitoramento e análise de logs em Application Insights. - Realização de troubleshooting e resolução de problemas. - Criação e automação de fluxos no Power Automate.  Requisitos - Graduação em Ciência da Computação ou áreas relacionadas - Experiência sólida em desenvolvimento C#. - Experiência sólida em Dynamics 365. - Experiência com Azure Functions e OData. - Experiência com Power Automate. - Experiência com JavaScript com SDK do Dynamics. - Conhecimento em programação, banco de dados e arquitetura de software. - Certificações na área de desenvolvimento de software serão um diferencial. - Capacidade de adaptação a diferentes cenários e trabalho em equipe.
+Empresa .....:  SYSMAP SOLUTIONS SOFTWARE E CONSULT LTDA</t>
+        </is>
+      </c>
+      <c r="H317" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 17/01/26 || Analista Programador Dynamics Sênior || Descrição - Desenvolvimento de plugins em C# para Dynamics. - Criação e manutenção de Azure Functions para integração com OData do Dynamics. - Integração com Kafka e Service Bus. - Monitoramento e análise de logs em Application Insights. - Realização de troubleshooting e resolução de problemas. - Criação e automação de fluxos no Power Automate.  Requisitos - Graduação em Ciência da Computação ou áreas relacionadas - Experiência sólida em desenvolvimento C#. - Experiência sólida em Dynamics 365. - Experiência com Azure Functions e OData. - Experiência com Power Automate. - Experiência com JavaScript com SDK do Dynamics. - Conhecimento em programação, banco de dados e arquitetura de software. - Certificações na área de desenvolvimento de software serão um diferencial. - Capacidade de adaptação a diferentes cenários e trabalho em equipe. || Empresa .....:  SYSMAP SOLUTIONS SOFTWARE E CONSULT LTDA</t>
+        </is>
+      </c>
+      <c r="I317" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>19/01/2026</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>81975</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>Consultor Engenheiro de Telecomunicações - Inglês</t>
+        </is>
+      </c>
+      <c r="D318" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E318" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F318" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 17/01/26</t>
+        </is>
+      </c>
+      <c r="G318" t="inlineStr">
+        <is>
+          <t>Consultor Engenheiro(a) de Telecomunicações Preferencialmente São Paulo (1x por semana no escritório do cliente/ 4x remoto).  Também serão considerados profissionais de outras localidades:  Rio de Janeiro, Brasília, Belo Horizonte, Recife, Salvador, Porto Alegre, Blumenau, Campinas, Curitiba, Fortaleza e Ribeirão Preto.  Contrato de 6 meses com possibilidade de renovação.  •	Projetar, implementar e manter sistemas e infraestrutura de telecomunicações que suportem as operações de negócio. •	Colaborar com equipes multifuncionais para coletar requisitos e garantir que as soluções de telecom atendam às necessidades da organização. •	Monitorar e solucionar problemas em sistemas de voz, dados e vídeo, assegurando desempenho e confiabilidade. •	Fornecer suporte técnico e atuar na resolução de interrupções e incidentes de telecomunicações. •	Avaliar regularmente os sistemas de telecom e recomendar melhorias para otimização de desempenho e segurança.
+Empresa .....:  k2 partnering Solutions</t>
+        </is>
+      </c>
+      <c r="H318" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 17/01/26 || Consultor Engenheiro de Telecomunicações - Inglês || Consultor Engenheiro(a) de Telecomunicações Preferencialmente São Paulo (1x por semana no escritório do cliente/ 4x remoto).  Também serão considerados profissionais de outras localidades:  Rio de Janeiro, Brasília, Belo Horizonte, Recife, Salvador, Porto Alegre, Blumenau, Campinas, Curitiba, Fortaleza e Ribeirão Preto.  Contrato de 6 meses com possibilidade de renovação.  •	Projetar, implementar e manter sistemas e infraestrutura de telecomunicações que suportem as operações de negócio. •	Colaborar com equipes multifuncionais para coletar requisitos e garantir que as soluções de telecom atendam às necessidades da organização. •	Monitorar e solucionar problemas em sistemas de voz, dados e vídeo, assegurando desempenho e confiabilidade. •	Fornecer suporte técnico e atuar na resolução de interrupções e incidentes de telecomunicações. •	Avaliar regularmente os sistemas de telecom e recomendar melhorias para otimização de desempenho e segurança. || Empresa .....:  k2 partnering Solutions</t>
+        </is>
+      </c>
+      <c r="I318" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>19/01/2026</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>82239</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>Consultor QA/Teste (Azure) Com inglês</t>
+        </is>
+      </c>
+      <c r="D319" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E319" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F319" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 17/01/26</t>
+        </is>
+      </c>
+      <c r="G319" t="inlineStr">
+        <is>
+          <t>Consultor QA (Azure)– inglês Totalmente remoto Inglês: Avançado/Fluente (Conversação em Inglês)  Importante: Para esse contrato específico, o início será em Janeiro de 2026.  O contrato de prestação de serviços abrange a responsabilidade de consultoria para atuar em um novo projeto de migração para a nuvem Azure, abrangendo a responsabilidade de  Testing com envolvimento direto em iniciativas de transformação digital e modernização de sistemas legados.  Requer ter atuado em contratos anteriores com: Testes em projetos de migração para nuvem Azure DevOps, Test Plans, e ferramentas de automação Projetos de  cloud migration e conhecimento sólido sobre os stacks de tecnologia Azure. Criar e executar planos e casos de teste para ambientes Azure Realizar testes funcionais, de regressão e de integração pós-migração Identificar, documentar e acompanhar defeitos até sua resolução Colaborar com analistas para garantir qualidade de entrega Automatizar testes quando aplicável
+Empresa .....:  k2 partnering Solutions</t>
+        </is>
+      </c>
+      <c r="H319" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 17/01/26 || Consultor QA/Teste (Azure) Com inglês || Consultor QA (Azure)– inglês Totalmente remoto Inglês: Avançado/Fluente (Conversação em Inglês)  Importante: Para esse contrato específico, o início será em Janeiro de 2026.  O contrato de prestação de serviços abrange a responsabilidade de consultoria para atuar em um novo projeto de migração para a nuvem Azure, abrangendo a responsabilidade de  Testing com envolvimento direto em iniciativas de transformação digital e modernização de sistemas legados.  Requer ter atuado em contratos anteriores com: Testes em projetos de migração para nuvem Azure DevOps, Test Plans, e ferramentas de automação Projetos de  cloud migration e conhecimento sólido sobre os stacks de tecnologia Azure. Criar e executar planos e casos de teste para ambientes Azure Realizar testes funcionais, de regressão e de integração pós-migração Identificar, documentar e acompanhar defeitos até sua resolução Colaborar com analistas para garantir qualidade de entrega Automatizar testes quando aplicável || Empresa .....:  k2 partnering Solutions</t>
+        </is>
+      </c>
+      <c r="I319" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>19/01/2026</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>81769</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>Consultor Tasy</t>
+        </is>
+      </c>
+      <c r="D320" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E320" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F320" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 17/01/26</t>
+        </is>
+      </c>
+      <c r="G320" t="inlineStr">
+        <is>
+          <t>Consultor Tasy (Espanhol avançado)  Local: Remoto Prazo de atuação: 6 meses, com chances de prorrogar Atuação: PJ/hora aberta  Requisitos: Implementar as integrações existentes, realizar levantamento e análise de novas integrações Contatar clientes para compreender e executar suas demandas Realizar análise de requisitos técnicos e funcionais Elaborar documentação técnica e funcional Desenvolver relatórios e dashboards Criar templates e avaliações Acompanhar processos de personalização.  Ferramentas: PL/SQL: Insert, Update, Procedures, Functions, Packages Triggers e Jobs: Tasy Interface Engine (broker de interoperabilidade Tasy) Tasy, HTML5: EMR, portais Tasy: Portal do Paciente, Portal de Resultados, Portal Clinico e Aprovações Pendentes.
+Empresa .....:  Entrust It</t>
+        </is>
+      </c>
+      <c r="H320" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 17/01/26 || Consultor Tasy || Consultor Tasy (Espanhol avançado)  Local: Remoto Prazo de atuação: 6 meses, com chances de prorrogar Atuação: PJ/hora aberta  Requisitos: Implementar as integrações existentes, realizar levantamento e análise de novas integrações Contatar clientes para compreender e executar suas demandas Realizar análise de requisitos técnicos e funcionais Elaborar documentação técnica e funcional Desenvolver relatórios e dashboards Criar templates e avaliações Acompanhar processos de personalização.  Ferramentas: PL/SQL: Insert, Update, Procedures, Functions, Packages Triggers e Jobs: Tasy Interface Engine (broker de interoperabilidade Tasy) Tasy, HTML5: EMR, portais Tasy: Portal do Paciente, Portal de Resultados, Portal Clinico e Aprovações Pendentes. || Empresa .....:  Entrust It</t>
+        </is>
+      </c>
+      <c r="I320" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>19/01/2026</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>82848</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>Coordenador Segurança da Informação AWS</t>
+        </is>
+      </c>
+      <c r="D321" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E321" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F321" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 17/01/26</t>
+        </is>
+      </c>
+      <c r="G321" t="inlineStr">
+        <is>
+          <t>Modelo: PJ + Benefícios Atuação: Totalmente Remoto Valor máximo da vaga: 20 K  Obrigatório ter atuado como coordenador de equipe de Segurança da Informação e ser especialista em AWS  Experiência consolidada em segurança da informação com foco em ambientes de nuvem AWS.  Vivência em coordenação de times e projetos de segurança, com foco em priorização e gestão de demandas.  Conhecimento de frameworks e benchmarks de segurança (CIS, NIST, ISO 27001, LGPD, GDPR).  Entendimento prático de ferramentas e serviços AWS relacionados à segurança (IAM, KMS, Security Hub, GuardDuty, CloudTrail, Config etc.), atuando mais na definição de diretrizes do que na execução.  Familiaridade com práticas de DevSecOps, CI/CD seguro e automação de políticas de segurança.  Capacidade de traduzir riscos técnicos em insumos de decisão para áreas executivas.  Excelente comunicação, habilidade de negociação e trabalho colaborativo entre áreas de negócio e tecnologia.
+Empresa .....:  Venice Tech</t>
+        </is>
+      </c>
+      <c r="H321" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 17/01/26 || Coordenador Segurança da Informação AWS || Modelo: PJ + Benefícios Atuação: Totalmente Remoto Valor máximo da vaga: 20 K  Obrigatório ter atuado como coordenador de equipe de Segurança da Informação e ser especialista em AWS  Experiência consolidada em segurança da informação com foco em ambientes de nuvem AWS.  Vivência em coordenação de times e projetos de segurança, com foco em priorização e gestão de demandas.  Conhecimento de frameworks e benchmarks de segurança (CIS, NIST, ISO 27001, LGPD, GDPR).  Entendimento prático de ferramentas e serviços AWS relacionados à segurança (IAM, KMS, Security Hub, GuardDuty, CloudTrail, Config etc.), atuando mais na definição de diretrizes do que na execução.  Familiaridade com práticas de DevSecOps, CI/CD seguro e automação de políticas de segurança.  Capacidade de traduzir riscos técnicos em insumos de decisão para áreas executivas.  Excelente comunicação, habilidade de negociação e trabalho colaborativo entre áreas de negócio e tecnologia. || Empresa .....:  Venice Tech</t>
+        </is>
+      </c>
+      <c r="I321" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>19/01/2026</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>83287</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>Desenvolvedor Fullstack – GO e Svelte - REMOTO</t>
+        </is>
+      </c>
+      <c r="D322" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E322" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F322" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 17/01/26</t>
+        </is>
+      </c>
+      <c r="G322" t="inlineStr">
+        <is>
+          <t>Buscamos um profissional para desenvolver e manter aplicações web robustas e escaláveis usando Go e SvelteKit.  Conhecimento: •	GO com framework CHI •	Svelte/Sveltekit •	HTML, CSS e Javascript •	Conhecimento em Banco de Dados SQL e NoSQL •	Experiência com ferramentas de controle de versão como GIT •	Conhecimentos em testes automatizados como Testes unitários, testes de integração e Robot. •	APIs RESTful •	Pré-processadores como SASS ou LESS •	Jenkins •	Conhecimento em boas práticas e padronização de projetos.  O que esperamos de você: •	Cumprir os ritos do Scrum •	Colaborar como front-end e back-end para garantir requisitos claros e entregas de alta qualidade •	Escrever código limpo, testável, bem documentado e realizar revisões de código. •	Familiaridades com práticas de CI/CD e ferramentas associadas  Superior completo. Preferencialmemte na área da tecnologia.da informação.
+Empresa .....:  Hammer Consult</t>
+        </is>
+      </c>
+      <c r="H322" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 17/01/26 || Desenvolvedor Fullstack – GO e Svelte - REMOTO || Buscamos um profissional para desenvolver e manter aplicações web robustas e escaláveis usando Go e SvelteKit.  Conhecimento: •	GO com framework CHI •	Svelte/Sveltekit •	HTML, CSS e Javascript •	Conhecimento em Banco de Dados SQL e NoSQL •	Experiência com ferramentas de controle de versão como GIT •	Conhecimentos em testes automatizados como Testes unitários, testes de integração e Robot. •	APIs RESTful •	Pré-processadores como SASS ou LESS •	Jenkins •	Conhecimento em boas práticas e padronização de projetos.  O que esperamos de você: •	Cumprir os ritos do Scrum •	Colaborar como front-end e back-end para garantir requisitos claros e entregas de alta qualidade •	Escrever código limpo, testável, bem documentado e realizar revisões de código. •	Familiaridades com práticas de CI/CD e ferramentas associadas  Superior completo. Preferencialmemte na área da tecnologia.da informação. || Empresa .....:  Hammer Consult</t>
+        </is>
+      </c>
+      <c r="I322" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>19/01/2026</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>82976</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>Desenvolvedor Nodejs Sênior</t>
+        </is>
+      </c>
+      <c r="D323" t="inlineStr">
+        <is>
+          <t>Sênior</t>
+        </is>
+      </c>
+      <c r="E323" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F323" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 17/01/26</t>
+        </is>
+      </c>
+      <c r="G323" t="inlineStr">
+        <is>
+          <t>- Desenvolver aplicações Backend em Node.Js com MongoDB e ORACLE - Desenvolver aplicações para ambientes CLOUD (AWS e GCP) - Desenvolverá sistemas voltados para estatística e cálculos com muito fluxo em ferramentas NoCode - O profissional realizará reuniões de refinamentos técnicos - O profissional atuará em sustentação e novos projetos  Requisitos Técnicos Obrigatórios - Desenvolvimento em Node.Js, JavaScript e APIs - Alto conhecimento em GCP - Conhecimento em AWS - GIT - ORACLE - MongoDB - Metodologia Ágil SCRUM e KANBAN - Manipulação de JSON - Alto conhecimento em Clean code - Alto conhecimento em aplicar Design Patterns em soluções - Visão ampla em Arquitetura de Sistemas - Conhecimentos em sistemas de filas (RabittMQ, entre outros) - Experiências em monitoramento de sistemas (Datadog, AppDynamic, Stack Elastic)  Diferenciais - Desenvolvimento em JAVA - Conhecimentos em Seguros de Automóveis - Conhecimentos em Node-RED  Home Office Contratação
+Empresa .....:  FORNAX CONSULTORIA EM INFORMATICA</t>
+        </is>
+      </c>
+      <c r="H323" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 17/01/26 || Desenvolvedor Nodejs Sênior || - Desenvolver aplicações Backend em Node.Js com MongoDB e ORACLE - Desenvolver aplicações para ambientes CLOUD (AWS e GCP) - Desenvolverá sistemas voltados para estatística e cálculos com muito fluxo em ferramentas NoCode - O profissional realizará reuniões de refinamentos técnicos - O profissional atuará em sustentação e novos projetos  Requisitos Técnicos Obrigatórios - Desenvolvimento em Node.Js, JavaScript e APIs - Alto conhecimento em GCP - Conhecimento em AWS - GIT - ORACLE - MongoDB - Metodologia Ágil SCRUM e KANBAN - Manipulação de JSON - Alto conhecimento em Clean code - Alto conhecimento em aplicar Design Patterns em soluções - Visão ampla em Arquitetura de Sistemas - Conhecimentos em sistemas de filas (RabittMQ, entre outros) - Experiências em monitoramento de sistemas (Datadog, AppDynamic, Stack Elastic)  Diferenciais - Desenvolvimento em JAVA - Conhecimentos em Seguros de Automóveis - Conhecimentos em Node-RED  Home Office Contratação || Empresa .....:  FORNAX CONSULTORIA EM INFORMATICA</t>
+        </is>
+      </c>
+      <c r="I323" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>19/01/2026</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>82861</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>Desenvolvedor React Native - Remoto</t>
+        </is>
+      </c>
+      <c r="D324" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E324" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F324" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 17/01/26</t>
+        </is>
+      </c>
+      <c r="G324" t="inlineStr">
+        <is>
+          <t>Vaga Remota – PJ  Desenvolvedor React Native  Fulltime  Responsável pelo desenvolvimento e manutenção de aplicativos React Native para Android e iOS, atuando em soluções escaláveis e de alta performance. Requer experiência sólida em TypeScript, arquitetura de software, design patterns, algoritmos e estruturas de dados. Necessário domínio avançado em MongoDB (modelagem, otimização) e conhecimentos em Message Brokers (Pub/Sub). Atuação com práticas DevOps, CI/CD, segurança de aplicações, testes avançados e monitoramento. Desejável experiência em liderança técnica, code review, definição de padrões, decisões arquiteturais e mentoria de times. Formação superior em áreas de tecnologia e experiência mínima de 5 anos em desenvolvimento de software (ideal 6 a 7 anos).
+Empresa .....:  Code Group</t>
+        </is>
+      </c>
+      <c r="H324" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 17/01/26 || Desenvolvedor React Native - Remoto || Vaga Remota – PJ  Desenvolvedor React Native  Fulltime  Responsável pelo desenvolvimento e manutenção de aplicativos React Native para Android e iOS, atuando em soluções escaláveis e de alta performance. Requer experiência sólida em TypeScript, arquitetura de software, design patterns, algoritmos e estruturas de dados. Necessário domínio avançado em MongoDB (modelagem, otimização) e conhecimentos em Message Brokers (Pub/Sub). Atuação com práticas DevOps, CI/CD, segurança de aplicações, testes avançados e monitoramento. Desejável experiência em liderança técnica, code review, definição de padrões, decisões arquiteturais e mentoria de times. Formação superior em áreas de tecnologia e experiência mínima de 5 anos em desenvolvimento de software (ideal 6 a 7 anos). || Empresa .....:  Code Group</t>
+        </is>
+      </c>
+      <c r="I324" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>19/01/2026</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>82073</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>Engenheiro de Integração</t>
+        </is>
+      </c>
+      <c r="D325" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E325" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F325" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 17/01/26</t>
+        </is>
+      </c>
+      <c r="G325" t="inlineStr">
+        <is>
+          <t>A 200DEV é uma consultoria de TI focada em Inovação e Transformação Digital, utilizando tecnologias de ponta e profissionais orientados a resultados.  Vaga: Engenheiro de Integração e Desenvolvimento de Infraestrutura  Habilidades obrigatórias Experiência comprovada com Terraform e Ansible (IAC) Proficiência em desenvolvimento orientado a objetos (Java, .NET) e em linguagem de script de alto nível (Python, Go, Bash, etc.). Vivência prática e sólida em serviços AWS (EC2, S3, Lambda, etc.). Expertise em integração de APIs (REST, SOAP) e protocolos de segurança relacionados. Conhecimento e experiência com sistemas como Prometheus, Grafana, CheckMK, Alert Manager, APIs de monitoramento, etc. Experiência em troubleshooting de alto nível, otimização de desempenho e implementação de prática  Idioma: Inglês Avançado (leitura, escrita e conversação).  Desejável: Experiência com IBM MQ e IBM Connect Direct (IBM CD) ou soluções equivalentes.
+Empresa .....:  200DEV SVCS LTDA.</t>
+        </is>
+      </c>
+      <c r="H325" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 17/01/26 || Engenheiro de Integração || A 200DEV é uma consultoria de TI focada em Inovação e Transformação Digital, utilizando tecnologias de ponta e profissionais orientados a resultados.  Vaga: Engenheiro de Integração e Desenvolvimento de Infraestrutura  Habilidades obrigatórias Experiência comprovada com Terraform e Ansible (IAC) Proficiência em desenvolvimento orientado a objetos (Java, .NET) e em linguagem de script de alto nível (Python, Go, Bash, etc.). Vivência prática e sólida em serviços AWS (EC2, S3, Lambda, etc.). Expertise em integração de APIs (REST, SOAP) e protocolos de segurança relacionados. Conhecimento e experiência com sistemas como Prometheus, Grafana, CheckMK, Alert Manager, APIs de monitoramento, etc. Experiência em troubleshooting de alto nível, otimização de desempenho e implementação de prática  Idioma: Inglês Avançado (leitura, escrita e conversação).  Desejável: Experiência com IBM MQ e IBM Connect Direct (IBM CD) ou soluções equivalentes. || Empresa .....:  200DEV SVCS LTDA.</t>
+        </is>
+      </c>
+      <c r="I325" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>19/01/2026</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>81823</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>Engenheiro de Machine Learning Sênior</t>
+        </is>
+      </c>
+      <c r="D326" t="inlineStr">
+        <is>
+          <t>Sênior</t>
+        </is>
+      </c>
+      <c r="E326" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F326" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 17/01/26</t>
+        </is>
+      </c>
+      <c r="G326" t="inlineStr">
+        <is>
+          <t>Buscamos Engenheiro(a) de Machine Learning Sênior para desenvolver e manter pipelines e soluções de ML em ambiente AWS, garantindo automação, escalabilidade e rastreabilidade dos modelos em produção. Atuará junto às equipes de Data Science, Engenharia de Dados e Produto, assegurando qualidade e boas práticas.  Responsabilidades: Projetar e implementar pipelines de validação e avaliação de modelos integrar dados e métricas em fluxos automatizados modularizar pipelines para reuso e testes garantir versionamento, logging, monitoramento e testes automatizados propor melhorias na arquitetura e processos.  Requisitos: Experiência sólida em engenharia de software aplicada a dados e ML domínio de Python, PySpark, Pandas, Scikit-learn vivência com AWS (S3, Lambda, Glue, SageMaker) conhecimento em MLOps, CI/CD e orquestração de workflows código limpo e testável.  Diferenciais: Terraform, CloudForma
+Empresa .....:  Grupo Taking</t>
+        </is>
+      </c>
+      <c r="H326" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 17/01/26 || Engenheiro de Machine Learning Sênior || Buscamos Engenheiro(a) de Machine Learning Sênior para desenvolver e manter pipelines e soluções de ML em ambiente AWS, garantindo automação, escalabilidade e rastreabilidade dos modelos em produção. Atuará junto às equipes de Data Science, Engenharia de Dados e Produto, assegurando qualidade e boas práticas.  Responsabilidades: Projetar e implementar pipelines de validação e avaliação de modelos integrar dados e métricas em fluxos automatizados modularizar pipelines para reuso e testes garantir versionamento, logging, monitoramento e testes automatizados propor melhorias na arquitetura e processos.  Requisitos: Experiência sólida em engenharia de software aplicada a dados e ML domínio de Python, PySpark, Pandas, Scikit-learn vivência com AWS (S3, Lambda, Glue, SageMaker) conhecimento em MLOps, CI/CD e orquestração de workflows código limpo e testável.  Diferenciais: Terraform, CloudForma || Empresa .....:  Grupo Taking</t>
+        </is>
+      </c>
+      <c r="I326" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>19/01/2026</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>82265</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>Engenheiro de Machine Learning Senior</t>
+        </is>
+      </c>
+      <c r="D327" t="inlineStr">
+        <is>
+          <t>Sênior</t>
+        </is>
+      </c>
+      <c r="E327" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F327" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 17/01/26</t>
+        </is>
+      </c>
+      <c r="G327" t="inlineStr">
+        <is>
+          <t>Contrato: CLT Atuação: Remoto Projeto: Indeterminado  Requisitos: - Experiência em varejo. - Experiência sólida com engenharia de software aplicada a dados e machine learning. - Proficiência em Python e frameworks como PySpark, Pandas, Scikit-learn ou similares. - Experiência com ferramentas e serviços AWS, como S3, Lambda, Step Functions, Glue, Athena, SageMaker ou ECS. - Conhecimento em MLOps e CI/CD para pipelines de dados e modelos. - Experiência com orquestração de workflows. - Capacidade de escrever código limpo, modular e testável.  Diferenciais: - Experiência com infraestrutura como código (Terraform, CloudFormation). - Participação em projetos de ML em produção com foco em confiabilidade e rastreabilidade.  Responsabilidades: Projetar e implementar pipelines de validação de dados e avaliação de modelos em ambiente cloud (AWS) entre outras atividades.
+Empresa .....:  Runtalent</t>
+        </is>
+      </c>
+      <c r="H327" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 17/01/26 || Engenheiro de Machine Learning Senior || Contrato: CLT Atuação: Remoto Projeto: Indeterminado  Requisitos: - Experiência em varejo. - Experiência sólida com engenharia de software aplicada a dados e machine learning. - Proficiência em Python e frameworks como PySpark, Pandas, Scikit-learn ou similares. - Experiência com ferramentas e serviços AWS, como S3, Lambda, Step Functions, Glue, Athena, SageMaker ou ECS. - Conhecimento em MLOps e CI/CD para pipelines de dados e modelos. - Experiência com orquestração de workflows. - Capacidade de escrever código limpo, modular e testável.  Diferenciais: - Experiência com infraestrutura como código (Terraform, CloudFormation). - Participação em projetos de ML em produção com foco em confiabilidade e rastreabilidade.  Responsabilidades: Projetar e implementar pipelines de validação de dados e avaliação de modelos em ambiente cloud (AWS) entre outras atividades. || Empresa .....:  Runtalent</t>
+        </is>
+      </c>
+      <c r="I327" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>19/01/2026</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>82914</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>Engenheiro DevOps</t>
+        </is>
+      </c>
+      <c r="D328" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E328" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F328" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 17/01/26</t>
+        </is>
+      </c>
+      <c r="G328" t="inlineStr">
+        <is>
+          <t>Realizar criação de pipelines de dados com DevOps, utilizando Terraform e Jenkins/github para automatizar criação de infraestrutura AWS e deploy de soluções Auxiliar analistas de dados na classificação de dados pessoais e sensíveis e sua configuração com AWS Lake Formation (permissão de acesso a colunas e linhas) Processar grandes volumes de dados com uso do Spark através do EMR Studio e AWS Glue Jobs e Workflow Auxiliar analistas de dados na criação de modelos dimensionais para anállise de dados (fatos e dimensões) Habilidades de programação em Python Relacionamento com a área de negócio para entendimento das origens e mapeamento dos dados Estruturação e consolidação de dados e indicadores na AWS, garantindo bases com os templates adequados para o consumo direto em ferramentas de PowerBi para construção de dashboards
+Empresa .....:  Ewave do Brasil</t>
+        </is>
+      </c>
+      <c r="H328" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 17/01/26 || Engenheiro DevOps || Realizar criação de pipelines de dados com DevOps, utilizando Terraform e Jenkins/github para automatizar criação de infraestrutura AWS e deploy de soluções Auxiliar analistas de dados na classificação de dados pessoais e sensíveis e sua configuração com AWS Lake Formation (permissão de acesso a colunas e linhas) Processar grandes volumes de dados com uso do Spark através do EMR Studio e AWS Glue Jobs e Workflow Auxiliar analistas de dados na criação de modelos dimensionais para anállise de dados (fatos e dimensões) Habilidades de programação em Python Relacionamento com a área de negócio para entendimento das origens e mapeamento dos dados Estruturação e consolidação de dados e indicadores na AWS, garantindo bases com os templates adequados para o consumo direto em ferramentas de PowerBi para construção de dashboards || Empresa .....:  Ewave do Brasil</t>
+        </is>
+      </c>
+      <c r="I328" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>19/01/2026</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>82105</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>Especialista em Redes - Palo Alto</t>
+        </is>
+      </c>
+      <c r="D329" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E329" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F329" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 17/01/26</t>
+        </is>
+      </c>
+      <c r="G329" t="inlineStr">
+        <is>
+          <t>Especialista em Redes – Palo Alto Prisma Contrato PJ  Remoto  Atuação em ambiente global  Buscamos um(a) Especialista em Redes para garantir continuidade operacional, segurança, conectividade e alta disponibilidade durante essa transição crítica.  Requisitos: Inglês fluente – uso diário com time global. Sênior/Especialista em redes e infraestrutura, +7 anos de experiência. Experiência prática com Palo Alto (Prisma Access, Prisma Cloud e SD-WAN). Conhecimento em protocolos de roteamento, especialmente BGP. Vivência em ambientes híbridos e multicloud. Certificações Palo Alto (PCNSE, PCNSA, PCCSE). Experiência com Cisco e transição de ambientes Cisco Palo Alto. Domínio de segurança em nuvem, Zero Trust e automação.
+Empresa .....:  2Brain Group</t>
+        </is>
+      </c>
+      <c r="H329" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 17/01/26 || Especialista em Redes - Palo Alto || Especialista em Redes – Palo Alto Prisma Contrato PJ  Remoto  Atuação em ambiente global  Buscamos um(a) Especialista em Redes para garantir continuidade operacional, segurança, conectividade e alta disponibilidade durante essa transição crítica.  Requisitos: Inglês fluente – uso diário com time global. Sênior/Especialista em redes e infraestrutura, +7 anos de experiência. Experiência prática com Palo Alto (Prisma Access, Prisma Cloud e SD-WAN). Conhecimento em protocolos de roteamento, especialmente BGP. Vivência em ambientes híbridos e multicloud. Certificações Palo Alto (PCNSE, PCNSA, PCCSE). Experiência com Cisco e transição de ambientes Cisco Palo Alto. Domínio de segurança em nuvem, Zero Trust e automação. || Empresa .....:  2Brain Group</t>
+        </is>
+      </c>
+      <c r="I329" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>19/01/2026</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>82038</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>Administrador de Redes Pl</t>
+        </is>
+      </c>
+      <c r="D330" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E330" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F330" t="inlineStr">
+        <is>
+          <t>Maringá - PR - 17/01/26</t>
+        </is>
+      </c>
+      <c r="G330" t="inlineStr">
+        <is>
+          <t>Atividades: Execução de atividades relacionadas à infraestrutura de TI. Concessão e revogação de acessos e usuários. Manutenção básica de servidores. Resolução de problemas básicos relacionados aos sistemas utilizados na empresa. Configuração básica de firewall, incluindo criação de regras e habilitação de recursos de forma supervisionada. Atualização de patches de segurança. Gerenciamento de configurações de segurança do ambiente. Monitoramento da disponibilidade do ambiente.  Requisitos Técnicos: Experiência com nuvem Azure e AWS. Familiaridade com JIRA. Conhecimento em firewall Fortinet. Experiência com a suíte Microsoft 365. Conhecimento em Grafana.  CLT - Totalmente presencial - MARINGÁ/PR Salário compatível com o mercado. Assistência médica Vale refeição/alimentação. Vale transporte. Seguro de Vida
+Empresa .....:  Zenvor</t>
+        </is>
+      </c>
+      <c r="H330" t="inlineStr">
+        <is>
+          <t>Maringá - PR - 17/01/26 || Administrador de Redes Pl || Atividades: Execução de atividades relacionadas à infraestrutura de TI. Concessão e revogação de acessos e usuários. Manutenção básica de servidores. Resolução de problemas básicos relacionados aos sistemas utilizados na empresa. Configuração básica de firewall, incluindo criação de regras e habilitação de recursos de forma supervisionada. Atualização de patches de segurança. Gerenciamento de configurações de segurança do ambiente. Monitoramento da disponibilidade do ambiente.  Requisitos Técnicos: Experiência com nuvem Azure e AWS. Familiaridade com JIRA. Conhecimento em firewall Fortinet. Experiência com a suíte Microsoft 365. Conhecimento em Grafana.  CLT - Totalmente presencial - MARINGÁ/PR Salário compatível com o mercado. Assistência médica Vale refeição/alimentação. Vale transporte. Seguro de Vida || Empresa .....:  Zenvor</t>
+        </is>
+      </c>
+      <c r="I330" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>19/01/2026</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>82051</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>Analista de Sustentação Cloud</t>
+        </is>
+      </c>
+      <c r="D331" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E331" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F331" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro - RJ - 17/01/26</t>
+        </is>
+      </c>
+      <c r="G331" t="inlineStr">
+        <is>
+          <t>Especialista em infraestrutura com foco em operações para absorver conhecimento sobre arquitetura cloud híbrida (SAP BTP + AWS + S/4).  • Absorver conhecimento sobre arquitetura de infraestrutura SAP BTP + AWS + S/4 • Criar documentação de procedimentos operacionais de infraestrutura • Participar do desenho de monitoramento e alertas • Criar runbooks para operação da infraestrutura híbrida  • 6+ anos de experiência em operação de infraestrutura • 3+ anos operando ambientes SAP (Basis) • Experiência sólida com Kubernetes • Experiência com monitoramento (CALM, Datadog) • Scripting para automação
+Empresa .....:  Blend IT Consultoria</t>
+        </is>
+      </c>
+      <c r="H331" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro - RJ - 17/01/26 || Analista de Sustentação Cloud || Especialista em infraestrutura com foco em operações para absorver conhecimento sobre arquitetura cloud híbrida (SAP BTP + AWS + S/4).  • Absorver conhecimento sobre arquitetura de infraestrutura SAP BTP + AWS + S/4 • Criar documentação de procedimentos operacionais de infraestrutura • Participar do desenho de monitoramento e alertas • Criar runbooks para operação da infraestrutura híbrida  • 6+ anos de experiência em operação de infraestrutura • 3+ anos operando ambientes SAP (Basis) • Experiência sólida com Kubernetes • Experiência com monitoramento (CALM, Datadog) • Scripting para automação || Empresa .....:  Blend IT Consultoria</t>
+        </is>
+      </c>
+      <c r="I331" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>19/01/2026</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>81755</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>Líder Técnico</t>
+        </is>
+      </c>
+      <c r="D332" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E332" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F332" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro - RJ - 17/01/26</t>
+        </is>
+      </c>
+      <c r="G332" t="inlineStr">
+        <is>
+          <t>Estamos contratando Líder Técnico Sênior  Entendemos que para essa evolução, é necessário experiência em: C# - MVC e Web API Dapper e Entity Framework SQL Server e Oracle SOA, Webservices, APIs, Microsserviços Frameworks JavaScript como React e Vue.js Padrões de Projeto Metodologias ágeis Promover a constante busca por excelência e inovação.  Principais responsabilidades: Realizar reuniões de status com o cliente Trabalhar de forma cross em diferentes projetos Participar na definição de arquiteturas em novos desenvolvimentos Definir melhores práticas para desenvolvimento de aplicações Definir padrões de qualidade e segurança Analisar os requisitos funcionais e técnicos de um sistema Estimar o tempo de desenvolvimento de um sistema. Garantir a equipe desenvolva seguindo as prática
+Empresa .....:  Innolevels</t>
+        </is>
+      </c>
+      <c r="H332" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro - RJ - 17/01/26 || Líder Técnico || Estamos contratando Líder Técnico Sênior  Entendemos que para essa evolução, é necessário experiência em: C# - MVC e Web API Dapper e Entity Framework SQL Server e Oracle SOA, Webservices, APIs, Microsserviços Frameworks JavaScript como React e Vue.js Padrões de Projeto Metodologias ágeis Promover a constante busca por excelência e inovação.  Principais responsabilidades: Realizar reuniões de status com o cliente Trabalhar de forma cross em diferentes projetos Participar na definição de arquiteturas em novos desenvolvimentos Definir melhores práticas para desenvolvimento de aplicações Definir padrões de qualidade e segurança Analisar os requisitos funcionais e técnicos de um sistema Estimar o tempo de desenvolvimento de um sistema. Garantir a equipe desenvolva seguindo as prática || Empresa .....:  Innolevels</t>
+        </is>
+      </c>
+      <c r="I332" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>19/01/2026</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>83282</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>Product Owner-Sr</t>
+        </is>
+      </c>
+      <c r="D333" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E333" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F333" t="inlineStr">
+        <is>
+          <t>Santo André - SP - 17/01/26</t>
+        </is>
+      </c>
+      <c r="G333" t="inlineStr">
+        <is>
+          <t>Requisitos Obrigatórios: Experiência sólida como Product Owner e/ou Analista de Negócios Sênior Vivência em projetos regulatórios ou no segmento financeiro Experiência prática com projetos que envolvam dados sensíveis, regras fiscais ou normativas Postura hands-on, senso de responsabilidade e tomada de decisão  Principais atividades a serem desenvolvidas: Atuará como Product Owner no projeto de Inclusão de CPF em formato Alfanumérico, garantindo alinhamento entre negócio, tecnologia e qualidade. Levantar, detalhar e priorizar requisitos junto aos stakeholders, assegurando clareza das regras de negócio e critérios de aceite. Gerenciar e priorizar o Product Backlog, mantendo foco em valor, risco e dependências técnicas. Definir e validar user stories, critérios de aceite e cenários de teste relacionados à mudança do formato do CPF. Conduzir alinhamentos com times de desenvolvimento e integrações para mitigar impactos em sistemas legados.  Contratação: PJ
+Empresa .....:  SEMPRE IT SERVICOS DE TECNOLOGIA LTDA</t>
+        </is>
+      </c>
+      <c r="H333" t="inlineStr">
+        <is>
+          <t>Santo André - SP - 17/01/26 || Product Owner-Sr || Requisitos Obrigatórios: Experiência sólida como Product Owner e/ou Analista de Negócios Sênior Vivência em projetos regulatórios ou no segmento financeiro Experiência prática com projetos que envolvam dados sensíveis, regras fiscais ou normativas Postura hands-on, senso de responsabilidade e tomada de decisão  Principais atividades a serem desenvolvidas: Atuará como Product Owner no projeto de Inclusão de CPF em formato Alfanumérico, garantindo alinhamento entre negócio, tecnologia e qualidade. Levantar, detalhar e priorizar requisitos junto aos stakeholders, assegurando clareza das regras de negócio e critérios de aceite. Gerenciar e priorizar o Product Backlog, mantendo foco em valor, risco e dependências técnicas. Definir e validar user stories, critérios de aceite e cenários de teste relacionados à mudança do formato do CPF. Conduzir alinhamentos com times de desenvolvimento e integrações para mitigar impactos em sistemas legados.  Contratação: PJ || Empresa .....:  SEMPRE IT SERVICOS DE TECNOLOGIA LTDA</t>
+        </is>
+      </c>
+      <c r="I333" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>19/01/2026</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>82941</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>Analista Dados Sênior</t>
+        </is>
+      </c>
+      <c r="D334" t="inlineStr">
+        <is>
+          <t>Sênior</t>
+        </is>
+      </c>
+      <c r="E334" t="inlineStr">
+        <is>
+          <t>Híbrido</t>
+        </is>
+      </c>
+      <c r="F334" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 17/01/26</t>
+        </is>
+      </c>
+      <c r="G334" t="inlineStr">
+        <is>
+          <t>Experiência sólida com Power BI (manutenção, DAX básica/intermediária, modelagem simples) Excel intermediário/avançado SQL intermediário/avançado (consultas, joins, agregações, filtros avançados) Vivência com Databricks (manipulação, consultas, extrações) Experiência comprovada com manutenção e evolução de relatórios Capacidade de comunicação, organização e alinhamento com times de negócio Autonomia para identificar inconsistências e resolver problemas sem supervisão constante. Vivência com automações simples (Power Automate, scripts básicos, etc.) Noções de ambientes de dados em nuvem Conhecimento de boas práticas de governança de dados.  Híbrido - SP Setor financeiro
+Empresa .....:  MJV SOLUCOES EM TECNOLOGIA LTDA</t>
+        </is>
+      </c>
+      <c r="H334" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 17/01/26 || Analista Dados Sênior || Experiência sólida com Power BI (manutenção, DAX básica/intermediária, modelagem simples) Excel intermediário/avançado SQL intermediário/avançado (consultas, joins, agregações, filtros avançados) Vivência com Databricks (manipulação, consultas, extrações) Experiência comprovada com manutenção e evolução de relatórios Capacidade de comunicação, organização e alinhamento com times de negócio Autonomia para identificar inconsistências e resolver problemas sem supervisão constante. Vivência com automações simples (Power Automate, scripts básicos, etc.) Noções de ambientes de dados em nuvem Conhecimento de boas práticas de governança de dados.  Híbrido - SP Setor financeiro || Empresa .....:  MJV SOLUCOES EM TECNOLOGIA LTDA</t>
+        </is>
+      </c>
+      <c r="I334" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>19/01/2026</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>83036</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>Analista de Infraestrutura Sênior</t>
+        </is>
+      </c>
+      <c r="D335" t="inlineStr">
+        <is>
+          <t>Sênior</t>
+        </is>
+      </c>
+      <c r="E335" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F335" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 17/01/26</t>
+        </is>
+      </c>
+      <c r="G335" t="inlineStr">
+        <is>
+          <t>Experiência Técnica: Foco em implementação de projetos. Possuir vivência com projetos de infraestrutura. Experiência na área de tecnologia, preferencialmente na área bancária/financeira. Administração de Windows Server (desejável/diferencial ter Certificação). Administração de Linux Server (RedHat). Básico de Telecom (Switches, Roteadores, Vlan, Link de Dados) - Telecom (manutenção de terminais IPC e testes de gravações Verint). DFS. Citrix e Virtualização (Vmware / Oracle OLVM). Ferramentas de backup: Veeam. Ferramentas de e-mail e ferramentas de monitoramento como: SCOM, HPOpenView for Linux, Fluke NetFlow, Cacti e NNMi. SCCM. Administração de Storage / servidores Blades. Noções de Cloud. DESEJÁVEL certificação ITIL V3.  Formação Acadêmica: Superior Completo.  Idioma: Inglês avançado para conversação.  Observações: Local de trabalho: Morumbi. Vaga Híbrida uma vez por semana presencial.
+Empresa .....:  Emphasys IT Services</t>
+        </is>
+      </c>
+      <c r="H335" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 17/01/26 || Analista de Infraestrutura Sênior || Experiência Técnica: Foco em implementação de projetos. Possuir vivência com projetos de infraestrutura. Experiência na área de tecnologia, preferencialmente na área bancária/financeira. Administração de Windows Server (desejável/diferencial ter Certificação). Administração de Linux Server (RedHat). Básico de Telecom (Switches, Roteadores, Vlan, Link de Dados) - Telecom (manutenção de terminais IPC e testes de gravações Verint). DFS. Citrix e Virtualização (Vmware / Oracle OLVM). Ferramentas de backup: Veeam. Ferramentas de e-mail e ferramentas de monitoramento como: SCOM, HPOpenView for Linux, Fluke NetFlow, Cacti e NNMi. SCCM. Administração de Storage / servidores Blades. Noções de Cloud. DESEJÁVEL certificação ITIL V3.  Formação Acadêmica: Superior Completo.  Idioma: Inglês avançado para conversação.  Observações: Local de trabalho: Morumbi. Vaga Híbrida uma vez por semana presencial. || Empresa .....:  Emphasys IT Services</t>
+        </is>
+      </c>
+      <c r="I335" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>19/01/2026</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>82815</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>Analista de Produto Pleno</t>
+        </is>
+      </c>
+      <c r="D336" t="inlineStr">
+        <is>
+          <t>Pleno</t>
+        </is>
+      </c>
+      <c r="E336" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F336" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 17/01/26</t>
+        </is>
+      </c>
+      <c r="G336" t="inlineStr">
+        <is>
+          <t>Definir, priorizar e gerenciar o backlog do produto, assegurando alinhamento com a visão estratégica e os objetivos do negócio. Colaborar com as equipes de desenvolvimento para elaboração de user stories completas, com critérios de aceitação bem definidos e compreensíveis. Assegurar entregas contínuas de valor para os stakeholders, acompanhando a evolução das funcionalidades e avaliando impactos. Participar de todas as cerimônias ágeis, incluindo planejamento, refinamento, reviews e retrospectivas, contribuindo de maneira ativa e orientada a resultados. Facilitar a comunicação entre stakeholders e a equipe de desenvolvimento, garantindo clareza, alinhamento e transparência ao longo de todo o ciclo de vida do produto.  Modelo híbrido (3x presencial, 2x home office) Local: Vila Congonhas Regime de contratação: PJ Budget: R$ 6.500,00
+Empresa .....:  Devpartner</t>
+        </is>
+      </c>
+      <c r="H336" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 17/01/26 || Analista de Produto Pleno || Definir, priorizar e gerenciar o backlog do produto, assegurando alinhamento com a visão estratégica e os objetivos do negócio. Colaborar com as equipes de desenvolvimento para elaboração de user stories completas, com critérios de aceitação bem definidos e compreensíveis. Assegurar entregas contínuas de valor para os stakeholders, acompanhando a evolução das funcionalidades e avaliando impactos. Participar de todas as cerimônias ágeis, incluindo planejamento, refinamento, reviews e retrospectivas, contribuindo de maneira ativa e orientada a resultados. Facilitar a comunicação entre stakeholders e a equipe de desenvolvimento, garantindo clareza, alinhamento e transparência ao longo de todo o ciclo de vida do produto.  Modelo híbrido (3x presencial, 2x home office) Local: Vila Congonhas Regime de contratação: PJ Budget: R$ 6.500,00 || Empresa .....:  Devpartner</t>
+        </is>
+      </c>
+      <c r="I336" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>19/01/2026</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>82110</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>Analista de Segurança Sr</t>
+        </is>
+      </c>
+      <c r="D337" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E337" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F337" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 17/01/26</t>
+        </is>
+      </c>
+      <c r="G337" t="inlineStr">
+        <is>
+          <t>•  Atuação na interface com fornecedores e com outras áreas •  Atividades relacionadas a administração, operação, implantação e suporte de equipamentos e soluções de segurança com ênfase no ambiente de Datacenter •  Proposição e execução de melhorias e projetos no ambiente •  Firewall (Checkpoint e Cisco ASA) •  IDS/IPS (Trellix) •  Packet broker (Gigamon) •  Algosec •  Cofre de Senhas •  VPN •  WAF •  NDR/XDR •  Certificação ITIL 4 Foundation  Treinamentos abaixo: •  EXIN - ISF -Information Security Foundation (ISO 27001) •  F5 101 •  F5 201 •  Cisco SCOR •  Cisco CyberOps •  Cisco CCNA •  CheckPoint CCSA •  CheckPoint CCSE •  ITILv4 Specialist Drive Stakeholder Value
+Empresa .....:  Cast</t>
+        </is>
+      </c>
+      <c r="H337" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 17/01/26 || Analista de Segurança Sr || •  Atuação na interface com fornecedores e com outras áreas •  Atividades relacionadas a administração, operação, implantação e suporte de equipamentos e soluções de segurança com ênfase no ambiente de Datacenter •  Proposição e execução de melhorias e projetos no ambiente •  Firewall (Checkpoint e Cisco ASA) •  IDS/IPS (Trellix) •  Packet broker (Gigamon) •  Algosec •  Cofre de Senhas •  VPN •  WAF •  NDR/XDR •  Certificação ITIL 4 Foundation  Treinamentos abaixo: •  EXIN - ISF -Information Security Foundation (ISO 27001) •  F5 101 •  F5 201 •  Cisco SCOR •  Cisco CyberOps •  Cisco CCNA •  CheckPoint CCSA •  CheckPoint CCSE •  ITILv4 Specialist Drive Stakeholder Value || Empresa .....:  Cast</t>
+        </is>
+      </c>
+      <c r="I337" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>19/01/2026</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>83284</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>Analista de Service Desk Jr. (PJ)</t>
+        </is>
+      </c>
+      <c r="D338" t="inlineStr">
+        <is>
+          <t>Júnior</t>
+        </is>
+      </c>
+      <c r="E338" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F338" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 17/01/26</t>
+        </is>
+      </c>
+      <c r="G338" t="inlineStr">
+        <is>
+          <t>Atuação como primeiro ponto de contato para suporte de TI, realizando registro, diagnóstico, resolução e acompanhamento de incidentes e requisições. Foco em atendimento ágil, organizado e dentro dos SLAs, garantindo a estabilidade do ambiente de Workplace.  - Modelo: PJ - Atuação: Presencial - Local: 3x no Butantã (Zona Oeste/SP), 2x em Barueri e 2 sábados do mês remoto  - Escalas: Seg a sex das 06:40 às 15:00 + 2 sábados/mês (06:40 às 15:00) Seg a sex das 10:40 às 19:00 + 2 sábados/mês (06:40 às 14:00)  - Remuneração: R$ 3.000,00 PJ + Totalpass  Atividades: Atendimento a usuários via telefone, portal e canais definidos Registro, classificação e tratamento de chamados em ferramenta ITSM Suporte N1 para Windows, macOS, Google Workspace, smartphones, impressoras e sistemas corporativos Acesso remoto (TeamViewer ou similares) Escalonamento e acompanhamento de tickets até a resolução Apoio à base de conhecimento, catálogo de serviços e cumprimento de SLAs
+Empresa .....:  FindUP</t>
+        </is>
+      </c>
+      <c r="H338" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 17/01/26 || Analista de Service Desk Jr. (PJ) || Atuação como primeiro ponto de contato para suporte de TI, realizando registro, diagnóstico, resolução e acompanhamento de incidentes e requisições. Foco em atendimento ágil, organizado e dentro dos SLAs, garantindo a estabilidade do ambiente de Workplace.  - Modelo: PJ - Atuação: Presencial - Local: 3x no Butantã (Zona Oeste/SP), 2x em Barueri e 2 sábados do mês remoto  - Escalas: Seg a sex das 06:40 às 15:00 + 2 sábados/mês (06:40 às 15:00) Seg a sex das 10:40 às 19:00 + 2 sábados/mês (06:40 às 14:00)  - Remuneração: R$ 3.000,00 PJ + Totalpass  Atividades: Atendimento a usuários via telefone, portal e canais definidos Registro, classificação e tratamento de chamados em ferramenta ITSM Suporte N1 para Windows, macOS, Google Workspace, smartphones, impressoras e sistemas corporativos Acesso remoto (TeamViewer ou similares) Escalonamento e acompanhamento de tickets até a resolução Apoio à base de conhecimento, catálogo de serviços e cumprimento de SLAs || Empresa .....:  FindUP</t>
+        </is>
+      </c>
+      <c r="I338" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>19/01/2026</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>82902</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>Analista de Sustentação</t>
+        </is>
+      </c>
+      <c r="D339" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E339" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F339" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 17/01/26</t>
+        </is>
+      </c>
+      <c r="G339" t="inlineStr">
+        <is>
+          <t>Analista – Sustentação de Sistemas e Aplicações – Sênior Presencial – Chácara Santo Antônio Horário a definir, com escalas diurnas e noturnas.  REQUISITOS E QUALIFICAÇÕES Inglês avançado (conversação e escrita) e espanhol básico. Graduação preferencialmente em Tecnologia da Informação, Análise e Desenvolvimento de Sistemas, Engenharias em geral, Administração ou outras formações com experiência em Tecnologia. Conhecimento em ambientes de infraestrutura de TI, datacenter, cloud, redes e telecom. Experiência na área de sustentação de sistemas (mínimo de 5 anos será um diferencial). Forte senso de autodisciplina, trabalho em equipe e prontidão para tomada de decisão e escalonamento de assuntos. Resiliência para atuar em ambiente crítico (crises). Vivência com sustentação de sistemas e continuidade de negócio. Excelentes habilidades de comunicação, com escuta ativa e clareza na transmissão de informações.
+Empresa .....:  Mazzatech</t>
+        </is>
+      </c>
+      <c r="H339" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 17/01/26 || Analista de Sustentação || Analista – Sustentação de Sistemas e Aplicações – Sênior Presencial – Chácara Santo Antônio Horário a definir, com escalas diurnas e noturnas.  REQUISITOS E QUALIFICAÇÕES Inglês avançado (conversação e escrita) e espanhol básico. Graduação preferencialmente em Tecnologia da Informação, Análise e Desenvolvimento de Sistemas, Engenharias em geral, Administração ou outras formações com experiência em Tecnologia. Conhecimento em ambientes de infraestrutura de TI, datacenter, cloud, redes e telecom. Experiência na área de sustentação de sistemas (mínimo de 5 anos será um diferencial). Forte senso de autodisciplina, trabalho em equipe e prontidão para tomada de decisão e escalonamento de assuntos. Resiliência para atuar em ambiente crítico (crises). Vivência com sustentação de sistemas e continuidade de negócio. Excelentes habilidades de comunicação, com escuta ativa e clareza na transmissão de informações. || Empresa .....:  Mazzatech</t>
+        </is>
+      </c>
+      <c r="I339" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>19/01/2026</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>81811</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>ANALISTA FUNCIONAL PLENO (PROTHEUS)</t>
+        </is>
+      </c>
+      <c r="D340" t="inlineStr">
+        <is>
+          <t>Pleno</t>
+        </is>
+      </c>
+      <c r="E340" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F340" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 17/01/26</t>
+        </is>
+      </c>
+      <c r="G340" t="inlineStr">
+        <is>
+          <t>Requisitos: Experiência funcional em TOTVS Protheus (módulos: Compras, Financeiro, Faturamento, Fiscal, Contábil, PCP e Estoque/Custos) Desejável conhecimento em módulos de logística (SIGAWMS, SIGAGFE) Formação ou experiência em Contabilidade Noções técnicas em ADVPL e SQL (para entendimento).  Atuação Híbrida – 2x por semana (1x Nações Unidas e 1x Bom Sucesso – Guarulhos).
+Empresa .....:  CAPITANI CONSULTORIA E SISTEMAS LTDA</t>
+        </is>
+      </c>
+      <c r="H340" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 17/01/26 || ANALISTA FUNCIONAL PLENO (PROTHEUS) || Requisitos: Experiência funcional em TOTVS Protheus (módulos: Compras, Financeiro, Faturamento, Fiscal, Contábil, PCP e Estoque/Custos) Desejável conhecimento em módulos de logística (SIGAWMS, SIGAGFE) Formação ou experiência em Contabilidade Noções técnicas em ADVPL e SQL (para entendimento).  Atuação Híbrida – 2x por semana (1x Nações Unidas e 1x Bom Sucesso – Guarulhos). || Empresa .....:  CAPITANI CONSULTORIA E SISTEMAS LTDA</t>
+        </is>
+      </c>
+      <c r="I340" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>19/01/2026</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>82291</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>Analista Sênior Python (Oracle/PLSQL)</t>
+        </is>
+      </c>
+      <c r="D341" t="inlineStr">
+        <is>
+          <t>Sênior</t>
+        </is>
+      </c>
+      <c r="E341" t="inlineStr">
+        <is>
+          <t>Híbrido</t>
+        </is>
+      </c>
+      <c r="F341" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 17/01/26</t>
+        </is>
+      </c>
+      <c r="G341" t="inlineStr">
+        <is>
+          <t>Analista Sênior de Desenvolvimento Python (Oracle/PLSQL - TOTVS RM)  Híbrido - 4 presenciais - Bom Retiro – São Paulo/SP PJ  Domínio de Python 3.x APIs (FastAPI/Flask), testes (pytest), logging/observabilidade, packaging, virtualenv/poetry, tratamento de filas (Celery/RQ), consumo/produção de ETL e integrações PL/SQL avançado (packages, procedures, triggers), tuning (explain plan, índices, hints, estatísticas), views/materialized views, jobs (DBMS_SCHEDULER), criação de objetos para BI (consultas SQL otimizadas para cubos/relatórios), gestão de permissões Leitura do modelo de dados, consultas para cubos/visões do RM, uso de consultas SQL associadas a cubos e painéis de cenário entendimento de conectividade Oracle com o RM.  Diferenciais: Experiência no setor autopeças/distribuição Monitoramento (Prometheus/Grafana), mensageria (RabbitMQ/Redis), PowerBI/Dataviz Experiência com portabilidade/migração RM em Oracle.
+Empresa .....:  Entrust It</t>
+        </is>
+      </c>
+      <c r="H341" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 17/01/26 || Analista Sênior Python (Oracle/PLSQL) || Analista Sênior de Desenvolvimento Python (Oracle/PLSQL - TOTVS RM)  Híbrido - 4 presenciais - Bom Retiro – São Paulo/SP PJ  Domínio de Python 3.x APIs (FastAPI/Flask), testes (pytest), logging/observabilidade, packaging, virtualenv/poetry, tratamento de filas (Celery/RQ), consumo/produção de ETL e integrações PL/SQL avançado (packages, procedures, triggers), tuning (explain plan, índices, hints, estatísticas), views/materialized views, jobs (DBMS_SCHEDULER), criação de objetos para BI (consultas SQL otimizadas para cubos/relatórios), gestão de permissões Leitura do modelo de dados, consultas para cubos/visões do RM, uso de consultas SQL associadas a cubos e painéis de cenário entendimento de conectividade Oracle com o RM.  Diferenciais: Experiência no setor autopeças/distribuição Monitoramento (Prometheus/Grafana), mensageria (RabbitMQ/Redis), PowerBI/Dataviz Experiência com portabilidade/migração RM em Oracle. || Empresa .....:  Entrust It</t>
+        </is>
+      </c>
+      <c r="I341" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>19/01/2026</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>82827</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>CIENTISTA DE DADOS - IA</t>
+        </is>
+      </c>
+      <c r="D342" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E342" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F342" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 17/01/26</t>
+        </is>
+      </c>
+      <c r="G342" t="inlineStr">
+        <is>
+          <t>Atuação Totalmente remoto  Contratação PJ  Requisitos: - Experiência sólida em projetos de Ciência de Dados. - Conhecimento avançado em Machine Learning, LLMs e AI Agents. - Experiência em deploy de modelos em nuvem (Azure). - Fluência em Python, SQL e frameworks de Big Data. - EXPERIÊNCIA PRÁTICA COM AI AGENTES (LANGCHAIN, AUTOGEN, RAG, FRAMEWORKS LLMOps). - Experiência com CI/CD e automação de pipelines. - Vivência com monitoramento e retraining de modelos em produção. - Capacidade de traduzir problemas complexos em soluções técnicas aplicáveis ao negócio.  Diferencial: - Inglês - Experiência com Framework Web de Python (Django, Flask, FastAPI) - Experiência com Docker, Kubernetes, - Experiência em Engenharia de Dados.
+Empresa .....:  KLB Group</t>
+        </is>
+      </c>
+      <c r="H342" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 17/01/26 || CIENTISTA DE DADOS - IA || Atuação Totalmente remoto  Contratação PJ  Requisitos: - Experiência sólida em projetos de Ciência de Dados. - Conhecimento avançado em Machine Learning, LLMs e AI Agents. - Experiência em deploy de modelos em nuvem (Azure). - Fluência em Python, SQL e frameworks de Big Data. - EXPERIÊNCIA PRÁTICA COM AI AGENTES (LANGCHAIN, AUTOGEN, RAG, FRAMEWORKS LLMOps). - Experiência com CI/CD e automação de pipelines. - Vivência com monitoramento e retraining de modelos em produção. - Capacidade de traduzir problemas complexos em soluções técnicas aplicáveis ao negócio.  Diferencial: - Inglês - Experiência com Framework Web de Python (Django, Flask, FastAPI) - Experiência com Docker, Kubernetes, - Experiência em Engenharia de Dados. || Empresa .....:  KLB Group</t>
+        </is>
+      </c>
+      <c r="I342" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>19/01/2026</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>81718</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>DA – Data Engineer</t>
+        </is>
+      </c>
+      <c r="D343" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E343" t="inlineStr">
+        <is>
+          <t>Híbrido</t>
+        </is>
+      </c>
+      <c r="F343" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 17/01/26</t>
+        </is>
+      </c>
+      <c r="G343" t="inlineStr">
+        <is>
+          <t>DA – Data Engineer Hibrido Esporadico Inglês avançado - CLT  Habilidade Principal: AWS, Databricks, Python, Pyspark, SQL  Qualificações Necessárias AWS, Databricks, Python, Pyspark, SQL  Principais Atividades e Responsabilidades Analista com 2 a 3 anos de experiência, com conhecimento em: Python / Spark SQL (para codificação em Databricks) Serviços AWS (S3, EC2, Lambda, SQS, SNS, DynamoDB, OpenSearch, etc.) GitHub (para controle de versão) GitHub Actions para CI/CD  Soft Skills (Características Pessoais) Boa capacidade analítica e fluência em comunicação em inglês.
+Empresa .....:  CIDIC</t>
+        </is>
+      </c>
+      <c r="H343" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 17/01/26 || DA – Data Engineer || DA – Data Engineer Hibrido Esporadico Inglês avançado - CLT  Habilidade Principal: AWS, Databricks, Python, Pyspark, SQL  Qualificações Necessárias AWS, Databricks, Python, Pyspark, SQL  Principais Atividades e Responsabilidades Analista com 2 a 3 anos de experiência, com conhecimento em: Python / Spark SQL (para codificação em Databricks) Serviços AWS (S3, EC2, Lambda, SQS, SNS, DynamoDB, OpenSearch, etc.) GitHub (para controle de versão) GitHub Actions para CI/CD  Soft Skills (Características Pessoais) Boa capacidade analítica e fluência em comunicação em inglês. || Empresa .....:  CIDIC</t>
+        </is>
+      </c>
+      <c r="I343" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>19/01/2026</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>83003</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>Desenvolvedor Fullstack</t>
+        </is>
+      </c>
+      <c r="D344" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E344" t="inlineStr">
+        <is>
+          <t>Híbrido</t>
+        </is>
+      </c>
+      <c r="F344" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 17/01/26</t>
+        </is>
+      </c>
+      <c r="G344" t="inlineStr">
+        <is>
+          <t>Prazo: 5 meses, com chances de prorrogar Local:Híbrido - São Paulo (Chácara Santo Antônio) Contratação: PJ  Requisitos: Experiência sólida com Angular (preferencialmente versões 12+) Conhecimento em TypeScript, HTML5, CSS3 e JavaScript (ES6+). Experiência com RxJS, Angular CLI, Lazy Loading e State Management (NgRx ou similar) Integração com APIs REST e consumo de serviços Conhecimento em Git/ DevOps e práticas de versionamento Familiaridade com Testes Unitários e boas práticas de qualidade Noções de CI/CD e ferramentas como Azure DevOps, GitHub Actions ou similares Conhecimento em PostgreSQL Experiência com RESTful APIs e boas práticas de arquitetura de software Plataforma .NET (C#) SQL Server 2012-2016 Github Copilot
+Empresa .....:  Entrust IT</t>
+        </is>
+      </c>
+      <c r="H344" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 17/01/26 || Desenvolvedor Fullstack || Prazo: 5 meses, com chances de prorrogar Local:Híbrido - São Paulo (Chácara Santo Antônio) Contratação: PJ  Requisitos: Experiência sólida com Angular (preferencialmente versões 12+) Conhecimento em TypeScript, HTML5, CSS3 e JavaScript (ES6+). Experiência com RxJS, Angular CLI, Lazy Loading e State Management (NgRx ou similar) Integração com APIs REST e consumo de serviços Conhecimento em Git/ DevOps e práticas de versionamento Familiaridade com Testes Unitários e boas práticas de qualidade Noções de CI/CD e ferramentas como Azure DevOps, GitHub Actions ou similares Conhecimento em PostgreSQL Experiência com RESTful APIs e boas práticas de arquitetura de software Plataforma .NET (C#) SQL Server 2012-2016 Github Copilot || Empresa .....:  Entrust IT</t>
+        </is>
+      </c>
+      <c r="I344" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>19/01/2026</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>82169</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>DESENVOLVEDOR JAVA PLENO - HÍBRIDO SÃO PAULO/SP</t>
+        </is>
+      </c>
+      <c r="D345" t="inlineStr">
+        <is>
+          <t>Pleno</t>
+        </is>
+      </c>
+      <c r="E345" t="inlineStr">
+        <is>
+          <t>Híbrido</t>
+        </is>
+      </c>
+      <c r="F345" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 17/01/26</t>
+        </is>
+      </c>
+      <c r="G345" t="inlineStr">
+        <is>
+          <t>ATUAÇÃO HÍBRIDA 3X POR SEMANA NO BAIRRO DO MORUMBI, ZONA SUL DE SÃO PAULO/SP Contratação CLT + Benefícios  Requisitos: · Superior completo na área de Tecnologia · INGLÊS INTERMEDIÁRIO (MANDATÓRIO) · Experiência com desenvolvimento em JAVA e nos frameworks Spring MVC e Spring Boot · Histórico do projeto de varejo/comércio eletrônico · Experiência com desenvolvimento orientado a testes e frameworks de testes automatizados, como JUnit. · Familiaridade com Git, pipelines de CI/CD e metodologias de desenvolvimento Ágil   Diferencial: · Experiência com projeto de E-commerce desenvolvidos em plataforma Hybris (SAP Commerce Cloud) · Experiência com plataformas de nuvem (AWS, Azure ou SAP Cloud Platform). · Espanhol básico  Escopo: · Aprender a desenvolver na SAP Commerce(Hybris) plataforma baseada em JAVA no framework SPRING e adicionalmente aprender das suas ferramentas tais como groovy e impex
+Empresa .....:  KLB Group</t>
+        </is>
+      </c>
+      <c r="H345" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 17/01/26 || DESENVOLVEDOR JAVA PLENO - HÍBRIDO SÃO PAULO/SP || ATUAÇÃO HÍBRIDA 3X POR SEMANA NO BAIRRO DO MORUMBI, ZONA SUL DE SÃO PAULO/SP Contratação CLT + Benefícios  Requisitos: · Superior completo na área de Tecnologia · INGLÊS INTERMEDIÁRIO (MANDATÓRIO) · Experiência com desenvolvimento em JAVA e nos frameworks Spring MVC e Spring Boot · Histórico do projeto de varejo/comércio eletrônico · Experiência com desenvolvimento orientado a testes e frameworks de testes automatizados, como JUnit. · Familiaridade com Git, pipelines de CI/CD e metodologias de desenvolvimento Ágil   Diferencial: · Experiência com projeto de E-commerce desenvolvidos em plataforma Hybris (SAP Commerce Cloud) · Experiência com plataformas de nuvem (AWS, Azure ou SAP Cloud Platform). · Espanhol básico  Escopo: · Aprender a desenvolver na SAP Commerce(Hybris) plataforma baseada em JAVA no framework SPRING e adicionalmente aprender das suas ferramentas tais como groovy e impex || Empresa .....:  KLB Group</t>
+        </is>
+      </c>
+      <c r="I345" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>19/01/2026</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>82759</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>Desenvolvedor Java Sênior Remoto ou Híbrido (SP)</t>
+        </is>
+      </c>
+      <c r="D346" t="inlineStr">
+        <is>
+          <t>Sênior</t>
+        </is>
+      </c>
+      <c r="E346" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F346" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 17/01/26</t>
+        </is>
+      </c>
+      <c r="G346" t="inlineStr">
+        <is>
+          <t>Obrigatório graduação superior completa, preferencialmente em Sistemas de Informação, Análise de Sistemas, Ciência da Computação, Engenharia da Computação ou áreas relacionadas  Experiência com Java, Design Patterns e Arquitetura de Microserviços Conhecimentos em Containers, Kubernetes e Microserviços Conhecimentos em diferentes tipos de mensageria (RabbitMQ, Kafka, etc) Conhecimentos em tecnologias AWS (EKS, SNS, SQS, S3, DocumentDB, Secret Manager, API Gateway, Lambda, Dynamo, etc) Conhecimentos com banco de dados (PostgreSQL, DocumentDB, Redis)  Desejável conhecimento de mercado financeiro Boa comunicação interpessoal e capacidade de colaboração com diferentes áreas da empresa.  Diferencial Inglês intermediário/avançado Remoto ou Híbrido (SP)
+Empresa .....:  MJV SOLUCOES EM TECNOLOGIA LTDA</t>
+        </is>
+      </c>
+      <c r="H346" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 17/01/26 || Desenvolvedor Java Sênior Remoto ou Híbrido (SP) || Obrigatório graduação superior completa, preferencialmente em Sistemas de Informação, Análise de Sistemas, Ciência da Computação, Engenharia da Computação ou áreas relacionadas  Experiência com Java, Design Patterns e Arquitetura de Microserviços Conhecimentos em Containers, Kubernetes e Microserviços Conhecimentos em diferentes tipos de mensageria (RabbitMQ, Kafka, etc) Conhecimentos em tecnologias AWS (EKS, SNS, SQS, S3, DocumentDB, Secret Manager, API Gateway, Lambda, Dynamo, etc) Conhecimentos com banco de dados (PostgreSQL, DocumentDB, Redis)  Desejável conhecimento de mercado financeiro Boa comunicação interpessoal e capacidade de colaboração com diferentes áreas da empresa.  Diferencial Inglês intermediário/avançado Remoto ou Híbrido (SP) || Empresa .....:  MJV SOLUCOES EM TECNOLOGIA LTDA</t>
+        </is>
+      </c>
+      <c r="I346" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>19/01/2026</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>81798</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>DESENVOLVEDOR RPA PLENO - INGLÊS - HÍBRIDO SP</t>
+        </is>
+      </c>
+      <c r="D347" t="inlineStr">
+        <is>
+          <t>Pleno</t>
+        </is>
+      </c>
+      <c r="E347" t="inlineStr">
+        <is>
+          <t>Híbrido</t>
+        </is>
+      </c>
+      <c r="F347" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 17/01/26</t>
+        </is>
+      </c>
+      <c r="G347" t="inlineStr">
+        <is>
+          <t>ATUAÇÃO HÍBRIDA 03 X POR SEMANA NO BAIRRO DO MORUMBI, ZONA SUL DE SÃO PAULO/SP  Horário de Trabalho: das 09hs às 18hs Contratação CLT + Benefícios  Requisitos: - Superior completo em Tecnologia - INGLÊS AVANÇADO (MANDATÓRIO) - Experiência de pelo menos dois anos em programação (Python ou Java). - Interesse em aprender e crescer na área de Automação de Processos Robóticos (RPA).   DESEJÁVEL: - Experiência prévia em desenvolvimento de software ou automação de processos. - Conhecimento básico em ferramentas de automação de processos RPA, como UiPath, Automation Anywhere ou Blue Prism. - Certificações em RPA ou áreas relacionadas.  Escopo* · Auxiliar no levantamento e análise de processos para identificar oportunidades de automação. · Participar do desenvolvimento e implementação de soluções de automação usando ferramentas RPA.
+Empresa .....:  KLB Group</t>
+        </is>
+      </c>
+      <c r="H347" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 17/01/26 || DESENVOLVEDOR RPA PLENO - INGLÊS - HÍBRIDO SP || ATUAÇÃO HÍBRIDA 03 X POR SEMANA NO BAIRRO DO MORUMBI, ZONA SUL DE SÃO PAULO/SP  Horário de Trabalho: das 09hs às 18hs Contratação CLT + Benefícios  Requisitos: - Superior completo em Tecnologia - INGLÊS AVANÇADO (MANDATÓRIO) - Experiência de pelo menos dois anos em programação (Python ou Java). - Interesse em aprender e crescer na área de Automação de Processos Robóticos (RPA).   DESEJÁVEL: - Experiência prévia em desenvolvimento de software ou automação de processos. - Conhecimento básico em ferramentas de automação de processos RPA, como UiPath, Automation Anywhere ou Blue Prism. - Certificações em RPA ou áreas relacionadas.  Escopo* · Auxiliar no levantamento e análise de processos para identificar oportunidades de automação. · Participar do desenvolvimento e implementação de soluções de automação usando ferramentas RPA. || Empresa .....:  KLB Group</t>
+        </is>
+      </c>
+      <c r="I347" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>19/01/2026</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>82949</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>Engenheiro de Dados</t>
+        </is>
+      </c>
+      <c r="D348" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E348" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F348" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 17/01/26</t>
+        </is>
+      </c>
+      <c r="G348" t="inlineStr">
+        <is>
+          <t>Responsabilidades Estruturar pipelines de dados usando Databricks Desenvolver e manter processos de ETL / ELT, desde a ingestão até a consolidação Integrar dados vindos de múltiplas fontes e bancos (MySQL, Oracle, etc.) Atuar fortemente em data quality, limpeza, padronização e consistência dos dados Consolidar bases financeiras de diferentes unidades de negócio Preparar os dados para consumo futuro por ferramentas de BI e Analytics Apoiar definições de arquitetura e melhores estratégias de dados Atuar como referência técnica e mentor para o time Contribuir com análises voltadas à performance e eficiência do negócio  Req. Obrigatórios Experiência sólida como Engenheiro de Dados Sênior Domínio de Databricks (essencial) Forte conhecimento em modelagem e conceitos de banco de dados Experiência com múltiplas fontes de dados (MySQL, Oracle, entre outras) Vivência com ETL / ELT, integração e consolidação de dados Conhecimento em data quality e governança dados
+Empresa .....:  2BRAIN CONSULTORIA E ESTRATEGIA LTDA</t>
+        </is>
+      </c>
+      <c r="H348" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 17/01/26 || Engenheiro de Dados || Responsabilidades Estruturar pipelines de dados usando Databricks Desenvolver e manter processos de ETL / ELT, desde a ingestão até a consolidação Integrar dados vindos de múltiplas fontes e bancos (MySQL, Oracle, etc.) Atuar fortemente em data quality, limpeza, padronização e consistência dos dados Consolidar bases financeiras de diferentes unidades de negócio Preparar os dados para consumo futuro por ferramentas de BI e Analytics Apoiar definições de arquitetura e melhores estratégias de dados Atuar como referência técnica e mentor para o time Contribuir com análises voltadas à performance e eficiência do negócio  Req. Obrigatórios Experiência sólida como Engenheiro de Dados Sênior Domínio de Databricks (essencial) Forte conhecimento em modelagem e conceitos de banco de dados Experiência com múltiplas fontes de dados (MySQL, Oracle, entre outras) Vivência com ETL / ELT, integração e consolidação de dados Conhecimento em data quality e governança dados || Empresa .....:  2BRAIN CONSULTORIA E ESTRATEGIA LTDA</t>
+        </is>
+      </c>
+      <c r="I348" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>19/01/2026</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>82643</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>Engenheiro(a) de Infraestrutura de Dados Pleno II</t>
+        </is>
+      </c>
+      <c r="D349" t="inlineStr">
+        <is>
+          <t>Pleno</t>
+        </is>
+      </c>
+      <c r="E349" t="inlineStr">
+        <is>
+          <t>Híbrido</t>
+        </is>
+      </c>
+      <c r="F349" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 17/01/26</t>
+        </is>
+      </c>
+      <c r="G349" t="inlineStr">
+        <is>
+          <t>Engenheiro(a) de Infraestrutura de Dados Pleno II  Local: Híbrido - São Paulo/SP Modelo de contratação: (CLT/ PJ) Área: Tecnologia  Dados  Implementar e Manter a Infraestrutura de Dados: Projetar, construir e gerenciar ambientes escaláveis e robustos para processamento e armazenamento de dados, com foco em plataformas como Databricks Automatizar Pipelines: Desenvolver e otimizar pipelines CI/CD para implantação de infraestrutura Suporte a MLOps: Colaborar com Cientistas e Engenheiros de Dados na implementação de práticas e ferramentas de MLOps Gerenciamento de Recursos: Utilizar Terraform para provisionar e gerenciar recursos em nuvem (AWS, Azure ou GCP) Orquestração e Automação: Criar e gerenciar fluxos de trabalho de automação utilizando ferramentas como Jenkins ou GitHub Actions para deployments de infraestrutura e orquestração de tarefas de dados.
+Empresa .....:  Always On Digital</t>
+        </is>
+      </c>
+      <c r="H349" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 17/01/26 || Engenheiro(a) de Infraestrutura de Dados Pleno II || Engenheiro(a) de Infraestrutura de Dados Pleno II  Local: Híbrido - São Paulo/SP Modelo de contratação: (CLT/ PJ) Área: Tecnologia  Dados  Implementar e Manter a Infraestrutura de Dados: Projetar, construir e gerenciar ambientes escaláveis e robustos para processamento e armazenamento de dados, com foco em plataformas como Databricks Automatizar Pipelines: Desenvolver e otimizar pipelines CI/CD para implantação de infraestrutura Suporte a MLOps: Colaborar com Cientistas e Engenheiros de Dados na implementação de práticas e ferramentas de MLOps Gerenciamento de Recursos: Utilizar Terraform para provisionar e gerenciar recursos em nuvem (AWS, Azure ou GCP) Orquestração e Automação: Criar e gerenciar fluxos de trabalho de automação utilizando ferramentas como Jenkins ou GitHub Actions para deployments de infraestrutura e orquestração de tarefas de dados. || Empresa .....:  Always On Digital</t>
+        </is>
+      </c>
+      <c r="I349" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>19/01/2026</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>81806</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>Especialista Angular  (PJ)</t>
+        </is>
+      </c>
+      <c r="D350" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E350" t="inlineStr">
+        <is>
+          <t>Híbrido</t>
+        </is>
+      </c>
+      <c r="F350" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 17/01/26</t>
+        </is>
+      </c>
+      <c r="G350" t="inlineStr">
+        <is>
+          <t>Especialista em Front-end/Angular  (PJ) Empresa portuguesa de Tecnologia em expansão no Brasil Híbrido 2X semana região de Santo Amaro ou Interlagos Contratação PJ (valor mensal  fixo + 22 dias úteis de férias / ano)  Requisitos: Experiência com micro-front-ends. Domínio de Webpack, CI/CD para front-end e server-side rendering (SSR). Conhecimento avançado em Angular (otimização de performance, state management), RxJS, testes unitários (Jasmine/Karma) e E2E (Cypress/Protractor). Conhecimento aprofundado em arquitetura de aplicações de grande escala.  Responsabilidades: Liderar o desenvolvimento de funcionalidades complexas. Definir e implementar a arquitetura de front-end. Mentoria para desenvolvedores menos experientes.Desenvolver a arquitetura de sistemas front-end críticos. Pesquisar e implementar novas tecnologias e frameworks. Garantir a performance, escalabilidade da aplicação.
+Empresa .....:  Performance and Mind</t>
+        </is>
+      </c>
+      <c r="H350" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 17/01/26 || Especialista Angular  (PJ) || Especialista em Front-end/Angular  (PJ) Empresa portuguesa de Tecnologia em expansão no Brasil Híbrido 2X semana região de Santo Amaro ou Interlagos Contratação PJ (valor mensal  fixo + 22 dias úteis de férias / ano)  Requisitos: Experiência com micro-front-ends. Domínio de Webpack, CI/CD para front-end e server-side rendering (SSR). Conhecimento avançado em Angular (otimização de performance, state management), RxJS, testes unitários (Jasmine/Karma) e E2E (Cypress/Protractor). Conhecimento aprofundado em arquitetura de aplicações de grande escala.  Responsabilidades: Liderar o desenvolvimento de funcionalidades complexas. Definir e implementar a arquitetura de front-end. Mentoria para desenvolvedores menos experientes.Desenvolver a arquitetura de sistemas front-end críticos. Pesquisar e implementar novas tecnologias e frameworks. Garantir a performance, escalabilidade da aplicação. || Empresa .....:  Performance and Mind</t>
+        </is>
+      </c>
+      <c r="I350" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>19/01/2026</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>82340</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>Especialista em operações BPO</t>
+        </is>
+      </c>
+      <c r="D351" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E351" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F351" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 17/01/26</t>
+        </is>
+      </c>
+      <c r="G351" t="inlineStr">
+        <is>
+          <t>Atuar na área de BPO com foco em otimização de processos, gestão operacional e melhoria
+contínua.
+Supervisionar as operações de BPO, garantir qualidade, eficiência e cumprimento dos SLAs.
+Gerenciar o desempenho das equipes de atendimento internas ou terceiras (Call Centers).
+Mapear, revisar e otimizar processos de atendimento, suporte técnico e operacionais
+Atuar de forma integrada com as áreas de Infraestrutura, Desenvolvimento e DevOps para
+identificar e propor melhorias em sistemas e fluxos de trabalho
+Definir e acompanhar indicadores de desempenho (KPIs)
+Garantir a satisfação do cliente final.
+Requisitos:
+Experiência em operações de BPO (setor aéreo ou em empresas de grande porte)
+Experiência em Gestão de Atendimento (Call Centers) e Suporte Técnico
+Familiaridade com processos de Infraestrutura de TI, Desenvolvimento de Sistemas e práticas
+DevOp
+Horário Comercial
+PJ
+Presencial na região de Santo Amaro-SP (sexta-feira home office)
+Salário a combinar
+Empresa .....:  Soue Tech Serviços de Tecnologia Ltda</t>
+        </is>
+      </c>
+      <c r="H351" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 17/01/26 || Especialista em operações BPO || Atuar na área de BPO com foco em otimização de processos, gestão operacional e melhoria || contínua. || Supervisionar as operações de BPO, garantir qualidade, eficiência e cumprimento dos SLAs. || Gerenciar o desempenho das equipes de atendimento internas ou terceiras (Call Centers). || Mapear, revisar e otimizar processos de atendimento, suporte técnico e operacionais || Atuar de forma integrada com as áreas de Infraestrutura, Desenvolvimento e DevOps para || identificar e propor melhorias em sistemas e fluxos de trabalho || Definir e acompanhar indicadores de desempenho (KPIs) || Garantir a satisfação do cliente final. || Requisitos: || Experiência em operações de BPO (setor aéreo ou em empresas de grande porte) || Experiência em Gestão de Atendimento (Call Centers) e Suporte Técnico || Familiaridade com processos de Infraestrutura de TI, Desenvolvimento de Sistemas e práticas || DevOp || Horário Comercial || PJ || Presencial na região de Santo Amaro-SP (sexta-feira home office) || Salário a combinar || Empresa .....:  Soue Tech Serviços de Tecnologia Ltda</t>
+        </is>
+      </c>
+      <c r="I351" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>19/01/2026</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>82983</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>Especialista em Suporte de TI</t>
+        </is>
+      </c>
+      <c r="D352" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E352" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F352" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 17/01/26</t>
+        </is>
+      </c>
+      <c r="G352" t="inlineStr">
+        <is>
+          <t>O Especialista atuará como segundo nível de contato para lidar com problemas de suporte técnico dos parceiros de negócios. O foco principal é suporte documental e resolução de incidentes/solicitações de serviço enviadas de analistas de suporte do Service Desk ou por autoatendimento. Além disso, o mesmo irá orientar novos funcionários da equipe, tratar de questões complexas e também liderar e participar do projeto e do trabalho de mudança.  REQUISITOS: Inglês avançado, espanhol desejável (para contato com o time internacional) Experiência com sistema operacional Windows, Apple OS, Active Directory, MS Office Suite, sistemas de bilhetagem, call center, dispositivos móveis e antivírus/spyware. Proficiência técnica: compreensão das tecnologias de telecomunicações, incluindo VoIP, PBX e SIP (Session Initiation Protocol). Familiarizado com os processos e estrutura ITIL. Certificação ITIL v3 ou 2011 uma vantagem.  Presencial 4x na semana - 1x remoto  Morumbi, SP
+Empresa .....:  TOPMIND IT</t>
+        </is>
+      </c>
+      <c r="H352" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 17/01/26 || Especialista em Suporte de TI || O Especialista atuará como segundo nível de contato para lidar com problemas de suporte técnico dos parceiros de negócios. O foco principal é suporte documental e resolução de incidentes/solicitações de serviço enviadas de analistas de suporte do Service Desk ou por autoatendimento. Além disso, o mesmo irá orientar novos funcionários da equipe, tratar de questões complexas e também liderar e participar do projeto e do trabalho de mudança.  REQUISITOS: Inglês avançado, espanhol desejável (para contato com o time internacional) Experiência com sistema operacional Windows, Apple OS, Active Directory, MS Office Suite, sistemas de bilhetagem, call center, dispositivos móveis e antivírus/spyware. Proficiência técnica: compreensão das tecnologias de telecomunicações, incluindo VoIP, PBX e SIP (Session Initiation Protocol). Familiarizado com os processos e estrutura ITIL. Certificação ITIL v3 ou 2011 uma vantagem.  Presencial 4x na semana - 1x remoto  Morumbi, SP || Empresa .....:  TOPMIND IT</t>
+        </is>
+      </c>
+      <c r="I352" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>19/01/2026</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>82666</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>Especialista em TOTVS RM</t>
+        </is>
+      </c>
+      <c r="D353" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E353" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F353" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 17/01/26</t>
+        </is>
+      </c>
+      <c r="G353" t="inlineStr">
+        <is>
+          <t>Suporte técnico aos usuários do sistema Totvs RH (Linha RM), solucionando problemas, analisando processos, desempenho, funcionalidades, melhorias e regras de negócios. Documentação de processos, customizações e particularidades do funcionamento do sistema. Análise e levantamento de necessidades para implantação de novos módulos e rotinas visando melhorias e automatização nos processos da empresa.  Contato com o fornecedor Totvs para acompanhamento da evolução e solução de problemas no sistema. Testes de pacotes de atualização e novas versões da Totvs antes da implantação em produção. Atualização do sistema em ambiente de produção e acompanhamento da execução. Desenvolvimento de relatórios, consultas e customizações para adequação do sistema às necessidades da entidade conforme as regras de negócio aplicáveis.  Preparação e apresentação de conteúdo para instrução e treinamento dos usuários do sistema. Preferencialmente com experiencia no modulo construção.
+Empresa .....:  CRA ENGENHARIA DE INFRAESTRUTURA LTDA</t>
+        </is>
+      </c>
+      <c r="H353" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 17/01/26 || Especialista em TOTVS RM || Suporte técnico aos usuários do sistema Totvs RH (Linha RM), solucionando problemas, analisando processos, desempenho, funcionalidades, melhorias e regras de negócios. Documentação de processos, customizações e particularidades do funcionamento do sistema. Análise e levantamento de necessidades para implantação de novos módulos e rotinas visando melhorias e automatização nos processos da empresa.  Contato com o fornecedor Totvs para acompanhamento da evolução e solução de problemas no sistema. Testes de pacotes de atualização e novas versões da Totvs antes da implantação em produção. Atualização do sistema em ambiente de produção e acompanhamento da execução. Desenvolvimento de relatórios, consultas e customizações para adequação do sistema às necessidades da entidade conforme as regras de negócio aplicáveis.  Preparação e apresentação de conteúdo para instrução e treinamento dos usuários do sistema. Preferencialmente com experiencia no modulo construção. || Empresa .....:  CRA ENGENHARIA DE INFRAESTRUTURA LTDA</t>
+        </is>
+      </c>
+      <c r="I353" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>19/01/2026</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>83006</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>Field - JR</t>
+        </is>
+      </c>
+      <c r="D354" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E354" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F354" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 17/01/26</t>
+        </is>
+      </c>
+      <c r="G354" t="inlineStr">
+        <is>
+          <t>execução do serviço de Mapeamento e Inventário Físico Detalhado dos ativos de tecnologia (servidores, switches, etc.) instalados em Data Centers Presencial - SP - 1 mês - PJ
+Empresa .....:  Randstad</t>
+        </is>
+      </c>
+      <c r="H354" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 17/01/26 || Field - JR || execução do serviço de Mapeamento e Inventário Físico Detalhado dos ativos de tecnologia (servidores, switches, etc.) instalados em Data Centers Presencial - SP - 1 mês - PJ || Empresa .....:  Randstad</t>
+        </is>
+      </c>
+      <c r="I354" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>19/01/2026</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>83292</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>Gerente de Projetos</t>
+        </is>
+      </c>
+      <c r="D355" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E355" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F355" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 17/01/26</t>
+        </is>
+      </c>
+      <c r="G355" t="inlineStr">
+        <is>
+          <t>Gerente de Projetos Sênior  Você é um(a) profissional experiente na gestão de iniciativas complexas e de grande escala, com histórico comprovado de entregas bem-sucedidas? Tem interesse em coordenar múltiplas atividades interdependentes e garantir a evolução contínua dos projetos?  Estamos em busca de um(a) Gerente de Projetos Sênior para liderar a integração geral do CS Latam. com foco principal na incorporação do stack tecnológico do Brasil ao Banco.  Principais responsabilidades: Apoiar a integração de soluções tecnológicas, viabilizando a expansão da oferta de produtos do Banco Desenvolver planos e garantir o progresso da refatoração de aplicações conforme os Padrões Tecnológicos do Banco, incluindo rebranding e integração de sistemas core em uma plataforma única Conduzir a reestruturação e padronização das aplicações para consumo de serviços bancários, substituindo modelos independentes
+Empresa .....:  Mazzatech</t>
+        </is>
+      </c>
+      <c r="H355" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 17/01/26 || Gerente de Projetos || Gerente de Projetos Sênior  Você é um(a) profissional experiente na gestão de iniciativas complexas e de grande escala, com histórico comprovado de entregas bem-sucedidas? Tem interesse em coordenar múltiplas atividades interdependentes e garantir a evolução contínua dos projetos?  Estamos em busca de um(a) Gerente de Projetos Sênior para liderar a integração geral do CS Latam. com foco principal na incorporação do stack tecnológico do Brasil ao Banco.  Principais responsabilidades: Apoiar a integração de soluções tecnológicas, viabilizando a expansão da oferta de produtos do Banco Desenvolver planos e garantir o progresso da refatoração de aplicações conforme os Padrões Tecnológicos do Banco, incluindo rebranding e integração de sistemas core em uma plataforma única Conduzir a reestruturação e padronização das aplicações para consumo de serviços bancários, substituindo modelos independentes || Empresa .....:  Mazzatech</t>
+        </is>
+      </c>
+      <c r="I355" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>19/01/2026</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>83293</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>Gerente de Projetos - CRM</t>
+        </is>
+      </c>
+      <c r="D356" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E356" t="inlineStr">
+        <is>
+          <t>Híbrido</t>
+        </is>
+      </c>
+      <c r="F356" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 17/01/26</t>
+        </is>
+      </c>
+      <c r="G356" t="inlineStr">
+        <is>
+          <t>Vaga: Gerente de Projetos — Implantação de CRM  Transformação Digital  Estamos buscando um(a) Gerente de Projetos com forte atuação em implantação de CRM e condução de iniciativas corporativas estratégicas. A pessoa ideal para a posição possui perfil estruturado, visão de negócios, excelente comunicação com executivos e experiência na liderança de times multidisciplinares.  Requisitos Técnicos Experiência sólida em gestão de projetos complexos e corporativos (7–10+ anos). Experiência comprovada em projetos de implantação de CRM. Vivência em transformação digital, integrações sistêmicas e otimização de processos. Domínio de ferramentas de gestão de projetos (MS Project, Project Online, Planner ou similares). Forte atuação com gestão de stakeholders e reporte executivo.  Modelo de Trabalho Híbrido — 2x por semana presencial Local: Consolação — São Paulo/SP
+Empresa .....:  Mazzatech</t>
+        </is>
+      </c>
+      <c r="H356" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 17/01/26 || Gerente de Projetos - CRM || Vaga: Gerente de Projetos — Implantação de CRM  Transformação Digital  Estamos buscando um(a) Gerente de Projetos com forte atuação em implantação de CRM e condução de iniciativas corporativas estratégicas. A pessoa ideal para a posição possui perfil estruturado, visão de negócios, excelente comunicação com executivos e experiência na liderança de times multidisciplinares.  Requisitos Técnicos Experiência sólida em gestão de projetos complexos e corporativos (7–10+ anos). Experiência comprovada em projetos de implantação de CRM. Vivência em transformação digital, integrações sistêmicas e otimização de processos. Domínio de ferramentas de gestão de projetos (MS Project, Project Online, Planner ou similares). Forte atuação com gestão de stakeholders e reporte executivo.  Modelo de Trabalho Híbrido — 2x por semana presencial Local: Consolação — São Paulo/SP || Empresa .....:  Mazzatech</t>
+        </is>
+      </c>
+      <c r="I356" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>19/01/2026</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>83296</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>Pessoa Desenvolvedora Full Stack (React + .Net)</t>
+        </is>
+      </c>
+      <c r="D357" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E357" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F357" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 17/01/26</t>
+        </is>
+      </c>
+      <c r="G357" t="inlineStr">
+        <is>
+          <t>VAGA REMOTA  Requisitos Obrigatórios: Experiência sólida com React, Hooks e TypeScript. Experiência com .NET Core / .NET 6/7 e C#. Vivência com Cloud (Azure ou AWS). Conhecimento em Docker e containerização. Experiência com consumo de APIs REST e definição de contratos (Swagger/OpenAPI). Conhecimentos de HTML5, CSS3, CSS-in-JS (styled-components, emotion) ou frameworks CSS. Experiência com testes front-end (Jest, React Testing Library) e testes backend. Familiaridade com Git e boas práticas de versionamento. Experiência com ferramentas de build/packaging (Webpack, Vite) e pipelines de CI/CD.  Diferenciais (Desejáveis): Experiência com SSR/Next.js. Conhecimento em bibliotecas de estado (Redux, Zustand) e otimização de performance. Vivência com mensageria ou WebSockets. Experiência prática com acessibilidade (a11y).
+Empresa .....:  MJV</t>
+        </is>
+      </c>
+      <c r="H357" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 17/01/26 || Pessoa Desenvolvedora Full Stack (React + .Net) || VAGA REMOTA  Requisitos Obrigatórios: Experiência sólida com React, Hooks e TypeScript. Experiência com .NET Core / .NET 6/7 e C#. Vivência com Cloud (Azure ou AWS). Conhecimento em Docker e containerização. Experiência com consumo de APIs REST e definição de contratos (Swagger/OpenAPI). Conhecimentos de HTML5, CSS3, CSS-in-JS (styled-components, emotion) ou frameworks CSS. Experiência com testes front-end (Jest, React Testing Library) e testes backend. Familiaridade com Git e boas práticas de versionamento. Experiência com ferramentas de build/packaging (Webpack, Vite) e pipelines de CI/CD.  Diferenciais (Desejáveis): Experiência com SSR/Next.js. Conhecimento em bibliotecas de estado (Redux, Zustand) e otimização de performance. Vivência com mensageria ou WebSockets. Experiência prática com acessibilidade (a11y). || Empresa .....:  MJV</t>
+        </is>
+      </c>
+      <c r="I357" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>19/01/2026</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>83289</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>Tecnico de Informatica em Campo</t>
+        </is>
+      </c>
+      <c r="D358" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E358" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F358" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 17/01/26</t>
+        </is>
+      </c>
+      <c r="G358" t="inlineStr">
+        <is>
+          <t>Estamos em busca de um Técnico de Campo para atuar em visitas técnicas a clientes, realizando entrega e retirada de equipamentos, troca de equipamentos e, em alguns casos, configuração de impressoras  Principais atividades: Realizar visitas técnicas a clientes externos Efetuar entrega e retirada de equipamentos Executar troca de equipamentos quando necessário Configurar impressoras e prestar suporte básico em alguns atendimentos Preencher registros de atendimento e seguir os processos internos.  Requisitos: Conhecimentos básicos em informática e equipamentos de TI Desejável experiência anterior como técnico de campo ou suporte técnico Boa comunicação, organização e responsabilidade Disponibilidade para trabalho externo.  Horário de trabalho: Segunda a sexta-feira, das 09h às 18h. Salario: R$ 2.250,00  Vale-refeição no valor R$ 30,00 Vale-Transporte
+Empresa .....:  Allugga</t>
+        </is>
+      </c>
+      <c r="H358" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 17/01/26 || Tecnico de Informatica em Campo || Estamos em busca de um Técnico de Campo para atuar em visitas técnicas a clientes, realizando entrega e retirada de equipamentos, troca de equipamentos e, em alguns casos, configuração de impressoras  Principais atividades: Realizar visitas técnicas a clientes externos Efetuar entrega e retirada de equipamentos Executar troca de equipamentos quando necessário Configurar impressoras e prestar suporte básico em alguns atendimentos Preencher registros de atendimento e seguir os processos internos.  Requisitos: Conhecimentos básicos em informática e equipamentos de TI Desejável experiência anterior como técnico de campo ou suporte técnico Boa comunicação, organização e responsabilidade Disponibilidade para trabalho externo.  Horário de trabalho: Segunda a sexta-feira, das 09h às 18h. Salario: R$ 2.250,00  Vale-refeição no valor R$ 30,00 Vale-Transporte || Empresa .....:  Allugga</t>
+        </is>
+      </c>
+      <c r="I358" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>19/01/2026</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>82133</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>UX Designer Freelancer – Validação e Otimização de</t>
+        </is>
+      </c>
+      <c r="D359" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E359" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F359" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 17/01/26</t>
+        </is>
+      </c>
+      <c r="G359" t="inlineStr">
+        <is>
+          <t>Estamos em busca de um UX Designer freelancer para validar e otimizar telas de um sistema web complexo, com grande volume de informações e múltiplos fluxos de uso. O objetivo é preservar a estrutura existente e melhorar a experiência do usuário, tornando a navegação mais fluida, intuitiva e eficiente.  O profissional deverá analisar telas e fluxos, propor soluções, criar protótipos, conduzir testes de usabilidade e documentar recomendações para a equipe de desenvolvimento.  Requisitos: experiência comprovada em UX para sistemas corporativos, ERPs ou CRMs domínio de ferramentas conhecimento em mapeamento de jornada, arquitetura da informação e testes de usabilidade capacidade analítica para transformar processos complexos em experiências intuitivas.  Formato freelancer remoto, com entregas por etapas.
+Empresa .....:  Poliview Tecnologia</t>
+        </is>
+      </c>
+      <c r="H359" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 17/01/26 || UX Designer Freelancer – Validação e Otimização de || Estamos em busca de um UX Designer freelancer para validar e otimizar telas de um sistema web complexo, com grande volume de informações e múltiplos fluxos de uso. O objetivo é preservar a estrutura existente e melhorar a experiência do usuário, tornando a navegação mais fluida, intuitiva e eficiente.  O profissional deverá analisar telas e fluxos, propor soluções, criar protótipos, conduzir testes de usabilidade e documentar recomendações para a equipe de desenvolvimento.  Requisitos: experiência comprovada em UX para sistemas corporativos, ERPs ou CRMs domínio de ferramentas conhecimento em mapeamento de jornada, arquitetura da informação e testes de usabilidade capacidade analítica para transformar processos complexos em experiências intuitivas.  Formato freelancer remoto, com entregas por etapas. || Empresa .....:  Poliview Tecnologia</t>
+        </is>
+      </c>
+      <c r="I359" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>19/01/2026</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>82978</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>Analista de Suporte NOC</t>
+        </is>
+      </c>
+      <c r="D360" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E360" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F360" t="inlineStr">
+        <is>
+          <t>Sorocaba - SP - 17/01/26</t>
+        </is>
+      </c>
+      <c r="G360" t="inlineStr">
+        <is>
+          <t>-Responsabilidades Monitorar redes/servidores/serviços críticos em tempo real Identificar/analisar/resolver incidentes de forma rápida e eficiente Escalar problemas conforme procedimentos Garantir a disponibilidade/performance dos sistemas monitorados Documentar ocorrências/manter registros atualizados Colaborar com equipes de suporte/engenharia para resolução de problemas  Trabalho presencial - Sorocaba  -Requisitos Técnicos Conhecimento em redes (TCP/IP, DNS, VPN, roteamento, switching) Experiência com ferramentas de monitoramento (Zabbix/Grafana/ITSM) Noções de SO’s (Linux/Windows) Familiaridade com protocolos/troubleshooting básico Inglês técnico - leitura/escrita/conversação  -Comportamental Atenção aos detalhes/proatividade Capacidade de trabalhar sob pressão/regime de plantão Boa comunicação/trabalho em equipe Organização/disciplina para seguir processos  -Desejável Certificações (ITIL/CCNA/similar). Experiência prévia em monitorar de ambientes críticos ou NOC
+Empresa .....:  VEGACON TECNOLOGIA EM INFORMATICA LTDA</t>
+        </is>
+      </c>
+      <c r="H360" t="inlineStr">
+        <is>
+          <t>Sorocaba - SP - 17/01/26 || Analista de Suporte NOC || -Responsabilidades Monitorar redes/servidores/serviços críticos em tempo real Identificar/analisar/resolver incidentes de forma rápida e eficiente Escalar problemas conforme procedimentos Garantir a disponibilidade/performance dos sistemas monitorados Documentar ocorrências/manter registros atualizados Colaborar com equipes de suporte/engenharia para resolução de problemas  Trabalho presencial - Sorocaba  -Requisitos Técnicos Conhecimento em redes (TCP/IP, DNS, VPN, roteamento, switching) Experiência com ferramentas de monitoramento (Zabbix/Grafana/ITSM) Noções de SO’s (Linux/Windows) Familiaridade com protocolos/troubleshooting básico Inglês técnico - leitura/escrita/conversação  -Comportamental Atenção aos detalhes/proatividade Capacidade de trabalhar sob pressão/regime de plantão Boa comunicação/trabalho em equipe Organização/disciplina para seguir processos  -Desejável Certificações (ITIL/CCNA/similar). Experiência prévia em monitorar de ambientes críticos ou NOC || Empresa .....:  VEGACON TECNOLOGIA EM INFORMATICA LTDA</t>
+        </is>
+      </c>
+      <c r="I360" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>19/01/2026</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>82691</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>Consultor SAP MM Sênior</t>
+        </is>
+      </c>
+      <c r="D361" t="inlineStr">
+        <is>
+          <t>Sênior</t>
+        </is>
+      </c>
+      <c r="E361" t="inlineStr">
+        <is>
+          <t>Híbrido</t>
+        </is>
+      </c>
+      <c r="F361" t="inlineStr">
+        <is>
+          <t>Campinas - SP - 16/01/26</t>
+        </is>
+      </c>
+      <c r="G361" t="inlineStr">
+        <is>
+          <t>Buscamos uma pessoa para aumentar nossa equipe de AMS.  Requisitos Obrigatórios:  Sólida experiência no módulo MM em projetos de implementação e suporte AMS Experiência em atendimento a Clientes atuando em equipes de Suportes Solido conhecimento de configurações e dos processos envolvidos no modulo: Compras, Tipos de documentos,Transferência, Subcontratação, Consignação, Estratégias de aprovação, Gestão de Estoques e Movimentações, Contabilização, Tipos de movimentos, Inventário, Movimentação de material, Integraçaõ com WM, Faturamento de Fornecedores, Faturas, Notas de Crédito, Impostos, BP Planejamento de necessidades de material (MRP) e políticas de reabastecimento Processos de devoluções, cancelamentos, notas de crédito e bloqueio de fatura Experiência e conhecimento de Localização Brasil Conhecimento de integração MM com FI, CO, SD e GRC Experiência em levantamento de requisitos, configuração, testes e suporte pós go-live  Híbrido em Campinas - SP
+Empresa .....:  Essence IT</t>
+        </is>
+      </c>
+      <c r="H361" t="inlineStr">
+        <is>
+          <t>Campinas - SP - 16/01/26 || Consultor SAP MM Sênior || Buscamos uma pessoa para aumentar nossa equipe de AMS.  Requisitos Obrigatórios:  Sólida experiência no módulo MM em projetos de implementação e suporte AMS Experiência em atendimento a Clientes atuando em equipes de Suportes Solido conhecimento de configurações e dos processos envolvidos no modulo: Compras, Tipos de documentos,Transferência, Subcontratação, Consignação, Estratégias de aprovação, Gestão de Estoques e Movimentações, Contabilização, Tipos de movimentos, Inventário, Movimentação de material, Integraçaõ com WM, Faturamento de Fornecedores, Faturas, Notas de Crédito, Impostos, BP Planejamento de necessidades de material (MRP) e políticas de reabastecimento Processos de devoluções, cancelamentos, notas de crédito e bloqueio de fatura Experiência e conhecimento de Localização Brasil Conhecimento de integração MM com FI, CO, SD e GRC Experiência em levantamento de requisitos, configuração, testes e suporte pós go-live  Híbrido em Campinas - SP || Empresa .....:  Essence IT</t>
+        </is>
+      </c>
+      <c r="I361" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>19/01/2026</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>82891</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>Consultor Oracle APEX Sr</t>
+        </is>
+      </c>
+      <c r="D362" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E362" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F362" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 16/01/26</t>
+        </is>
+      </c>
+      <c r="G362" t="inlineStr">
+        <is>
+          <t>Responsabilidades Criar aplicações web seguras utilizando Oracle APEX. Construir interfaces rápidas, funcionais e responsivas. Desenvolver lógica de negócio utilizando PL/SQL. Integrar APIs internas e externas (REST). Configurar autenticação, controle de acessos e auditoria. Garantir a qualidade das entregas e realizar testes funcionais. Documentar soluções de maneira objetiva e clara. Competências Técnicas Experiência com Oracle APEX (versões recentes). Domínio de PL/SQL avançado. Forte conhecimento em Oracle Database (índices, planos de execução, performance tuning). Conhecimento em JavaScript e HTML para customizações. Experiência com RESTful Web Services / ORDS. Uso de Git para versionamento de código.
+Empresa .....:  GRUPO TAKING</t>
+        </is>
+      </c>
+      <c r="H362" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 16/01/26 || Consultor Oracle APEX Sr || Responsabilidades Criar aplicações web seguras utilizando Oracle APEX. Construir interfaces rápidas, funcionais e responsivas. Desenvolver lógica de negócio utilizando PL/SQL. Integrar APIs internas e externas (REST). Configurar autenticação, controle de acessos e auditoria. Garantir a qualidade das entregas e realizar testes funcionais. Documentar soluções de maneira objetiva e clara. Competências Técnicas Experiência com Oracle APEX (versões recentes). Domínio de PL/SQL avançado. Forte conhecimento em Oracle Database (índices, planos de execução, performance tuning). Conhecimento em JavaScript e HTML para customizações. Experiência com RESTful Web Services / ORDS. Uso de Git para versionamento de código. || Empresa .....:  GRUPO TAKING</t>
+        </is>
+      </c>
+      <c r="I362" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>19/01/2026</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>81876</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>Oracle Cloud Operations-Líder de Suporte Funcional</t>
+        </is>
+      </c>
+      <c r="D363" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E363" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F363" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 16/01/26</t>
+        </is>
+      </c>
+      <c r="G363" t="inlineStr">
+        <is>
+          <t>Requisitos: Sólido conhecimento funcional em Oracle ERP Cloud, especialmente nos módulos General Ledger, Ativos Fixos e Cash Management. Participação em 3+ implementações completas do Oracle Cloud Financials. Familiaridade com localizações e relatórios LACLS para o Brasil. Experiência em liderança de equipe (5 a 10 pessoas) e gestão de demandas dentro de SLAs. Domínio de BIP, PLSQL, FBDI, ADFDi, integrações SOAP/REST e boas práticas contábeis.  Excelente comunicação, resolução de problemas e capacidade de colaboração com times globais.  Fluência em português e inglês (mandatório).
+Empresa .....:  LIGHTHOUSE SOLUCOES EM INFORMATICA LTDA</t>
+        </is>
+      </c>
+      <c r="H363" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 16/01/26 || Oracle Cloud Operations-Líder de Suporte Funcional || Requisitos: Sólido conhecimento funcional em Oracle ERP Cloud, especialmente nos módulos General Ledger, Ativos Fixos e Cash Management. Participação em 3+ implementações completas do Oracle Cloud Financials. Familiaridade com localizações e relatórios LACLS para o Brasil. Experiência em liderança de equipe (5 a 10 pessoas) e gestão de demandas dentro de SLAs. Domínio de BIP, PLSQL, FBDI, ADFDi, integrações SOAP/REST e boas práticas contábeis.  Excelente comunicação, resolução de problemas e capacidade de colaboração com times globais.  Fluência em português e inglês (mandatório). || Empresa .....:  LIGHTHOUSE SOLUCOES EM INFORMATICA LTDA</t>
+        </is>
+      </c>
+      <c r="I363" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>19/01/2026</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>81761</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>Profissional de TI com Experiência em Licitações e</t>
+        </is>
+      </c>
+      <c r="D364" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E364" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F364" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro - RJ - 16/01/26</t>
+        </is>
+      </c>
+      <c r="G364" t="inlineStr">
+        <is>
+          <t>Vaga para Analista de TI com experiência em licitações públicas, contratos administrativos e termos de referência. O profissional atuará na elaboração de documentos técnicos, planilhas de custos e especificações de equipamentos, além de apoiar processos de aquisição e acompanhar projetos de infraestrutura de rede. É necessário conhecimento em servidores, switches, access points, fibra óptica e demais equipamentos de TI, bem como compreensão das exigências legais da Lei nº 14.133/2021.  Desejável formação em TI, Engenharia de Redes, Sistemas ou áreas correlatas, experiência com licitações, boa redação técnica, organização e atenção a detalhes.  Conhecimento intermediário em Excel e ferramentas Google Workspace é essencial. Conhecimentos em certificações como FCC, CE, RoHS e ISO serão considerados diferenciais. Modalidade home office, regime PJ ou autônomo, horário flexível.
+Empresa .....:  Santa Alianca Serviços de Tecnologia</t>
+        </is>
+      </c>
+      <c r="H364" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro - RJ - 16/01/26 || Profissional de TI com Experiência em Licitações e || Vaga para Analista de TI com experiência em licitações públicas, contratos administrativos e termos de referência. O profissional atuará na elaboração de documentos técnicos, planilhas de custos e especificações de equipamentos, além de apoiar processos de aquisição e acompanhar projetos de infraestrutura de rede. É necessário conhecimento em servidores, switches, access points, fibra óptica e demais equipamentos de TI, bem como compreensão das exigências legais da Lei nº 14.133/2021.  Desejável formação em TI, Engenharia de Redes, Sistemas ou áreas correlatas, experiência com licitações, boa redação técnica, organização e atenção a detalhes.  Conhecimento intermediário em Excel e ferramentas Google Workspace é essencial. Conhecimentos em certificações como FCC, CE, RoHS e ISO serão considerados diferenciais. Modalidade home office, regime PJ ou autônomo, horário flexível. || Empresa .....:  Santa Alianca Serviços de Tecnologia</t>
+        </is>
+      </c>
+      <c r="I364" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>19/01/2026</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>82775</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>ANALISTA DE SISTEMAS</t>
+        </is>
+      </c>
+      <c r="D365" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E365" t="inlineStr">
+        <is>
+          <t>Híbrido</t>
+        </is>
+      </c>
+      <c r="F365" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 16/01/26</t>
+        </is>
+      </c>
+      <c r="G365" t="inlineStr">
+        <is>
+          <t>Analista de Sistemas  Requisitos: Conhecimentos avançados em : Fullstack (SpringBoot + Angular) Experiência e conhecimento com: Frontend: Angular 14+ Backend (SpringBoot) Linguagem: Java 17 Conhecimento em APIs REST, integração com serviços externos Conhecimento: com CI/CD e versionamento (Git) Familiaridade com bancos de dados relacionais Experiência e vivência, com projetos de desenvolvimento  Modelo de atuação: Hibrido (Região da Bela Vista - São Paulo - SP)  O que oferecemos? Contratação CLT Vale Refeição ou Alimentação Assistência Médica e Assistência Odontológica Auxílio creche Convênio com Farmácia Parcerias com Universidades e Escolas de Idiomas Parceria de descontos com Seguro Auto e Residência Gympass Seguro de Vida
+Empresa .....:  PSM COMPANY</t>
+        </is>
+      </c>
+      <c r="H365" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 16/01/26 || ANALISTA DE SISTEMAS || Analista de Sistemas  Requisitos: Conhecimentos avançados em : Fullstack (SpringBoot + Angular) Experiência e conhecimento com: Frontend: Angular 14+ Backend (SpringBoot) Linguagem: Java 17 Conhecimento em APIs REST, integração com serviços externos Conhecimento: com CI/CD e versionamento (Git) Familiaridade com bancos de dados relacionais Experiência e vivência, com projetos de desenvolvimento  Modelo de atuação: Hibrido (Região da Bela Vista - São Paulo - SP)  O que oferecemos? Contratação CLT Vale Refeição ou Alimentação Assistência Médica e Assistência Odontológica Auxílio creche Convênio com Farmácia Parcerias com Universidades e Escolas de Idiomas Parceria de descontos com Seguro Auto e Residência Gympass Seguro de Vida || Empresa .....:  PSM COMPANY</t>
+        </is>
+      </c>
+      <c r="I365" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>19/01/2026</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>82836</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>Analista Protheus</t>
+        </is>
+      </c>
+      <c r="D366" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E366" t="inlineStr">
+        <is>
+          <t>Híbrido</t>
+        </is>
+      </c>
+      <c r="F366" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 16/01/26</t>
+        </is>
+      </c>
+      <c r="G366" t="inlineStr">
+        <is>
+          <t>O profissional será responsável pela administração do sistema Totvs PROTHEUS e demais sistemas utilizados pela empresa, gerenciando correções, automações e ferramentas de IA. Atuará na coordenação da implantação de novos clientes, organização e personalização dos sistemas, além de treinar as áreas para uso correto e integral das ferramentas. Também será o ponto focal para suporte diário da equipe.  É necessário: - Possuir domínio do sistema Protheus - Ter experiência com implantação de sistemas - Possuir superior completo ou cursando TI - Ser apaixonado por inovação tecnológica - Disponibilidade para trabalhar híbrido (3 dias presencial e 2 dias home-office) - ficamos localizados próximo a estação de metrô Brigadeiro.
+Empresa .....:  Baker Tilly BPO</t>
+        </is>
+      </c>
+      <c r="H366" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 16/01/26 || Analista Protheus || O profissional será responsável pela administração do sistema Totvs PROTHEUS e demais sistemas utilizados pela empresa, gerenciando correções, automações e ferramentas de IA. Atuará na coordenação da implantação de novos clientes, organização e personalização dos sistemas, além de treinar as áreas para uso correto e integral das ferramentas. Também será o ponto focal para suporte diário da equipe.  É necessário: - Possuir domínio do sistema Protheus - Ter experiência com implantação de sistemas - Possuir superior completo ou cursando TI - Ser apaixonado por inovação tecnológica - Disponibilidade para trabalhar híbrido (3 dias presencial e 2 dias home-office) - ficamos localizados próximo a estação de metrô Brigadeiro. || Empresa .....:  Baker Tilly BPO</t>
+        </is>
+      </c>
+      <c r="I366" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>19/01/2026</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>82125</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>Cloud Migration Data to Analytics Senior</t>
+        </is>
+      </c>
+      <c r="D367" t="inlineStr">
+        <is>
+          <t>Sênior</t>
+        </is>
+      </c>
+      <c r="E367" t="inlineStr">
+        <is>
+          <t>Híbrido</t>
+        </is>
+      </c>
+      <c r="F367" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 16/01/26</t>
+        </is>
+      </c>
+      <c r="G367" t="inlineStr">
+        <is>
+          <t>Cargo: Cloud Migration Data to Analytics Senior Atuação: Barueri/SP – Híbrido (1x presencial) Modelo de contratação: CLT + Benefícios  Skill / Requisitos obrigatórios: Experiência com ETL  Integração de dados Planejamento estratégico com base em dados Conhecimento em Algorithms and Data Structures Capacidade analítica e resolutiva Agilidade e proatividade Inglês  Diferenciais: Experiência com pipelines de dados e validações pré e pós ETL Experiência com governança e qualidade de dados Experiência atuando junto a áreas de Analytics  Benefícios: Assistência médica e odontológica VR e VA flexível Gympass e Wellz Parceria com o SESC Descontos em restaurantes Descontos em cursos técnicos e de ensino superior Descontos em escolas e plataformas de idiomas
+Empresa .....:  Foursys</t>
+        </is>
+      </c>
+      <c r="H367" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 16/01/26 || Cloud Migration Data to Analytics Senior || Cargo: Cloud Migration Data to Analytics Senior Atuação: Barueri/SP – Híbrido (1x presencial) Modelo de contratação: CLT + Benefícios  Skill / Requisitos obrigatórios: Experiência com ETL  Integração de dados Planejamento estratégico com base em dados Conhecimento em Algorithms and Data Structures Capacidade analítica e resolutiva Agilidade e proatividade Inglês  Diferenciais: Experiência com pipelines de dados e validações pré e pós ETL Experiência com governança e qualidade de dados Experiência atuando junto a áreas de Analytics  Benefícios: Assistência médica e odontológica VR e VA flexível Gympass e Wellz Parceria com o SESC Descontos em restaurantes Descontos em cursos técnicos e de ensino superior Descontos em escolas e plataformas de idiomas || Empresa .....:  Foursys</t>
+        </is>
+      </c>
+      <c r="I367" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>19/01/2026</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>82801</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>Desenvolvedor Backend Python</t>
+        </is>
+      </c>
+      <c r="D368" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E368" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F368" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 16/01/26</t>
+        </is>
+      </c>
+      <c r="G368" t="inlineStr">
+        <is>
+          <t>Prazo: 5 meses, com chance de prorrogar Contratação: PJ Local: Remoto - 1x no mês no escritório, Grande SP  Inglês avançado Experiência em Python e desenvolvimento backend, incluindo boas práticas e padrões de projetos, testes automatizados e otimização de código. (FastAPI, Flask, Django) Conhecimento profundo em frameworks para IA generativa, especialmente LangChain e LangGraph, e familiaridade com conceitos de Orquestração de Multi-Agentes Sólida base em arquitetura de containers, com habilidade para criar imagens eficientes e configurar orquestradores para ambientes escaláveis utilizando Kubernetes Proficiência em bancos de dados relacionais, com foco em modelagem, tuning de performance e integridade em PostgreSQL Experiência com construção de ferramentas utilizando MCP (Model Context Protocol) e sistemas RAG (Retrieval-Augmented Generation). Experiência em ambientes cloud (AWS, Azure ou GCP), envolvendo deploy, monitoramento e otimização de recursos.
+Empresa .....:  Entrust IT</t>
+        </is>
+      </c>
+      <c r="H368" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 16/01/26 || Desenvolvedor Backend Python || Prazo: 5 meses, com chance de prorrogar Contratação: PJ Local: Remoto - 1x no mês no escritório, Grande SP  Inglês avançado Experiência em Python e desenvolvimento backend, incluindo boas práticas e padrões de projetos, testes automatizados e otimização de código. (FastAPI, Flask, Django) Conhecimento profundo em frameworks para IA generativa, especialmente LangChain e LangGraph, e familiaridade com conceitos de Orquestração de Multi-Agentes Sólida base em arquitetura de containers, com habilidade para criar imagens eficientes e configurar orquestradores para ambientes escaláveis utilizando Kubernetes Proficiência em bancos de dados relacionais, com foco em modelagem, tuning de performance e integridade em PostgreSQL Experiência com construção de ferramentas utilizando MCP (Model Context Protocol) e sistemas RAG (Retrieval-Augmented Generation). Experiência em ambientes cloud (AWS, Azure ou GCP), envolvendo deploy, monitoramento e otimização de recursos. || Empresa .....:  Entrust IT</t>
+        </is>
+      </c>
+      <c r="I368" t="n">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Atualização automática: Tue Feb  3 04:08:11 UTC 2026
</commit_message>
<xml_diff>
--- a/vagas_apinfo.xlsx
+++ b/vagas_apinfo.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I606"/>
+  <dimension ref="A1:I700"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -28460,6 +28460,4330 @@
         <v>20</v>
       </c>
     </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>03/02/2026</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t>83552</t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>Analista de Infraestrutura e Cloud 365</t>
+        </is>
+      </c>
+      <c r="D607" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E607" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F607" t="inlineStr">
+        <is>
+          <t>Barueri - SP - 03/02/26</t>
+        </is>
+      </c>
+      <c r="G607" t="inlineStr">
+        <is>
+          <t>Responsável por administrar, manter e evoluir ambientes de Infraestrutura e Cloud, com foco em Microsoft Office 365, garantindo segurança, disponibilidade, desempenho e conformidade dos serviços. Atuará na gestão das plataformas Microsoft, apoiando usuários e áreas de negócio, além de contribuir para projetos de melhoria contínua e governança do ambiente  Administrar e manter o ambiente Microsoft 365 (Exchange Online, SharePoint Online, Teams, OneDrive e Power Apps). Gerenciar políticas de segurança e conformidade utilizando Microsoft Defender e Microsoft Purview. Atuar na administração de dispositivos e identidades por meio do Microsoft Intune e Entra ID (Azure AD). Prestar suporte técnico de nível avançado (N2/N3) aos usuários e áreas internas. Atuar na resolução de incidentes, análise de causa raiz e melhoria contínua dos serviços. Apoiar projetos de migração, integração e otimização
+Empresa .....:  Mk Tech</t>
+        </is>
+      </c>
+      <c r="H607" t="inlineStr">
+        <is>
+          <t>Barueri - SP - 03/02/26 || Analista de Infraestrutura e Cloud 365 || Responsável por administrar, manter e evoluir ambientes de Infraestrutura e Cloud, com foco em Microsoft Office 365, garantindo segurança, disponibilidade, desempenho e conformidade dos serviços. Atuará na gestão das plataformas Microsoft, apoiando usuários e áreas de negócio, além de contribuir para projetos de melhoria contínua e governança do ambiente  Administrar e manter o ambiente Microsoft 365 (Exchange Online, SharePoint Online, Teams, OneDrive e Power Apps). Gerenciar políticas de segurança e conformidade utilizando Microsoft Defender e Microsoft Purview. Atuar na administração de dispositivos e identidades por meio do Microsoft Intune e Entra ID (Azure AD). Prestar suporte técnico de nível avançado (N2/N3) aos usuários e áreas internas. Atuar na resolução de incidentes, análise de causa raiz e melhoria contínua dos serviços. Apoiar projetos de migração, integração e otimização || Empresa .....:  Mk Tech</t>
+        </is>
+      </c>
+      <c r="I607" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>03/02/2026</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t>82591</t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>Product Owner - Meios de Pagamento</t>
+        </is>
+      </c>
+      <c r="D608" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E608" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F608" t="inlineStr">
+        <is>
+          <t>Brasília - DF - 03/02/26</t>
+        </is>
+      </c>
+      <c r="G608" t="inlineStr">
+        <is>
+          <t>A Tech For está com oportunidade para Product Owner Sênior, atuar em projeto de sustentação em cliente do segmento bancário.  PJ  Requisitos Mandatórios: - Ter atuado nos segmentos de Tecnologia da Informação - Ter atuado em squads ágeis (frameworks Scrum e/ou Kanban) - Ferramentas de Gestão de backlog: Jira, Asana, GenTi, BusinessMap - Experiência nas áreas de negócio com Foco em Meios de Pagamento - CARTÕES - Experiência em levantamento de requisitos e detalhamento das necessidades (especificações funcionais) - Perfil integrador / dinâmico, flexível, boa desenvoltura (condução de reuniões) - Foco em melhoria contínua e qualidade na entrega de resultados.
+Empresa .....:  Tech For TI</t>
+        </is>
+      </c>
+      <c r="H608" t="inlineStr">
+        <is>
+          <t>Brasília - DF - 03/02/26 || Product Owner - Meios de Pagamento || A Tech For está com oportunidade para Product Owner Sênior, atuar em projeto de sustentação em cliente do segmento bancário.  PJ  Requisitos Mandatórios: - Ter atuado nos segmentos de Tecnologia da Informação - Ter atuado em squads ágeis (frameworks Scrum e/ou Kanban) - Ferramentas de Gestão de backlog: Jira, Asana, GenTi, BusinessMap - Experiência nas áreas de negócio com Foco em Meios de Pagamento - CARTÕES - Experiência em levantamento de requisitos e detalhamento das necessidades (especificações funcionais) - Perfil integrador / dinâmico, flexível, boa desenvoltura (condução de reuniões) - Foco em melhoria contínua e qualidade na entrega de resultados. || Empresa .....:  Tech For TI</t>
+        </is>
+      </c>
+      <c r="I608" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>03/02/2026</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t>82518</t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>QA Sênior</t>
+        </is>
+      </c>
+      <c r="D609" t="inlineStr">
+        <is>
+          <t>Sênior</t>
+        </is>
+      </c>
+      <c r="E609" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F609" t="inlineStr">
+        <is>
+          <t>Cascavel - PR - 03/02/26</t>
+        </is>
+      </c>
+      <c r="G609" t="inlineStr">
+        <is>
+          <t>Missão Principal Ser o responsável por implantar, padronizar e evoluir o processo de QA, garantindo entregas consistentes, automatizadas e integradas ao fluxo de desenvolvimento do produto.  Requisitos e Experiências: -Experiência com testes manuais e automatizados -Experiência na definição e implementação de estratégias de teste (unitário, integração, E2E, contrato) -Experiência prática com BDD (Cucumber, Gherkin) e/ou TDD -Experiência com testes de API REST (validação, autenticação e headers) -Domínio das ferramentas: Postman, Selenium, Cypress, Jira, TestRail, JMeter e k6 -Conhecimento em GitHub, PostgreSQL e pipelines de CI/CD (CircleCI) -Conhecimento básico em JavaScript/TypeScript aplicado à automação de testes.  Formação: Ensino superior completo ou em andamento na área de tecnologia. Idioma: Inglês técnico básico (leitura de documentação).
+Empresa .....:  CODE GROUP</t>
+        </is>
+      </c>
+      <c r="H609" t="inlineStr">
+        <is>
+          <t>Cascavel - PR - 03/02/26 || QA Sênior || Missão Principal Ser o responsável por implantar, padronizar e evoluir o processo de QA, garantindo entregas consistentes, automatizadas e integradas ao fluxo de desenvolvimento do produto.  Requisitos e Experiências: -Experiência com testes manuais e automatizados -Experiência na definição e implementação de estratégias de teste (unitário, integração, E2E, contrato) -Experiência prática com BDD (Cucumber, Gherkin) e/ou TDD -Experiência com testes de API REST (validação, autenticação e headers) -Domínio das ferramentas: Postman, Selenium, Cypress, Jira, TestRail, JMeter e k6 -Conhecimento em GitHub, PostgreSQL e pipelines de CI/CD (CircleCI) -Conhecimento básico em JavaScript/TypeScript aplicado à automação de testes.  Formação: Ensino superior completo ou em andamento na área de tecnologia. Idioma: Inglês técnico básico (leitura de documentação). || Empresa .....:  CODE GROUP</t>
+        </is>
+      </c>
+      <c r="I609" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>03/02/2026</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>83554</t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>Analista de Infraestrutura e Cloud 365</t>
+        </is>
+      </c>
+      <c r="D610" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E610" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F610" t="inlineStr">
+        <is>
+          <t>Conceição do Jacuípe - BA - 03/02/26</t>
+        </is>
+      </c>
+      <c r="G610" t="inlineStr">
+        <is>
+          <t>Responsável por administrar, manter e evoluir ambientes de Infraestrutura e Cloud, com foco em Microsoft Office 365, garantindo segurança, disponibilidade, desempenho e conformidade dos serviços. Atuará na gestão das plataformas Microsoft, apoiando usuários e áreas de negócio, além de contribuir para projetos de melhoria contínua e governança do ambiente Administrar e manter o ambiente Microsoft 365 (Exchange Online, SharePoint Online, Teams, OneDrive e Power Apps). Gerenciar políticas de segurança e conformidade utilizando Microsoft Defender e Microsoft Purview. Atuar na administração de dispositivos e identidades por meio do Microsoft Intune e Entra ID (Azure AD). Implementar e manter políticas de acesso condicional, DLP, classificação e retenção de dados. Prestar suporte técnico de nível avançado (N2/N3) aos usuários e áreas internas. Atuar na resolução de incidentes, análise de causa raiz e melhoria contínua dos serviços.
+Empresa .....:  Mk Tech</t>
+        </is>
+      </c>
+      <c r="H610" t="inlineStr">
+        <is>
+          <t>Conceição do Jacuípe - BA - 03/02/26 || Analista de Infraestrutura e Cloud 365 || Responsável por administrar, manter e evoluir ambientes de Infraestrutura e Cloud, com foco em Microsoft Office 365, garantindo segurança, disponibilidade, desempenho e conformidade dos serviços. Atuará na gestão das plataformas Microsoft, apoiando usuários e áreas de negócio, além de contribuir para projetos de melhoria contínua e governança do ambiente Administrar e manter o ambiente Microsoft 365 (Exchange Online, SharePoint Online, Teams, OneDrive e Power Apps). Gerenciar políticas de segurança e conformidade utilizando Microsoft Defender e Microsoft Purview. Atuar na administração de dispositivos e identidades por meio do Microsoft Intune e Entra ID (Azure AD). Implementar e manter políticas de acesso condicional, DLP, classificação e retenção de dados. Prestar suporte técnico de nível avançado (N2/N3) aos usuários e áreas internas. Atuar na resolução de incidentes, análise de causa raiz e melhoria contínua dos serviços. || Empresa .....:  Mk Tech</t>
+        </is>
+      </c>
+      <c r="I610" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>03/02/2026</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t>83548</t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>Consultor Tasy - Espahol Avançado</t>
+        </is>
+      </c>
+      <c r="D611" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E611" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F611" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 03/02/26</t>
+        </is>
+      </c>
+      <c r="G611" t="inlineStr">
+        <is>
+          <t>Vaga: Consultor Tasy Prazo: 6 meses, com chances de prorrogar Local: Remoto  Requisitos Tecnicos: Espanhol Avançado Implementar as integrações existentes, realizar levantamento e analise de novas integrações, contatar  clientes para compreender e executar suas demandas, realizar análise de requisitos técnicos e funcionais elaborar documentação técnica e funcional, desenvolver relatórios e dashboards, criar templates e avaliações, acompanhar processos de personalização.  Ferramentas: PL/SQL: Insert, Update, Procedures, Functions, Packages, Triggers e Jobs: Tasy Interface Engine (broker de interoperabilidade Tasy), Tasy, HTML5: EMR, portais Tasy: Portal do Paciente, Portal de Resultados, Portal Clinico e Aprovações Pendentes.
+Empresa .....:  Entrust IT</t>
+        </is>
+      </c>
+      <c r="H611" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 03/02/26 || Consultor Tasy - Espahol Avançado || Vaga: Consultor Tasy Prazo: 6 meses, com chances de prorrogar Local: Remoto  Requisitos Tecnicos: Espanhol Avançado Implementar as integrações existentes, realizar levantamento e analise de novas integrações, contatar  clientes para compreender e executar suas demandas, realizar análise de requisitos técnicos e funcionais elaborar documentação técnica e funcional, desenvolver relatórios e dashboards, criar templates e avaliações, acompanhar processos de personalização.  Ferramentas: PL/SQL: Insert, Update, Procedures, Functions, Packages, Triggers e Jobs: Tasy Interface Engine (broker de interoperabilidade Tasy), Tasy, HTML5: EMR, portais Tasy: Portal do Paciente, Portal de Resultados, Portal Clinico e Aprovações Pendentes. || Empresa .....:  Entrust IT</t>
+        </is>
+      </c>
+      <c r="I611" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>03/02/2026</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t>82587</t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>Desenvolvedor C/C++ Sênior</t>
+        </is>
+      </c>
+      <c r="D612" t="inlineStr">
+        <is>
+          <t>Sênior</t>
+        </is>
+      </c>
+      <c r="E612" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F612" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 03/02/26</t>
+        </is>
+      </c>
+      <c r="G612" t="inlineStr">
+        <is>
+          <t>Desenvolvedor C/C++  - Totalmente REMOTO   Estamos em busca de um Desenvolvedor de Software Embarcado para integrar nossa equipe de engenharia. O profissional será responsável pelo desenvolvimento e manutenção de soluções em sistemas embarcados, com foco em performance, confiabilidade e escalabilidade.  Responsabilidades Desenvolver e manter aplicações em Linux embarcado. Programar em C/C++ para sistemas de alto desempenho. Utilizar Qt 5 para desenvolvimento de interfaces gráficas. Gerenciar versionamento de código utilizando Git. Colaborar com equipes multidisciplinares em ambiente internacional. Documentar processos e soluções técnicas de forma clara e organizada.  Requisitos Experiência comprovada em Linux embarcado. Domínio de C/C++. Experiência com Qt 5. Conhecimento em Git e boas práticas de versionamento. Inglês intermediário ou superior (capaz de participar de reuniões técnicas e compreender documentação).
+Empresa .....:  Mazzatech</t>
+        </is>
+      </c>
+      <c r="H612" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 03/02/26 || Desenvolvedor C/C++ Sênior || Desenvolvedor C/C++  - Totalmente REMOTO   Estamos em busca de um Desenvolvedor de Software Embarcado para integrar nossa equipe de engenharia. O profissional será responsável pelo desenvolvimento e manutenção de soluções em sistemas embarcados, com foco em performance, confiabilidade e escalabilidade.  Responsabilidades Desenvolver e manter aplicações em Linux embarcado. Programar em C/C++ para sistemas de alto desempenho. Utilizar Qt 5 para desenvolvimento de interfaces gráficas. Gerenciar versionamento de código utilizando Git. Colaborar com equipes multidisciplinares em ambiente internacional. Documentar processos e soluções técnicas de forma clara e organizada.  Requisitos Experiência comprovada em Linux embarcado. Domínio de C/C++. Experiência com Qt 5. Conhecimento em Git e boas práticas de versionamento. Inglês intermediário ou superior (capaz de participar de reuniões técnicas e compreender documentação). || Empresa .....:  Mazzatech</t>
+        </is>
+      </c>
+      <c r="I612" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>03/02/2026</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t>82773</t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>Desenvolvedor Full Stack - Remoto</t>
+        </is>
+      </c>
+      <c r="D613" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E613" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F613" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 03/02/26</t>
+        </is>
+      </c>
+      <c r="G613" t="inlineStr">
+        <is>
+          <t>- Atuar no suporte técnico de nível avançado, realizando atendimentos, interações com clientes e aplicando correções ou soluções no sistema. - Apoiar processos de implantação do sistema junto a clientes, garantindo boa comunicação e estabilidade no deploy. - Corrigir falhas e implementar melhorias contínuas nas aplicações existentes. - Criar e manter documentações técnicas, arquiteturais e operacionais. - Participar da definição de projetos e tarefas, avaliando arquitetura, impactos, estratégias de deploy e entregáveis. - Desenvolver e manter pipelines de Integração Contínua (CI). - Estruturar monitoramento, alarmes, logs e ferramentas de troubleshooting. - Investigar incidentes de produção, realizando análise detalhada e correção da causa raiz. - Antecipar impactos de mudanças e novos produtos na arquitetura existente, propondo ações de mitigação. - Contribuir para a construção de soluções escaláveis, resilientes e observáveis.  Segunda a sexta-feira, das 09h às 18h
+Empresa .....:  Infonova</t>
+        </is>
+      </c>
+      <c r="H613" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 03/02/26 || Desenvolvedor Full Stack - Remoto || - Atuar no suporte técnico de nível avançado, realizando atendimentos, interações com clientes e aplicando correções ou soluções no sistema. - Apoiar processos de implantação do sistema junto a clientes, garantindo boa comunicação e estabilidade no deploy. - Corrigir falhas e implementar melhorias contínuas nas aplicações existentes. - Criar e manter documentações técnicas, arquiteturais e operacionais. - Participar da definição de projetos e tarefas, avaliando arquitetura, impactos, estratégias de deploy e entregáveis. - Desenvolver e manter pipelines de Integração Contínua (CI). - Estruturar monitoramento, alarmes, logs e ferramentas de troubleshooting. - Investigar incidentes de produção, realizando análise detalhada e correção da causa raiz. - Antecipar impactos de mudanças e novos produtos na arquitetura existente, propondo ações de mitigação. - Contribuir para a construção de soluções escaláveis, resilientes e observáveis.  Segunda a sexta-feira, das 09h às 18h || Empresa .....:  Infonova</t>
+        </is>
+      </c>
+      <c r="I613" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>03/02/2026</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t>83162</t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>Desenvolvedor Full Stack PHP/Vue Sr</t>
+        </is>
+      </c>
+      <c r="D614" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E614" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F614" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 03/02/26</t>
+        </is>
+      </c>
+      <c r="G614" t="inlineStr">
+        <is>
+          <t>A Tech For TI está com oportunidade para Desenvolvedor Full Stack PHP/Vue Sr, atuar em projeto de cliente AutoTech, focada no mercado B2B, presente em diversos países.  - PJ - Totalmente home  Backend - Sólida experiência com PHP, incluindo domínio das versões 5.6 e 7.0 - Proficiência em MySQL 5.6, incluindo otimização de queries e performance - Experiência com Docker e containerização - Domínio de Git e boas práticas de controle de versão - Experiência com sistemas de cache, especialmente Redis - Desejável conhecimentos em Google Cloud Platform.  Frontend - Experiência sólida com Vue.js e seus ecossistemas (Se encontrar com as outras características exceto esta, pode nos enviar mesmo assim) - Domínio de JavaScript - Experiência com jQuery em sistemas legados - Conhecimentos em HTML5 e CSS3 - Experiência com integração de APIs RESTful.
+Empresa .....:  Tech For TI</t>
+        </is>
+      </c>
+      <c r="H614" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 03/02/26 || Desenvolvedor Full Stack PHP/Vue Sr || A Tech For TI está com oportunidade para Desenvolvedor Full Stack PHP/Vue Sr, atuar em projeto de cliente AutoTech, focada no mercado B2B, presente em diversos países.  - PJ - Totalmente home  Backend - Sólida experiência com PHP, incluindo domínio das versões 5.6 e 7.0 - Proficiência em MySQL 5.6, incluindo otimização de queries e performance - Experiência com Docker e containerização - Domínio de Git e boas práticas de controle de versão - Experiência com sistemas de cache, especialmente Redis - Desejável conhecimentos em Google Cloud Platform.  Frontend - Experiência sólida com Vue.js e seus ecossistemas (Se encontrar com as outras características exceto esta, pode nos enviar mesmo assim) - Domínio de JavaScript - Experiência com jQuery em sistemas legados - Conhecimentos em HTML5 e CSS3 - Experiência com integração de APIs RESTful. || Empresa .....:  Tech For TI</t>
+        </is>
+      </c>
+      <c r="I614" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>03/02/2026</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>83116</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>Desenvolvedor FullStack PHP</t>
+        </is>
+      </c>
+      <c r="D615" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E615" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F615" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 03/02/26</t>
+        </is>
+      </c>
+      <c r="G615" t="inlineStr">
+        <is>
+          <t>- Experiência comprovada em desenvolvimento fullstack utilizando tecnologias como PHP, JavaScript, HTML5 e CSS3. - Experiência com frameworks modernos de frontend (React, Vue ou similares). - Conhecimento e experiência com WordPress é um diferencial, especialmente em ambientes de mídia. - Familiaridade com bancos de dados relacionais (MySQL, PostgreSQL), não relacionais e vetoriais. - *Habilidades sólidas de resolução de problemas e depuração.* - Capacidade de trabalho colaborativo com equipes multidisciplinares. - Excelentes habilidades de comunicação verbal e escrita. - *Compromisso com qualidade de código, escalabilidade e desempenho.* - Flexibilidade para lidar com tecnologias emergentes e ambientes dinâmicos.  - Experiência com arquitetura em Cloud (AWS, Google Cloud) - Familiaridade com ferramentas como Google Analytics, Chartbeat - Conhecimento prático em Google Search Console - Noções de SEO e AEO aplicadas a produtos digitais
+Empresa .....:  Tessa IT</t>
+        </is>
+      </c>
+      <c r="H615" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 03/02/26 || Desenvolvedor FullStack PHP || - Experiência comprovada em desenvolvimento fullstack utilizando tecnologias como PHP, JavaScript, HTML5 e CSS3. - Experiência com frameworks modernos de frontend (React, Vue ou similares). - Conhecimento e experiência com WordPress é um diferencial, especialmente em ambientes de mídia. - Familiaridade com bancos de dados relacionais (MySQL, PostgreSQL), não relacionais e vetoriais. - *Habilidades sólidas de resolução de problemas e depuração.* - Capacidade de trabalho colaborativo com equipes multidisciplinares. - Excelentes habilidades de comunicação verbal e escrita. - *Compromisso com qualidade de código, escalabilidade e desempenho.* - Flexibilidade para lidar com tecnologias emergentes e ambientes dinâmicos.  - Experiência com arquitetura em Cloud (AWS, Google Cloud) - Familiaridade com ferramentas como Google Analytics, Chartbeat - Conhecimento prático em Google Search Console - Noções de SEO e AEO aplicadas a produtos digitais || Empresa .....:  Tessa IT</t>
+        </is>
+      </c>
+      <c r="I615" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>03/02/2026</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t>83544</t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>Desenvolvedor Java Sênior</t>
+        </is>
+      </c>
+      <c r="D616" t="inlineStr">
+        <is>
+          <t>Sênior</t>
+        </is>
+      </c>
+      <c r="E616" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F616" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 03/02/26</t>
+        </is>
+      </c>
+      <c r="G616" t="inlineStr">
+        <is>
+          <t>Experiência com ferramentas de desenvolvimento: IntelliJ, Visual Studio, Chrome DevTools Monitoramento e observabilidade: Grafana, Kibana, Elastic, Dynatrace Frameworks Java: Spring, Spring Boot, Spring Cloud, Spring Data, Spring Security Linguagens de programação: Java (principal), JavaScript Relacionais: SQL Server, DBeaver, Google Cloud SQL Não-relacionais: Redis Plataformas de Integração: Sensedia, Mulesoft API Clients: Postman, Insomnia Arquitetura SOA Versionamento de código: Git Serviços em nuvem: AWS Desenvolvimento e documentação de APIs REST: Swagger, HTML Docs Automação: Jenkins Testes automatizados: Cucumber, Teste de Mutação  Diferenciais Desejáveis Ter trabalhado no RE Porto, ou em times relacionados a sistemas Financeiros Conhecimento em metodologias ágeis: Scrum, Kanban Criação de scripts para automação de tarefas repetitivas Experiência com DataStage Experiência com API Gateway Vivência no segmento de seguros
+Empresa .....:  FORNAX CONSULTORIA EM INFORMATICA</t>
+        </is>
+      </c>
+      <c r="H616" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 03/02/26 || Desenvolvedor Java Sênior || Experiência com ferramentas de desenvolvimento: IntelliJ, Visual Studio, Chrome DevTools Monitoramento e observabilidade: Grafana, Kibana, Elastic, Dynatrace Frameworks Java: Spring, Spring Boot, Spring Cloud, Spring Data, Spring Security Linguagens de programação: Java (principal), JavaScript Relacionais: SQL Server, DBeaver, Google Cloud SQL Não-relacionais: Redis Plataformas de Integração: Sensedia, Mulesoft API Clients: Postman, Insomnia Arquitetura SOA Versionamento de código: Git Serviços em nuvem: AWS Desenvolvimento e documentação de APIs REST: Swagger, HTML Docs Automação: Jenkins Testes automatizados: Cucumber, Teste de Mutação  Diferenciais Desejáveis Ter trabalhado no RE Porto, ou em times relacionados a sistemas Financeiros Conhecimento em metodologias ágeis: Scrum, Kanban Criação de scripts para automação de tarefas repetitivas Experiência com DataStage Experiência com API Gateway Vivência no segmento de seguros || Empresa .....:  FORNAX CONSULTORIA EM INFORMATICA</t>
+        </is>
+      </c>
+      <c r="I616" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>03/02/2026</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>82516</t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>Especialista em Infraestrutura  Segurança Genetec</t>
+        </is>
+      </c>
+      <c r="D617" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E617" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F617" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 03/02/26</t>
+        </is>
+      </c>
+      <c r="G617" t="inlineStr">
+        <is>
+          <t>Consultor / Especialista em Infraestrutura  Segurança (Genetec)  Local: Totalmente remoto  (atuação remota e com interação internacional) Inglês fluente obrigatório  Buscamos, parceiro, prestador de serviços para integrar o time de Produto responsável por soluções de Segurança Global, atuando diretamente no suporte a sistemas críticos utilizados em todas as unidades do cliente.  Senioridade em consultoria em Infraestrutura (Fundação). Domínio de servidores, dispositivos de rede, bancos de dados e Azure. Certificação Genetec Security Center (ou disponibilidade para se certificar). Proficiência em PowerShell e/ou scripts SQL. Responsável por implantar e manter o sistema de controle de acesso físico e vídeo (Genetec), garantindo a segurança dos colaboradores e ativos da empresa.
+Empresa .....:  k2 partnering Solutions</t>
+        </is>
+      </c>
+      <c r="H617" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 03/02/26 || Especialista em Infraestrutura  Segurança Genetec || Consultor / Especialista em Infraestrutura  Segurança (Genetec)  Local: Totalmente remoto  (atuação remota e com interação internacional) Inglês fluente obrigatório  Buscamos, parceiro, prestador de serviços para integrar o time de Produto responsável por soluções de Segurança Global, atuando diretamente no suporte a sistemas críticos utilizados em todas as unidades do cliente.  Senioridade em consultoria em Infraestrutura (Fundação). Domínio de servidores, dispositivos de rede, bancos de dados e Azure. Certificação Genetec Security Center (ou disponibilidade para se certificar). Proficiência em PowerShell e/ou scripts SQL. Responsável por implantar e manter o sistema de controle de acesso físico e vídeo (Genetec), garantindo a segurança dos colaboradores e ativos da empresa. || Empresa .....:  k2 partnering Solutions</t>
+        </is>
+      </c>
+      <c r="I617" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>03/02/2026</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t>82708</t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>Analista de Suporte a Sistemas Pleno</t>
+        </is>
+      </c>
+      <c r="D618" t="inlineStr">
+        <is>
+          <t>Pleno</t>
+        </is>
+      </c>
+      <c r="E618" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F618" t="inlineStr">
+        <is>
+          <t>Santo André - SP - 03/02/26</t>
+        </is>
+      </c>
+      <c r="G618" t="inlineStr">
+        <is>
+          <t>Responsabilidades: Prestar suporte técnico a sistemas internos e externos, garantindo o funcionamento adequado das aplicações. Realizar análise, extração e consultas em banco de dados para investigação e solução de incidentes. Interpretar e manipular arquivos XML para apoio às atividades de suporte. Monitorar aplicações e serviços utilizando ferramentas de observabilidade. Registrar, acompanhar e atualizar chamados técnicos em ferramentas de gestão.  Requisitos Técnicos: Experiência com suporte a sistemas e análise de incidentes. Conhecimento sólido em XML. Capacidade de realizar consultas e extrações em banco de dados (SQL). Conhecimento em Jira para gerenciamento de demandas. Conhecimento em Grafana para monitoramento e análise de indicadores.  Inglês avançado (leitura, escrita e conversação).  Disponibilidade: Disponibilidade para atuar em escala, incluindo períodos diurnos e noturnos.
+Empresa .....:  TAKING</t>
+        </is>
+      </c>
+      <c r="H618" t="inlineStr">
+        <is>
+          <t>Santo André - SP - 03/02/26 || Analista de Suporte a Sistemas Pleno || Responsabilidades: Prestar suporte técnico a sistemas internos e externos, garantindo o funcionamento adequado das aplicações. Realizar análise, extração e consultas em banco de dados para investigação e solução de incidentes. Interpretar e manipular arquivos XML para apoio às atividades de suporte. Monitorar aplicações e serviços utilizando ferramentas de observabilidade. Registrar, acompanhar e atualizar chamados técnicos em ferramentas de gestão.  Requisitos Técnicos: Experiência com suporte a sistemas e análise de incidentes. Conhecimento sólido em XML. Capacidade de realizar consultas e extrações em banco de dados (SQL). Conhecimento em Jira para gerenciamento de demandas. Conhecimento em Grafana para monitoramento e análise de indicadores.  Inglês avançado (leitura, escrita e conversação).  Disponibilidade: Disponibilidade para atuar em escala, incluindo períodos diurnos e noturnos. || Empresa .....:  TAKING</t>
+        </is>
+      </c>
+      <c r="I618" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>03/02/2026</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>83550</t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>Estágio de TI - Monitoramento e suporte</t>
+        </is>
+      </c>
+      <c r="D619" t="inlineStr">
+        <is>
+          <t>Estágio</t>
+        </is>
+      </c>
+      <c r="E619" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F619" t="inlineStr">
+        <is>
+          <t>Santo André - SP - 03/02/26</t>
+        </is>
+      </c>
+      <c r="G619" t="inlineStr">
+        <is>
+          <t>ATIVIDADES • Monitorar performance dos sistemas e disponibilidade dos serviços (Milvus) • Manter e alimentar a ferramenta de monitoramento • Instalar e configurar agentes, drivers e aplicativos • Acompanhar rotinas de backup • Auxiliar na manutenção física e lógica de computadores • Identificar e registrar falhas de hardware e software • Elaborar relatórios • Criar e manter documentações.  REQUISITOS • Cursando ensino superior em TI, Redes de Computadores, Sistemas de Informação ou áreas relacionadas • Noções básicas de manutenção de computadores e sistemas operacionais • Boa comunicação, organização, adaptabilidade e trabalho em equipe • Conhecimentos em Pacote Office e sistemas operacionais Windows e/ou Linux.  EXPERIÊNCIA • Não é necessária.  BENEFÍCIOS • Regime de estágio, com possibilidade de efetivação • Bolsa auxílio: R$ 1.000,00 + Ajuda de custo: R$ 900,00 • Local: Santo André – SP • Segunda a sexta-feira, das 11h às 18h.
+Empresa .....:  TC do Brasil</t>
+        </is>
+      </c>
+      <c r="H619" t="inlineStr">
+        <is>
+          <t>Santo André - SP - 03/02/26 || Estágio de TI - Monitoramento e suporte || ATIVIDADES • Monitorar performance dos sistemas e disponibilidade dos serviços (Milvus) • Manter e alimentar a ferramenta de monitoramento • Instalar e configurar agentes, drivers e aplicativos • Acompanhar rotinas de backup • Auxiliar na manutenção física e lógica de computadores • Identificar e registrar falhas de hardware e software • Elaborar relatórios • Criar e manter documentações.  REQUISITOS • Cursando ensino superior em TI, Redes de Computadores, Sistemas de Informação ou áreas relacionadas • Noções básicas de manutenção de computadores e sistemas operacionais • Boa comunicação, organização, adaptabilidade e trabalho em equipe • Conhecimentos em Pacote Office e sistemas operacionais Windows e/ou Linux.  EXPERIÊNCIA • Não é necessária.  BENEFÍCIOS • Regime de estágio, com possibilidade de efetivação • Bolsa auxílio: R$ 1.000,00 + Ajuda de custo: R$ 900,00 • Local: Santo André – SP • Segunda a sexta-feira, das 11h às 18h. || Empresa .....:  TC do Brasil</t>
+        </is>
+      </c>
+      <c r="I619" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>03/02/2026</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t>82295</t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>Analista de Automação de Processos (VBA)</t>
+        </is>
+      </c>
+      <c r="D620" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E620" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F620" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 03/02/26</t>
+        </is>
+      </c>
+      <c r="G620" t="inlineStr">
+        <is>
+          <t>Requisitos: Conhecimentos em VBA Mapeamento de processos e sistemas  Atividades: Identificar, mapear e documentar várias macros em VBA construídas no âmbito departamental do extinto DCPS.  Presencial Osasco SP Contratação CLT
+Empresa .....:  TO Brasil</t>
+        </is>
+      </c>
+      <c r="H620" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 03/02/26 || Analista de Automação de Processos (VBA) || Requisitos: Conhecimentos em VBA Mapeamento de processos e sistemas  Atividades: Identificar, mapear e documentar várias macros em VBA construídas no âmbito departamental do extinto DCPS.  Presencial Osasco SP Contratação CLT || Empresa .....:  TO Brasil</t>
+        </is>
+      </c>
+      <c r="I620" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>03/02/2026</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>82894</t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>Analista de Implantação e Sustentação Sênior</t>
+        </is>
+      </c>
+      <c r="D621" t="inlineStr">
+        <is>
+          <t>Sênior</t>
+        </is>
+      </c>
+      <c r="E621" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F621" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 03/02/26</t>
+        </is>
+      </c>
+      <c r="G621" t="inlineStr">
+        <is>
+          <t>Atividades: - Liderar tecnicamente a equipe e atuar como ponto de escala final (N3) antes do fornecedor - Gerenciar o relacionamento técnico com o fornecedor externo - Garantir padronização e qualidade dos processos de implantação e sustentação - Assegurar a consistência técnica na estruturação de processos de Service Desk ou reestruturações de Suporte.  Requisitos: - Experiência em Suporte (N2 e N3) ou Análise de Sistemas - Sólidos conhecimentos em ITIL - Experiência em gestão de fornecedores de T.I - Conhecimento em SLA s, OLA s e Gestão de problemas (análise de causa raiz) - Habilidade de comunicação com diretoria, fornecedores e clientes - Experiência prévia na estruturação de processos de Service Desk ou Reestruturações de Suporte.  Informações Adicionais: - Salário: A combinar - Benefícios: Assistência Médica + Seguro de Vida + Cesta Básica + Vale Transporte - Regime de contratação: CLT (Efetivo) - Horário: A combinar
+Empresa .....:  UNIP</t>
+        </is>
+      </c>
+      <c r="H621" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 03/02/26 || Analista de Implantação e Sustentação Sênior || Atividades: - Liderar tecnicamente a equipe e atuar como ponto de escala final (N3) antes do fornecedor - Gerenciar o relacionamento técnico com o fornecedor externo - Garantir padronização e qualidade dos processos de implantação e sustentação - Assegurar a consistência técnica na estruturação de processos de Service Desk ou reestruturações de Suporte.  Requisitos: - Experiência em Suporte (N2 e N3) ou Análise de Sistemas - Sólidos conhecimentos em ITIL - Experiência em gestão de fornecedores de T.I - Conhecimento em SLA s, OLA s e Gestão de problemas (análise de causa raiz) - Habilidade de comunicação com diretoria, fornecedores e clientes - Experiência prévia na estruturação de processos de Service Desk ou Reestruturações de Suporte.  Informações Adicionais: - Salário: A combinar - Benefícios: Assistência Médica + Seguro de Vida + Cesta Básica + Vale Transporte - Regime de contratação: CLT (Efetivo) - Horário: A combinar || Empresa .....:  UNIP</t>
+        </is>
+      </c>
+      <c r="I621" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>03/02/2026</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t>83165</t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>Analista de Infraestrutura Pleno</t>
+        </is>
+      </c>
+      <c r="D622" t="inlineStr">
+        <is>
+          <t>Pleno</t>
+        </is>
+      </c>
+      <c r="E622" t="inlineStr">
+        <is>
+          <t>Híbrido</t>
+        </is>
+      </c>
+      <c r="F622" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 03/02/26</t>
+        </is>
+      </c>
+      <c r="G622" t="inlineStr">
+        <is>
+          <t>• Experiência com criação e sustentação de ambientes de Infraestrutura de TI nível Datacenter • Vivência em JBOSS EAP, realizando Deploy de aplicações e atuando na correção de problemas de instalação de aplicações baseadas em JAVA • Experiência em gestão de ambientes Linux Redhat, tratativa de vulnerabilidades em sistemas operacionais, rotinas de Backup e gestão de Storage e administração de recursos de servidores (provisionamento de memória, processador e disco) • Conhecimento com GMUD e Middleware  Hibrido (Vila Olímpia - São Paulo/SP) Contratação CLT  Oferecemos: VR ou VA, Assistência Médica e Odontológica, Auxílio creche, parcerias com Universidades e WellHub.
+Empresa .....:  PSM COM PROFESSIONAL SERVICES MANAGEMENT</t>
+        </is>
+      </c>
+      <c r="H622" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 03/02/26 || Analista de Infraestrutura Pleno || • Experiência com criação e sustentação de ambientes de Infraestrutura de TI nível Datacenter • Vivência em JBOSS EAP, realizando Deploy de aplicações e atuando na correção de problemas de instalação de aplicações baseadas em JAVA • Experiência em gestão de ambientes Linux Redhat, tratativa de vulnerabilidades em sistemas operacionais, rotinas de Backup e gestão de Storage e administração de recursos de servidores (provisionamento de memória, processador e disco) • Conhecimento com GMUD e Middleware  Hibrido (Vila Olímpia - São Paulo/SP) Contratação CLT  Oferecemos: VR ou VA, Assistência Médica e Odontológica, Auxílio creche, parcerias com Universidades e WellHub. || Empresa .....:  PSM COM PROFESSIONAL SERVICES MANAGEMENT</t>
+        </is>
+      </c>
+      <c r="I622" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>03/02/2026</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t>82682</t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>Analista de Redes Sênior</t>
+        </is>
+      </c>
+      <c r="D623" t="inlineStr">
+        <is>
+          <t>Sênior</t>
+        </is>
+      </c>
+      <c r="E623" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F623" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 03/02/26</t>
+        </is>
+      </c>
+      <c r="G623" t="inlineStr">
+        <is>
+          <t>Analista de Redes Sênior Profissional responsável pela administração e manutenção de redes LAN, WAN e WLAN, atuando em troubleshooting avançado de conectividade, roteamento e desempenho. Irá gerenciar equipamentos como switches, roteadores, firewalls e access points, além de implementar políticas de segurança (VPNs, segmentação, regras de firewall e controle de acesso). Também realizará monitoramento (Zabbix/Grafana), documentação técnica e participação em projetos de evolução da infraestrutura, seguindo boas práticas de gestão de mudanças.  Requisitos essenciais: – Experiência em redes de médio/grande porte e forte vivência em ambiente Cisco (Catalyst/Nexus). – Domínio de TCP/IP, VLAN, STP, OSPF, BGP, DNS, DHCP, switching L2/L3 e Wi-Fi corporativo. – Experiência com firewall Palo Alto, Cisco ISE/NAC e troubleshooting de LAN/WAN. – Noções de ITIL – Certificação CCNA.  -Contratação CLT - Atuação hibrida - (3x presencial na região de Bela Vista - SP)
+Empresa .....:  PSM COMPANY</t>
+        </is>
+      </c>
+      <c r="H623" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 03/02/26 || Analista de Redes Sênior || Analista de Redes Sênior Profissional responsável pela administração e manutenção de redes LAN, WAN e WLAN, atuando em troubleshooting avançado de conectividade, roteamento e desempenho. Irá gerenciar equipamentos como switches, roteadores, firewalls e access points, além de implementar políticas de segurança (VPNs, segmentação, regras de firewall e controle de acesso). Também realizará monitoramento (Zabbix/Grafana), documentação técnica e participação em projetos de evolução da infraestrutura, seguindo boas práticas de gestão de mudanças.  Requisitos essenciais: – Experiência em redes de médio/grande porte e forte vivência em ambiente Cisco (Catalyst/Nexus). – Domínio de TCP/IP, VLAN, STP, OSPF, BGP, DNS, DHCP, switching L2/L3 e Wi-Fi corporativo. – Experiência com firewall Palo Alto, Cisco ISE/NAC e troubleshooting de LAN/WAN. – Noções de ITIL – Certificação CCNA.  -Contratação CLT - Atuação hibrida - (3x presencial na região de Bela Vista - SP) || Empresa .....:  PSM COMPANY</t>
+        </is>
+      </c>
+      <c r="I623" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>03/02/2026</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t>82792</t>
+        </is>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>Analista de Segurança da Informação - Híbrido 1x</t>
+        </is>
+      </c>
+      <c r="D624" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E624" t="inlineStr">
+        <is>
+          <t>Híbrido</t>
+        </is>
+      </c>
+      <c r="F624" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 03/02/26</t>
+        </is>
+      </c>
+      <c r="G624" t="inlineStr">
+        <is>
+          <t>A missão do Analista de Segurança é garantir a proteção e o bom funcionamento da infraestrutura local e em nuvem da empresa. Atuando no monitoramento de redes, servidores e dispositivos, identificando vulnerabilidades e implementando soluções de segurança. Configura firewalls, políticas de acesso e criptografia, além de realizar análises de risco e troubleshooting. .  Requisitos necessários:  Conhecimentos em  ZTNA, Conhecimento em Netskope e/ou Fortinet e/ou CDN (Cloudflare). Firewall Fortinet e filtro de conteúdo EDR, cofre de senha, Tunnel GRE/IpSec, Abrangente conhecimento em redes. Conhecimento de protocolos web.  *Atuação: Híbrido - 1x presencial na Chácara Santo Antônio - São Paulo - SP* Formação: Graduação  Concluída ou cursando  Ramo da empresa: Segurança da Informação  Contratação CLT R$3.000,00 + Benefícios
+Empresa .....:  Moot Consulting</t>
+        </is>
+      </c>
+      <c r="H624" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 03/02/26 || Analista de Segurança da Informação - Híbrido 1x || A missão do Analista de Segurança é garantir a proteção e o bom funcionamento da infraestrutura local e em nuvem da empresa. Atuando no monitoramento de redes, servidores e dispositivos, identificando vulnerabilidades e implementando soluções de segurança. Configura firewalls, políticas de acesso e criptografia, além de realizar análises de risco e troubleshooting. .  Requisitos necessários:  Conhecimentos em  ZTNA, Conhecimento em Netskope e/ou Fortinet e/ou CDN (Cloudflare). Firewall Fortinet e filtro de conteúdo EDR, cofre de senha, Tunnel GRE/IpSec, Abrangente conhecimento em redes. Conhecimento de protocolos web.  *Atuação: Híbrido - 1x presencial na Chácara Santo Antônio - São Paulo - SP* Formação: Graduação  Concluída ou cursando  Ramo da empresa: Segurança da Informação  Contratação CLT R$3.000,00 + Benefícios || Empresa .....:  Moot Consulting</t>
+        </is>
+      </c>
+      <c r="I624" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>03/02/2026</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t>82614</t>
+        </is>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>Analista de Service Desk Bilingue</t>
+        </is>
+      </c>
+      <c r="D625" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E625" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F625" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 03/02/26</t>
+        </is>
+      </c>
+      <c r="G625" t="inlineStr">
+        <is>
+          <t>Vaga Remota para Analistas de Service Desk.  Requisitos Essenciais: Inglês Fluente (Atendimento global). Residência em SP (Obrigatório devido à contratação e CCT). Disponibilidade total para escala 12 x 36 (incluindo fins de semana/feriados). Experiência (ou interesse em aprender) com ServiceNow.  Atividades: Atendimento de chamados (tickets globais) com escopo fechado (6 tipos principais - FCR). Treinamento inicial de 2-3 semanas será fornecido pelo cliente. Equipamento de trabalho fornecido pelo cliente.  Buscamos profissionais com disciplina para a escala 12x36 e foco em qualidade de atendimento sob pressão (alta demanda). Início imediato.
+Empresa .....:  Randstad</t>
+        </is>
+      </c>
+      <c r="H625" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 03/02/26 || Analista de Service Desk Bilingue || Vaga Remota para Analistas de Service Desk.  Requisitos Essenciais: Inglês Fluente (Atendimento global). Residência em SP (Obrigatório devido à contratação e CCT). Disponibilidade total para escala 12 x 36 (incluindo fins de semana/feriados). Experiência (ou interesse em aprender) com ServiceNow.  Atividades: Atendimento de chamados (tickets globais) com escopo fechado (6 tipos principais - FCR). Treinamento inicial de 2-3 semanas será fornecido pelo cliente. Equipamento de trabalho fornecido pelo cliente.  Buscamos profissionais com disciplina para a escala 12x36 e foco em qualidade de atendimento sob pressão (alta demanda). Início imediato. || Empresa .....:  Randstad</t>
+        </is>
+      </c>
+      <c r="I625" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>03/02/2026</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t>83174</t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>Analista de Sistema Jr / Analista de Requisitos Jr</t>
+        </is>
+      </c>
+      <c r="D626" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E626" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F626" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 03/02/26</t>
+        </is>
+      </c>
+      <c r="G626" t="inlineStr">
+        <is>
+          <t>Principais responsabilidades Receber, registrar e acompanhar demandas dos clientes. Elaborar, organizar e controlar backlog de projetos de baixa complexidade. Gerar e compartilhar status recorrentes dos projetos. Atender clientes, esclarecendo prazos, consumos e andamento das demandas. Abrir, atualizar e acompanhar chamados e demandas no Jira. Realizar follow-ups com clientes e equipe técnica, garantindo alinhamento e prazos. Preparar e conduzir homologações junto aos clientes. Executar operação assistida após entregas. Acompanhar e atualizar projetos na Release Wiki, conforme entregáveis. Apoiar chamados da área de suporte. Atuar em apoio aos analistas de processos na execução e tratativa das demandas.  Competências Técnicas Obrigatórias Experiência mínima de 1 ano em organizações públicas ou privadas, atuando com: inovação de modelos de negócio, configuração, parametrização e uso de sistemas, apoio à gestão e operação de soluções tecnológicas. Pacote Office.
+Empresa .....:  BRBPO</t>
+        </is>
+      </c>
+      <c r="H626" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 03/02/26 || Analista de Sistema Jr / Analista de Requisitos Jr || Principais responsabilidades Receber, registrar e acompanhar demandas dos clientes. Elaborar, organizar e controlar backlog de projetos de baixa complexidade. Gerar e compartilhar status recorrentes dos projetos. Atender clientes, esclarecendo prazos, consumos e andamento das demandas. Abrir, atualizar e acompanhar chamados e demandas no Jira. Realizar follow-ups com clientes e equipe técnica, garantindo alinhamento e prazos. Preparar e conduzir homologações junto aos clientes. Executar operação assistida após entregas. Acompanhar e atualizar projetos na Release Wiki, conforme entregáveis. Apoiar chamados da área de suporte. Atuar em apoio aos analistas de processos na execução e tratativa das demandas.  Competências Técnicas Obrigatórias Experiência mínima de 1 ano em organizações públicas ou privadas, atuando com: inovação de modelos de negócio, configuração, parametrização e uso de sistemas, apoio à gestão e operação de soluções tecnológicas. Pacote Office. || Empresa .....:  BRBPO</t>
+        </is>
+      </c>
+      <c r="I626" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>03/02/2026</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t>83542</t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>CONSULTOR DE PROCESSOS</t>
+        </is>
+      </c>
+      <c r="D627" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E627" t="inlineStr">
+        <is>
+          <t>Híbrido</t>
+        </is>
+      </c>
+      <c r="F627" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 03/02/26</t>
+        </is>
+      </c>
+      <c r="G627" t="inlineStr">
+        <is>
+          <t>Local: Híbrido - 1x semana - Chácara Santo Antônio/SP Prazo: 6 meses, com chances de prorrogação Contratação: PJ  Requisitos: Inglês intermediário/avançado Ensino superior completo em Engenharia de Produção, Administração, Contabilidade, Economia, Análise e Desenvolvimento de Sistemas, ou áreas correlatas Conhecimento de processos financeiros, fiscais e contábeis Mapeamento e otimização de processos Documentação de processos e fluxos BPMN Projetos de melhoria contínua e implantação de sistemas Análise de tempos e métodos Levantamento de requisitos e análise de causa raiz.  Diferenciais: Sistemas ERP (Oracle, SAP, entre outros) Sistemas fiscais (Ex: Mastersaf Dfe, entre outros) Arquitetura de sistemas com foco fiscal Ferramentas de automação de processos Metodologias Lean e Seis Sigma.
+Empresa .....:  Entrust It</t>
+        </is>
+      </c>
+      <c r="H627" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 03/02/26 || CONSULTOR DE PROCESSOS || Local: Híbrido - 1x semana - Chácara Santo Antônio/SP Prazo: 6 meses, com chances de prorrogação Contratação: PJ  Requisitos: Inglês intermediário/avançado Ensino superior completo em Engenharia de Produção, Administração, Contabilidade, Economia, Análise e Desenvolvimento de Sistemas, ou áreas correlatas Conhecimento de processos financeiros, fiscais e contábeis Mapeamento e otimização de processos Documentação de processos e fluxos BPMN Projetos de melhoria contínua e implantação de sistemas Análise de tempos e métodos Levantamento de requisitos e análise de causa raiz.  Diferenciais: Sistemas ERP (Oracle, SAP, entre outros) Sistemas fiscais (Ex: Mastersaf Dfe, entre outros) Arquitetura de sistemas com foco fiscal Ferramentas de automação de processos Metodologias Lean e Seis Sigma. || Empresa .....:  Entrust It</t>
+        </is>
+      </c>
+      <c r="I627" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>03/02/2026</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t>83540</t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>Consultor PJ_Suporte Sistemas Bancários</t>
+        </is>
+      </c>
+      <c r="D628" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E628" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F628" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 03/02/26</t>
+        </is>
+      </c>
+      <c r="G628" t="inlineStr">
+        <is>
+          <t>Empresa Portuguesa de Tecnologia, busca profissionais em modalidade PJ para atuar em cliente do ramo Financeiro / Banco.  Local de trabalho: híbrido na Faria Lima - SP (4xsemana) e Home Office (1xsemana) Contratação PJ (valor fixo mensal + 22 dias de férias/ano).  Requisitos: Experiência com suporte Nível 1 a sistemas bancários (Altbank, Função, Altair, outros) Inglês avançado para escrever relatórios  Já tenha atuado em Suporte à Produção Nivel 1, ou seja: Abertura de tickets Análise preliminar para definição e encaminhamento da resolução de defeitos Monitorar a resolução de tickets por parte do provedor Preparar estatísticas sobre tickets de problemas de Produção Comunicar o status de resolução de incidentes aos usuários  Desejável: experiência com Matera ou Change e conhecimento de Espanhol (oral e escrita)
+Empresa .....:  Performance and Mind</t>
+        </is>
+      </c>
+      <c r="H628" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 03/02/26 || Consultor PJ_Suporte Sistemas Bancários || Empresa Portuguesa de Tecnologia, busca profissionais em modalidade PJ para atuar em cliente do ramo Financeiro / Banco.  Local de trabalho: híbrido na Faria Lima - SP (4xsemana) e Home Office (1xsemana) Contratação PJ (valor fixo mensal + 22 dias de férias/ano).  Requisitos: Experiência com suporte Nível 1 a sistemas bancários (Altbank, Função, Altair, outros) Inglês avançado para escrever relatórios  Já tenha atuado em Suporte à Produção Nivel 1, ou seja: Abertura de tickets Análise preliminar para definição e encaminhamento da resolução de defeitos Monitorar a resolução de tickets por parte do provedor Preparar estatísticas sobre tickets de problemas de Produção Comunicar o status de resolução de incidentes aos usuários  Desejável: experiência com Matera ou Change e conhecimento de Espanhol (oral e escrita) || Empresa .....:  Performance and Mind</t>
+        </is>
+      </c>
+      <c r="I628" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>03/02/2026</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t>83553</t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>Desenvolvedor Full Stack Pleno</t>
+        </is>
+      </c>
+      <c r="D629" t="inlineStr">
+        <is>
+          <t>Pleno</t>
+        </is>
+      </c>
+      <c r="E629" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F629" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 03/02/26</t>
+        </is>
+      </c>
+      <c r="G629" t="inlineStr">
+        <is>
+          <t>A GTI Solution é uma das maiores integradoras de Soluções de TI, onde temos como premissa a liberdade de criação e a busca pelo bem-estar dos colaboradores, além de acreditarmos na diversidade da oferta, especialização do atendimento e na valorização da demanda do cliente.  Estamos buscando: Desenvolvedor Full Stack Pleno Node.js Next.js Experiência com APIs REST Boas práticas de desenvolvimento (código limpo, segurança, testes, versionamento) Ter atuado na área de Seguros  Desejáveis AWS (Lambda, API Gateway, S3, SQS, Elastic Beanstalk, RDS, DynamoDB, CodePipeline) SQL Server DynamoDB Docker PHP (para lidar pontualmente com sistemas legados) Conhecimento básico de LGPD (opcional, mas valorizado)  CLT do cliente Atuação híbrida: 03 x presencial por semana - zona sul
+Empresa .....:  GTI SOLUTION</t>
+        </is>
+      </c>
+      <c r="H629" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 03/02/26 || Desenvolvedor Full Stack Pleno || A GTI Solution é uma das maiores integradoras de Soluções de TI, onde temos como premissa a liberdade de criação e a busca pelo bem-estar dos colaboradores, além de acreditarmos na diversidade da oferta, especialização do atendimento e na valorização da demanda do cliente.  Estamos buscando: Desenvolvedor Full Stack Pleno Node.js Next.js Experiência com APIs REST Boas práticas de desenvolvimento (código limpo, segurança, testes, versionamento) Ter atuado na área de Seguros  Desejáveis AWS (Lambda, API Gateway, S3, SQS, Elastic Beanstalk, RDS, DynamoDB, CodePipeline) SQL Server DynamoDB Docker PHP (para lidar pontualmente com sistemas legados) Conhecimento básico de LGPD (opcional, mas valorizado)  CLT do cliente Atuação híbrida: 03 x presencial por semana - zona sul || Empresa .....:  GTI SOLUTION</t>
+        </is>
+      </c>
+      <c r="I629" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>03/02/2026</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t>82477</t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>Desenvolvedor FullStack</t>
+        </is>
+      </c>
+      <c r="D630" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E630" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F630" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 03/02/26</t>
+        </is>
+      </c>
+      <c r="G630" t="inlineStr">
+        <is>
+          <t>Prazo: 12 meses, com chances de prorrogar Local: Remoto Contratação: PJ  Inglês Avançado para conversação Desenvolver interfaces de usuário a partir de mockups de design utilizando HTML, CSS e JavaScript Criar funcionalidades interativas com frameworks como React, Angular ou Vue.js Garantir experiências de usuário responsivas e compatíveis com diferentes navegadores Projetar e implementar lógica do lado do servidor utilizando Python, Java, Node.js ou linguagens similares Criar e manter APIs e gerenciar interações com bancos de dados Integrar software com sistemas e plataformas de terceiros Escrever testes unitários e depurar código em toda a pilha de tecnologia Implementar medidas de segurança para integridade de dados e aplicações Colaborar com designers, desenvolvedores e stakeholders ao longo do ciclo de vida de desenvolvimento de software (SDLC), especialmente em ambientes ágeis Manter-se atualizado com as tecnologias e tendências de front-end e back-end
+Empresa .....:  Entrust IT</t>
+        </is>
+      </c>
+      <c r="H630" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 03/02/26 || Desenvolvedor FullStack || Prazo: 12 meses, com chances de prorrogar Local: Remoto Contratação: PJ  Inglês Avançado para conversação Desenvolver interfaces de usuário a partir de mockups de design utilizando HTML, CSS e JavaScript Criar funcionalidades interativas com frameworks como React, Angular ou Vue.js Garantir experiências de usuário responsivas e compatíveis com diferentes navegadores Projetar e implementar lógica do lado do servidor utilizando Python, Java, Node.js ou linguagens similares Criar e manter APIs e gerenciar interações com bancos de dados Integrar software com sistemas e plataformas de terceiros Escrever testes unitários e depurar código em toda a pilha de tecnologia Implementar medidas de segurança para integridade de dados e aplicações Colaborar com designers, desenvolvedores e stakeholders ao longo do ciclo de vida de desenvolvimento de software (SDLC), especialmente em ambientes ágeis Manter-se atualizado com as tecnologias e tendências de front-end e back-end || Empresa .....:  Entrust IT</t>
+        </is>
+      </c>
+      <c r="I630" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>03/02/2026</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t>82673</t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>Desenvolvedor Fullstack</t>
+        </is>
+      </c>
+      <c r="D631" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E631" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F631" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 03/02/26</t>
+        </is>
+      </c>
+      <c r="G631" t="inlineStr">
+        <is>
+          <t>Prazo: 6 meses, com chances de prorrogação Local: remoto Contratação: PJ  Experiência em .Net e Angular Conhecimento em GCP.
+Empresa .....:  Entrust IT</t>
+        </is>
+      </c>
+      <c r="H631" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 03/02/26 || Desenvolvedor Fullstack || Prazo: 6 meses, com chances de prorrogação Local: remoto Contratação: PJ  Experiência em .Net e Angular Conhecimento em GCP. || Empresa .....:  Entrust IT</t>
+        </is>
+      </c>
+      <c r="I631" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>03/02/2026</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t>82388</t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>Desenvolvedor FullStack (.Net e ReactJS)</t>
+        </is>
+      </c>
+      <c r="D632" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E632" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F632" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 03/02/26</t>
+        </is>
+      </c>
+      <c r="G632" t="inlineStr">
+        <is>
+          <t>Prazo: 12 meses, com chances de prorrogar Local: Remoto Contratação: PJ  Requisitos: Inglês - Avançado para conversação Experiência em Projetos Globais, Melhorias ou Suporte a AMS. Experiência prática em Microsoft .NET Framework (.NET Core) e ReactJS. Conhecimento em Azure Cloud e experiência prática em DevOps são imprescindíveis. Conhecimento em banco de dados é imprescindível.
+Empresa .....:  Entrust IT</t>
+        </is>
+      </c>
+      <c r="H632" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 03/02/26 || Desenvolvedor FullStack (.Net e ReactJS) || Prazo: 12 meses, com chances de prorrogar Local: Remoto Contratação: PJ  Requisitos: Inglês - Avançado para conversação Experiência em Projetos Globais, Melhorias ou Suporte a AMS. Experiência prática em Microsoft .NET Framework (.NET Core) e ReactJS. Conhecimento em Azure Cloud e experiência prática em DevOps são imprescindíveis. Conhecimento em banco de dados é imprescindível. || Empresa .....:  Entrust IT</t>
+        </is>
+      </c>
+      <c r="I632" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>03/02/2026</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>82470</t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>DESENVOLVEDOR JAVA PLENO PRESENCIAL</t>
+        </is>
+      </c>
+      <c r="D633" t="inlineStr">
+        <is>
+          <t>Pleno</t>
+        </is>
+      </c>
+      <c r="E633" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F633" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 03/02/26</t>
+        </is>
+      </c>
+      <c r="G633" t="inlineStr">
+        <is>
+          <t>ANALISTA PROGRAMADOR JAVA PLENO PRESENCIAL Experiência em Java, MySQL, Docker (desejável). Análise e desenvolvimento de sistemas. Contratação PJ: 4 dias presenciais e 1 dia home office
+Empresa .....:  ARTIUM SOLUÇÕES</t>
+        </is>
+      </c>
+      <c r="H633" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 03/02/26 || DESENVOLVEDOR JAVA PLENO PRESENCIAL || ANALISTA PROGRAMADOR JAVA PLENO PRESENCIAL Experiência em Java, MySQL, Docker (desejável). Análise e desenvolvimento de sistemas. Contratação PJ: 4 dias presenciais e 1 dia home office || Empresa .....:  ARTIUM SOLUÇÕES</t>
+        </is>
+      </c>
+      <c r="I633" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>03/02/2026</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>83555</t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>Desenvolvedor Java Sênior</t>
+        </is>
+      </c>
+      <c r="D634" t="inlineStr">
+        <is>
+          <t>Sênior</t>
+        </is>
+      </c>
+      <c r="E634" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F634" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 03/02/26</t>
+        </is>
+      </c>
+      <c r="G634" t="inlineStr">
+        <is>
+          <t>A GTI Solution é uma das maiores integradoras de Soluções de TI, onde temos como premissa a liberdade de criação e a busca pelo bem-estar dos colaboradores, além de acreditarmos na diversidade da oferta, especialização do atendimento e na valorização da demanda do cliente.  Requisitos Obrigatórios Java 8+ Spring Boot 2+ Angular 16+ SQL e NoSQL Filas  Diferencial: Clean Architecture Clean Code Design Patterns  Atuação híbrida: 03 x presencial por semana - SP - SP CLT + benefícios GTI Solution
+Empresa .....:  GTI SOLUTION</t>
+        </is>
+      </c>
+      <c r="H634" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 03/02/26 || Desenvolvedor Java Sênior || A GTI Solution é uma das maiores integradoras de Soluções de TI, onde temos como premissa a liberdade de criação e a busca pelo bem-estar dos colaboradores, além de acreditarmos na diversidade da oferta, especialização do atendimento e na valorização da demanda do cliente.  Requisitos Obrigatórios Java 8+ Spring Boot 2+ Angular 16+ SQL e NoSQL Filas  Diferencial: Clean Architecture Clean Code Design Patterns  Atuação híbrida: 03 x presencial por semana - SP - SP CLT + benefícios GTI Solution || Empresa .....:  GTI SOLUTION</t>
+        </is>
+      </c>
+      <c r="I634" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>03/02/2026</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t>83117</t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>Desenvolvedor JR</t>
+        </is>
+      </c>
+      <c r="D635" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E635" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F635" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 03/02/26</t>
+        </is>
+      </c>
+      <c r="G635" t="inlineStr">
+        <is>
+          <t>Requisitos obrigatórios - JavaScript (lógica, funções, estruturas condicionais) - Node.js (conceitos básicos de backend, APIs, scripts) - SQL (Postgres, Oracle ou similar) - Git (clone, commit, branch, pull request) - React ou Vue.js (conceitos básicos)  Conhecimentos desejáveis (diferencial) - Linux (linha de comando básicos) - Shell Script  Caso não possua esses conhecimentos, há espaço para aprendizado.
+Empresa .....:  Amix Serviços de Informatica Ltda</t>
+        </is>
+      </c>
+      <c r="H635" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 03/02/26 || Desenvolvedor JR || Requisitos obrigatórios - JavaScript (lógica, funções, estruturas condicionais) - Node.js (conceitos básicos de backend, APIs, scripts) - SQL (Postgres, Oracle ou similar) - Git (clone, commit, branch, pull request) - React ou Vue.js (conceitos básicos)  Conhecimentos desejáveis (diferencial) - Linux (linha de comando básicos) - Shell Script  Caso não possua esses conhecimentos, há espaço para aprendizado. || Empresa .....:  Amix Serviços de Informatica Ltda</t>
+        </is>
+      </c>
+      <c r="I635" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>03/02/2026</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t>82570</t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>Desenvolvedor Web Sênior</t>
+        </is>
+      </c>
+      <c r="D636" t="inlineStr">
+        <is>
+          <t>Sênior</t>
+        </is>
+      </c>
+      <c r="E636" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F636" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 03/02/26</t>
+        </is>
+      </c>
+      <c r="G636" t="inlineStr">
+        <is>
+          <t>Requisitos Técnicos : C#: Proficiência na linguagem. NET 8+: Experiência comprovada no desenvolvimento de aplicações escaláveis utilizando as versões mais recentes do framework .NET. Conhecimento avançado e experiência na implementação de Event Sourcing e CQRS DDD (Domain-Driven Design): Sólida vivência na aplicação dos princípios e padrões do DDD. Bancos de Dados Relacionais: Experiência prática e otimização de consultas com SQL Server e Firebird. Vivência com mensageria e processamento assíncrono  Habilidades: Demonstrar proatividade na identificação e resolução de problemas, e comprometimento com a equipe e a qualidade dos projetos. Capacidade de cumprir prazos de entrega previamente definidos, com organização e foco na finalização das tarefas Possuir boa comunicação e facilidade de interação com a equipe interna. Habilidade para liderar novos projetos WEB e transmitir o conhecimento para o time como um todo.
+Empresa .....:  Poliview Tecnologia S/A</t>
+        </is>
+      </c>
+      <c r="H636" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 03/02/26 || Desenvolvedor Web Sênior || Requisitos Técnicos : C#: Proficiência na linguagem. NET 8+: Experiência comprovada no desenvolvimento de aplicações escaláveis utilizando as versões mais recentes do framework .NET. Conhecimento avançado e experiência na implementação de Event Sourcing e CQRS DDD (Domain-Driven Design): Sólida vivência na aplicação dos princípios e padrões do DDD. Bancos de Dados Relacionais: Experiência prática e otimização de consultas com SQL Server e Firebird. Vivência com mensageria e processamento assíncrono  Habilidades: Demonstrar proatividade na identificação e resolução de problemas, e comprometimento com a equipe e a qualidade dos projetos. Capacidade de cumprir prazos de entrega previamente definidos, com organização e foco na finalização das tarefas Possuir boa comunicação e facilidade de interação com a equipe interna. Habilidade para liderar novos projetos WEB e transmitir o conhecimento para o time como um todo. || Empresa .....:  Poliview Tecnologia S/A</t>
+        </is>
+      </c>
+      <c r="I636" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>03/02/2026</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t>82594</t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>Especialista de Suporte</t>
+        </is>
+      </c>
+      <c r="D637" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E637" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F637" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 03/02/26</t>
+        </is>
+      </c>
+      <c r="G637" t="inlineStr">
+        <is>
+          <t>A Emphasys it Services:contrata:  Fornecer suporte técnico oportuno e eficaz aos usuários finais. Diagnosticar e resolver problemas de hardware e software. Auxiliar na instalação, configuração e manutenção de equipamentos de TI Assistência ao usuário Responder às dúvidas dos usuários e fornecer orientação sobre assuntos relacionados a TI. Gerenciamento de incidentes: Implante construções de estações de trabalho e laptops, mantenha o inventário de equipamentos Forte conhecimento em solução de problemas de hardware e software. A certificação ITIL é uma vantagem. Compreensão avançada do SCCM para implantação de pacotes e gerenciamento de patches. Paciência e comunicação clara com os usuários finais internos. Experiência de arquiteto de soluções com Microsoft Windows 11 e Office 365 conhecimento de scripts do Windows PowerShell. A experiência VDI é uma vantagem  Inglês avançado
+Empresa .....:  Emphasys</t>
+        </is>
+      </c>
+      <c r="H637" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 03/02/26 || Especialista de Suporte || A Emphasys it Services:contrata:  Fornecer suporte técnico oportuno e eficaz aos usuários finais. Diagnosticar e resolver problemas de hardware e software. Auxiliar na instalação, configuração e manutenção de equipamentos de TI Assistência ao usuário Responder às dúvidas dos usuários e fornecer orientação sobre assuntos relacionados a TI. Gerenciamento de incidentes: Implante construções de estações de trabalho e laptops, mantenha o inventário de equipamentos Forte conhecimento em solução de problemas de hardware e software. A certificação ITIL é uma vantagem. Compreensão avançada do SCCM para implantação de pacotes e gerenciamento de patches. Paciência e comunicação clara com os usuários finais internos. Experiência de arquiteto de soluções com Microsoft Windows 11 e Office 365 conhecimento de scripts do Windows PowerShell. A experiência VDI é uma vantagem  Inglês avançado || Empresa .....:  Emphasys</t>
+        </is>
+      </c>
+      <c r="I637" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>03/02/2026</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t>82450</t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>Gerente de Projetos/Trade</t>
+        </is>
+      </c>
+      <c r="D638" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E638" t="inlineStr">
+        <is>
+          <t>Híbrido</t>
+        </is>
+      </c>
+      <c r="F638" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 03/02/26</t>
+        </is>
+      </c>
+      <c r="G638" t="inlineStr">
+        <is>
+          <t>Buscamos um Gerente de Projetos com experiência na área de Trade.  Responsabilidades: Garantir comunicação clara e eficaz com stakeholders internos e externos Acompanhar tendências e movimentações do mercado de vendas, propondo estratégias eficazes por canal Garantir rastreabilidade e compliance Suporte e treinamento às áreas de negócio Construção de dashboards em BI para KPIs de promoção Integração de dados de sell in e sell out por SKU/PLU com foco em desempenho de vendas, rentabilidade e cobertura de portfólio Reduzir atividades manuais e conciliação de promoções.  Requisitos: Experiência comprovada em trade Conhecimento de SKU/PLU Visão estratégica sobre o mercado de vendas no geral, incluindo canais diretos e indiretos Forte habilidade analítica e orientação a resultados Conhecimento em Visualfabriq, O9 e Osprey.  Necessário espanhol avançado Desejável inglês avançado.  Híbrido 2x por semana Enviar pretensão PJ e CV
+Empresa .....:  TOPMIND IT</t>
+        </is>
+      </c>
+      <c r="H638" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 03/02/26 || Gerente de Projetos/Trade || Buscamos um Gerente de Projetos com experiência na área de Trade.  Responsabilidades: Garantir comunicação clara e eficaz com stakeholders internos e externos Acompanhar tendências e movimentações do mercado de vendas, propondo estratégias eficazes por canal Garantir rastreabilidade e compliance Suporte e treinamento às áreas de negócio Construção de dashboards em BI para KPIs de promoção Integração de dados de sell in e sell out por SKU/PLU com foco em desempenho de vendas, rentabilidade e cobertura de portfólio Reduzir atividades manuais e conciliação de promoções.  Requisitos: Experiência comprovada em trade Conhecimento de SKU/PLU Visão estratégica sobre o mercado de vendas no geral, incluindo canais diretos e indiretos Forte habilidade analítica e orientação a resultados Conhecimento em Visualfabriq, O9 e Osprey.  Necessário espanhol avançado Desejável inglês avançado.  Híbrido 2x por semana Enviar pretensão PJ e CV || Empresa .....:  TOPMIND IT</t>
+        </is>
+      </c>
+      <c r="I638" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>03/02/2026</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t>82484</t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>Product Owner</t>
+        </is>
+      </c>
+      <c r="D639" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E639" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F639" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 03/02/26</t>
+        </is>
+      </c>
+      <c r="G639" t="inlineStr">
+        <is>
+          <t>Buscamos um Product Owner para liderar iniciativas de implementação de dados, transformação digital e soluções estratégicas para a área de Vendas em um ambiente multinacional.  Requisitos: Experiência sólida como Product Owner ou Analista Funcional Sênior com atuação equivalente. Experiência com projetos de dados, transformação digital e soluções para Vendas. Atuação em projetos complexos e ambientes corporativos multinacionais. Experiência LATAM. Inglês e espanhol avançados para conversação. Perfil analítico, comunicativo e orientado a valor de negócio.  Diferenciais: Experiência com metodologias ágeis (Scrum/Kanban). Conhecimento em CRM, BI ou ferramentas de integração de dados. Híbrido: 3x presencial no escritório e 2x home office  Contratação PJ Horário de trabalho das 09h às 18h
+Empresa .....:  TOPMIND</t>
+        </is>
+      </c>
+      <c r="H639" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 03/02/26 || Product Owner || Buscamos um Product Owner para liderar iniciativas de implementação de dados, transformação digital e soluções estratégicas para a área de Vendas em um ambiente multinacional.  Requisitos: Experiência sólida como Product Owner ou Analista Funcional Sênior com atuação equivalente. Experiência com projetos de dados, transformação digital e soluções para Vendas. Atuação em projetos complexos e ambientes corporativos multinacionais. Experiência LATAM. Inglês e espanhol avançados para conversação. Perfil analítico, comunicativo e orientado a valor de negócio.  Diferenciais: Experiência com metodologias ágeis (Scrum/Kanban). Conhecimento em CRM, BI ou ferramentas de integração de dados. Híbrido: 3x presencial no escritório e 2x home office  Contratação PJ Horário de trabalho das 09h às 18h || Empresa .....:  TOPMIND</t>
+        </is>
+      </c>
+      <c r="I639" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>03/02/2026</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t>82215</t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>Programador Web Pleno - São Paulo - Zona Leste</t>
+        </is>
+      </c>
+      <c r="D640" t="inlineStr">
+        <is>
+          <t>Pleno</t>
+        </is>
+      </c>
+      <c r="E640" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F640" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 03/02/26</t>
+        </is>
+      </c>
+      <c r="G640" t="inlineStr">
+        <is>
+          <t>* Escrever códigos bem estruturados, eficientes e testáveis utilizando as melhores práticas de desenvolvimento de softwares * Criar layout/interface de usuário de sites * Integrar dados de vários serviços de back-end e bancos de dados * Reunir e refinar especificações e requisitos com base em necessidades técnicas * Criar e manter documentação de softwares * Manter-se atualizado sobre tecnologias emergentes e tendências da indústria e aplicá-las em operações e atividades * Cooperar com web designers para atender à concepção visual do projeto.  Conhecimentos necessários: * Angular (JavaScript, typescript) * C# * Python * Versionamento com Git (github) * SQL Server/MySQL * APIs * Webservices  Conhecimentos desejáveis * PHP * Laravel * Nuvem Pública * Desenvolvimento mobile * Sharepoint * UX  Salário Compatível com mercado e benefícios: AM. AO, VR, VA, SV e 2 Bolsas para filhos após o período de experiência.
+Empresa .....:  SAEA  - Educação e Assistência</t>
+        </is>
+      </c>
+      <c r="H640" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 03/02/26 || Programador Web Pleno - São Paulo - Zona Leste || * Escrever códigos bem estruturados, eficientes e testáveis utilizando as melhores práticas de desenvolvimento de softwares * Criar layout/interface de usuário de sites * Integrar dados de vários serviços de back-end e bancos de dados * Reunir e refinar especificações e requisitos com base em necessidades técnicas * Criar e manter documentação de softwares * Manter-se atualizado sobre tecnologias emergentes e tendências da indústria e aplicá-las em operações e atividades * Cooperar com web designers para atender à concepção visual do projeto.  Conhecimentos necessários: * Angular (JavaScript, typescript) * C# * Python * Versionamento com Git (github) * SQL Server/MySQL * APIs * Webservices  Conhecimentos desejáveis * PHP * Laravel * Nuvem Pública * Desenvolvimento mobile * Sharepoint * UX  Salário Compatível com mercado e benefícios: AM. AO, VR, VA, SV e 2 Bolsas para filhos após o período de experiência. || Empresa .....:  SAEA  - Educação e Assistência</t>
+        </is>
+      </c>
+      <c r="I640" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>03/02/2026</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t>83189</t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>Suporte Técnico Campo</t>
+        </is>
+      </c>
+      <c r="D641" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E641" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F641" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 03/02/26</t>
+        </is>
+      </c>
+      <c r="G641" t="inlineStr">
+        <is>
+          <t>Estamos contratando técnico de suporte: Conhecimento em sistemas operacionais windows 10/11 Pró Conhecimento em hardware Conhecimento comprovado em redes, lan e wan.  Desejável Conhecimento em switchs Conhecimento em roteadores Possuir CNH  Contratação: CLT Benefícios: VR/VT/VA e Auxilio Saúde
+Empresa .....:  DryIT Services Intermediação de Negócios</t>
+        </is>
+      </c>
+      <c r="H641" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 03/02/26 || Suporte Técnico Campo || Estamos contratando técnico de suporte: Conhecimento em sistemas operacionais windows 10/11 Pró Conhecimento em hardware Conhecimento comprovado em redes, lan e wan.  Desejável Conhecimento em switchs Conhecimento em roteadores Possuir CNH  Contratação: CLT Benefícios: VR/VT/VA e Auxilio Saúde || Empresa .....:  DryIT Services Intermediação de Negócios</t>
+        </is>
+      </c>
+      <c r="I641" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>03/02/2026</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t>83547</t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>Supply Analyst SR</t>
+        </is>
+      </c>
+      <c r="D642" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E642" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F642" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 03/02/26</t>
+        </is>
+      </c>
+      <c r="G642" t="inlineStr">
+        <is>
+          <t>O Supply Analyst conectará a estratégia comercial às dinâmicas de mercado, garantindo decisões eficientes de compra, hedge e precificação de energia, com foco em confiabilidade e custo-benefício. Atuará em parceria com a célula de dados, apoiando previsão de carga, avaliação de estratégias, monitoramento de riscos e decisões orientadas por dados.  Responsabilidades Avaliar e otimizar processos de supply ponta a ponta Desenvolver e acompanhar KPIs do portfólio (previsibilidade, hedge, custos e margens) Produzir previsões de carga, análises de cenário e impactos de sazonalidade, clima e mix Apoiar decisões de compra e hedge, monitorando posições vs. políticas e limites Acompanhar fundamentos de mercado e gerar relatórios de performance e margem Documentar e comunicar análises e recomendações a stakeholders  Requisitos 3+ anos de experiência (5+ diferencial) Experiência com SQL Formação em Engenharia, Matemática ou áreas correlatas Forte capacidade analítica e autonomia.
+Empresa .....:  Farol plus (Consultoria de RH)</t>
+        </is>
+      </c>
+      <c r="H642" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 03/02/26 || Supply Analyst SR || O Supply Analyst conectará a estratégia comercial às dinâmicas de mercado, garantindo decisões eficientes de compra, hedge e precificação de energia, com foco em confiabilidade e custo-benefício. Atuará em parceria com a célula de dados, apoiando previsão de carga, avaliação de estratégias, monitoramento de riscos e decisões orientadas por dados.  Responsabilidades Avaliar e otimizar processos de supply ponta a ponta Desenvolver e acompanhar KPIs do portfólio (previsibilidade, hedge, custos e margens) Produzir previsões de carga, análises de cenário e impactos de sazonalidade, clima e mix Apoiar decisões de compra e hedge, monitorando posições vs. políticas e limites Acompanhar fundamentos de mercado e gerar relatórios de performance e margem Documentar e comunicar análises e recomendações a stakeholders  Requisitos 3+ anos de experiência (5+ diferencial) Experiência com SQL Formação em Engenharia, Matemática ou áreas correlatas Forte capacidade analítica e autonomia. || Empresa .....:  Farol plus (Consultoria de RH)</t>
+        </is>
+      </c>
+      <c r="I642" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>03/02/2026</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t>83191</t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>Trainee Analista de Sistemas</t>
+        </is>
+      </c>
+      <c r="D643" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E643" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F643" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 03/02/26</t>
+        </is>
+      </c>
+      <c r="G643" t="inlineStr">
+        <is>
+          <t>Estamos contratando analista de sistemas trainee / junior.  Formado em análise de sistemas ou correlato.  Contratação: CLT Benefícios: VT / VR / VA - Aux. Saúde
+Empresa .....:  DryIT Services Intermediação de Negócios</t>
+        </is>
+      </c>
+      <c r="H643" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 03/02/26 || Trainee Analista de Sistemas || Estamos contratando analista de sistemas trainee / junior.  Formado em análise de sistemas ou correlato.  Contratação: CLT Benefícios: VT / VR / VA - Aux. Saúde || Empresa .....:  DryIT Services Intermediação de Negócios</t>
+        </is>
+      </c>
+      <c r="I643" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>03/02/2026</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t>82476</t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>Desenvolvedor Pleno DELPHI</t>
+        </is>
+      </c>
+      <c r="D644" t="inlineStr">
+        <is>
+          <t>Pleno</t>
+        </is>
+      </c>
+      <c r="E644" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F644" t="inlineStr">
+        <is>
+          <t>Americana - SP - 02/02/26</t>
+        </is>
+      </c>
+      <c r="G644" t="inlineStr">
+        <is>
+          <t>Desenvolvedor de Software em linguagem DELPHI  Requisitos: Experiência em desenvolvimento de software em Delphi nível Pleno Domino de TSQL
+Empresa .....:  Microdata Sistemas</t>
+        </is>
+      </c>
+      <c r="H644" t="inlineStr">
+        <is>
+          <t>Americana - SP - 02/02/26 || Desenvolvedor Pleno DELPHI || Desenvolvedor de Software em linguagem DELPHI  Requisitos: Experiência em desenvolvimento de software em Delphi nível Pleno Domino de TSQL || Empresa .....:  Microdata Sistemas</t>
+        </is>
+      </c>
+      <c r="I644" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>03/02/2026</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t>83140</t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>Analista de Infraestrutura Cloud Azure e Segurança</t>
+        </is>
+      </c>
+      <c r="D645" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E645" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F645" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 02/02/26</t>
+        </is>
+      </c>
+      <c r="G645" t="inlineStr">
+        <is>
+          <t>Modelo: Remoto  Nível: Pleno  -- Responsabilidades: - Administração da infraestrutura em Azure incluindo: Web Apps, Azure SQL, Virtual Machines, Data Factory, Databricks e Blob Storage - Implementação de automação de scaling e boas práticas de FinOps (controle, análise e otimização de custos) - Gestão do Cloudflare, domínios, DNS e WAF - Implementação e manutenção de políticas de DLP (Data Loss Prevention) - Monitoramento dos recursos com Grafana, dashboards e alertas - Atuação preventiva e corretiva em incidentes de infraestrutura - Gestão do ambiente Microsoft 365, com administração de contas, acessos e licenças  -- Requisitos: - Experiência sólida com Azure e seus principais serviços - Vivência com Cloudflare e firewalls  **Obrigatório conhecimento implantação de ferramentas para DLP
+Empresa .....:  Target Software</t>
+        </is>
+      </c>
+      <c r="H645" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 02/02/26 || Analista de Infraestrutura Cloud Azure e Segurança || Modelo: Remoto  Nível: Pleno  -- Responsabilidades: - Administração da infraestrutura em Azure incluindo: Web Apps, Azure SQL, Virtual Machines, Data Factory, Databricks e Blob Storage - Implementação de automação de scaling e boas práticas de FinOps (controle, análise e otimização de custos) - Gestão do Cloudflare, domínios, DNS e WAF - Implementação e manutenção de políticas de DLP (Data Loss Prevention) - Monitoramento dos recursos com Grafana, dashboards e alertas - Atuação preventiva e corretiva em incidentes de infraestrutura - Gestão do ambiente Microsoft 365, com administração de contas, acessos e licenças  -- Requisitos: - Experiência sólida com Azure e seus principais serviços - Vivência com Cloudflare e firewalls  **Obrigatório conhecimento implantação de ferramentas para DLP || Empresa .....:  Target Software</t>
+        </is>
+      </c>
+      <c r="I645" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>03/02/2026</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t>83093</t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>Arquiteto de Soluções Corporativas Temporário</t>
+        </is>
+      </c>
+      <c r="D646" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E646" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F646" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 02/02/26</t>
+        </is>
+      </c>
+      <c r="G646" t="inlineStr">
+        <is>
+          <t>Buscamos Arquiteto(a) de Soluções corporativas com atuação estratégica e transversal, focado em automações, IA, integrações, cloud e dados. Perfil voltado a desenho e governança de arquitetura, apoiando decisões técnicas sem atuação como desenvolvedor full-time.  Responsabilidades: •	Definição de arquitetura de soluções (AS-IS / TO-BE) •	Desenho de integrações (APIs, eventos, mensageria, dados) •	Avaliação técnica de soluções, fornecedores e riscos •	Apoio técnico a times internos, parceiros e áreas de negócio •	Atuação em padrões, governança, segurança e escalabilidade  Requisitos: •	Experiência em arquitetura corporativa •	Visão multicloud (AWS, Azure, GCP) •	Conhecimento em APIs, microsserviços, eventos, dados e automação •	Segurança (OAuth2, OIDC) e observabilidade  Obs: Vaga temporária por 6 meses mas, com chances de se estender. Contratação PJ.
+Empresa .....:  CBYK</t>
+        </is>
+      </c>
+      <c r="H646" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 02/02/26 || Arquiteto de Soluções Corporativas Temporário || Buscamos Arquiteto(a) de Soluções corporativas com atuação estratégica e transversal, focado em automações, IA, integrações, cloud e dados. Perfil voltado a desenho e governança de arquitetura, apoiando decisões técnicas sem atuação como desenvolvedor full-time.  Responsabilidades: •	Definição de arquitetura de soluções (AS-IS / TO-BE) •	Desenho de integrações (APIs, eventos, mensageria, dados) •	Avaliação técnica de soluções, fornecedores e riscos •	Apoio técnico a times internos, parceiros e áreas de negócio •	Atuação em padrões, governança, segurança e escalabilidade  Requisitos: •	Experiência em arquitetura corporativa •	Visão multicloud (AWS, Azure, GCP) •	Conhecimento em APIs, microsserviços, eventos, dados e automação •	Segurança (OAuth2, OIDC) e observabilidade  Obs: Vaga temporária por 6 meses mas, com chances de se estender. Contratação PJ. || Empresa .....:  CBYK</t>
+        </is>
+      </c>
+      <c r="I646" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>03/02/2026</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t>83109</t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>Engenheiro FullStack</t>
+        </is>
+      </c>
+      <c r="D647" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E647" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F647" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 02/02/26</t>
+        </is>
+      </c>
+      <c r="G647" t="inlineStr">
+        <is>
+          <t>Vaga: Engenheiro FullStack Prazo: 6 meses, com chances de prorrogar Local: Remoto Contratação: PJ  Requisitos Técnicos: Buscamos um(a) Desenvolvedor(a) Full Stack com foco em Inteligência Artificial para atuar no desenvolvimento de aplicações ponta a ponta, integrando frontend, backend e modelos de IA/ML. A pessoa colaborará com times de produto e dados na criação de soluções escaláveis, testáveis e orientadas ao valor de negócio. Experiência em frontend (React, Angular ou Vue HTML, CSS, JavaScript/TypeScript), backend (Node.js, Python, Java ou .NET), APIs REST/GraphQL, integração com serviços de IA/LLMs, fundamentos de IA/ML, bancos de dados relacionais e NoSQL, testes automatizados, boas práticas de engenharia e arquiteturas RAG com uso de vetores e mecanismos de busca.
+Empresa .....:  Entrust IT</t>
+        </is>
+      </c>
+      <c r="H647" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 02/02/26 || Engenheiro FullStack || Vaga: Engenheiro FullStack Prazo: 6 meses, com chances de prorrogar Local: Remoto Contratação: PJ  Requisitos Técnicos: Buscamos um(a) Desenvolvedor(a) Full Stack com foco em Inteligência Artificial para atuar no desenvolvimento de aplicações ponta a ponta, integrando frontend, backend e modelos de IA/ML. A pessoa colaborará com times de produto e dados na criação de soluções escaláveis, testáveis e orientadas ao valor de negócio. Experiência em frontend (React, Angular ou Vue HTML, CSS, JavaScript/TypeScript), backend (Node.js, Python, Java ou .NET), APIs REST/GraphQL, integração com serviços de IA/LLMs, fundamentos de IA/ML, bancos de dados relacionais e NoSQL, testes automatizados, boas práticas de engenharia e arquiteturas RAG com uso de vetores e mecanismos de busca. || Empresa .....:  Entrust IT</t>
+        </is>
+      </c>
+      <c r="I647" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>03/02/2026</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t>82511</t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>Técnicos de operações de TI São Paulo</t>
+        </is>
+      </c>
+      <c r="D648" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E648" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F648" t="inlineStr">
+        <is>
+          <t>Osasco - SP - 02/02/26</t>
+        </is>
+      </c>
+      <c r="G648" t="inlineStr">
+        <is>
+          <t>Possui conhecimento amplo e aprofundado sobre operações de TI e seus processos relacionados. É capaz de realizar análises proativas de risco, identificar potenciais ameaças e definir medidas de controle para as atividades de TI em datacenters (IDC) ou parques tecnológicos. Atua na otimização contínua dos processos de EOP e SOP.
+Empresa .....:  KUNYUCOMM TECH BRASIL LTDA.</t>
+        </is>
+      </c>
+      <c r="H648" t="inlineStr">
+        <is>
+          <t>Osasco - SP - 02/02/26 || Técnicos de operações de TI São Paulo || Possui conhecimento amplo e aprofundado sobre operações de TI e seus processos relacionados. É capaz de realizar análises proativas de risco, identificar potenciais ameaças e definir medidas de controle para as atividades de TI em datacenters (IDC) ou parques tecnológicos. Atua na otimização contínua dos processos de EOP e SOP. || Empresa .....:  KUNYUCOMM TECH BRASIL LTDA.</t>
+        </is>
+      </c>
+      <c r="I648" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>03/02/2026</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t>82818</t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>Analista de Infraestrutura Pleno</t>
+        </is>
+      </c>
+      <c r="D649" t="inlineStr">
+        <is>
+          <t>Pleno</t>
+        </is>
+      </c>
+      <c r="E649" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F649" t="inlineStr">
+        <is>
+          <t>São Caetano do Sul - SP - 02/02/26</t>
+        </is>
+      </c>
+      <c r="G649" t="inlineStr">
+        <is>
+          <t>Suporte e sustentação de servidores, redes, firewalls, cloud e segurança.  Conhecimentos necessários: Microsoft 365 Nextgen Firewall Windows Server / AD Antivírus EDR / XDR Backup (Acromis, Arcserv ou outro) Administração de Redes  CLT VAGAS PARA PLENO: a partir de R$ 3.000,00 + Beneficios (VR, VT, GYMPASS. PLANO DE SAUDE SULAMERICA)
+Empresa .....:  Multipoint It Solutions</t>
+        </is>
+      </c>
+      <c r="H649" t="inlineStr">
+        <is>
+          <t>São Caetano do Sul - SP - 02/02/26 || Analista de Infraestrutura Pleno || Suporte e sustentação de servidores, redes, firewalls, cloud e segurança.  Conhecimentos necessários: Microsoft 365 Nextgen Firewall Windows Server / AD Antivírus EDR / XDR Backup (Acromis, Arcserv ou outro) Administração de Redes  CLT VAGAS PARA PLENO: a partir de R$ 3.000,00 + Beneficios (VR, VT, GYMPASS. PLANO DE SAUDE SULAMERICA) || Empresa .....:  Multipoint It Solutions</t>
+        </is>
+      </c>
+      <c r="I649" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>03/02/2026</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t>83536</t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>Analista de Dados Power BI – Pleno</t>
+        </is>
+      </c>
+      <c r="D650" t="inlineStr">
+        <is>
+          <t>Pleno</t>
+        </is>
+      </c>
+      <c r="E650" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F650" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 02/02/26</t>
+        </is>
+      </c>
+      <c r="G650" t="inlineStr">
+        <is>
+          <t>Criar e manter dashboards e relatórios interativos no Power BI Desenvolver modelos de dados eficientes e performáticos Aplicar DAX e Power Query para criação de métricas e transformação de dados Integrar diferentes fontes (MySQL, APIs, Excel, SharePoint, DW e Data Lake) Transformar dados em insights acionáveis para o negócio Garantir qualidade, governança e segurança dos dados Colaborar com times multidisciplinares em soluções analíticas  - Requisitos Experiência com Power BI (DAX, Power Query e modelagem de dados) Conhecimento em SQL Experiência com ETL e tratamento de dados Noções de Data Warehouse, Data Lake e governança de dados Perfil analítico e boa comunicação com stakeholders  Conhecimento em Figma será considerado diferencial  - O que oferecemos - R$ 7.500,00 - Bônus anual - Cartão FLASH (refeição/alimentação) - TotalPass - Clude Saúde + Cartão de TODOS - Modelo híbrido (3x presencial / 2x remoto
+Empresa .....:  NCM Sistemas e Consultoria</t>
+        </is>
+      </c>
+      <c r="H650" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 02/02/26 || Analista de Dados Power BI – Pleno || Criar e manter dashboards e relatórios interativos no Power BI Desenvolver modelos de dados eficientes e performáticos Aplicar DAX e Power Query para criação de métricas e transformação de dados Integrar diferentes fontes (MySQL, APIs, Excel, SharePoint, DW e Data Lake) Transformar dados em insights acionáveis para o negócio Garantir qualidade, governança e segurança dos dados Colaborar com times multidisciplinares em soluções analíticas  - Requisitos Experiência com Power BI (DAX, Power Query e modelagem de dados) Conhecimento em SQL Experiência com ETL e tratamento de dados Noções de Data Warehouse, Data Lake e governança de dados Perfil analítico e boa comunicação com stakeholders  Conhecimento em Figma será considerado diferencial  - O que oferecemos - R$ 7.500,00 - Bônus anual - Cartão FLASH (refeição/alimentação) - TotalPass - Clude Saúde + Cartão de TODOS - Modelo híbrido (3x presencial / 2x remoto || Empresa .....:  NCM Sistemas e Consultoria</t>
+        </is>
+      </c>
+      <c r="I650" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>03/02/2026</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t>83115</t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>Analista de Infraestrutura Sênior (hibrido)</t>
+        </is>
+      </c>
+      <c r="D651" t="inlineStr">
+        <is>
+          <t>Sênior</t>
+        </is>
+      </c>
+      <c r="E651" t="inlineStr">
+        <is>
+          <t>Híbrido</t>
+        </is>
+      </c>
+      <c r="F651" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 02/02/26</t>
+        </is>
+      </c>
+      <c r="G651" t="inlineStr">
+        <is>
+          <t>REQUISITOS E QUALIFICAÇÕES Experiência comprovada em ambientes Oracle Cloud e AWS Domínio em VMWare e projetos de migração para Cloud Conhecimentos avançados em sistemas operacionais Windows e Linux Capacidade de análise crítica, resolução de problemas e trabalho colaborativo Boa comunicação e organização.  Diferenciais: Certificações em Cloud (AWS, Oracle) ou VMWare Experiência com ferramentas de automação e infraestrutura como código (IaC) Vivência em ambientes corporativos com alta disponibilidade.
+Empresa .....:  3CON CONSULTORIA E SISTEMAS</t>
+        </is>
+      </c>
+      <c r="H651" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 02/02/26 || Analista de Infraestrutura Sênior (hibrido) || REQUISITOS E QUALIFICAÇÕES Experiência comprovada em ambientes Oracle Cloud e AWS Domínio em VMWare e projetos de migração para Cloud Conhecimentos avançados em sistemas operacionais Windows e Linux Capacidade de análise crítica, resolução de problemas e trabalho colaborativo Boa comunicação e organização.  Diferenciais: Certificações em Cloud (AWS, Oracle) ou VMWare Experiência com ferramentas de automação e infraestrutura como código (IaC) Vivência em ambientes corporativos com alta disponibilidade. || Empresa .....:  3CON CONSULTORIA E SISTEMAS</t>
+        </is>
+      </c>
+      <c r="I651" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>03/02/2026</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t>83103</t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>Analista de Segurança da Informação</t>
+        </is>
+      </c>
+      <c r="D652" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E652" t="inlineStr">
+        <is>
+          <t>Híbrido</t>
+        </is>
+      </c>
+      <c r="F652" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 02/02/26</t>
+        </is>
+      </c>
+      <c r="G652" t="inlineStr">
+        <is>
+          <t>Requisitos necessários:  Conhecimentos em  ZTNA, Conhecimento em Netskope e/ou Fortinet e/ou CDN (Cloudflare).#8203 Firewall Fortinet e filtro de conteúdo EDR, cofre de senha, Tunnel GRE/IpSec, Abrangente conhecimento em redes. Conhecimento de protocolos web.#8203 Inglês Intermediário (leitura, escrita e conversação).  Atuação: Híbrido - 1x presencial na Chácara Santo Antônio - São Paulo - SP  Formação: Graduação  Concluída ou cursando Vaga efetiva Ramo da empresa: Segurança da Informação Contratação CLT + Benefícios
+Empresa .....:  Moot Consulting</t>
+        </is>
+      </c>
+      <c r="H652" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 02/02/26 || Analista de Segurança da Informação || Requisitos necessários:  Conhecimentos em  ZTNA, Conhecimento em Netskope e/ou Fortinet e/ou CDN (Cloudflare).#8203 Firewall Fortinet e filtro de conteúdo EDR, cofre de senha, Tunnel GRE/IpSec, Abrangente conhecimento em redes. Conhecimento de protocolos web.#8203 Inglês Intermediário (leitura, escrita e conversação).  Atuação: Híbrido - 1x presencial na Chácara Santo Antônio - São Paulo - SP  Formação: Graduação  Concluída ou cursando Vaga efetiva Ramo da empresa: Segurança da Informação Contratação CLT + Benefícios || Empresa .....:  Moot Consulting</t>
+        </is>
+      </c>
+      <c r="I652" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>03/02/2026</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t>82234</t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>Analista de sistemas MV Pleno</t>
+        </is>
+      </c>
+      <c r="D653" t="inlineStr">
+        <is>
+          <t>Pleno</t>
+        </is>
+      </c>
+      <c r="E653" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F653" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 02/02/26</t>
+        </is>
+      </c>
+      <c r="G653" t="inlineStr">
+        <is>
+          <t>• Experiência com sistemas de gestão hospitalar (ERP MV Saúde). • Domínio de banco de dados e consultas SQL. • Vivência com ferramentas de análise e visualização de dados (Power BI ou equivalentes). • Conhecimento em mapeamento e modelagem de processos (fluxogramas, BPMN, Visio). • Habilidade em documentação técnica, elaboração de manuais e definição de fluxos operacionais. • Conhecimento em boas práticas de governança de TI e controle de acessos. • Domínio do pacote Microsoft Office, especialmente Excel avançado, PowerQuery e PowerPivot.
+Empresa .....:  WTime</t>
+        </is>
+      </c>
+      <c r="H653" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 02/02/26 || Analista de sistemas MV Pleno || • Experiência com sistemas de gestão hospitalar (ERP MV Saúde). • Domínio de banco de dados e consultas SQL. • Vivência com ferramentas de análise e visualização de dados (Power BI ou equivalentes). • Conhecimento em mapeamento e modelagem de processos (fluxogramas, BPMN, Visio). • Habilidade em documentação técnica, elaboração de manuais e definição de fluxos operacionais. • Conhecimento em boas práticas de governança de TI e controle de acessos. • Domínio do pacote Microsoft Office, especialmente Excel avançado, PowerQuery e PowerPivot. || Empresa .....:  WTime</t>
+        </is>
+      </c>
+      <c r="I653" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>03/02/2026</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t>83182</t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>ANALISTA DE TECNOLOGIA DA INFORMAÇÃO JR</t>
+        </is>
+      </c>
+      <c r="D654" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E654" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F654" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 02/02/26</t>
+        </is>
+      </c>
+      <c r="G654" t="inlineStr">
+        <is>
+          <t>ANALISTA DE TECNOLOGIA DA INFORMAÇÃO JÚNIOR I – PRESENCIAL São Paulo/SP  Ambiente leve, ético, diverso e comprometido com impacto positivo na sociedade e no meio ambiente.  Buscamos uma pessoa responsável, organizada, proativa e com bom relacionamento interpessoal, que queira se desenvolver na área de Tecnologia da Informação.  Principais responsabilidades: Suporte e manutenção de hardware, realização de testes lógicos e físicos, troca de componentes, conhecimentos básicos em VPN, Microsoft Teams e Office 365, boa comunicação escrita e verbal, organização, dinamismo e capacidade de trabalhar sob pressão.  Competências necessárias: Cursando Ciência da Computação, Sistemas de Informação, Redes ou áreas correlatas. Conhecimento básico em sistemas operacionais, hardware, software, Excel, além de empatia e boa comunicação.  Benefícios: Vale Refeição, Vale Transporte, Assistência Médica e Odontológica, Auxílio Creche e Seguro de Vida.  Salario R$ 2.245,00
+Empresa .....:  KVM TECNOLOGIA</t>
+        </is>
+      </c>
+      <c r="H654" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 02/02/26 || ANALISTA DE TECNOLOGIA DA INFORMAÇÃO JR || ANALISTA DE TECNOLOGIA DA INFORMAÇÃO JÚNIOR I – PRESENCIAL São Paulo/SP  Ambiente leve, ético, diverso e comprometido com impacto positivo na sociedade e no meio ambiente.  Buscamos uma pessoa responsável, organizada, proativa e com bom relacionamento interpessoal, que queira se desenvolver na área de Tecnologia da Informação.  Principais responsabilidades: Suporte e manutenção de hardware, realização de testes lógicos e físicos, troca de componentes, conhecimentos básicos em VPN, Microsoft Teams e Office 365, boa comunicação escrita e verbal, organização, dinamismo e capacidade de trabalhar sob pressão.  Competências necessárias: Cursando Ciência da Computação, Sistemas de Informação, Redes ou áreas correlatas. Conhecimento básico em sistemas operacionais, hardware, software, Excel, além de empatia e boa comunicação.  Benefícios: Vale Refeição, Vale Transporte, Assistência Médica e Odontológica, Auxílio Creche e Seguro de Vida.  Salario R$ 2.245,00 || Empresa .....:  KVM TECNOLOGIA</t>
+        </is>
+      </c>
+      <c r="I654" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>03/02/2026</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t>82512</t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>Arquiteto de Software - Java</t>
+        </is>
+      </c>
+      <c r="D655" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E655" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F655" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 02/02/26</t>
+        </is>
+      </c>
+      <c r="G655" t="inlineStr">
+        <is>
+          <t>- Escrever um código limpo e eficiente usando Java e suas tecnologias relacionadas, aderindo às melhores práticas e padrões de codificação. - Utilizar ferramentas de automação de testes, como JUnit, para garantir a qualidade do software desenvolvido.  Experiência em desenvolvimento de software, com sólidos conhecimentos em Java e arquitetura de sistemas. Experiência com tecnologias como Spring, Hibernate, Maven, JUnit, Docker, Kubernetes e cloud Azure é necessária.  Modelo de Alocação: Híbrida - 2x por semana na Vila Olímpia. Período de Alocação: Tempo indeterminado - PJ
+Empresa .....:  SOW Serviços</t>
+        </is>
+      </c>
+      <c r="H655" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 02/02/26 || Arquiteto de Software - Java || - Escrever um código limpo e eficiente usando Java e suas tecnologias relacionadas, aderindo às melhores práticas e padrões de codificação. - Utilizar ferramentas de automação de testes, como JUnit, para garantir a qualidade do software desenvolvido.  Experiência em desenvolvimento de software, com sólidos conhecimentos em Java e arquitetura de sistemas. Experiência com tecnologias como Spring, Hibernate, Maven, JUnit, Docker, Kubernetes e cloud Azure é necessária.  Modelo de Alocação: Híbrida - 2x por semana na Vila Olímpia. Período de Alocação: Tempo indeterminado - PJ || Empresa .....:  SOW Serviços</t>
+        </is>
+      </c>
+      <c r="I655" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>03/02/2026</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t>82564</t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>Consultor de Transformação de Negócios/Treinamento</t>
+        </is>
+      </c>
+      <c r="D656" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E656" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F656" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 02/02/26</t>
+        </is>
+      </c>
+      <c r="G656" t="inlineStr">
+        <is>
+          <t>Acompanhar o requisitos do treinamento junto com time de projeto •    Acompanhar a estratégia de execução do treinamento •    Acompanhar e validar formatos de treinamentos •    Produzir os materiais de treinamentos •    Acompanhar  sessões de treinamentos com Key Users •    Revisar e manter os treinamentos atualizados  Vaga remota Enviar cv com pretensão CLT e PJ
+Empresa .....:  TOPMIND IT</t>
+        </is>
+      </c>
+      <c r="H656" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 02/02/26 || Consultor de Transformação de Negócios/Treinamento || Acompanhar o requisitos do treinamento junto com time de projeto •    Acompanhar a estratégia de execução do treinamento •    Acompanhar e validar formatos de treinamentos •    Produzir os materiais de treinamentos •    Acompanhar  sessões de treinamentos com Key Users •    Revisar e manter os treinamentos atualizados  Vaga remota Enviar cv com pretensão CLT e PJ || Empresa .....:  TOPMIND IT</t>
+        </is>
+      </c>
+      <c r="I656" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>03/02/2026</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t>82502</t>
+        </is>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>Desenvolvedor Full Stack</t>
+        </is>
+      </c>
+      <c r="D657" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E657" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F657" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 02/02/26</t>
+        </is>
+      </c>
+      <c r="G657" t="inlineStr">
+        <is>
+          <t>Local: Vila Congonhas – São Paulo/SP Modalidade: Híbrido (3x presencial  2x remoto) Contratação: PJ Remuneração: A combinar  Requisitos Técnicos: • Back-end: .NET, ASP.NET Core, MVC, Web Forms • Front-end: React ou Angular (desejável) • Arquitetura: Microservices • Sistemas: Experiência com sistema de controle de fila e mensageria • Banco de Dados: SQL Server e MongoDB • Metodologias: Atuação com metodologias ágeis (preferencialmente Scrum)
+Empresa .....:  Devpartner</t>
+        </is>
+      </c>
+      <c r="H657" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 02/02/26 || Desenvolvedor Full Stack || Local: Vila Congonhas – São Paulo/SP Modalidade: Híbrido (3x presencial  2x remoto) Contratação: PJ Remuneração: A combinar  Requisitos Técnicos: • Back-end: .NET, ASP.NET Core, MVC, Web Forms • Front-end: React ou Angular (desejável) • Arquitetura: Microservices • Sistemas: Experiência com sistema de controle de fila e mensageria • Banco de Dados: SQL Server e MongoDB • Metodologias: Atuação com metodologias ágeis (preferencialmente Scrum) || Empresa .....:  Devpartner</t>
+        </is>
+      </c>
+      <c r="I657" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>03/02/2026</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t>82720</t>
+        </is>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>Desenvolvedor Java Oracle Híbrido SP</t>
+        </is>
+      </c>
+      <c r="D658" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E658" t="inlineStr">
+        <is>
+          <t>Híbrido</t>
+        </is>
+      </c>
+      <c r="F658" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 02/02/26</t>
+        </is>
+      </c>
+      <c r="G658" t="inlineStr">
+        <is>
+          <t>•	Ensino Superior em Tecnologia ou Ciência da Computação. •	Domínio em Java (JSE, JEE, JSP, Servlets, Spring Boot, Spring MVC, Hibernate, JPA) e JavaScript, HTML5, CSS3, JSON, AJAX. •	Experiência com APIs RESTful e SOAP. •	Conhecimento em Spring (Boot, Data, Security), Hibernate, Angular ou React, Bootstrap, Maven, Git, Jenkins ou GitLab CI/CD. •	Vivência com IDEs (Eclipse, IntelliJ, VS Code, NetBeans) e servidores de aplicação (Apache Tomcat, JBoss, WebLogic). •	Sólido conhecimento em SQL e PL/SQL (Oracle, PostgreSQL ou MySQL), modelagem de dados (DER) e integração via JDBC/JPA. •	Experiência com arquitetura e padrões de projeto (MVC, DAO, Factory, Singleton, Observer, UML). •	Atuação com metodologias ágeis (Scrum, Kanban) e práticas de Integração Contínua e Entrega Contínua (CI/CD).  Contratação CLT Híbrido SP  Caso tenha interesse é só enviar o cv atualizado com a pretensão salarial CLT
+Empresa .....:  TO Brasil</t>
+        </is>
+      </c>
+      <c r="H658" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 02/02/26 || Desenvolvedor Java Oracle Híbrido SP || •	Ensino Superior em Tecnologia ou Ciência da Computação. •	Domínio em Java (JSE, JEE, JSP, Servlets, Spring Boot, Spring MVC, Hibernate, JPA) e JavaScript, HTML5, CSS3, JSON, AJAX. •	Experiência com APIs RESTful e SOAP. •	Conhecimento em Spring (Boot, Data, Security), Hibernate, Angular ou React, Bootstrap, Maven, Git, Jenkins ou GitLab CI/CD. •	Vivência com IDEs (Eclipse, IntelliJ, VS Code, NetBeans) e servidores de aplicação (Apache Tomcat, JBoss, WebLogic). •	Sólido conhecimento em SQL e PL/SQL (Oracle, PostgreSQL ou MySQL), modelagem de dados (DER) e integração via JDBC/JPA. •	Experiência com arquitetura e padrões de projeto (MVC, DAO, Factory, Singleton, Observer, UML). •	Atuação com metodologias ágeis (Scrum, Kanban) e práticas de Integração Contínua e Entrega Contínua (CI/CD).  Contratação CLT Híbrido SP  Caso tenha interesse é só enviar o cv atualizado com a pretensão salarial CLT || Empresa .....:  TO Brasil</t>
+        </is>
+      </c>
+      <c r="I658" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>03/02/2026</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t>82561</t>
+        </is>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>Engenheiro de Dados</t>
+        </is>
+      </c>
+      <c r="D659" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E659" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F659" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 02/02/26</t>
+        </is>
+      </c>
+      <c r="G659" t="inlineStr">
+        <is>
+          <t>Prazo: 3 meses, com chance de prorrogação. Local: Remoto Contratação: PJ  Python: Para scripts de ETL, análise ou automações. C# e .NET Core(desejável): Experiência em desenvolvimento de serviços de dados. Desenvolver soluções em linguagens como: Python, SQL e .NET * Bancos de Dados SQL Server / PostgreSQL: Domínio em consultas, modelagem e tuning. NoSQL: Conhecimento em MongoDB e Redis é um diferencial. Mensageria RabbitMQ e/ou Kafka: Experiência com processamento assíncrono, eventos e alta performance. ETL e Pipelines Construção e manutenção de pipelines de dados automatizados (batch ou streaming). Experiência com ferramentas de orquestração (ex: Apache Airflow, Azure Data Factory, Luigi, etc.). DevOps / Integração Contínua Experiência com Git, Azure DevOps ou ferramentas similares para versionamento e CI/CD. Automatização de deploys de pipelines e monitoramento. Distribuição e Sincronização de Dados
+Empresa .....:  Entrust IT</t>
+        </is>
+      </c>
+      <c r="H659" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 02/02/26 || Engenheiro de Dados || Prazo: 3 meses, com chance de prorrogação. Local: Remoto Contratação: PJ  Python: Para scripts de ETL, análise ou automações. C# e .NET Core(desejável): Experiência em desenvolvimento de serviços de dados. Desenvolver soluções em linguagens como: Python, SQL e .NET * Bancos de Dados SQL Server / PostgreSQL: Domínio em consultas, modelagem e tuning. NoSQL: Conhecimento em MongoDB e Redis é um diferencial. Mensageria RabbitMQ e/ou Kafka: Experiência com processamento assíncrono, eventos e alta performance. ETL e Pipelines Construção e manutenção de pipelines de dados automatizados (batch ou streaming). Experiência com ferramentas de orquestração (ex: Apache Airflow, Azure Data Factory, Luigi, etc.). DevOps / Integração Contínua Experiência com Git, Azure DevOps ou ferramentas similares para versionamento e CI/CD. Automatização de deploys de pipelines e monitoramento. Distribuição e Sincronização de Dados || Empresa .....:  Entrust IT</t>
+        </is>
+      </c>
+      <c r="I659" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>03/02/2026</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t>83535</t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>Gerente de Inteligência de Negócios</t>
+        </is>
+      </c>
+      <c r="D660" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E660" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F660" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 02/02/26</t>
+        </is>
+      </c>
+      <c r="G660" t="inlineStr">
+        <is>
+          <t>Liderar e desenvolver a equipe de Inteligência de Negócios e BI, promovendo alta performance e aprendizado contínuo Definir e executar a estratégia de BI alinhada aos objetivos corporativos e à evolução do Marketplace das Oportunidades Antecipar necessidades de dados das áreas de Vendas, Marketing, Operações, Finanças e Produto Desenvolver e manter dashboards, relatórios e modelos de dados complexos Analisar tendências de mercado, desempenho da plataforma, métricas de crescimento e concorrência Avaliar e implementar novas ferramentas e tecnologias de BI Atuar como agente de disseminação da cultura data-driven Garantir governança, qualidade e segurança da informação (LGPD)  - Desafios da posição Garantir a integridade, governança e escalabilidade dos dados Apresentar insights estratégicos para a alta gestão e parceiros do ecossistema  - Requisitos Formação superior em Ciência da Computação, Engenharia, Estatística
+Empresa .....:  NCM Sistemas e Consultoria</t>
+        </is>
+      </c>
+      <c r="H660" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 02/02/26 || Gerente de Inteligência de Negócios || Liderar e desenvolver a equipe de Inteligência de Negócios e BI, promovendo alta performance e aprendizado contínuo Definir e executar a estratégia de BI alinhada aos objetivos corporativos e à evolução do Marketplace das Oportunidades Antecipar necessidades de dados das áreas de Vendas, Marketing, Operações, Finanças e Produto Desenvolver e manter dashboards, relatórios e modelos de dados complexos Analisar tendências de mercado, desempenho da plataforma, métricas de crescimento e concorrência Avaliar e implementar novas ferramentas e tecnologias de BI Atuar como agente de disseminação da cultura data-driven Garantir governança, qualidade e segurança da informação (LGPD)  - Desafios da posição Garantir a integridade, governança e escalabilidade dos dados Apresentar insights estratégicos para a alta gestão e parceiros do ecossistema  - Requisitos Formação superior em Ciência da Computação, Engenharia, Estatística || Empresa .....:  NCM Sistemas e Consultoria</t>
+        </is>
+      </c>
+      <c r="I660" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>03/02/2026</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t>83089</t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>Técnico de Informatica JR II - Guarulhos</t>
+        </is>
+      </c>
+      <c r="D661" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E661" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F661" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 02/02/26</t>
+        </is>
+      </c>
+      <c r="G661" t="inlineStr">
+        <is>
+          <t>Realizar atendimento para solucionar problemas de baixa a media complexidade. Conceder acesso as telas do sistema Metodo. Instalar e configurar programas no ambiente Windows, pacote office e outros executados nesse ambiente. Realizar a movimentação de computadores, impressoras e demais ativos de TI.  Criar usuários e alterar senhas na rede. Criar conta de e-mail e alterar senha de acesso. Criar usuário e alterar senha no portal. Criar usuários, alteração e bloqueio de acesso ao sistema Metodo.  Realizar suporte remoto aos computadores por VNC. Prestar atendimento aos colaboradores da Unidade. Realizar manutenção e reparos em ativos de TI (Computadores). Realizar suporte remoto nos polos por team viewer. Atuar em ações voltadas à captação e retenção dos alunos, a partir de orientações prévias. Apoiar eventos e outras atividades que tem como objetivo a promoção da marca e dos cursos da instituição.
+Empresa .....:  OBRAS SOCIAIS E EDUCACIONAIS DE LUZ</t>
+        </is>
+      </c>
+      <c r="H661" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 02/02/26 || Técnico de Informatica JR II - Guarulhos || Realizar atendimento para solucionar problemas de baixa a media complexidade. Conceder acesso as telas do sistema Metodo. Instalar e configurar programas no ambiente Windows, pacote office e outros executados nesse ambiente. Realizar a movimentação de computadores, impressoras e demais ativos de TI.  Criar usuários e alterar senhas na rede. Criar conta de e-mail e alterar senha de acesso. Criar usuário e alterar senha no portal. Criar usuários, alteração e bloqueio de acesso ao sistema Metodo.  Realizar suporte remoto aos computadores por VNC. Prestar atendimento aos colaboradores da Unidade. Realizar manutenção e reparos em ativos de TI (Computadores). Realizar suporte remoto nos polos por team viewer. Atuar em ações voltadas à captação e retenção dos alunos, a partir de orientações prévias. Apoiar eventos e outras atividades que tem como objetivo a promoção da marca e dos cursos da instituição. || Empresa .....:  OBRAS SOCIAIS E EDUCACIONAIS DE LUZ</t>
+        </is>
+      </c>
+      <c r="I661" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>03/02/2026</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t>83215</t>
+        </is>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>Analista de Sistemas Sr (Protheus)</t>
+        </is>
+      </c>
+      <c r="D662" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E662" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F662" t="inlineStr">
+        <is>
+          <t>Barueri - SP - 31/01/26</t>
+        </is>
+      </c>
+      <c r="G662" t="inlineStr">
+        <is>
+          <t>• Atender as demandas de suporte e sustentação, visando a continuidade das atividades • Analisar, diagnosticar e resolver erros sistêmicos, chamados recorrentes e demandas de evolução. • Realizar parametrizações, ajustes e configurações nos módulos utilizados pela empresa. • Construir e revisar documentações técnicas e funcionais dos processos. • Realizar testes, validações, homologações e acompanhamento pós-implantação. • Colaborar com times internos (TI, negócios, infraestrutura) e parceiros TOTVS em demandas sistêmicas.  Conhecimentos técnicos necessários: • Experiência com ERP Protheus (TOTVS) em sustentação e suporte. • Conhecimento em Linguagem ADVPL e TL++ (leitura / ajustes básicos). • Parametrização de módulos, ajustar conforme necessidade da empresa). • Utilização de ferramentas TOTVS: • TDS / VS Code • DBAccess / AppServer • Configuração de ambientes e Builds • Conhecimento em bancos de dados SQL Server ou Progress. • Noções de arquit. Protheus.
+Empresa .....:  Grupo MPR</t>
+        </is>
+      </c>
+      <c r="H662" t="inlineStr">
+        <is>
+          <t>Barueri - SP - 31/01/26 || Analista de Sistemas Sr (Protheus) || • Atender as demandas de suporte e sustentação, visando a continuidade das atividades • Analisar, diagnosticar e resolver erros sistêmicos, chamados recorrentes e demandas de evolução. • Realizar parametrizações, ajustes e configurações nos módulos utilizados pela empresa. • Construir e revisar documentações técnicas e funcionais dos processos. • Realizar testes, validações, homologações e acompanhamento pós-implantação. • Colaborar com times internos (TI, negócios, infraestrutura) e parceiros TOTVS em demandas sistêmicas.  Conhecimentos técnicos necessários: • Experiência com ERP Protheus (TOTVS) em sustentação e suporte. • Conhecimento em Linguagem ADVPL e TL++ (leitura / ajustes básicos). • Parametrização de módulos, ajustar conforme necessidade da empresa). • Utilização de ferramentas TOTVS: • TDS / VS Code • DBAccess / AppServer • Configuração de ambientes e Builds • Conhecimento em bancos de dados SQL Server ou Progress. • Noções de arquit. Protheus. || Empresa .....:  Grupo MPR</t>
+        </is>
+      </c>
+      <c r="I662" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>03/02/2026</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t>83520</t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>DCEO</t>
+        </is>
+      </c>
+      <c r="D663" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E663" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F663" t="inlineStr">
+        <is>
+          <t>Barueri - SP - 31/01/26</t>
+        </is>
+      </c>
+      <c r="G663" t="inlineStr">
+        <is>
+          <t>Estamos com uma oportunidade para atuar como Operador de Datacenter - Eletricidade em um de nossos clientes, do setor Telecomunicações, localizada na região São Paulo/SP com mais de 07 unidades espalhadas por todo o país.  Descrição das atividades:  Gerenciar e supervisionar as operações e a manutenção diária de equipamentos mecânicos e elétricos em um datacenter.  Identificar riscos e realizar avaliação da qualidade de operação e manutenção de fornecedores de IDC.  Atuar como profissional técnico para todas as questões relacionadas às instalações dentro do datacenter, escalando para a equipe técnica da sede (HQ) conforme necessário.  Realizar Análise de Causa Raiz (RCA) de falhas críticas de equipamentos.  Solucionar problemas e reportar eventos de nível de instalação e servidor dentro dos SLAs internos.  Criar e implementar novas práticas padrão para técnicos e equipes de suporte de fornecedores de IDC.
+Empresa .....:  Randstad</t>
+        </is>
+      </c>
+      <c r="H663" t="inlineStr">
+        <is>
+          <t>Barueri - SP - 31/01/26 || DCEO || Estamos com uma oportunidade para atuar como Operador de Datacenter - Eletricidade em um de nossos clientes, do setor Telecomunicações, localizada na região São Paulo/SP com mais de 07 unidades espalhadas por todo o país.  Descrição das atividades:  Gerenciar e supervisionar as operações e a manutenção diária de equipamentos mecânicos e elétricos em um datacenter.  Identificar riscos e realizar avaliação da qualidade de operação e manutenção de fornecedores de IDC.  Atuar como profissional técnico para todas as questões relacionadas às instalações dentro do datacenter, escalando para a equipe técnica da sede (HQ) conforme necessário.  Realizar Análise de Causa Raiz (RCA) de falhas críticas de equipamentos.  Solucionar problemas e reportar eventos de nível de instalação e servidor dentro dos SLAs internos.  Criar e implementar novas práticas padrão para técnicos e equipes de suporte de fornecedores de IDC. || Empresa .....:  Randstad</t>
+        </is>
+      </c>
+      <c r="I663" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>03/02/2026</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>82641</t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>Desenvolvedor Mainframe Sr. (Híbrido - São Paulo)</t>
+        </is>
+      </c>
+      <c r="D664" t="inlineStr">
+        <is>
+          <t>Sênior</t>
+        </is>
+      </c>
+      <c r="E664" t="inlineStr">
+        <is>
+          <t>Híbrido</t>
+        </is>
+      </c>
+      <c r="F664" t="inlineStr">
+        <is>
+          <t>Barueri - SP - 31/01/26</t>
+        </is>
+      </c>
+      <c r="G664" t="inlineStr">
+        <is>
+          <t>Resumo das atividades: Executar levantamento e documentação de programas, subprogramas e base de dados (VSAMS e tabelas DB2) Entender o ambiente de testes mainframe do cliente Analisar e entender o teste do analista de sistemas do cliente Analisar transações, jobs e programas COBOL e, a partir deste contexto Levantar requisitos e mapear/documentar processos Levantamento de árvore de impacto  Conhecimentos obrigatórios:  Linguagem COBOL e JCL Desenvolvimento de CICS (Programação CICS em Command Level: CEDF/CEDX, CEMT/CECI, acesso arquivos VSAMs, CICS c/ DB2, análise de programas CICS...) ISPF/ TSO (SDSF, Skells, Criação de arquivos e Análise de Dumps) DB2 (Table Space, Database, Comandos SQL/Querys, Catálogo DB2, Comandos DB2 e Utilitários DB2) ChangeMan e Control-M para Mainframe VSAM, z/OS e Utilitários IBM XPEDITER – Monitor de testes. Ambiente de desenvolvimento e testes de Bancos e Seguradoras.
+Empresa .....:  Eccox Software S.A</t>
+        </is>
+      </c>
+      <c r="H664" t="inlineStr">
+        <is>
+          <t>Barueri - SP - 31/01/26 || Desenvolvedor Mainframe Sr. (Híbrido - São Paulo) || Resumo das atividades: Executar levantamento e documentação de programas, subprogramas e base de dados (VSAMS e tabelas DB2) Entender o ambiente de testes mainframe do cliente Analisar e entender o teste do analista de sistemas do cliente Analisar transações, jobs e programas COBOL e, a partir deste contexto Levantar requisitos e mapear/documentar processos Levantamento de árvore de impacto  Conhecimentos obrigatórios:  Linguagem COBOL e JCL Desenvolvimento de CICS (Programação CICS em Command Level: CEDF/CEDX, CEMT/CECI, acesso arquivos VSAMs, CICS c/ DB2, análise de programas CICS...) ISPF/ TSO (SDSF, Skells, Criação de arquivos e Análise de Dumps) DB2 (Table Space, Database, Comandos SQL/Querys, Catálogo DB2, Comandos DB2 e Utilitários DB2) ChangeMan e Control-M para Mainframe VSAM, z/OS e Utilitários IBM XPEDITER – Monitor de testes. Ambiente de desenvolvimento e testes de Bancos e Seguradoras. || Empresa .....:  Eccox Software S.A</t>
+        </is>
+      </c>
+      <c r="I664" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>03/02/2026</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t>83072</t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>Tester</t>
+        </is>
+      </c>
+      <c r="D665" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E665" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F665" t="inlineStr">
+        <is>
+          <t>Campinas - SP - 31/01/26</t>
+        </is>
+      </c>
+      <c r="G665" t="inlineStr">
+        <is>
+          <t>Principais Responsabilidades: •	Elaborar Planejamento para execução de testes •	Preparar dados e Ambiente para testes •	Descrever, documentar e manter os casos de teste •	Executar, validar e registrar os resultados dos casos de teste  Perfil da função: •	Comunicação •	Habilidade Analítica •	Gestão do Tempo •	Aprendizado •	Foco no Usuário  Formação/ Pré-requisitos: •	Cursando ou Superior completo em Sistemas de Informação, Engenharia de Software, Ciência da Computação ou área afins •	Desejável: Certificações: QAI ou ISTQB
+Empresa .....:  Ti9  Sistemas de Informação Ltda</t>
+        </is>
+      </c>
+      <c r="H665" t="inlineStr">
+        <is>
+          <t>Campinas - SP - 31/01/26 || Tester || Principais Responsabilidades: •	Elaborar Planejamento para execução de testes •	Preparar dados e Ambiente para testes •	Descrever, documentar e manter os casos de teste •	Executar, validar e registrar os resultados dos casos de teste  Perfil da função: •	Comunicação •	Habilidade Analítica •	Gestão do Tempo •	Aprendizado •	Foco no Usuário  Formação/ Pré-requisitos: •	Cursando ou Superior completo em Sistemas de Informação, Engenharia de Software, Ciência da Computação ou área afins •	Desejável: Certificações: QAI ou ISTQB || Empresa .....:  Ti9  Sistemas de Informação Ltda</t>
+        </is>
+      </c>
+      <c r="I665" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>03/02/2026</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>82238</t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>Analista de Requisitos Sênior</t>
+        </is>
+      </c>
+      <c r="D666" t="inlineStr">
+        <is>
+          <t>Sênior</t>
+        </is>
+      </c>
+      <c r="E666" t="inlineStr">
+        <is>
+          <t>Híbrido</t>
+        </is>
+      </c>
+      <c r="F666" t="inlineStr">
+        <is>
+          <t>Curitiba - PR - 31/01/26</t>
+        </is>
+      </c>
+      <c r="G666" t="inlineStr">
+        <is>
+          <t>A FábricaDS está buscando profissional no seguinte perfil:  Experiência como Analista de Requisitos/ Funcional, realizando a interface entre as áreas de negócios e a área de desenvolvimento ( atuando em Mapear, descrever e documentar os requisitos funcionais e não funcionais dos projetos). O projeto é para uma grande empresa. Local: Curitiba -  Híbrido ( 03 x por semana presencial)..  Os interessados favor encaminhar currículo atualizado e pretensão salarial por hora
+Empresa .....:  FábricaDS Soluções em Tecnologia</t>
+        </is>
+      </c>
+      <c r="H666" t="inlineStr">
+        <is>
+          <t>Curitiba - PR - 31/01/26 || Analista de Requisitos Sênior || A FábricaDS está buscando profissional no seguinte perfil:  Experiência como Analista de Requisitos/ Funcional, realizando a interface entre as áreas de negócios e a área de desenvolvimento ( atuando em Mapear, descrever e documentar os requisitos funcionais e não funcionais dos projetos). O projeto é para uma grande empresa. Local: Curitiba -  Híbrido ( 03 x por semana presencial)..  Os interessados favor encaminhar currículo atualizado e pretensão salarial por hora || Empresa .....:  FábricaDS Soluções em Tecnologia</t>
+        </is>
+      </c>
+      <c r="I666" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>03/02/2026</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t>83522</t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>Desenvolvedor .NET Sênior</t>
+        </is>
+      </c>
+      <c r="D667" t="inlineStr">
+        <is>
+          <t>Sênior</t>
+        </is>
+      </c>
+      <c r="E667" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F667" t="inlineStr">
+        <is>
+          <t>Curitiba - PR - 31/01/26</t>
+        </is>
+      </c>
+      <c r="G667" t="inlineStr">
+        <is>
+          <t>Requisitos essenciais - Superior completo ou cursando em TI, Engenharia de Software ou áreas correlatas - 5+ anos de experiência com desenvolvimento (mínimo 1 ano como sênior) - Domínio em .NET (C# – Core e Framework) - Criação de bibliotecas internas, SDKs ou frameworks - Desenvolvimento de APIs RESTful - Bancos: SQL Server e PostgreSQL - Mensageria (RabbitMQ, Kafka ou similares) - CI/CD, Git, Azure DevOps (ou similares) - Segurança no desenvolvimento - Docker - Boas práticas: SOLID, Clean Code, DDD, Design Patterns  Diferenciais - Contribuições em open source (especialmente em .NET) - Experiência com engenharia de plataforma ou developer experience - Ferramentas como: SonarQube, StyleCop, FxCop, Roslyn Analyzers - Arquitetura orientada a eventos - DevOps e automação de infraestrutura - Participação na definição de padrões técnicos corporativos - Templates de projeto, linters, automações de dev - MongoDB,
+Empresa .....:  Code Group</t>
+        </is>
+      </c>
+      <c r="H667" t="inlineStr">
+        <is>
+          <t>Curitiba - PR - 31/01/26 || Desenvolvedor .NET Sênior || Requisitos essenciais - Superior completo ou cursando em TI, Engenharia de Software ou áreas correlatas - 5+ anos de experiência com desenvolvimento (mínimo 1 ano como sênior) - Domínio em .NET (C# – Core e Framework) - Criação de bibliotecas internas, SDKs ou frameworks - Desenvolvimento de APIs RESTful - Bancos: SQL Server e PostgreSQL - Mensageria (RabbitMQ, Kafka ou similares) - CI/CD, Git, Azure DevOps (ou similares) - Segurança no desenvolvimento - Docker - Boas práticas: SOLID, Clean Code, DDD, Design Patterns  Diferenciais - Contribuições em open source (especialmente em .NET) - Experiência com engenharia de plataforma ou developer experience - Ferramentas como: SonarQube, StyleCop, FxCop, Roslyn Analyzers - Arquitetura orientada a eventos - DevOps e automação de infraestrutura - Participação na definição de padrões técnicos corporativos - Templates de projeto, linters, automações de dev - MongoDB, || Empresa .....:  Code Group</t>
+        </is>
+      </c>
+      <c r="I667" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>03/02/2026</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t>82526</t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>Analista Funcional EBS</t>
+        </is>
+      </c>
+      <c r="D668" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E668" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F668" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 31/01/26</t>
+        </is>
+      </c>
+      <c r="G668" t="inlineStr">
+        <is>
+          <t>Ser referência funcional de produtos digitais voltados a meios de pagamento. Levantamento e análise de requisitos funcionais - área de produto / negócio. Atuação em módulos Oracle EBS (principalmente AR (Contas a Receber), AP (Contas a Pagar), OM (Vendas) - processo OTC. Experiência comprovada como Analista Funcional em projetos com Oracle EBS. Conhecimento funcional nos módulos financeiros e de faturamento (AR, AP, OM). Vivência com meios de pagamento: gateways, adquirentes, APIs de pagamento, conciliação. Capacidade de traduzir requisitos de negócio em especificações funcionais claras. Habilidade de comunicação com áreas técnicas e não técnicas. Boa visão analítica sobre produtos.  Superior Completo. Vaga Home Office.
+Empresa .....:  Emphasys IT Services</t>
+        </is>
+      </c>
+      <c r="H668" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 31/01/26 || Analista Funcional EBS || Ser referência funcional de produtos digitais voltados a meios de pagamento. Levantamento e análise de requisitos funcionais - área de produto / negócio. Atuação em módulos Oracle EBS (principalmente AR (Contas a Receber), AP (Contas a Pagar), OM (Vendas) - processo OTC. Experiência comprovada como Analista Funcional em projetos com Oracle EBS. Conhecimento funcional nos módulos financeiros e de faturamento (AR, AP, OM). Vivência com meios de pagamento: gateways, adquirentes, APIs de pagamento, conciliação. Capacidade de traduzir requisitos de negócio em especificações funcionais claras. Habilidade de comunicação com áreas técnicas e não técnicas. Boa visão analítica sobre produtos.  Superior Completo. Vaga Home Office. || Empresa .....:  Emphasys IT Services</t>
+        </is>
+      </c>
+      <c r="I668" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>03/02/2026</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t>82374</t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>CONSULTOR PROTHEUS - TOTVS</t>
+        </is>
+      </c>
+      <c r="D669" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E669" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F669" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 31/01/26</t>
+        </is>
+      </c>
+      <c r="G669" t="inlineStr">
+        <is>
+          <t>Configurador de Tributos com sólida experiência em TOTVS Protheus para atuar de forma remota (PJ) em projetos desafiadores e com excelente remuneração.  Responsabilidades - Configurar e parametrizar regras fiscais no Protheus (TOTVS) - Realizar ajustes em rotinas de ICMS, IPI, PIS, COFINS, ISS e demais tributos - Apoiar as áreas contábil e fiscal na análise e correção de inconsistências - Implementar melhorias e garantir conformidade com a legislação tributária - Acompanhar atualizações e evoluções do sistema.  Requisitos - Experiência comprovada como Configurador de Tributos ou Analista Fiscal Protheus - Domínio dos módulos SIGAFIS, SIGACFG, SIGAFAT, SIGACTB - Conhecimento em TSS, SPED Fiscal, SPED Contribuições e Bloco K - Entendimento atualizado da legislação fiscal brasileira - Perfil analítico, detalhista e com boa comunicação.  Condições - Contratação PJ - Totalmente Remoto - Excelente remuneração, compatível com o nível de experiência
+Empresa .....:  DMS</t>
+        </is>
+      </c>
+      <c r="H669" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 31/01/26 || CONSULTOR PROTHEUS - TOTVS || Configurador de Tributos com sólida experiência em TOTVS Protheus para atuar de forma remota (PJ) em projetos desafiadores e com excelente remuneração.  Responsabilidades - Configurar e parametrizar regras fiscais no Protheus (TOTVS) - Realizar ajustes em rotinas de ICMS, IPI, PIS, COFINS, ISS e demais tributos - Apoiar as áreas contábil e fiscal na análise e correção de inconsistências - Implementar melhorias e garantir conformidade com a legislação tributária - Acompanhar atualizações e evoluções do sistema.  Requisitos - Experiência comprovada como Configurador de Tributos ou Analista Fiscal Protheus - Domínio dos módulos SIGAFIS, SIGACFG, SIGAFAT, SIGACTB - Conhecimento em TSS, SPED Fiscal, SPED Contribuições e Bloco K - Entendimento atualizado da legislação fiscal brasileira - Perfil analítico, detalhista e com boa comunicação.  Condições - Contratação PJ - Totalmente Remoto - Excelente remuneração, compatível com o nível de experiência || Empresa .....:  DMS</t>
+        </is>
+      </c>
+      <c r="I669" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>03/02/2026</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t>83517</t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>Consultor RM Totvs Backoffice</t>
+        </is>
+      </c>
+      <c r="D670" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E670" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F670" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 31/01/26</t>
+        </is>
+      </c>
+      <c r="G670" t="inlineStr">
+        <is>
+          <t>Buscamos um(a) Consultor(a) RM TOTVS Backoffice para atuar na implantação, parametrização e sustentação dos módulos administrativos e financeiros do TOTVS RM.  Conhecimentos Técnicos: - Domínio dos módulos do TOTVS RM (Folha, Financeiro, Contábil, Patrimônio e Compras). - Conhecimento em integração entre módulos e rotinas operacionais do RM. - Experiência na criação e customização de relatórios RM. - Noções de processos contábeis, financeiros e administrativos. - Conhecimento em boas práticas de implantação e sustentação de sistemas ERP.  Competências Comportamentais: - Perfil analítico e organizado. - Boa comunicação e facilidade para lidar com usuários e clientes. - Capacidade de diagnóstico e resolução de problemas. - Comprometimento com prazos e qualidade das entregas.  Diferenciais: Certificações TOTVS RM. - Experiência em projetos de migração ou upgrade de versão. - Conhecimento em SQL ou banco de dados aplicado ao RM. - Atuação em consultorias/ projetos
+Empresa .....:  Onebrain</t>
+        </is>
+      </c>
+      <c r="H670" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 31/01/26 || Consultor RM Totvs Backoffice || Buscamos um(a) Consultor(a) RM TOTVS Backoffice para atuar na implantação, parametrização e sustentação dos módulos administrativos e financeiros do TOTVS RM.  Conhecimentos Técnicos: - Domínio dos módulos do TOTVS RM (Folha, Financeiro, Contábil, Patrimônio e Compras). - Conhecimento em integração entre módulos e rotinas operacionais do RM. - Experiência na criação e customização de relatórios RM. - Noções de processos contábeis, financeiros e administrativos. - Conhecimento em boas práticas de implantação e sustentação de sistemas ERP.  Competências Comportamentais: - Perfil analítico e organizado. - Boa comunicação e facilidade para lidar com usuários e clientes. - Capacidade de diagnóstico e resolução de problemas. - Comprometimento com prazos e qualidade das entregas.  Diferenciais: Certificações TOTVS RM. - Experiência em projetos de migração ou upgrade de versão. - Conhecimento em SQL ou banco de dados aplicado ao RM. - Atuação em consultorias/ projetos || Empresa .....:  Onebrain</t>
+        </is>
+      </c>
+      <c r="I670" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>03/02/2026</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t>82658</t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>Coordenadora  Segurança AWS</t>
+        </is>
+      </c>
+      <c r="D671" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E671" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F671" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 31/01/26</t>
+        </is>
+      </c>
+      <c r="G671" t="inlineStr">
+        <is>
+          <t>Vaga Afirmativa para Mulheres – Coordenadora de Segurança em Cloud AWS  A Venice Tech busca profissional para atuar como Coordenadora de Segurança em AWS, responsável por arquitetura de segurança, IAM, monitoramento e resposta a incidentes, automação, proteção de dados, gestão de riscos e liderança do time. Necessário experiência sólida em Segurança da Informação com foco em AWS, vivência em liderança, conhecimento em CIS, NIST, ISO 27001, LGPD/GDPR e domínio de serviços como IAM, KMS, GuardDuty, Security Hub e CloudTrail. Diferenciais: AWS Security Specialty, outras certificações (CISSP, CISM, Architect), inglês técnico e experiência com compliance e ambientes híbridos.  Modelo PJ, home office, horário comercial e notebook fornecido.
+Empresa .....:  Venice Tech</t>
+        </is>
+      </c>
+      <c r="H671" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 31/01/26 || Coordenadora  Segurança AWS || Vaga Afirmativa para Mulheres – Coordenadora de Segurança em Cloud AWS  A Venice Tech busca profissional para atuar como Coordenadora de Segurança em AWS, responsável por arquitetura de segurança, IAM, monitoramento e resposta a incidentes, automação, proteção de dados, gestão de riscos e liderança do time. Necessário experiência sólida em Segurança da Informação com foco em AWS, vivência em liderança, conhecimento em CIS, NIST, ISO 27001, LGPD/GDPR e domínio de serviços como IAM, KMS, GuardDuty, Security Hub e CloudTrail. Diferenciais: AWS Security Specialty, outras certificações (CISSP, CISM, Architect), inglês técnico e experiência com compliance e ambientes híbridos.  Modelo PJ, home office, horário comercial e notebook fornecido. || Empresa .....:  Venice Tech</t>
+        </is>
+      </c>
+      <c r="I671" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>03/02/2026</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t>83523</t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>Desenvolvedor FullStack - React Node</t>
+        </is>
+      </c>
+      <c r="D672" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E672" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F672" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 31/01/26</t>
+        </is>
+      </c>
+      <c r="G672" t="inlineStr">
+        <is>
+          <t>A Tech For TI está com oportunidade para Desenvolvedor (a) de Software FullStack Sênior atuar em projeto de cliente AutoTech.  Uma plataforma de inteligência automotiva que utiliza IA e Machine Learning para transformar a forma como o mercado compra e vende veículos. Processamos uma grande massa de dados para gerar insights estratégicos que ajudam concessionárias e revendedores a tomar decisões mais inteligentes.  O Desafio: Você vai atuar em um produto já existente em Go e React, com foco em: - Escalar a aplicação para suportar o crescimento acelerado - Evoluir features que utilizam IA/ML para geração de insights - Trabalhar com grande volume de dados do mercado automotivo  Requisitos imprescindíveis: - Experiência comprovada com GoLang no desenvolvimento backend - Sólida experiência com React em projetos de produção - Domínio de MySQL em aplicações de alta escala. - Experiência com ferramentas de IA para desenvolvimento (Copilot, Claude, etc.)
+Empresa .....:  Tech For TI</t>
+        </is>
+      </c>
+      <c r="H672" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 31/01/26 || Desenvolvedor FullStack - React Node || A Tech For TI está com oportunidade para Desenvolvedor (a) de Software FullStack Sênior atuar em projeto de cliente AutoTech.  Uma plataforma de inteligência automotiva que utiliza IA e Machine Learning para transformar a forma como o mercado compra e vende veículos. Processamos uma grande massa de dados para gerar insights estratégicos que ajudam concessionárias e revendedores a tomar decisões mais inteligentes.  O Desafio: Você vai atuar em um produto já existente em Go e React, com foco em: - Escalar a aplicação para suportar o crescimento acelerado - Evoluir features que utilizam IA/ML para geração de insights - Trabalhar com grande volume de dados do mercado automotivo  Requisitos imprescindíveis: - Experiência comprovada com GoLang no desenvolvimento backend - Sólida experiência com React em projetos de produção - Domínio de MySQL em aplicações de alta escala. - Experiência com ferramentas de IA para desenvolvimento (Copilot, Claude, etc.) || Empresa .....:  Tech For TI</t>
+        </is>
+      </c>
+      <c r="I672" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>03/02/2026</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t>83136</t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>Desenvolvedor Fullstack - Remoto</t>
+        </is>
+      </c>
+      <c r="D673" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E673" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F673" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 31/01/26</t>
+        </is>
+      </c>
+      <c r="G673" t="inlineStr">
+        <is>
+          <t>O Desafio: Atuar em modelo de alocação em um projeto para um cliente do setor financeiro, contribuindo na migração de sistemas legados para soluções modernas.Também dará suporte na definição de soluções técnicas, garantindo alinhamento com os padrões arquiteturais e com os requisitos do negócio.  O Que Esperamos de Você:     Backend: - Java – JEE - Servidor de aplicação JBoss EAP 7.+ - Spring Boot - SGBD Oracle 11g ou superior - JPA/Hibernate, JDBC - CDI, EJB - JUnit 4 ou superior - Mensageria, Web Services, REST API - Maven - Jenkins / Sonar - Métodos ágeis (Scrum e Kanban) - Containers (Docker, Kubernetes/OpenShift) - Segurança: OAuth2, OpenID Connect - Git para controle de versão  Frontend: - Java – JEE - Frameworks de interface: AngularJS, Angular 2+, React - JavaScript e TypeScript - Maven - Jenkins / Sonar  Informar pretensão salarial no currículo.
+Empresa .....:  Pitang</t>
+        </is>
+      </c>
+      <c r="H673" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 31/01/26 || Desenvolvedor Fullstack - Remoto || O Desafio: Atuar em modelo de alocação em um projeto para um cliente do setor financeiro, contribuindo na migração de sistemas legados para soluções modernas.Também dará suporte na definição de soluções técnicas, garantindo alinhamento com os padrões arquiteturais e com os requisitos do negócio.  O Que Esperamos de Você:     Backend: - Java – JEE - Servidor de aplicação JBoss EAP 7.+ - Spring Boot - SGBD Oracle 11g ou superior - JPA/Hibernate, JDBC - CDI, EJB - JUnit 4 ou superior - Mensageria, Web Services, REST API - Maven - Jenkins / Sonar - Métodos ágeis (Scrum e Kanban) - Containers (Docker, Kubernetes/OpenShift) - Segurança: OAuth2, OpenID Connect - Git para controle de versão  Frontend: - Java – JEE - Frameworks de interface: AngularJS, Angular 2+, React - JavaScript e TypeScript - Maven - Jenkins / Sonar  Informar pretensão salarial no currículo. || Empresa .....:  Pitang</t>
+        </is>
+      </c>
+      <c r="I673" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>03/02/2026</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t>83521</t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>Desenvolvedor Fullstack Java</t>
+        </is>
+      </c>
+      <c r="D674" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E674" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F674" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 31/01/26</t>
+        </is>
+      </c>
+      <c r="G674" t="inlineStr">
+        <is>
+          <t>Vem fazer parte da Spassu Estamos em uma busca de Desenvolvedor Fullstack Java com angular para atuar em projeto de transformação digital e financeiro.  Requisitos: Graduação completa na área de Tecnologia da Informação. Experiência comprovada com desenvolvimento de sistemas Experiência em Java SE 8+, Java EE, Spring Framework 3.x+, Microprofile JPA, JDBC, Hibernate, Angular 8+ SQL Design Patterns, MVC, arquitetura em 3 camadas APIs RESTful, SOAP, Swagger/OpenAPI Servidores de aplicação: IBM WebSphere Application Server (WAS), IBM WebSphere Liberty (Liberty Profile), Red Hat JBoss EAP (WildFly), Quarkus (Red Hat) Jenkins, Git, Maven, SonarQube Testes: JUnit, TDD, ATDD Mensageria com MQ Series (IBM WebSphere MQ, JMS).  Atuação Híbrido/Remoto Contratação CLT  Favor enviar pretensão salarial CLT.  Benefícios: Plano de Saúde Plano Odontológico Seguro de Vida Vale Alimentação ou Refeição Vale Transporte WellHub - Gympass Parcerias com empresas educacionais
+Empresa .....:  Spassu</t>
+        </is>
+      </c>
+      <c r="H674" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 31/01/26 || Desenvolvedor Fullstack Java || Vem fazer parte da Spassu Estamos em uma busca de Desenvolvedor Fullstack Java com angular para atuar em projeto de transformação digital e financeiro.  Requisitos: Graduação completa na área de Tecnologia da Informação. Experiência comprovada com desenvolvimento de sistemas Experiência em Java SE 8+, Java EE, Spring Framework 3.x+, Microprofile JPA, JDBC, Hibernate, Angular 8+ SQL Design Patterns, MVC, arquitetura em 3 camadas APIs RESTful, SOAP, Swagger/OpenAPI Servidores de aplicação: IBM WebSphere Application Server (WAS), IBM WebSphere Liberty (Liberty Profile), Red Hat JBoss EAP (WildFly), Quarkus (Red Hat) Jenkins, Git, Maven, SonarQube Testes: JUnit, TDD, ATDD Mensageria com MQ Series (IBM WebSphere MQ, JMS).  Atuação Híbrido/Remoto Contratação CLT  Favor enviar pretensão salarial CLT.  Benefícios: Plano de Saúde Plano Odontológico Seguro de Vida Vale Alimentação ou Refeição Vale Transporte WellHub - Gympass Parcerias com empresas educacionais || Empresa .....:  Spassu</t>
+        </is>
+      </c>
+      <c r="I674" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>03/02/2026</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>83099</t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>Desenvolvedor Python (IA / LLM)</t>
+        </is>
+      </c>
+      <c r="D675" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E675" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F675" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 31/01/26</t>
+        </is>
+      </c>
+      <c r="G675" t="inlineStr">
+        <is>
+          <t>Estamos ampliando nosso time de tecnologia para atuar em projetos estratégicos de Inteligência Artificial. Buscamos um(a) Desenvolvedor(a) Python com foco em IA/LLM para trabalhar com aplicações reais, integrações complexas e soluções de alto impacto.  O que você vai fazer: - Desenvolver e manter aplicações em Python - Integrar e ajustar modelos LLM (RAG, fine-tuning, embeddings) - Estruturar e otimizar prompts e bases de conhecimento - Integrar soluções de IA com sistemas legados e APIs corporativas - Atuar próximo ao time de negócio e tecnologia do cliente  O que esperamos de você: - Python em nível Pleno - Experiência com LangChain, LlamaIndex, CrewAI ou similares - Conhecimento prático em LLMs e arquiteturas RAG - Boa capacidade de comunicação e autonomia técnica - Experiência prévia em ambientes corporativos é um diferencial  O que oferecemos: - Projeto de longo prazo - Atuação em soluções reais de IA (não apenas POCs) - Ambiente técnico desafiador e colaborativo
+Empresa .....:  CADS DIGITAL</t>
+        </is>
+      </c>
+      <c r="H675" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 31/01/26 || Desenvolvedor Python (IA / LLM) || Estamos ampliando nosso time de tecnologia para atuar em projetos estratégicos de Inteligência Artificial. Buscamos um(a) Desenvolvedor(a) Python com foco em IA/LLM para trabalhar com aplicações reais, integrações complexas e soluções de alto impacto.  O que você vai fazer: - Desenvolver e manter aplicações em Python - Integrar e ajustar modelos LLM (RAG, fine-tuning, embeddings) - Estruturar e otimizar prompts e bases de conhecimento - Integrar soluções de IA com sistemas legados e APIs corporativas - Atuar próximo ao time de negócio e tecnologia do cliente  O que esperamos de você: - Python em nível Pleno - Experiência com LangChain, LlamaIndex, CrewAI ou similares - Conhecimento prático em LLMs e arquiteturas RAG - Boa capacidade de comunicação e autonomia técnica - Experiência prévia em ambientes corporativos é um diferencial  O que oferecemos: - Projeto de longo prazo - Atuação em soluções reais de IA (não apenas POCs) - Ambiente técnico desafiador e colaborativo || Empresa .....:  CADS DIGITAL</t>
+        </is>
+      </c>
+      <c r="I675" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>03/02/2026</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t>83529</t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>Desenvolvedor(a) Full Stack  Sr</t>
+        </is>
+      </c>
+      <c r="D676" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E676" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F676" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 31/01/26</t>
+        </is>
+      </c>
+      <c r="G676" t="inlineStr">
+        <is>
+          <t>Sólida experiência em desenvolvimento e manutenção de features em .NET Core e React. Conhecimento avançado em AWS (Lambda, API Gateway, S3, SQS, SNS, Step Functions, CloudFormation). •	Publica no SNS #8594 SQS consome #8594 Lambda executa a lógica •	RabbitMQ e IBM MQ •	SOLID e Design Patterns  Design Patterns, com uso frequente de: •	Strategy •	Command •	Repository •	Injeção de Dependência (DI)  Bancos de Dados: •	PostgreSQL •	DynamoDB •	SQL Server (diferencial em projetos legados)  Azure DevOps: •	Repositórios Git •	Pipelines (CI/CD) •	Boards para acompanhamento de features e entregas  Atividades desenvolvidas: Desenvolvimento e manutenção de features em .NET Core e React. Arquiteturas baseadas em mensageria, principalmente em AWS. Desenvolver soluções usando: SNS, SQS  e Lambda.  Formato de contratação: CLT/ PJ Local de trabalho: Home Office
+Empresa .....:  SEMPRE IT SERVICOS DE TECNOLOGIA LTDA</t>
+        </is>
+      </c>
+      <c r="H676" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 31/01/26 || Desenvolvedor(a) Full Stack  Sr || Sólida experiência em desenvolvimento e manutenção de features em .NET Core e React. Conhecimento avançado em AWS (Lambda, API Gateway, S3, SQS, SNS, Step Functions, CloudFormation). •	Publica no SNS #8594 SQS consome #8594 Lambda executa a lógica •	RabbitMQ e IBM MQ •	SOLID e Design Patterns  Design Patterns, com uso frequente de: •	Strategy •	Command •	Repository •	Injeção de Dependência (DI)  Bancos de Dados: •	PostgreSQL •	DynamoDB •	SQL Server (diferencial em projetos legados)  Azure DevOps: •	Repositórios Git •	Pipelines (CI/CD) •	Boards para acompanhamento de features e entregas  Atividades desenvolvidas: Desenvolvimento e manutenção de features em .NET Core e React. Arquiteturas baseadas em mensageria, principalmente em AWS. Desenvolver soluções usando: SNS, SQS  e Lambda.  Formato de contratação: CLT/ PJ Local de trabalho: Home Office || Empresa .....:  SEMPRE IT SERVICOS DE TECNOLOGIA LTDA</t>
+        </is>
+      </c>
+      <c r="I676" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>03/02/2026</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t>82646</t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>Engenheiro Machine Learning Sr.</t>
+        </is>
+      </c>
+      <c r="D677" t="inlineStr">
+        <is>
+          <t>Sênior</t>
+        </is>
+      </c>
+      <c r="E677" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F677" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 31/01/26</t>
+        </is>
+      </c>
+      <c r="G677" t="inlineStr">
+        <is>
+          <t>Totalmente Remoto - 6 meses com possibilidade de renovação - PJ  O profissional será responsável por projetar, desenvolver e implantar soluções de Machine Learning, e IA Generativa aplicada a diferentes áreas de negócio.  Requisitos Técnicos (Obrigatórios) · Domínio de SQL e ferramentas de processamento de dados (PySpark, Pandas). · Experiência em plataformas de nuvem (Azure, AWS ou GCP) e serviços de IA. · Familiaridade com Databricks ou plataformas equivalentes de dados/ML. · Conhecimento sólido em integração de APIs (REST, GraphQL).  Diferenciais Desejáveis · Experiência com LLMs, LangChain, LangGraph ou orquestração multiagente. · Conhecimento em arquitetura de MLOps e deploy de modelos em produção. · Vivência com ferramentas de observabilidade de IA (ex: MLflow, Weights  Biases). · Inglês técnico para leitura e documentação.
+Empresa .....:  4Solution Group</t>
+        </is>
+      </c>
+      <c r="H677" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 31/01/26 || Engenheiro Machine Learning Sr. || Totalmente Remoto - 6 meses com possibilidade de renovação - PJ  O profissional será responsável por projetar, desenvolver e implantar soluções de Machine Learning, e IA Generativa aplicada a diferentes áreas de negócio.  Requisitos Técnicos (Obrigatórios) · Domínio de SQL e ferramentas de processamento de dados (PySpark, Pandas). · Experiência em plataformas de nuvem (Azure, AWS ou GCP) e serviços de IA. · Familiaridade com Databricks ou plataformas equivalentes de dados/ML. · Conhecimento sólido em integração de APIs (REST, GraphQL).  Diferenciais Desejáveis · Experiência com LLMs, LangChain, LangGraph ou orquestração multiagente. · Conhecimento em arquitetura de MLOps e deploy de modelos em produção. · Vivência com ferramentas de observabilidade de IA (ex: MLflow, Weights  Biases). · Inglês técnico para leitura e documentação. || Empresa .....:  4Solution Group</t>
+        </is>
+      </c>
+      <c r="I677" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>03/02/2026</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>82732</t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>Analista de Produtos Sr.</t>
+        </is>
+      </c>
+      <c r="D678" t="inlineStr">
+        <is>
+          <t>Sênior</t>
+        </is>
+      </c>
+      <c r="E678" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F678" t="inlineStr">
+        <is>
+          <t>Osasco - SP - 31/01/26</t>
+        </is>
+      </c>
+      <c r="G678" t="inlineStr">
+        <is>
+          <t>Esta oportunidade é destinada para pessoas com deficiência (PcD). Se você procura um ambiente onde suas habilidades são reconhecidas e deseja crescer ao lado de uma empresa de grande porte, inscreva-se agora e venha fazer parte do nosso time  A Randstad, líder mundial em soluções de talentos, busca um(a) Analista Sênior e/ou Especialista de Produtos para gerir e liderar iniciativas estratégicas. Os desafios envolvem atuar com equipes de TI e Negócio, gerir o product backlog definindo prioridades, objetivos e roadmaps de curto a longo prazo, e liderar a definição de iniciativas, negociando trade-offs para garantir a melhor experiência do usuário e o benefício global da empresa. O profissional será responsável por acompanhar a performance e o impacto dos projetos, garantindo a visibilidade para os stakeholders, e realizando análises de mercado/concorrência. É essencial ter experiência comprovada em Produto e/ou Gerenciamento de Projetos.
+Empresa .....:  randstad Brasil</t>
+        </is>
+      </c>
+      <c r="H678" t="inlineStr">
+        <is>
+          <t>Osasco - SP - 31/01/26 || Analista de Produtos Sr. || Esta oportunidade é destinada para pessoas com deficiência (PcD). Se você procura um ambiente onde suas habilidades são reconhecidas e deseja crescer ao lado de uma empresa de grande porte, inscreva-se agora e venha fazer parte do nosso time  A Randstad, líder mundial em soluções de talentos, busca um(a) Analista Sênior e/ou Especialista de Produtos para gerir e liderar iniciativas estratégicas. Os desafios envolvem atuar com equipes de TI e Negócio, gerir o product backlog definindo prioridades, objetivos e roadmaps de curto a longo prazo, e liderar a definição de iniciativas, negociando trade-offs para garantir a melhor experiência do usuário e o benefício global da empresa. O profissional será responsável por acompanhar a performance e o impacto dos projetos, garantindo a visibilidade para os stakeholders, e realizando análises de mercado/concorrência. É essencial ter experiência comprovada em Produto e/ou Gerenciamento de Projetos. || Empresa .....:  randstad Brasil</t>
+        </is>
+      </c>
+      <c r="I678" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>03/02/2026</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>82728</t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>Desenvolvedor Java Sr.</t>
+        </is>
+      </c>
+      <c r="D679" t="inlineStr">
+        <is>
+          <t>Sênior</t>
+        </is>
+      </c>
+      <c r="E679" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F679" t="inlineStr">
+        <is>
+          <t>Osasco - SP - 31/01/26</t>
+        </is>
+      </c>
+      <c r="G679" t="inlineStr">
+        <is>
+          <t>Estamos buscando um(a) S.r. Software Engineer Backend (Online Payments).  Esta oportunidade é destinada para pessoas com deficiência (PcD).  Se você procura um ambiente onde suas habilidades são reconhecidas e deseja crescer ao lado de uma empresa de grande porte, inscreva-se agora e venha fazer parte do nosso time), para atuar em um ambiente de grande porte onde suas habilidades serão valorizadas.  Procuramos um profissional experiente, curioso(a) e com iniciativa, com amplo conhecimento em arquitetura, microsserviços, bancos de dados e observabilidade. É essencial ter experiência prática em Java e/ou Golang, familiaridade com AWS e dominar conceitos como SOLID, Design Patterns, Clean ou Hexagonal Architecture.  As responsabilidades incluem desenvolver software escalável e de alto desempenho, oferecer mentoria à equipe, apoiar a evolução tecnológica do projeto e colaborar em demandas Cross. Se você busca crescimento e possui este background técnico avançado, candidate-se.
+Empresa .....:  randstad Brasil</t>
+        </is>
+      </c>
+      <c r="H679" t="inlineStr">
+        <is>
+          <t>Osasco - SP - 31/01/26 || Desenvolvedor Java Sr. || Estamos buscando um(a) S.r. Software Engineer Backend (Online Payments).  Esta oportunidade é destinada para pessoas com deficiência (PcD).  Se você procura um ambiente onde suas habilidades são reconhecidas e deseja crescer ao lado de uma empresa de grande porte, inscreva-se agora e venha fazer parte do nosso time), para atuar em um ambiente de grande porte onde suas habilidades serão valorizadas.  Procuramos um profissional experiente, curioso(a) e com iniciativa, com amplo conhecimento em arquitetura, microsserviços, bancos de dados e observabilidade. É essencial ter experiência prática em Java e/ou Golang, familiaridade com AWS e dominar conceitos como SOLID, Design Patterns, Clean ou Hexagonal Architecture.  As responsabilidades incluem desenvolver software escalável e de alto desempenho, oferecer mentoria à equipe, apoiar a evolução tecnológica do projeto e colaborar em demandas Cross. Se você busca crescimento e possui este background técnico avançado, candidate-se. || Empresa .....:  randstad Brasil</t>
+        </is>
+      </c>
+      <c r="I679" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>03/02/2026</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>82693</t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>Desenvolvedor PHP Pleno</t>
+        </is>
+      </c>
+      <c r="D680" t="inlineStr">
+        <is>
+          <t>Pleno</t>
+        </is>
+      </c>
+      <c r="E680" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F680" t="inlineStr">
+        <is>
+          <t>Presidente Prudente - SP - 31/01/26</t>
+        </is>
+      </c>
+      <c r="G680" t="inlineStr">
+        <is>
+          <t>Desenvolvedor PHP Pleno, atuar na modalidade PJ, presencial em cliente situado no interior SP (Presidente Prudente).  Requisitos imprescindíveis: - Experiência com frameworks PHP (Laravel, CodeIgniter, entre outros). - Experiência com bancos de dados relacionais e NoSQL. - Experiência com ferramentas de versionamento de código como Git. - Experiência com metodologias ágeis de desenvolvimento. - Excelentes conhecimentos em PHP e frameworks relacionados. - Conhecimento em Arquitetura de Software. - Habilidade para escrever código limpo, eficiente e bem documentado. - Habilidade para solucionar problemas complexos de forma criativa. - Excelentes habilidades de comunicação escrita e verbal. - Capacidade de trabalhar de forma independente e como parte de uma equipe. - Entendimento de Processos de Negócio.
+Empresa .....:  Tech For TI</t>
+        </is>
+      </c>
+      <c r="H680" t="inlineStr">
+        <is>
+          <t>Presidente Prudente - SP - 31/01/26 || Desenvolvedor PHP Pleno || Desenvolvedor PHP Pleno, atuar na modalidade PJ, presencial em cliente situado no interior SP (Presidente Prudente).  Requisitos imprescindíveis: - Experiência com frameworks PHP (Laravel, CodeIgniter, entre outros). - Experiência com bancos de dados relacionais e NoSQL. - Experiência com ferramentas de versionamento de código como Git. - Experiência com metodologias ágeis de desenvolvimento. - Excelentes conhecimentos em PHP e frameworks relacionados. - Conhecimento em Arquitetura de Software. - Habilidade para escrever código limpo, eficiente e bem documentado. - Habilidade para solucionar problemas complexos de forma criativa. - Excelentes habilidades de comunicação escrita e verbal. - Capacidade de trabalhar de forma independente e como parte de uma equipe. - Entendimento de Processos de Negócio. || Empresa .....:  Tech For TI</t>
+        </is>
+      </c>
+      <c r="I680" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>03/02/2026</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t>82706</t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>Desenvolvedor Full Stack Jr III - RJ</t>
+        </is>
+      </c>
+      <c r="D681" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E681" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F681" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro - RJ - 31/01/26</t>
+        </is>
+      </c>
+      <c r="G681" t="inlineStr">
+        <is>
+          <t>Atividades - Atuar na manutenção e sustentação dos produtos SIPE e DJE - Diagnosticar, corrigir e evoluir sistemas em produção - Implementar integrações, automações e ajustes pontuais em APIs  Requisitos - Formação superior completa ou em andamento em Análise e Desenvolvimento de Sistemas, Ciência da Computação ou áreas correlatas. - Possuir experiência mínima de 1 ano em desenvolvimento de softwares - .NET / C# - SQL Server - Conhecimento desejável em ASP.NET MVC - Git - Residir na cidade do RJ (imprescindível)  Escala: 2ª à 5ª de 9h às 18h / sexta-feira home office, até às 17h (39h/semanais) Modelo de contratação: CLT  Remuneração: R$ 5.299,00  Benefícios: Vale transporte / Vale refeição / Assistência médica / Assistência odontológica / Convênio com faculdades / TotalPass
+Empresa .....:  Iprazos Tecnologia e Serviços</t>
+        </is>
+      </c>
+      <c r="H681" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro - RJ - 31/01/26 || Desenvolvedor Full Stack Jr III - RJ || Atividades - Atuar na manutenção e sustentação dos produtos SIPE e DJE - Diagnosticar, corrigir e evoluir sistemas em produção - Implementar integrações, automações e ajustes pontuais em APIs  Requisitos - Formação superior completa ou em andamento em Análise e Desenvolvimento de Sistemas, Ciência da Computação ou áreas correlatas. - Possuir experiência mínima de 1 ano em desenvolvimento de softwares - .NET / C# - SQL Server - Conhecimento desejável em ASP.NET MVC - Git - Residir na cidade do RJ (imprescindível)  Escala: 2ª à 5ª de 9h às 18h / sexta-feira home office, até às 17h (39h/semanais) Modelo de contratação: CLT  Remuneração: R$ 5.299,00  Benefícios: Vale transporte / Vale refeição / Assistência médica / Assistência odontológica / Convênio com faculdades / TotalPass || Empresa .....:  Iprazos Tecnologia e Serviços</t>
+        </is>
+      </c>
+      <c r="I681" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>03/02/2026</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t>82599</t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>Gerente de Projetos SAP</t>
+        </is>
+      </c>
+      <c r="D682" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E682" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F682" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro - RJ - 31/01/26</t>
+        </is>
+      </c>
+      <c r="G682" t="inlineStr">
+        <is>
+          <t>Local: Rio de Janeiro – Centro (presencial 3x/semana) Início imediato  Projeto de 6 meses (prorrogável)  Estamos buscando um(a) Gerente de Projetos SAP para liderar projeto de implementação (carve-in), migração e melhoria contínua do SAP S/4 RISE 2021 Foundation na EDF Power Solutions.  Requisitos: - +10 anos de experiência em gestão de projetos de TI - Forte atuação em projetos SAP (S/4HANA, ECC, etc.) - Experiência com PMBOK/PMI e metodologias ágeis - Excelentes habilidades de liderança e gestão de stakeholders  Diferenciais: PMP, CSM, SAP Activate, inglês avançado.
+Empresa .....:  Ultracon</t>
+        </is>
+      </c>
+      <c r="H682" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro - RJ - 31/01/26 || Gerente de Projetos SAP || Local: Rio de Janeiro – Centro (presencial 3x/semana) Início imediato  Projeto de 6 meses (prorrogável)  Estamos buscando um(a) Gerente de Projetos SAP para liderar projeto de implementação (carve-in), migração e melhoria contínua do SAP S/4 RISE 2021 Foundation na EDF Power Solutions.  Requisitos: - +10 anos de experiência em gestão de projetos de TI - Forte atuação em projetos SAP (S/4HANA, ECC, etc.) - Experiência com PMBOK/PMI e metodologias ágeis - Excelentes habilidades de liderança e gestão de stakeholders  Diferenciais: PMP, CSM, SAP Activate, inglês avançado. || Empresa .....:  Ultracon</t>
+        </is>
+      </c>
+      <c r="I682" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>03/02/2026</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>83082</t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>Analista de Suporte  Junior</t>
+        </is>
+      </c>
+      <c r="D683" t="inlineStr">
+        <is>
+          <t>Júnior</t>
+        </is>
+      </c>
+      <c r="E683" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F683" t="inlineStr">
+        <is>
+          <t>Santana de Parnaíba - SP - 31/01/26</t>
+        </is>
+      </c>
+      <c r="G683" t="inlineStr">
+        <is>
+          <t>Estamos buscando um profissional com experiência em suporte técnico voltado para voz e dados, incluindo configuração, implantação e manutenção de sistemas de telefonia e redes IP. Executara manutenção preventiva e corretiva em equipamentos e hardware do sistema de telefonia Alcatel-Lucent.  É essencial ter boa comunicação, habilidade para solucionar problemas e facilidade no relacionamento com clientes e equipe.   Diferenciais:  Certificações em Alcatel, Huawei, CCNA, Voice ou similares  Inglês desejável  CNH B será um diferencial  Vivencia com sistemas de telefonia: PABX, ASTERISK, e Voip   Perfil Ideal:  Comunicação clara  Raciocínio rápido  Organização e precisão  Abertura para aprender sempre  Local de Trabalho: Santana de Parnaiba   Horário: Escala: 12x36 - Diurno 07:00 as 19hs  Salário: R$ 2.800,00 (CLT)   Benefícios:  Refeição na Empresa  TotalPass  Assistência médica Bradesco +odontológica  VT Pago em Dinheiro  Seguro de Vida
+Empresa .....:  3CORPTECHNOLOGY</t>
+        </is>
+      </c>
+      <c r="H683" t="inlineStr">
+        <is>
+          <t>Santana de Parnaíba - SP - 31/01/26 || Analista de Suporte  Junior || Estamos buscando um profissional com experiência em suporte técnico voltado para voz e dados, incluindo configuração, implantação e manutenção de sistemas de telefonia e redes IP. Executara manutenção preventiva e corretiva em equipamentos e hardware do sistema de telefonia Alcatel-Lucent.  É essencial ter boa comunicação, habilidade para solucionar problemas e facilidade no relacionamento com clientes e equipe.   Diferenciais:  Certificações em Alcatel, Huawei, CCNA, Voice ou similares  Inglês desejável  CNH B será um diferencial  Vivencia com sistemas de telefonia: PABX, ASTERISK, e Voip   Perfil Ideal:  Comunicação clara  Raciocínio rápido  Organização e precisão  Abertura para aprender sempre  Local de Trabalho: Santana de Parnaiba   Horário: Escala: 12x36 - Diurno 07:00 as 19hs  Salário: R$ 2.800,00 (CLT)   Benefícios:  Refeição na Empresa  TotalPass  Assistência médica Bradesco +odontológica  VT Pago em Dinheiro  Seguro de Vida || Empresa .....:  3CORPTECHNOLOGY</t>
+        </is>
+      </c>
+      <c r="I683" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>03/02/2026</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t>82480</t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>Programador / Desenvolvedor</t>
+        </is>
+      </c>
+      <c r="D684" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E684" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F684" t="inlineStr">
+        <is>
+          <t>São Bernardo do Campo - SP - 31/01/26</t>
+        </is>
+      </c>
+      <c r="G684" t="inlineStr">
+        <is>
+          <t>Requisitos: Conhecimento em Vue 2 e/ou 3 Domínio de HTML, CSS e JavaScript Domínio em NodeJS express, axios, mssql Conhecimentos em MSSQL Conhecimento básico em versionamento com Git Habilidade em integração / criação de APIs RESTful  Horário de trabalho: seg - sex, 07:00 - 16:48, presencial  Beneficios : Vale Transporte , Restaurante café da manhã e almoço, Convênio Médico Notredame ( opcional) a empresa paga 50  + Convênio Dental Amil a empresa paga 50  opcional + Cartão Alimentação Alelo ( R$ 257,00) + Convênio Farmacia.
+Empresa .....:  RM Empresarial</t>
+        </is>
+      </c>
+      <c r="H684" t="inlineStr">
+        <is>
+          <t>São Bernardo do Campo - SP - 31/01/26 || Programador / Desenvolvedor || Requisitos: Conhecimento em Vue 2 e/ou 3 Domínio de HTML, CSS e JavaScript Domínio em NodeJS express, axios, mssql Conhecimentos em MSSQL Conhecimento básico em versionamento com Git Habilidade em integração / criação de APIs RESTful  Horário de trabalho: seg - sex, 07:00 - 16:48, presencial  Beneficios : Vale Transporte , Restaurante café da manhã e almoço, Convênio Médico Notredame ( opcional) a empresa paga 50  + Convênio Dental Amil a empresa paga 50  opcional + Cartão Alimentação Alelo ( R$ 257,00) + Convênio Farmacia. || Empresa .....:  RM Empresarial</t>
+        </is>
+      </c>
+      <c r="I684" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>03/02/2026</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t>82429</t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>Analista de Migração de Dados</t>
+        </is>
+      </c>
+      <c r="D685" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E685" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F685" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 31/01/26</t>
+        </is>
+      </c>
+      <c r="G685" t="inlineStr">
+        <is>
+          <t>Migração de Dados (SAS para PySpark)  Área: Dados e Analytics / Engenharia de Dados Modalidade: PJ Modelo: Remoto  Projeto estratégico de modernização de uma plataforma de dados, efetuando a migração de processos e códigos legados em SAS para uma arquitetura moderna baseada em PySpark e Microsoft Fabric.  Profundo conhecimento em SAS, sendo capaz de interpretar, otimizar e traduzir lógicas complexas, e ao mesmo tempo, dominar o ecossistema PySpark para desenvolver soluções de dados escaláveis e eficientes.  Requisitos: -Exp. em SAS: linguagem SAS, incluindo SAS Base, SAS Macro e PROC SQL -Exp.prática na análise e manutenção de códigos SAS complexos e de grande volume. -Proficiência em PySpark:desenvolvimento de soluções de processamento de dados com PySpark, incluindo otimização de performance (tuning de jobs Spark) -Ecossistemas de Big Data-conceitos de computação distribuída e arquiteturas de dados modernas
+Empresa .....:  Tech For TI</t>
+        </is>
+      </c>
+      <c r="H685" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 31/01/26 || Analista de Migração de Dados || Migração de Dados (SAS para PySpark)  Área: Dados e Analytics / Engenharia de Dados Modalidade: PJ Modelo: Remoto  Projeto estratégico de modernização de uma plataforma de dados, efetuando a migração de processos e códigos legados em SAS para uma arquitetura moderna baseada em PySpark e Microsoft Fabric.  Profundo conhecimento em SAS, sendo capaz de interpretar, otimizar e traduzir lógicas complexas, e ao mesmo tempo, dominar o ecossistema PySpark para desenvolver soluções de dados escaláveis e eficientes.  Requisitos: -Exp. em SAS: linguagem SAS, incluindo SAS Base, SAS Macro e PROC SQL -Exp.prática na análise e manutenção de códigos SAS complexos e de grande volume. -Proficiência em PySpark:desenvolvimento de soluções de processamento de dados com PySpark, incluindo otimização de performance (tuning de jobs Spark) -Ecossistemas de Big Data-conceitos de computação distribuída e arquiteturas de dados modernas || Empresa .....:  Tech For TI</t>
+        </is>
+      </c>
+      <c r="I685" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>03/02/2026</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>83158</t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>ANALISTA DE PROCESSOS PLENO</t>
+        </is>
+      </c>
+      <c r="D686" t="inlineStr">
+        <is>
+          <t>Pleno</t>
+        </is>
+      </c>
+      <c r="E686" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F686" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 31/01/26</t>
+        </is>
+      </c>
+      <c r="G686" t="inlineStr">
+        <is>
+          <t>Transformação digital de serviços, participando diretamente da construção de soluções inovadoras, com impacto real no negócio e na experiência do usuário.  O que você vai fazer no dia a dia Planejamento estratégico: Participar de discussões e planejamento de demandas, conduzir reuniões e realizar visitas técnicas aos clientes. Mapeamento e modelagem de processos: Analisar processos atuais (AS-IS) e desenhar cenários futuros (TO-BE), focando eficiência, inovação e digitalização. Pesquisa e experiência do usuário: Conduzir pesquisas com usuários, elaborar jornadas, blueprints de serviços e pesquisas online. Levantamento de requisitos: Apoiar a definição de requisitos e regras de negócio em conjunto com stakeholders. Documentação e implantação: Criar diagramas em BPMN, estruturar requisitos de formulários e apoiar o time de implantação com parâmetros técnicos. Melhoria contínua: Analisar legislações, normas e regras internas para propor melhorias
+Empresa .....:  BR BPO TECNOLOGIA S/A</t>
+        </is>
+      </c>
+      <c r="H686" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 31/01/26 || ANALISTA DE PROCESSOS PLENO || Transformação digital de serviços, participando diretamente da construção de soluções inovadoras, com impacto real no negócio e na experiência do usuário.  O que você vai fazer no dia a dia Planejamento estratégico: Participar de discussões e planejamento de demandas, conduzir reuniões e realizar visitas técnicas aos clientes. Mapeamento e modelagem de processos: Analisar processos atuais (AS-IS) e desenhar cenários futuros (TO-BE), focando eficiência, inovação e digitalização. Pesquisa e experiência do usuário: Conduzir pesquisas com usuários, elaborar jornadas, blueprints de serviços e pesquisas online. Levantamento de requisitos: Apoiar a definição de requisitos e regras de negócio em conjunto com stakeholders. Documentação e implantação: Criar diagramas em BPMN, estruturar requisitos de formulários e apoiar o time de implantação com parâmetros técnicos. Melhoria contínua: Analisar legislações, normas e regras internas para propor melhorias || Empresa .....:  BR BPO TECNOLOGIA S/A</t>
+        </is>
+      </c>
+      <c r="I686" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>03/02/2026</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t>82704</t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>Analista de Redes Sênior</t>
+        </is>
+      </c>
+      <c r="D687" t="inlineStr">
+        <is>
+          <t>Sênior</t>
+        </is>
+      </c>
+      <c r="E687" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F687" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 31/01/26</t>
+        </is>
+      </c>
+      <c r="G687" t="inlineStr">
+        <is>
+          <t>Oportunidade para Analista de Redes Sênior, atuar no REMOTAMENTE, PORÉM COM IDAS AO ESCRITÓRIO ESPORÁDICAS E PROGRAMADAS (região Sul de SP, Berrini), em projeto de cliente do segmento de seguro.  Requisitos técnicos: - Cisco Switches (L2 e L3): Políticas de roteamento (VRFs), OSPF, BGP - Avançado. - Cisco Firewalls: Validação de vazamento e fluxo de tráfego, criação de regras, SSL Inspection, Intrusion Rules, VPNs (Site-to-Site e - Remote Access)  - Intermediário. - Redes Wi-Fi: Meraki / Aironet - Básico. - F5: GTM, LTM, publicação de URLs, configuração de WAF, mitigação DDoS, Anti-Bot, iRules, Global DNS  - Intermediário. - Cisco ISE: Controle de acesso via VPN, rede cabeada e Wireless, postura  - Intermediário. - Cloud Networking: VPC, Direct Connect, Transit Gateway (AWS / Google) - Intermediário.  Diferencial: Certificações CCIE e CCNP
+Empresa .....:  Tech For TI</t>
+        </is>
+      </c>
+      <c r="H687" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 31/01/26 || Analista de Redes Sênior || Oportunidade para Analista de Redes Sênior, atuar no REMOTAMENTE, PORÉM COM IDAS AO ESCRITÓRIO ESPORÁDICAS E PROGRAMADAS (região Sul de SP, Berrini), em projeto de cliente do segmento de seguro.  Requisitos técnicos: - Cisco Switches (L2 e L3): Políticas de roteamento (VRFs), OSPF, BGP - Avançado. - Cisco Firewalls: Validação de vazamento e fluxo de tráfego, criação de regras, SSL Inspection, Intrusion Rules, VPNs (Site-to-Site e - Remote Access)  - Intermediário. - Redes Wi-Fi: Meraki / Aironet - Básico. - F5: GTM, LTM, publicação de URLs, configuração de WAF, mitigação DDoS, Anti-Bot, iRules, Global DNS  - Intermediário. - Cisco ISE: Controle de acesso via VPN, rede cabeada e Wireless, postura  - Intermediário. - Cloud Networking: VPC, Direct Connect, Transit Gateway (AWS / Google) - Intermediário.  Diferencial: Certificações CCIE e CCNP || Empresa .....:  Tech For TI</t>
+        </is>
+      </c>
+      <c r="I687" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>03/02/2026</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t>82563</t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>Analista de Segurança Operacional</t>
+        </is>
+      </c>
+      <c r="D688" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E688" t="inlineStr">
+        <is>
+          <t>Híbrido</t>
+        </is>
+      </c>
+      <c r="F688" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 31/01/26</t>
+        </is>
+      </c>
+      <c r="G688" t="inlineStr">
+        <is>
+          <t>Analista de Segurança Operacional  Requisitos: Experiencia e conhecimento, conforme abaixo: Controles de KPI Controles de planos de ação Controles de remediação Comunicação com os owners Políticas de Segurança Compliance check Análises Semanais Monitoração de Remediação Ferramenta de PAM TAM - Technical Account Manager IAM - Identity and Access Management PAM - Privileged Access Management Revisão de acessos de contas privilegiadas  Requisitos obrigatórios: Inglês nível: intermediário Espanhol nível: intermediário  Modelo de atuação: Hibrido (zona sul de São Paulo - SP)  Contratação CLT Vale Refeição ou Alimentação Assistência Médica e Assistência Odontológica Auxílio creche Convênio com Farmácia Parcerias com Universidades e Escolas de Idiomas Parceria de descontos com Seguro Auto e Residência Gympass Seguro de Vida
+Empresa .....:  PSM COMPANY</t>
+        </is>
+      </c>
+      <c r="H688" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 31/01/26 || Analista de Segurança Operacional || Analista de Segurança Operacional  Requisitos: Experiencia e conhecimento, conforme abaixo: Controles de KPI Controles de planos de ação Controles de remediação Comunicação com os owners Políticas de Segurança Compliance check Análises Semanais Monitoração de Remediação Ferramenta de PAM TAM - Technical Account Manager IAM - Identity and Access Management PAM - Privileged Access Management Revisão de acessos de contas privilegiadas  Requisitos obrigatórios: Inglês nível: intermediário Espanhol nível: intermediário  Modelo de atuação: Hibrido (zona sul de São Paulo - SP)  Contratação CLT Vale Refeição ou Alimentação Assistência Médica e Assistência Odontológica Auxílio creche Convênio com Farmácia Parcerias com Universidades e Escolas de Idiomas Parceria de descontos com Seguro Auto e Residência Gympass Seguro de Vida || Empresa .....:  PSM COMPANY</t>
+        </is>
+      </c>
+      <c r="I688" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>03/02/2026</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t>83090</t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>Analista de Sistemas WEB JR I - Marechal Deodoro</t>
+        </is>
+      </c>
+      <c r="D689" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E689" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F689" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 31/01/26</t>
+        </is>
+      </c>
+      <c r="G689" t="inlineStr">
+        <is>
+          <t>Analisar, avaliar a viabilidade, desenvolver , testar e homologar os sistemas de informações, utilizando ferramentas e procedimento adequados à sua implantação. Analisar o desempenho dos sistemas implantados, reavaliar e/ou atualizar os procedimentos, conversando e colhendo informações dos usuários. Treinar e acompanhar os usuários na utilização dos sistemas desenvolvidos, demonstrando e realizando suporte quanto a sua utilização. Corrigir eventuais falhas nos sistemas e/ou dados, através da análise, dos chamados técnicos e outros meios de atendimento. Alterar ou atualizar os sistemas devido à mudanças nas regras de procedimentos ou mudanças nas leis, através das solicitações dos seus superiores. Apresentar, treinar e orientar em relação ao desenvolvimento e manutenção dos sistemas. Prover a integração sistêmica/suporte entre os sistemas desenvolvidos internamente, no ambiente Web, com sistemas de fornecedores prestadores de serviços.
+Empresa .....:  OBRAS SOCIAIS E EDUCACIONAIS DE LUZ</t>
+        </is>
+      </c>
+      <c r="H689" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 31/01/26 || Analista de Sistemas WEB JR I - Marechal Deodoro || Analisar, avaliar a viabilidade, desenvolver , testar e homologar os sistemas de informações, utilizando ferramentas e procedimento adequados à sua implantação. Analisar o desempenho dos sistemas implantados, reavaliar e/ou atualizar os procedimentos, conversando e colhendo informações dos usuários. Treinar e acompanhar os usuários na utilização dos sistemas desenvolvidos, demonstrando e realizando suporte quanto a sua utilização. Corrigir eventuais falhas nos sistemas e/ou dados, através da análise, dos chamados técnicos e outros meios de atendimento. Alterar ou atualizar os sistemas devido à mudanças nas regras de procedimentos ou mudanças nas leis, através das solicitações dos seus superiores. Apresentar, treinar e orientar em relação ao desenvolvimento e manutenção dos sistemas. Prover a integração sistêmica/suporte entre os sistemas desenvolvidos internamente, no ambiente Web, com sistemas de fornecedores prestadores de serviços. || Empresa .....:  OBRAS SOCIAIS E EDUCACIONAIS DE LUZ</t>
+        </is>
+      </c>
+      <c r="I689" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>03/02/2026</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t>83527</t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>Analista de Suporte Sênior</t>
+        </is>
+      </c>
+      <c r="D690" t="inlineStr">
+        <is>
+          <t>Sênior</t>
+        </is>
+      </c>
+      <c r="E690" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F690" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 31/01/26</t>
+        </is>
+      </c>
+      <c r="G690" t="inlineStr">
+        <is>
+          <t>Analista de Suporte SR – Temporário  Empresa localizada na Vila Olímpia contrata Analista de Suporte SR para cobertura de férias (de 30 a 60 dias), início em Fev/2026.  Atividades: Atuação no Service Desk, organizando e controlando processos técnicos suporte aos usuários presencial, remoto e telefônico manutenção básica de hardware gestão de telefonia fixa e móvel suporte a ambiente Microsoft (Windows) acessos de rede, e-mail, internet, Active Directory e segurança da informação suporte a salas de reunião diagnóstico de falhas em hardware, redes e sistemas uso de Google Workspace SAP desejável controle de chamados, relatórios semanais e mensais inventário e gerenciamento de ativos de hardware e software. Requisitos: Formação em TI ou áreas correlatas experiência como Suporte/Service Desk Sênior inglês ou espanhol intermediário (escrita) / avançado disponibilidade presencial de segunda a sexta, das 8h às 18h.  R$ 6.500 + VA e VR 650,00  VT (Pagos em dinheiro)
+Empresa .....:  Enfok RH</t>
+        </is>
+      </c>
+      <c r="H690" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 31/01/26 || Analista de Suporte Sênior || Analista de Suporte SR – Temporário  Empresa localizada na Vila Olímpia contrata Analista de Suporte SR para cobertura de férias (de 30 a 60 dias), início em Fev/2026.  Atividades: Atuação no Service Desk, organizando e controlando processos técnicos suporte aos usuários presencial, remoto e telefônico manutenção básica de hardware gestão de telefonia fixa e móvel suporte a ambiente Microsoft (Windows) acessos de rede, e-mail, internet, Active Directory e segurança da informação suporte a salas de reunião diagnóstico de falhas em hardware, redes e sistemas uso de Google Workspace SAP desejável controle de chamados, relatórios semanais e mensais inventário e gerenciamento de ativos de hardware e software. Requisitos: Formação em TI ou áreas correlatas experiência como Suporte/Service Desk Sênior inglês ou espanhol intermediário (escrita) / avançado disponibilidade presencial de segunda a sexta, das 8h às 18h.  R$ 6.500 + VA e VR 650,00  VT (Pagos em dinheiro) || Empresa .....:  Enfok RH</t>
+        </is>
+      </c>
+      <c r="I690" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>03/02/2026</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t>82189</t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>Analista Funcional Protheus (Negócios) - Sr</t>
+        </is>
+      </c>
+      <c r="D691" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E691" t="inlineStr">
+        <is>
+          <t>Híbrido</t>
+        </is>
+      </c>
+      <c r="F691" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 31/01/26</t>
+        </is>
+      </c>
+      <c r="G691" t="inlineStr">
+        <is>
+          <t>Estamos em busca de um Consultor Funcional Protheus Sênior para atuar em projetos de implantação do ERP Protheus.  Híbrido 2x na Semana – Bairro Saúde - São Paulo   Atuar como consultor funcional nos módulos de Backoffice (COM, FAT, EST, FIN, FIS, CTB, ATF) Conduzir parametrizações e ajustes no módulo de Gestão de Contratos Apoiar em demais módulos (CRM, PCP, etc.) – considerado diferencial Realizar levantamento de requisitos, testes, homologações e treinamentos Apoiar desenvolvedores com conhecimento básico de ADVPL (nível intermediário será diferencial)  Participar ativamente das fases de implantação do ERP junto ao cliente.  Requisitos: Experiência sólida como Consultor Funcional Protheus em implantação de ERP Forte conhecimento nos módulos de Backoffice e Gestão de Contratos Conhecimento em demais módulos (CRM, PCP, etc.) será considerado diferencial Conhecimento em ADVPL básico  Diferencial: conhecimento da Metodologia de Implantação TOTVS (MIT).
+Empresa .....:  Mazzatech</t>
+        </is>
+      </c>
+      <c r="H691" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 31/01/26 || Analista Funcional Protheus (Negócios) - Sr || Estamos em busca de um Consultor Funcional Protheus Sênior para atuar em projetos de implantação do ERP Protheus.  Híbrido 2x na Semana – Bairro Saúde - São Paulo   Atuar como consultor funcional nos módulos de Backoffice (COM, FAT, EST, FIN, FIS, CTB, ATF) Conduzir parametrizações e ajustes no módulo de Gestão de Contratos Apoiar em demais módulos (CRM, PCP, etc.) – considerado diferencial Realizar levantamento de requisitos, testes, homologações e treinamentos Apoiar desenvolvedores com conhecimento básico de ADVPL (nível intermediário será diferencial)  Participar ativamente das fases de implantação do ERP junto ao cliente.  Requisitos: Experiência sólida como Consultor Funcional Protheus em implantação de ERP Forte conhecimento nos módulos de Backoffice e Gestão de Contratos Conhecimento em demais módulos (CRM, PCP, etc.) será considerado diferencial Conhecimento em ADVPL básico  Diferencial: conhecimento da Metodologia de Implantação TOTVS (MIT). || Empresa .....:  Mazzatech</t>
+        </is>
+      </c>
+      <c r="I691" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>03/02/2026</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t>82397</t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>Arquiteto Corporativo</t>
+        </is>
+      </c>
+      <c r="D692" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E692" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F692" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 31/01/26</t>
+        </is>
+      </c>
+      <c r="G692" t="inlineStr">
+        <is>
+          <t>Vaga: Arquiteto(a) Corporativo(a)  Requisitos: •	Domínio do padrão estratégico de DDD (Domain-Driven Design), ADM do TOGAF e, preferencialmente, conhecimento em Microservices. •	Experiência com mapas de cadeia de valor, Diagrama de Ishikawa e fluxos de valor.  Principais Atividades e Desafios: •	Definir padrões, convenções e boas práticas para identificação de subdomínios, contextos de negócios e funcionalidades que emergem desses contextos. •	Atuar de forma estratégica na modelagem e evolução da arquitetura corporativa, alinhando soluções às necessidades do negócio. •	Contribuir para a integração entre áreas de negócio e tecnologia, garantindo que os princípios arquiteturais apoiem objetivos de longo prazo. •	Auxiliar na identificação de oportunidades de melhoria e inovação, utilizando mapas de valor e técnicas analíticas para apoiar decisões de arquitetura.
+Empresa .....:  Verx Tecnologia e Inovação</t>
+        </is>
+      </c>
+      <c r="H692" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 31/01/26 || Arquiteto Corporativo || Vaga: Arquiteto(a) Corporativo(a)  Requisitos: •	Domínio do padrão estratégico de DDD (Domain-Driven Design), ADM do TOGAF e, preferencialmente, conhecimento em Microservices. •	Experiência com mapas de cadeia de valor, Diagrama de Ishikawa e fluxos de valor.  Principais Atividades e Desafios: •	Definir padrões, convenções e boas práticas para identificação de subdomínios, contextos de negócios e funcionalidades que emergem desses contextos. •	Atuar de forma estratégica na modelagem e evolução da arquitetura corporativa, alinhando soluções às necessidades do negócio. •	Contribuir para a integração entre áreas de negócio e tecnologia, garantindo que os princípios arquiteturais apoiem objetivos de longo prazo. •	Auxiliar na identificação de oportunidades de melhoria e inovação, utilizando mapas de valor e técnicas analíticas para apoiar decisões de arquitetura. || Empresa .....:  Verx Tecnologia e Inovação</t>
+        </is>
+      </c>
+      <c r="I692" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>03/02/2026</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>82327</t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>Arquiteto de Software Sênior/Google Cloud</t>
+        </is>
+      </c>
+      <c r="D693" t="inlineStr">
+        <is>
+          <t>Sênior</t>
+        </is>
+      </c>
+      <c r="E693" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F693" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 31/01/26</t>
+        </is>
+      </c>
+      <c r="G693" t="inlineStr">
+        <is>
+          <t>A Tech For TI está com oportunidade para Arquiteto de Software Sênior, atuar em projeto de cliente - AutoTech, focada no mercado B2B, presente em diversos países. - pj - Remoto  Requisitos mandatórios: Experiência prática comprovada como Arquiteto de Software em ambientes complexos. Experiência com PHP, Node.js e C# Experiência em front-end (Angular, React, Vue) Integração com apps mobile (Android/iOS via APIs) Experiência com Google Cloud Platform (GCP), incluindo práticas para otimização de custos. (Mandatório) Conhecimentos em segurança de aplicações e performance. Capacidade de traduzir requisitos de negócio em soluções técnicas claras.
+Empresa .....:  Tech For TI</t>
+        </is>
+      </c>
+      <c r="H693" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 31/01/26 || Arquiteto de Software Sênior/Google Cloud || A Tech For TI está com oportunidade para Arquiteto de Software Sênior, atuar em projeto de cliente - AutoTech, focada no mercado B2B, presente em diversos países. - pj - Remoto  Requisitos mandatórios: Experiência prática comprovada como Arquiteto de Software em ambientes complexos. Experiência com PHP, Node.js e C# Experiência em front-end (Angular, React, Vue) Integração com apps mobile (Android/iOS via APIs) Experiência com Google Cloud Platform (GCP), incluindo práticas para otimização de custos. (Mandatório) Conhecimentos em segurança de aplicações e performance. Capacidade de traduzir requisitos de negócio em soluções técnicas claras. || Empresa .....:  Tech For TI</t>
+        </is>
+      </c>
+      <c r="I693" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>03/02/2026</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t>82449</t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>Arquiteto de Soluções (presencial 3x/semana)</t>
+        </is>
+      </c>
+      <c r="D694" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E694" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F694" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 31/01/26</t>
+        </is>
+      </c>
+      <c r="G694" t="inlineStr">
+        <is>
+          <t>Definir a arquitetura de produtos bancários com foco em antecipação de recebíveis: modelagem de fluxos, regras de negócio, integração e escalabilidade da solução. Projetar e validar a solução completa — da captura dos recebíveis, registro, liquidação, à antecipação e repasse — garantindo conformidade regulatória, performance e segurança. Trabalhar com equipes multifuncionais (produto, TI, compliance, operações, risco) para transformar requisitos de negócio em soluções técnicas robustas. Selecionar, configurar ou propor plataformas tecnológicas (ex: módulo de antecipação, integração com registradoras, APIs de análise de crédito) e definir padrões de integração (REST, event-driven, microserviços). Garantir que a arquitetura atenda aos requisitos de compliance, normas do mercado financeiro e integração de dados (como registro de recebíveis em entidades autorizadas). Fomentar boas práticas de arquitetura: modularidade, reutilização, governança, monitoramento e segurança
+Empresa .....:  CBDS</t>
+        </is>
+      </c>
+      <c r="H694" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 31/01/26 || Arquiteto de Soluções (presencial 3x/semana) || Definir a arquitetura de produtos bancários com foco em antecipação de recebíveis: modelagem de fluxos, regras de negócio, integração e escalabilidade da solução. Projetar e validar a solução completa — da captura dos recebíveis, registro, liquidação, à antecipação e repasse — garantindo conformidade regulatória, performance e segurança. Trabalhar com equipes multifuncionais (produto, TI, compliance, operações, risco) para transformar requisitos de negócio em soluções técnicas robustas. Selecionar, configurar ou propor plataformas tecnológicas (ex: módulo de antecipação, integração com registradoras, APIs de análise de crédito) e definir padrões de integração (REST, event-driven, microserviços). Garantir que a arquitetura atenda aos requisitos de compliance, normas do mercado financeiro e integração de dados (como registro de recebíveis em entidades autorizadas). Fomentar boas práticas de arquitetura: modularidade, reutilização, governança, monitoramento e segurança || Empresa .....:  CBDS</t>
+        </is>
+      </c>
+      <c r="I694" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>03/02/2026</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t>83066</t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>Delivery Manager Sênior</t>
+        </is>
+      </c>
+      <c r="D695" t="inlineStr">
+        <is>
+          <t>Sênior</t>
+        </is>
+      </c>
+      <c r="E695" t="inlineStr">
+        <is>
+          <t>Híbrido</t>
+        </is>
+      </c>
+      <c r="F695" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 31/01/26</t>
+        </is>
+      </c>
+      <c r="G695" t="inlineStr">
+        <is>
+          <t>Cargo: Delivery Manager Sênior (SDM) Empresa: Venice Technology Modelo: Híbrido – Santo André/SP (1x por semana presencial) Contratação: PJ + Benefícios  Descrição: Atuar como Delivery Manager Sênior apoiando Scrum Masters e Product Owners, garantindo a correta aplicação de frameworks ágeis (Scrum/Kanban), qualidade das entregas, previsibilidade e melhoria contínua. Responsável por acompanhar performance dos times, apoiar priorização de backlog, garantir ritos ágeis, remover impedimentos e atuar em iniciativas estratégicas junto ao cliente, promovendo governança e boas práticas ágeis.  Requisitos: Certificações em Agilidade (CSM, PSM, CSPO, PSPO ou similares) – obrigatório. Experiência com múltiplos times ágeis, conhecimento sólido em práticas, frameworks e métricas ágeis, experiência com Jira e indicadores. Excelente comunicação, gestão de stakeholders e capacidade analítica.
+Empresa .....:  Venice Tech</t>
+        </is>
+      </c>
+      <c r="H695" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 31/01/26 || Delivery Manager Sênior || Cargo: Delivery Manager Sênior (SDM) Empresa: Venice Technology Modelo: Híbrido – Santo André/SP (1x por semana presencial) Contratação: PJ + Benefícios  Descrição: Atuar como Delivery Manager Sênior apoiando Scrum Masters e Product Owners, garantindo a correta aplicação de frameworks ágeis (Scrum/Kanban), qualidade das entregas, previsibilidade e melhoria contínua. Responsável por acompanhar performance dos times, apoiar priorização de backlog, garantir ritos ágeis, remover impedimentos e atuar em iniciativas estratégicas junto ao cliente, promovendo governança e boas práticas ágeis.  Requisitos: Certificações em Agilidade (CSM, PSM, CSPO, PSPO ou similares) – obrigatório. Experiência com múltiplos times ágeis, conhecimento sólido em práticas, frameworks e métricas ágeis, experiência com Jira e indicadores. Excelente comunicação, gestão de stakeholders e capacidade analítica. || Empresa .....:  Venice Tech</t>
+        </is>
+      </c>
+      <c r="I695" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>03/02/2026</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>83533</t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>Desenvolvedor Backend (AWS Lambda)</t>
+        </is>
+      </c>
+      <c r="D696" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E696" t="inlineStr">
+        <is>
+          <t>Híbrido</t>
+        </is>
+      </c>
+      <c r="F696" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 31/01/26</t>
+        </is>
+      </c>
+      <c r="G696" t="inlineStr">
+        <is>
+          <t>Híbrido (3x por semana no escritório em São Paulo - Morumbi) CLT e por tempo indeterminado  Você fará parte de um time que está conduzindo a transformação de sistemas legados para uma arquitetura moderna em microserviços e serverless na AWS.  Requisitos Experiência em AWS Domínio AWS Lambda (codificação) Experiência em migração de sistema legado para arquitetura moderna. Experiência sólida Node.js. e/ou Java Experiência sólida Typescript Forte domínio de boas práticas back-end e arquitetura.  Responsabilidades Desenvolver e manter APIs back-end escaláveis. Criar e manter APIs serverless (Lambda). Implementar testes unitários garantindo qualidade e cobertura. Atuar com PostgreSQL, DynamoDB e PL/SQL quando necessário. Contribuir em soluções e integrações utilizando serviços AWS: Lambda, API Gateway, SQS, S3, Step Functions, CloudWatch, entre outros.
+Empresa .....:  Conquest One</t>
+        </is>
+      </c>
+      <c r="H696" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 31/01/26 || Desenvolvedor Backend (AWS Lambda) || Híbrido (3x por semana no escritório em São Paulo - Morumbi) CLT e por tempo indeterminado  Você fará parte de um time que está conduzindo a transformação de sistemas legados para uma arquitetura moderna em microserviços e serverless na AWS.  Requisitos Experiência em AWS Domínio AWS Lambda (codificação) Experiência em migração de sistema legado para arquitetura moderna. Experiência sólida Node.js. e/ou Java Experiência sólida Typescript Forte domínio de boas práticas back-end e arquitetura.  Responsabilidades Desenvolver e manter APIs back-end escaláveis. Criar e manter APIs serverless (Lambda). Implementar testes unitários garantindo qualidade e cobertura. Atuar com PostgreSQL, DynamoDB e PL/SQL quando necessário. Contribuir em soluções e integrações utilizando serviços AWS: Lambda, API Gateway, SQS, S3, Step Functions, CloudWatch, entre outros. || Empresa .....:  Conquest One</t>
+        </is>
+      </c>
+      <c r="I696" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>03/02/2026</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t>83173</t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>DESENVOLVEDOR FRONT-END</t>
+        </is>
+      </c>
+      <c r="D697" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E697" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F697" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 31/01/26</t>
+        </is>
+      </c>
+      <c r="G697" t="inlineStr">
+        <is>
+          <t>Atividades: Atuação em evolução e manutenção de aplicações, ajustes de layout, testes unitários, integração com APIs, code review e colaboração técnica com o time.  Requisitos: Angular ou React Metodologias ágeis Git  CLT  Presencial – Av. Paulista (Brazilian Financial Center)
+Empresa .....:  CAPITANI CONSULTORIA E SISTEMAS LTDA</t>
+        </is>
+      </c>
+      <c r="H697" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 31/01/26 || DESENVOLVEDOR FRONT-END || Atividades: Atuação em evolução e manutenção de aplicações, ajustes de layout, testes unitários, integração com APIs, code review e colaboração técnica com o time.  Requisitos: Angular ou React Metodologias ágeis Git  CLT  Presencial – Av. Paulista (Brazilian Financial Center) || Empresa .....:  CAPITANI CONSULTORIA E SISTEMAS LTDA</t>
+        </is>
+      </c>
+      <c r="I697" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>03/02/2026</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t>83532</t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>DESENVOLVEDOR FRONT-END PLENO</t>
+        </is>
+      </c>
+      <c r="D698" t="inlineStr">
+        <is>
+          <t>Pleno</t>
+        </is>
+      </c>
+      <c r="E698" t="inlineStr">
+        <is>
+          <t>Híbrido</t>
+        </is>
+      </c>
+      <c r="F698" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 31/01/26</t>
+        </is>
+      </c>
+      <c r="G698" t="inlineStr">
+        <is>
+          <t>REQUISITOS: Javascript TypeScript Git Teste unitarios jasmine ou jest Teste end-to-end Angular 2+ SASS Métodologia BEM Gerenciamento de estado Clean Code Jenkins  Atuação: Hibrido 4x/semana  (Av. Paulista - Bela Vista.)
+Empresa .....:  CAPITANI CONSULTORIA E SISTEMAS LTDA</t>
+        </is>
+      </c>
+      <c r="H698" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 31/01/26 || DESENVOLVEDOR FRONT-END PLENO || REQUISITOS: Javascript TypeScript Git Teste unitarios jasmine ou jest Teste end-to-end Angular 2+ SASS Métodologia BEM Gerenciamento de estado Clean Code Jenkins  Atuação: Hibrido 4x/semana  (Av. Paulista - Bela Vista.) || Empresa .....:  CAPITANI CONSULTORIA E SISTEMAS LTDA</t>
+        </is>
+      </c>
+      <c r="I698" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>03/02/2026</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t>83178</t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>Desenvolvedor Full Stack (PHP/React)</t>
+        </is>
+      </c>
+      <c r="D699" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E699" t="inlineStr">
+        <is>
+          <t>Híbrido</t>
+        </is>
+      </c>
+      <c r="F699" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 31/01/26</t>
+        </is>
+      </c>
+      <c r="G699" t="inlineStr">
+        <is>
+          <t>Buscamos profissionais Pleno/Senior para atuar no desenvolvimento, manutenção e evolução dos nossos sistemas web, com visão completa da aplicação (frontend, backend e banco de dados).  Como será o seu dia a dia: Desenvolver e manter novas funcionalidades nos sistemas web utilizando PHP (com framework Laravel) no backend.  Criar e implementar interfaces de usuário responsivas e interativas utilizando JavaScript e React.  Projetar, otimizar e gerenciar estruturas de banco de dados PostgreSQL, escrevendo queries eficientes para relatórios.  Integrar os sistemas internos com APIs externas e desenvolver suas próprias APIs RESTful.  Atuar na correção de bugs e resolução de problemas técnicos reportados pelos usuários e pela equipe de produto.  Utilizar Git para versionamento de código e colaborar através de fluxos de trabalho como Git Flow ou GitHub Flow.  Forma de trabalho: híbrido no centro de São Paulo Contratação: PJ  Faixa Salarial entre R$ 6.000 - R$ 8.000
+Empresa .....:  Análise Editorial</t>
+        </is>
+      </c>
+      <c r="H699" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 31/01/26 || Desenvolvedor Full Stack (PHP/React) || Buscamos profissionais Pleno/Senior para atuar no desenvolvimento, manutenção e evolução dos nossos sistemas web, com visão completa da aplicação (frontend, backend e banco de dados).  Como será o seu dia a dia: Desenvolver e manter novas funcionalidades nos sistemas web utilizando PHP (com framework Laravel) no backend.  Criar e implementar interfaces de usuário responsivas e interativas utilizando JavaScript e React.  Projetar, otimizar e gerenciar estruturas de banco de dados PostgreSQL, escrevendo queries eficientes para relatórios.  Integrar os sistemas internos com APIs externas e desenvolver suas próprias APIs RESTful.  Atuar na correção de bugs e resolução de problemas técnicos reportados pelos usuários e pela equipe de produto.  Utilizar Git para versionamento de código e colaborar através de fluxos de trabalho como Git Flow ou GitHub Flow.  Forma de trabalho: híbrido no centro de São Paulo Contratação: PJ  Faixa Salarial entre R$ 6.000 - R$ 8.000 || Empresa .....:  Análise Editorial</t>
+        </is>
+      </c>
+      <c r="I699" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>03/02/2026</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>83080</t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>Desenvolvedor Fullstack Net Sênior</t>
+        </is>
+      </c>
+      <c r="D700" t="inlineStr">
+        <is>
+          <t>Sênior</t>
+        </is>
+      </c>
+      <c r="E700" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F700" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 31/01/26</t>
+        </is>
+      </c>
+      <c r="G700" t="inlineStr">
+        <is>
+          <t>VAGA  Desenvolvedor Fullstack .NET / Vue.js Sênior  Presencial – Av. Juscelino Kubitschek  São Paulo (Cliente do setor financeiro)  Estamos em busca de um(a) Desenvolvedor(a) Fullstack Sênior para atuar em um ambiente desafiador, com foco em tecnologia e inovação no mercado financeiro.  Requisitos Forte experiência com C# e .NET Core Sólidos conhecimentos em front-end, incluindo HTML, CSS responsivo e JavaScript, além de experiência com Single Page Applications (SPA), especificamente com Vue.JS e Flutter. Vivência em desenvolvimento back-end utilizando ASP.NET Web Forms e ASP.NET MVC. Conhecimento em microsserviços, design patterns e mensageria Bancos de dados SQL / T-SQL e NoSQL Metodologias ágeis e Git  Diferenciais Experiência no setor financeiro Uso de IA no desenvolvimento (ex: GitHub Copilot) Docker / Kubernetes e CI/CD Monitoramento com Splunk e Dynatrace Análise de performance de banco de dados (DPA)
+Empresa .....:  CBYK</t>
+        </is>
+      </c>
+      <c r="H700" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 31/01/26 || Desenvolvedor Fullstack Net Sênior || VAGA  Desenvolvedor Fullstack .NET / Vue.js Sênior  Presencial – Av. Juscelino Kubitschek  São Paulo (Cliente do setor financeiro)  Estamos em busca de um(a) Desenvolvedor(a) Fullstack Sênior para atuar em um ambiente desafiador, com foco em tecnologia e inovação no mercado financeiro.  Requisitos Forte experiência com C# e .NET Core Sólidos conhecimentos em front-end, incluindo HTML, CSS responsivo e JavaScript, além de experiência com Single Page Applications (SPA), especificamente com Vue.JS e Flutter. Vivência em desenvolvimento back-end utilizando ASP.NET Web Forms e ASP.NET MVC. Conhecimento em microsserviços, design patterns e mensageria Bancos de dados SQL / T-SQL e NoSQL Metodologias ágeis e Git  Diferenciais Experiência no setor financeiro Uso de IA no desenvolvimento (ex: GitHub Copilot) Docker / Kubernetes e CI/CD Monitoramento com Splunk e Dynatrace Análise de performance de banco de dados (DPA) || Empresa .....:  CBYK</t>
+        </is>
+      </c>
+      <c r="I700" t="n">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Atualização automática: Wed Feb  4 04:05:56 UTC 2026
</commit_message>
<xml_diff>
--- a/vagas_apinfo.xlsx
+++ b/vagas_apinfo.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I700"/>
+  <dimension ref="A1:I776"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -32784,6 +32784,3509 @@
         <v>20</v>
       </c>
     </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>04/02/2026</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>82497</t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>Product Owner</t>
+        </is>
+      </c>
+      <c r="D701" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E701" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F701" t="inlineStr">
+        <is>
+          <t>Barueri - SP - 04/02/26</t>
+        </is>
+      </c>
+      <c r="G701" t="inlineStr">
+        <is>
+          <t>Oportunidade híbrida 2x  Alphaville Modalidade PJ  Responsabilidades: Gerenciar e priorizar o Product Backlog Garantir clareza e transparência dos itens para o time Maximizar valor das entregas Atuar junto ao Scrum Master nas cerimônias Assegurar entendimento do backlog pelo time de desenvolvimento.  Requisitos: Inglês fluente Experiência sólida como PO Conhecimento em Trello, Jira, Kanban, SAFe, XP  Desejável: Design Thinking, Design Sprint, Lean Inception Boa comunicação e organização.
+Empresa .....:  Entrust IT</t>
+        </is>
+      </c>
+      <c r="H701" t="inlineStr">
+        <is>
+          <t>Barueri - SP - 04/02/26 || Product Owner || Oportunidade híbrida 2x  Alphaville Modalidade PJ  Responsabilidades: Gerenciar e priorizar o Product Backlog Garantir clareza e transparência dos itens para o time Maximizar valor das entregas Atuar junto ao Scrum Master nas cerimônias Assegurar entendimento do backlog pelo time de desenvolvimento.  Requisitos: Inglês fluente Experiência sólida como PO Conhecimento em Trello, Jira, Kanban, SAFe, XP  Desejável: Design Thinking, Design Sprint, Lean Inception Boa comunicação e organização. || Empresa .....:  Entrust IT</t>
+        </is>
+      </c>
+      <c r="I701" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>04/02/2026</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t>82573</t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>Especialista de Sistemas e TI - Presencial</t>
+        </is>
+      </c>
+      <c r="D702" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E702" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F702" t="inlineStr">
+        <is>
+          <t>Campinas - SP - 04/02/26</t>
+        </is>
+      </c>
+      <c r="G702" t="inlineStr">
+        <is>
+          <t>Profissional com formação superior completa em Análise de Sistemas, Ciências da Computação ou Engenharia da Computação, experiência sólida em gestão de sistemas e projetos.  Principais responsabilidades Ser referência técnica para o time de Analistas Atuar como ponto focal entre empresa e fornecedores, garantindo qualidade, prazo e escopo Sustentação de sistemas: atendimento a incidentes, problemas e mudanças Gestão de projetos (Waterfall e Ágil) Monitoramento de performance e integração entre sistemas Levantamento de requisitos técnicos e funcionais Desenho e implementação de APIs Mapeamento de processos (BPMN) e análise de melhorias.  Conhecimentos desejados Bancos de dados Oracle, MS SQL Server e Progress ITIL e COBIT (desejável).
+Empresa .....:  Aeroporto Internacional de Viracopos</t>
+        </is>
+      </c>
+      <c r="H702" t="inlineStr">
+        <is>
+          <t>Campinas - SP - 04/02/26 || Especialista de Sistemas e TI - Presencial || Profissional com formação superior completa em Análise de Sistemas, Ciências da Computação ou Engenharia da Computação, experiência sólida em gestão de sistemas e projetos.  Principais responsabilidades Ser referência técnica para o time de Analistas Atuar como ponto focal entre empresa e fornecedores, garantindo qualidade, prazo e escopo Sustentação de sistemas: atendimento a incidentes, problemas e mudanças Gestão de projetos (Waterfall e Ágil) Monitoramento de performance e integração entre sistemas Levantamento de requisitos técnicos e funcionais Desenho e implementação de APIs Mapeamento de processos (BPMN) e análise de melhorias.  Conhecimentos desejados Bancos de dados Oracle, MS SQL Server e Progress ITIL e COBIT (desejável). || Empresa .....:  Aeroporto Internacional de Viracopos</t>
+        </is>
+      </c>
+      <c r="I702" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>04/02/2026</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t>83558</t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>Desenvolvedor ADVPL Pleno</t>
+        </is>
+      </c>
+      <c r="D703" t="inlineStr">
+        <is>
+          <t>Pleno</t>
+        </is>
+      </c>
+      <c r="E703" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F703" t="inlineStr">
+        <is>
+          <t>Curitiba - PR - 04/02/26</t>
+        </is>
+      </c>
+      <c r="G703" t="inlineStr">
+        <is>
+          <t>Buscamos profissionais com experiência em desenvolvimento ADVPL Protheus, com boa comunicação e habilidade de relacionamento. Espera-se atuação próxima ao cliente, com postura consultiva, colaborativa e foco em solução, além de maturidade profissional para interação com diferentes áreas e forte espírito de equipe.  Detalhes da Vaga Modelo: Presencial – Curitiba/PR Contratação: Cooperado Carga horária: Full-time  Segunda a sexta-feira  Horário comercial  9Atividades Desenvolvimento e manutenção de aplicações em ADVPL/TL++ Criação de Jobs e Schedules Desenvolvimento de Webservices (SOAP e REST).  Requisitos Conhecimento em regras de negócio Banco de dados SQL Programação em ADVPL/TL++.  Perfil Comportamental Boa comunicação, atuação consultiva, perfil colaborativo, senso de responsabilidade e foco em entregas com qualidade.
+Empresa .....:  CODE GROUP</t>
+        </is>
+      </c>
+      <c r="H703" t="inlineStr">
+        <is>
+          <t>Curitiba - PR - 04/02/26 || Desenvolvedor ADVPL Pleno || Buscamos profissionais com experiência em desenvolvimento ADVPL Protheus, com boa comunicação e habilidade de relacionamento. Espera-se atuação próxima ao cliente, com postura consultiva, colaborativa e foco em solução, além de maturidade profissional para interação com diferentes áreas e forte espírito de equipe.  Detalhes da Vaga Modelo: Presencial – Curitiba/PR Contratação: Cooperado Carga horária: Full-time  Segunda a sexta-feira  Horário comercial  9Atividades Desenvolvimento e manutenção de aplicações em ADVPL/TL++ Criação de Jobs e Schedules Desenvolvimento de Webservices (SOAP e REST).  Requisitos Conhecimento em regras de negócio Banco de dados SQL Programação em ADVPL/TL++.  Perfil Comportamental Boa comunicação, atuação consultiva, perfil colaborativo, senso de responsabilidade e foco em entregas com qualidade. || Empresa .....:  CODE GROUP</t>
+        </is>
+      </c>
+      <c r="I703" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>04/02/2026</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t>83579</t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>Arquiteto de Softwares</t>
+        </is>
+      </c>
+      <c r="D704" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E704" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F704" t="inlineStr">
+        <is>
+          <t>Gravataí - RS - 04/02/26</t>
+        </is>
+      </c>
+      <c r="G704" t="inlineStr">
+        <is>
+          <t>Profissional generalista com capacidade de desenhar e evoluir arquiteturas escaláveis, seguras e operáveis, selecionando o estilo adequado ao contexto (monólito modular, microservices, SOA, event-driven, arquitetura hexagonal, DDD, serverless) com foco em NFRs  Linguagens e Ecossistema Principal: desejável com C e C++ e .NET (C#)  Cloud AWS: domínio de fundamentos de AWS Apoiar discovery e priorização, e estruturar soluções considerando roadmap de produto, reutilização (plataforma) e time-to-market.  Modelagem e Documentação de Arquitetura: produzir diagramas e documentação objetiva usando o Modelo C4 (Contexto, Contêiner, Componente) e UML.  DevOps: entendimento de CI/CD, automação de infraestrutura (IaC), containers (Docker) .  Dados e Integrações: conhecimento em bancos relacionais e não relacionais e em integração de sistemas.  Ambiente de engenharia: domínio de controle de versão (Git) e práticas de qualidade (code review, testes automatizados,
+Empresa .....:  Scope</t>
+        </is>
+      </c>
+      <c r="H704" t="inlineStr">
+        <is>
+          <t>Gravataí - RS - 04/02/26 || Arquiteto de Softwares || Profissional generalista com capacidade de desenhar e evoluir arquiteturas escaláveis, seguras e operáveis, selecionando o estilo adequado ao contexto (monólito modular, microservices, SOA, event-driven, arquitetura hexagonal, DDD, serverless) com foco em NFRs  Linguagens e Ecossistema Principal: desejável com C e C++ e .NET (C#)  Cloud AWS: domínio de fundamentos de AWS Apoiar discovery e priorização, e estruturar soluções considerando roadmap de produto, reutilização (plataforma) e time-to-market.  Modelagem e Documentação de Arquitetura: produzir diagramas e documentação objetiva usando o Modelo C4 (Contexto, Contêiner, Componente) e UML.  DevOps: entendimento de CI/CD, automação de infraestrutura (IaC), containers (Docker) .  Dados e Integrações: conhecimento em bancos relacionais e não relacionais e em integração de sistemas.  Ambiente de engenharia: domínio de controle de versão (Git) e práticas de qualidade (code review, testes automatizados, || Empresa .....:  Scope</t>
+        </is>
+      </c>
+      <c r="I704" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>04/02/2026</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t>83580</t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>Desenvolvedor de Softwares</t>
+        </is>
+      </c>
+      <c r="D705" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E705" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F705" t="inlineStr">
+        <is>
+          <t>Gravataí - RS - 04/02/26</t>
+        </is>
+      </c>
+      <c r="G705" t="inlineStr">
+        <is>
+          <t>Atuará  tanto no frontend quanto no backend e deverá participar da construção e evolução de sistemas robustos e modernos.  •	Criar e manter interfaces web utilizando Angular (preferencialmente versões recentes), •	Manter e evoluir sistemas legados baseados em ASP.NET e WINDOWS FORMS (.NET Framework e C#) •	Experiência com Angular, HTML5, CSS3 e TypeScript •	Conhecimento em C# com Windows Forms, .NET Framework (e desejável .NET Core •	Desenvolver e integrar middlewares e serviços REST para comunicação entre camadas de negócio e aplicações web •	Bancos de dados relacionais, especialmente Oracle (CRUD, Procedures, Views) •	Garantir a qualidade do código com boas práticas de desenvolvimento e testes unitários e funcionais •	Documentar requisitos, fluxos de dados, APIs e regras de negócio •	Participar de reuniões técnicas, revisões de código e contribuir com soluções inovadoras. •	Diferencial: Conhecimentos básicos de Docker, Git, DevOps ou CI
+Empresa .....:  Scope</t>
+        </is>
+      </c>
+      <c r="H705" t="inlineStr">
+        <is>
+          <t>Gravataí - RS - 04/02/26 || Desenvolvedor de Softwares || Atuará  tanto no frontend quanto no backend e deverá participar da construção e evolução de sistemas robustos e modernos.  •	Criar e manter interfaces web utilizando Angular (preferencialmente versões recentes), •	Manter e evoluir sistemas legados baseados em ASP.NET e WINDOWS FORMS (.NET Framework e C#) •	Experiência com Angular, HTML5, CSS3 e TypeScript •	Conhecimento em C# com Windows Forms, .NET Framework (e desejável .NET Core •	Desenvolver e integrar middlewares e serviços REST para comunicação entre camadas de negócio e aplicações web •	Bancos de dados relacionais, especialmente Oracle (CRUD, Procedures, Views) •	Garantir a qualidade do código com boas práticas de desenvolvimento e testes unitários e funcionais •	Documentar requisitos, fluxos de dados, APIs e regras de negócio •	Participar de reuniões técnicas, revisões de código e contribuir com soluções inovadoras. •	Diferencial: Conhecimentos básicos de Docker, Git, DevOps ou CI || Empresa .....:  Scope</t>
+        </is>
+      </c>
+      <c r="I705" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>04/02/2026</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>83571</t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>Analista de Configuração</t>
+        </is>
+      </c>
+      <c r="D706" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E706" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F706" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 04/02/26</t>
+        </is>
+      </c>
+      <c r="G706" t="inlineStr">
+        <is>
+          <t>Sólida experiência em controle de configuração de software, revisão de código (Code Review) e automação de pipelines em esteiras DevOps.  Experiência prática na definição e manutenção de processos de versionamento, gestão de branches, políticas de merge, padronização de commits e governança de código.  Superior completo em cursos relacionados a TI Atuação Totalmente remota
+Empresa .....:  Spassu Tecnologia</t>
+        </is>
+      </c>
+      <c r="H706" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 04/02/26 || Analista de Configuração || Sólida experiência em controle de configuração de software, revisão de código (Code Review) e automação de pipelines em esteiras DevOps.  Experiência prática na definição e manutenção de processos de versionamento, gestão de branches, políticas de merge, padronização de commits e governança de código.  Superior completo em cursos relacionados a TI Atuação Totalmente remota || Empresa .....:  Spassu Tecnologia</t>
+        </is>
+      </c>
+      <c r="I706" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>04/02/2026</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t>83060</t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>Analista Desenvolvedor Full Stack Sênior</t>
+        </is>
+      </c>
+      <c r="D707" t="inlineStr">
+        <is>
+          <t>Sênior</t>
+        </is>
+      </c>
+      <c r="E707" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F707" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 04/02/26</t>
+        </is>
+      </c>
+      <c r="G707" t="inlineStr">
+        <is>
+          <t>Experiência Técnica:  Capacidade de elaborar e compreender System Design e arquiteturas de software. Forte compreensão dos princípios do Ciclo de Vida de Desenvolvimento de Software (SDLC). Conhecimentos sólidos em desenvolvimento seguro, incluindo práticas de pentest, SAST e DAST. Experiência na implementação de boas práticas de autenticação e autorização, incluindo OAuth 2.0. Conhecimento em IdentityServer / Keycloak. Vivência com soluções Multi-Tenant (multi-cliente). Conhecimento em padrões e boas práticas como Design Patterns, Cloud Patterns, SOA e Web Standards. Experiência comprovada em metodologias ágeis (Scrum e Kanban), além de DevOps e CI/CD. .NET (.NET Framework / .NET Core) – C# ASP.NET APIs REST JavaScript / jQuery AngularJS / Angular (2+) SQL Server NoSQL: ElasticSearch Entity Framework Core Redis Cache HTML5 / CSS Git IIS Implementação de controles de segurança alinhados ao OWASP Top 10  Superior Completo  Inglês Intermediário.
+Empresa .....:  Emphasys IT Services</t>
+        </is>
+      </c>
+      <c r="H707" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 04/02/26 || Analista Desenvolvedor Full Stack Sênior || Experiência Técnica:  Capacidade de elaborar e compreender System Design e arquiteturas de software. Forte compreensão dos princípios do Ciclo de Vida de Desenvolvimento de Software (SDLC). Conhecimentos sólidos em desenvolvimento seguro, incluindo práticas de pentest, SAST e DAST. Experiência na implementação de boas práticas de autenticação e autorização, incluindo OAuth 2.0. Conhecimento em IdentityServer / Keycloak. Vivência com soluções Multi-Tenant (multi-cliente). Conhecimento em padrões e boas práticas como Design Patterns, Cloud Patterns, SOA e Web Standards. Experiência comprovada em metodologias ágeis (Scrum e Kanban), além de DevOps e CI/CD. .NET (.NET Framework / .NET Core) – C# ASP.NET APIs REST JavaScript / jQuery AngularJS / Angular (2+) SQL Server NoSQL: ElasticSearch Entity Framework Core Redis Cache HTML5 / CSS Git IIS Implementação de controles de segurança alinhados ao OWASP Top 10  Superior Completo  Inglês Intermediário. || Empresa .....:  Emphasys IT Services</t>
+        </is>
+      </c>
+      <c r="I707" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>04/02/2026</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t>83565</t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>Analista Funcional Salesforce (Industries) - SR</t>
+        </is>
+      </c>
+      <c r="D708" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E708" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F708" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 04/02/26</t>
+        </is>
+      </c>
+      <c r="G708" t="inlineStr">
+        <is>
+          <t>Analista Funcional Salesforce (Industries) – Sênior  Modelo: Totalmente remoto Localidade obrigatória do candidato(a): SP, Recife, Nova Lima/MG ou RJ Prazo de contrato: 1 ano (com possibilidade de efetivação) Horário: 9h às 18h Regime: PJ (precisa ter empresa aberta) ou CLT  Principais requisitos: Experiência como Analista Funcional Salesforce Atuação com Salesforce Industries (Communications Cloud) Levantamento de requisitos e documentação funcional Interface direta com o cliente Conhecimento em telecom (diferencial)  Observação: Para essa posição o candidato precisa ter experiência profissional comprovada em Salesforce Industries (Communications Cloud).  Enviar currículo atualizado.
+Empresa .....:  ITeam</t>
+        </is>
+      </c>
+      <c r="H708" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 04/02/26 || Analista Funcional Salesforce (Industries) - SR || Analista Funcional Salesforce (Industries) – Sênior  Modelo: Totalmente remoto Localidade obrigatória do candidato(a): SP, Recife, Nova Lima/MG ou RJ Prazo de contrato: 1 ano (com possibilidade de efetivação) Horário: 9h às 18h Regime: PJ (precisa ter empresa aberta) ou CLT  Principais requisitos: Experiência como Analista Funcional Salesforce Atuação com Salesforce Industries (Communications Cloud) Levantamento de requisitos e documentação funcional Interface direta com o cliente Conhecimento em telecom (diferencial)  Observação: Para essa posição o candidato precisa ter experiência profissional comprovada em Salesforce Industries (Communications Cloud).  Enviar currículo atualizado. || Empresa .....:  ITeam</t>
+        </is>
+      </c>
+      <c r="I708" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>04/02/2026</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>Desenvolvedor (Remoto)</t>
+        </is>
+      </c>
+      <c r="D709" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E709" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F709" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 04/02/26</t>
+        </is>
+      </c>
+      <c r="G709" t="inlineStr"/>
+      <c r="H709" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 04/02/26 || Desenvolvedor (Remoto)</t>
+        </is>
+      </c>
+      <c r="I709" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>04/02/2026</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t>83556</t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>Empresa .....:  Milkbox</t>
+        </is>
+      </c>
+      <c r="D710" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E710" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F710" t="inlineStr">
+        <is>
+          <t>Não Informado</t>
+        </is>
+      </c>
+      <c r="G710" t="inlineStr"/>
+      <c r="H710" t="inlineStr">
+        <is>
+          <t>Empresa .....:  Milkbox</t>
+        </is>
+      </c>
+      <c r="I710" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>04/02/2026</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t>83169</t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>Desenvolvedor Back-end Sênior</t>
+        </is>
+      </c>
+      <c r="D711" t="inlineStr">
+        <is>
+          <t>Sênior</t>
+        </is>
+      </c>
+      <c r="E711" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F711" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 04/02/26</t>
+        </is>
+      </c>
+      <c r="G711" t="inlineStr">
+        <is>
+          <t>Responsabilidades e requisitos: •Atuação principal em projetos de meios de pagamento, incluindo PIX (estático, dinâmico e automático), análise de dados e integrações com gateways como GetNet, Cielo e Stone. •Conhecimento sólido em .NET, Clean Code, SOLID, TDD e DDD. •Experiência prévia em empresas de pagamentos, bancos, fintechs ou consultorias do setor financeiro será altamente valorizada. •Perfil colaborativo, boa comunicação e maturidade para atuação em ambiente remoto. •Diferencial para quem já atuou com integração de sistemas, arquivos Febraban, transações em tempo real, análise de risco e prevenção a fraudes. •Espera-se senioridade técnica comprovada, autonomia e capacidade de adaptação a diferentes tribos e squads de tecnologia.
+Empresa .....:  Farol plus (Consultoria de RH)</t>
+        </is>
+      </c>
+      <c r="H711" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 04/02/26 || Desenvolvedor Back-end Sênior || Responsabilidades e requisitos: •Atuação principal em projetos de meios de pagamento, incluindo PIX (estático, dinâmico e automático), análise de dados e integrações com gateways como GetNet, Cielo e Stone. •Conhecimento sólido em .NET, Clean Code, SOLID, TDD e DDD. •Experiência prévia em empresas de pagamentos, bancos, fintechs ou consultorias do setor financeiro será altamente valorizada. •Perfil colaborativo, boa comunicação e maturidade para atuação em ambiente remoto. •Diferencial para quem já atuou com integração de sistemas, arquivos Febraban, transações em tempo real, análise de risco e prevenção a fraudes. •Espera-se senioridade técnica comprovada, autonomia e capacidade de adaptação a diferentes tribos e squads de tecnologia. || Empresa .....:  Farol plus (Consultoria de RH)</t>
+        </is>
+      </c>
+      <c r="I711" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>04/02/2026</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t>83047</t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>Desenvolvedor Full Stack - JAVA</t>
+        </is>
+      </c>
+      <c r="D712" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E712" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F712" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 04/02/26</t>
+        </is>
+      </c>
+      <c r="G712" t="inlineStr">
+        <is>
+          <t>A Pentacom IT Solutions, há mais de 20 anos no mercado, busca Desenvolvedor Full Stack -J AVA:  Requisitos e Conhecimentos Essenciais: - Experiência em Java (versão 8+), Spring framework (Springboot , Spring Cloud , Spring Batch) - Experiência em Angular (versão 8+, 20, 21) , CSS , TypeScript - Conhecimento em Jenkins e GitLab - Desejável conhecimento nos bancos de dados Oracle e MongoDB - Conhecimento em processos e ferramentas de automação de testes (Junit, Jasmine, Karma) - Desejável conhecimento em Openshift, Docker, Kubernetes, Kafka, Rabbit MQ - Desejável conhecimento em Redis - Experiência com integrações nos formatos de contrato: Swagger / Yaml - Experiência no desenvolvimento de micro serviços - Conhecimento de metodologia Ágil / Scrum - Conhecimento das práticas DevSecOps.  Período: Indeterminado Início: Imediato Contratação: CLT Atuação: Home Office  Profissionais interessados, enviar currículo informando disponibilidade para início
+Empresa .....:  Pentacom IT Solutions</t>
+        </is>
+      </c>
+      <c r="H712" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 04/02/26 || Desenvolvedor Full Stack - JAVA || A Pentacom IT Solutions, há mais de 20 anos no mercado, busca Desenvolvedor Full Stack -J AVA:  Requisitos e Conhecimentos Essenciais: - Experiência em Java (versão 8+), Spring framework (Springboot , Spring Cloud , Spring Batch) - Experiência em Angular (versão 8+, 20, 21) , CSS , TypeScript - Conhecimento em Jenkins e GitLab - Desejável conhecimento nos bancos de dados Oracle e MongoDB - Conhecimento em processos e ferramentas de automação de testes (Junit, Jasmine, Karma) - Desejável conhecimento em Openshift, Docker, Kubernetes, Kafka, Rabbit MQ - Desejável conhecimento em Redis - Experiência com integrações nos formatos de contrato: Swagger / Yaml - Experiência no desenvolvimento de micro serviços - Conhecimento de metodologia Ágil / Scrum - Conhecimento das práticas DevSecOps.  Período: Indeterminado Início: Imediato Contratação: CLT Atuação: Home Office  Profissionais interessados, enviar currículo informando disponibilidade para início || Empresa .....:  Pentacom IT Solutions</t>
+        </is>
+      </c>
+      <c r="I712" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>04/02/2026</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>82741</t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>Desenvolvedor Java Sênior</t>
+        </is>
+      </c>
+      <c r="D713" t="inlineStr">
+        <is>
+          <t>Sênior</t>
+        </is>
+      </c>
+      <c r="E713" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F713" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 04/02/26</t>
+        </is>
+      </c>
+      <c r="G713" t="inlineStr">
+        <is>
+          <t>Estamos em busca de um(a) Desenvolvedor(a) Java Back-end experiente para integrar nossa Squad de Negócios Digitais. Procuramos um profissional com forte atuação em Spring Boot e conhecimentos sólidos em Spring WebFlowm, WebFlux e programação reativa.  Requisitos e Conhecimentos Essenciais:  Linguagens e Frameworks: Forte experiência em Java (versão 17 ou superior) e Spring Boot. Conhecimentos em Spring WebFlux e programação reativa são diferenciais importantes.  Testes: Experiência com testes em Java e familiaridade com Cucumber. DevOps e Ferramentas: Conhecimento em Jenkins (CI/CD), Docker, Redis e sistemas de mensageria. Monitoramento e Observabilidade: Familiaridade com ferramentas de monitoramento e observabilidade.  Metodologias Ágeis: Experiência com Scrum e/ou Kanban.  Modalidade: CLT Local: Home Office
+Empresa .....:  Taking Results e Informatica Ltda</t>
+        </is>
+      </c>
+      <c r="H713" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 04/02/26 || Desenvolvedor Java Sênior || Estamos em busca de um(a) Desenvolvedor(a) Java Back-end experiente para integrar nossa Squad de Negócios Digitais. Procuramos um profissional com forte atuação em Spring Boot e conhecimentos sólidos em Spring WebFlowm, WebFlux e programação reativa.  Requisitos e Conhecimentos Essenciais:  Linguagens e Frameworks: Forte experiência em Java (versão 17 ou superior) e Spring Boot. Conhecimentos em Spring WebFlux e programação reativa são diferenciais importantes.  Testes: Experiência com testes em Java e familiaridade com Cucumber. DevOps e Ferramentas: Conhecimento em Jenkins (CI/CD), Docker, Redis e sistemas de mensageria. Monitoramento e Observabilidade: Familiaridade com ferramentas de monitoramento e observabilidade.  Metodologias Ágeis: Experiência com Scrum e/ou Kanban.  Modalidade: CLT Local: Home Office || Empresa .....:  Taking Results e Informatica Ltda</t>
+        </is>
+      </c>
+      <c r="I713" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>04/02/2026</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>82774</t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>Desenvolvedor PL SQL</t>
+        </is>
+      </c>
+      <c r="D714" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E714" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F714" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 04/02/26</t>
+        </is>
+      </c>
+      <c r="G714" t="inlineStr">
+        <is>
+          <t>Graduação em curso de nível superior em TI Experiência sólida em PL/SQL (Oracle): criação de packages, procedures, otimização de queries e tunning. Experiência com ETL e processos de tratamento de dados. Conhecimento em modelagem de bancos relacionais. Habilidade com análise, debugging e resolução de incidentes em rotinas de dados. Experiência prévia como Analista de Sistemas/Desenvolvedor ou Analista de Dados. Boa comunicação e capacidade de interação com times multidisciplinares. Capacidade de trabalhar de forma autônoma e organizada. #8203  Remoto contratação PJ
+Empresa .....:  TO Brasil</t>
+        </is>
+      </c>
+      <c r="H714" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 04/02/26 || Desenvolvedor PL SQL || Graduação em curso de nível superior em TI Experiência sólida em PL/SQL (Oracle): criação de packages, procedures, otimização de queries e tunning. Experiência com ETL e processos de tratamento de dados. Conhecimento em modelagem de bancos relacionais. Habilidade com análise, debugging e resolução de incidentes em rotinas de dados. Experiência prévia como Analista de Sistemas/Desenvolvedor ou Analista de Dados. Boa comunicação e capacidade de interação com times multidisciplinares. Capacidade de trabalhar de forma autônoma e organizada. #8203  Remoto contratação PJ || Empresa .....:  TO Brasil</t>
+        </is>
+      </c>
+      <c r="I714" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>04/02/2026</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>82842</t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>Desenvolvedor(a) Fullstack .NET Core / Angular</t>
+        </is>
+      </c>
+      <c r="D715" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E715" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F715" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 04/02/26</t>
+        </is>
+      </c>
+      <c r="G715" t="inlineStr">
+        <is>
+          <t>A 200DEV é uma consultoria de TI focada em Inovação e Transformação Digital, utilizando tecnologias de ponta e profissionais orientados a resultados.  VAGA REMOTA: Desenvolvedor(a) Fullstack .NET Core / Angular Sênior  REQUISITOS OBRIGATÓRIOS: Exp. em desenvolvimento com .NET Core (C#). Conhecimento avançado em Angular (versão 8 ou superior). Domínio de Entity Framework, Dapper e LINQ. Exp. no desenvolvimento de APIs REST. Conhecimento em bancos de dados relacionais, especialmente Oracle. Conhecimento em Arquitetura de Software, Design Patterns e Boas Práticas. Exp.com Controle de Versão (Git, etc.). Exp. com pelo menos uma das plataformas de Cloud Computing (Azure, AWS, Google Cloud). Exp.com Metodologias Ágeis (Scrum, Kanban).  Modelo: Remoto Contratação: PJ
+Empresa .....:  200DEV SVCS LTDA.</t>
+        </is>
+      </c>
+      <c r="H715" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 04/02/26 || Desenvolvedor(a) Fullstack .NET Core / Angular || A 200DEV é uma consultoria de TI focada em Inovação e Transformação Digital, utilizando tecnologias de ponta e profissionais orientados a resultados.  VAGA REMOTA: Desenvolvedor(a) Fullstack .NET Core / Angular Sênior  REQUISITOS OBRIGATÓRIOS: Exp. em desenvolvimento com .NET Core (C#). Conhecimento avançado em Angular (versão 8 ou superior). Domínio de Entity Framework, Dapper e LINQ. Exp. no desenvolvimento de APIs REST. Conhecimento em bancos de dados relacionais, especialmente Oracle. Conhecimento em Arquitetura de Software, Design Patterns e Boas Práticas. Exp.com Controle de Versão (Git, etc.). Exp. com pelo menos uma das plataformas de Cloud Computing (Azure, AWS, Google Cloud). Exp.com Metodologias Ágeis (Scrum, Kanban).  Modelo: Remoto Contratação: PJ || Empresa .....:  200DEV SVCS LTDA.</t>
+        </is>
+      </c>
+      <c r="I715" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>04/02/2026</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>82180</t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>Engenheiro de Dados</t>
+        </is>
+      </c>
+      <c r="D716" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E716" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F716" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 04/02/26</t>
+        </is>
+      </c>
+      <c r="G716" t="inlineStr">
+        <is>
+          <t>Engenheiro de Dados Disponibilidade imediata Contratação PJ Período estimado de 06 a 12 meses (podendo ser prorrogado) Atuação Remoto  Experiência comprovada em projetos usando IA ( MLs, deep learning, LLMs) Engajamento, senso de dono, comunicação, capacidade de traduzir problemas de negócio em soluções praticas, fazer apresentações gerenciais, comunicação e trabalho em equipe.
+Empresa .....:  THERA CONSULTING</t>
+        </is>
+      </c>
+      <c r="H716" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 04/02/26 || Engenheiro de Dados || Engenheiro de Dados Disponibilidade imediata Contratação PJ Período estimado de 06 a 12 meses (podendo ser prorrogado) Atuação Remoto  Experiência comprovada em projetos usando IA ( MLs, deep learning, LLMs) Engajamento, senso de dono, comunicação, capacidade de traduzir problemas de negócio em soluções praticas, fazer apresentações gerenciais, comunicação e trabalho em equipe. || Empresa .....:  THERA CONSULTING</t>
+        </is>
+      </c>
+      <c r="I716" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>04/02/2026</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t>83573</t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>Gerente de Configuração e Mudança</t>
+        </is>
+      </c>
+      <c r="D717" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E717" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F717" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 04/02/26</t>
+        </is>
+      </c>
+      <c r="G717" t="inlineStr">
+        <is>
+          <t>Gerenciar os processos de Configuração e Mudança, assegurando aderência às boas práticas de ITIL. Planejar, avaliar, aprovar e acompanhar mudanças em ambientes Mainframe (z/OS). Garantir a integridade da CMDB, mantendo informações atualizadas e confiáveis. Experiência em ambientes de missão crítica (bancos, seguradoras, telecom, etc.). Forte atuação em ambientes Mainframe (z/OS, JCL, CICS, DB2, IMS, entre outros) Superior completo em cursos relacionados a TI Atuação Totalmente remota
+Empresa .....:  Spassu Tecnologia</t>
+        </is>
+      </c>
+      <c r="H717" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 04/02/26 || Gerente de Configuração e Mudança || Gerenciar os processos de Configuração e Mudança, assegurando aderência às boas práticas de ITIL. Planejar, avaliar, aprovar e acompanhar mudanças em ambientes Mainframe (z/OS). Garantir a integridade da CMDB, mantendo informações atualizadas e confiáveis. Experiência em ambientes de missão crítica (bancos, seguradoras, telecom, etc.). Forte atuação em ambientes Mainframe (z/OS, JCL, CICS, DB2, IMS, entre outros) Superior completo em cursos relacionados a TI Atuação Totalmente remota || Empresa .....:  Spassu Tecnologia</t>
+        </is>
+      </c>
+      <c r="I717" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>04/02/2026</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t>83576</t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>Gerente de Projetos</t>
+        </is>
+      </c>
+      <c r="D718" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E718" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F718" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 04/02/26</t>
+        </is>
+      </c>
+      <c r="G718" t="inlineStr">
+        <is>
+          <t>Requisitos: Graduação completa na área de Tecnologia da Informação, ou conclusão de qualquer curso superior acompanhado de certificado de curso de pós graduação (especialização, mestrado ou doutorado) na área de Tecnologia da Informação de, no mínimo, 360 horas.  Experiência comprovada com atuação em gestão de projetos de tecnologia, com liderança de equipes técnicas, planejamento de entregas e acompanhamento de escopo, custo, prazo e qualidade.  CONHECIMENTOS: Ter background técnico, experiência em projetos de desenvolvimento Experiência em Gerência de Projetos com base em PMBOK ou equivalente Métodos ágeis: Scrum, SAFe, Lean Kanban, Lean Startup Ferramentas: Jira, Confluence, MS Project, Planner, Trello ou equivalentes Técnicas de análise de valor agregado, EAP, curva S, matriz de stakeholders Noções de DevOps e integração continua Gestão de backlog e priorização em ciclos iterative.  Contratação CLT + benefícios  Favor enviar pretensão salarial CL
+Empresa .....:  Spassu</t>
+        </is>
+      </c>
+      <c r="H718" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 04/02/26 || Gerente de Projetos || Requisitos: Graduação completa na área de Tecnologia da Informação, ou conclusão de qualquer curso superior acompanhado de certificado de curso de pós graduação (especialização, mestrado ou doutorado) na área de Tecnologia da Informação de, no mínimo, 360 horas.  Experiência comprovada com atuação em gestão de projetos de tecnologia, com liderança de equipes técnicas, planejamento de entregas e acompanhamento de escopo, custo, prazo e qualidade.  CONHECIMENTOS: Ter background técnico, experiência em projetos de desenvolvimento Experiência em Gerência de Projetos com base em PMBOK ou equivalente Métodos ágeis: Scrum, SAFe, Lean Kanban, Lean Startup Ferramentas: Jira, Confluence, MS Project, Planner, Trello ou equivalentes Técnicas de análise de valor agregado, EAP, curva S, matriz de stakeholders Noções de DevOps e integração continua Gestão de backlog e priorização em ciclos iterative.  Contratação CLT + benefícios  Favor enviar pretensão salarial CL || Empresa .....:  Spassu</t>
+        </is>
+      </c>
+      <c r="I718" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>04/02/2026</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>82537</t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>Support Operations Junior  c/ Inglês - Remoto</t>
+        </is>
+      </c>
+      <c r="D719" t="inlineStr">
+        <is>
+          <t>Júnior</t>
+        </is>
+      </c>
+      <c r="E719" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F719" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 04/02/26</t>
+        </is>
+      </c>
+      <c r="G719" t="inlineStr">
+        <is>
+          <t>Support Operations Junior Remoto Contrato com prestação de serviços PJ Inglês  avançado Support Operations Junior  Fornecer suporte técnico de nível especializado para o conjunto de aplicativos, abordando problemas de usuários, solucionando incidentes e garantindo resolução oportuna para manter a alta disponibilidade do sistema.  Desenvolver planos de ação preventivos para atender as métricas dos Indicadores Chave de Desempenho (KPIs) e dos Acordos de Nível de Serviço (SLAs). Responsável por manter a documentação precisa do sistema enquanto segue as regulamentações Sarbanes-Oxley (SOX).  Gerenciar e solucionar problemas de sistemas de transporte de telemetria de enfileiramento de mensagens, garantindo comunicação de dados confiável e eficiente.  Mantenha integrações de mensagens com o Azure Service Bus e o EventHub, garantindo que os dados fluam de maneira suave e segura entre os sistemas. Utilização do Datadog para análise de registros e monitores
+Empresa .....:  k2 partnering Solutions</t>
+        </is>
+      </c>
+      <c r="H719" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 04/02/26 || Support Operations Junior  c/ Inglês - Remoto || Support Operations Junior Remoto Contrato com prestação de serviços PJ Inglês  avançado Support Operations Junior  Fornecer suporte técnico de nível especializado para o conjunto de aplicativos, abordando problemas de usuários, solucionando incidentes e garantindo resolução oportuna para manter a alta disponibilidade do sistema.  Desenvolver planos de ação preventivos para atender as métricas dos Indicadores Chave de Desempenho (KPIs) e dos Acordos de Nível de Serviço (SLAs). Responsável por manter a documentação precisa do sistema enquanto segue as regulamentações Sarbanes-Oxley (SOX).  Gerenciar e solucionar problemas de sistemas de transporte de telemetria de enfileiramento de mensagens, garantindo comunicação de dados confiável e eficiente.  Mantenha integrações de mensagens com o Azure Service Bus e o EventHub, garantindo que os dados fluam de maneira suave e segura entre os sistemas. Utilização do Datadog para análise de registros e monitores || Empresa .....:  k2 partnering Solutions</t>
+        </is>
+      </c>
+      <c r="I719" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>04/02/2026</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>83572</t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>Estágio de Suporte</t>
+        </is>
+      </c>
+      <c r="D720" t="inlineStr">
+        <is>
+          <t>Estágio</t>
+        </is>
+      </c>
+      <c r="E720" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F720" t="inlineStr">
+        <is>
+          <t>Osasco - SP - 04/02/26</t>
+        </is>
+      </c>
+      <c r="G720" t="inlineStr">
+        <is>
+          <t>REQUISITOS: Ensino Superior em cursos da área de TI. Disponibilidade para trabalhar 30 horas semanais, em formato presencial, das 08:00 às 14:00.  Conhecimentos desejados: Windows Gerenciamento de logins Gerenciamento de impressora Conhecimento no arquivo XML. Excel - Básico Gramática.  LOCAL: Escritório CBTECH - Osasco - Centro (Próximo à estação de trem Osasco)  BOLSA: R$ 1.000,00 + Auxílio-transporte  AÇÕES: - Auxiliar nas  demandas do suporte  em geral - Realizar atividades específicas ou massiva - Gerenciamento de itens de configuração.  SOFT SKILLS: - Boa comunicação - Proatividade - Trabalho em equipe - Organização
+Empresa .....:  COCO BAMBU RESTAURANTES</t>
+        </is>
+      </c>
+      <c r="H720" t="inlineStr">
+        <is>
+          <t>Osasco - SP - 04/02/26 || Estágio de Suporte || REQUISITOS: Ensino Superior em cursos da área de TI. Disponibilidade para trabalhar 30 horas semanais, em formato presencial, das 08:00 às 14:00.  Conhecimentos desejados: Windows Gerenciamento de logins Gerenciamento de impressora Conhecimento no arquivo XML. Excel - Básico Gramática.  LOCAL: Escritório CBTECH - Osasco - Centro (Próximo à estação de trem Osasco)  BOLSA: R$ 1.000,00 + Auxílio-transporte  AÇÕES: - Auxiliar nas  demandas do suporte  em geral - Realizar atividades específicas ou massiva - Gerenciamento de itens de configuração.  SOFT SKILLS: - Boa comunicação - Proatividade - Trabalho em equipe - Organização || Empresa .....:  COCO BAMBU RESTAURANTES</t>
+        </is>
+      </c>
+      <c r="I720" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>04/02/2026</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t>82232</t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>Gerente de Projetos Pleno</t>
+        </is>
+      </c>
+      <c r="D721" t="inlineStr">
+        <is>
+          <t>Pleno</t>
+        </is>
+      </c>
+      <c r="E721" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F721" t="inlineStr">
+        <is>
+          <t>Paranapanema - SP - 04/02/26</t>
+        </is>
+      </c>
+      <c r="G721" t="inlineStr">
+        <is>
+          <t>WA FENIX contrata: Gerente de Projetos  Requisitos: Experiência como PMO ou com gerenciamento de projetos são bem vistas Necessário experiência com projetos de implantação SAP e do S4/hana Conhecimentos com Solution Manager,  ALM e Clean Core Necessário boa postura, boa comunicação e iniciativa  Local: Região de Avaré - SP - presencial Duração da contratação: 12 meses, podendo renovar, visto que projeto vai até Março 2028.
+Empresa .....:  WA FENIX IT SERVICES  SOLUTIONS</t>
+        </is>
+      </c>
+      <c r="H721" t="inlineStr">
+        <is>
+          <t>Paranapanema - SP - 04/02/26 || Gerente de Projetos Pleno || WA FENIX contrata: Gerente de Projetos  Requisitos: Experiência como PMO ou com gerenciamento de projetos são bem vistas Necessário experiência com projetos de implantação SAP e do S4/hana Conhecimentos com Solution Manager,  ALM e Clean Core Necessário boa postura, boa comunicação e iniciativa  Local: Região de Avaré - SP - presencial Duração da contratação: 12 meses, podendo renovar, visto que projeto vai até Março 2028. || Empresa .....:  WA FENIX IT SERVICES  SOLUTIONS</t>
+        </is>
+      </c>
+      <c r="I721" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>04/02/2026</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>82228</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>Analista de Suporte Pleno</t>
+        </is>
+      </c>
+      <c r="D722" t="inlineStr">
+        <is>
+          <t>Pleno</t>
+        </is>
+      </c>
+      <c r="E722" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F722" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro - RJ - 04/02/26</t>
+        </is>
+      </c>
+      <c r="G722" t="inlineStr">
+        <is>
+          <t>Realizar suporte técnico Nível 1 e Nível 2 ao usuário final, provendo soluções para incidentes e problemas em estações de trabalho Windows, Linux e MacOS e periféricos, como pacote Office e outros softwares Atender pronta e corretamente as solicitações dos clientes, registrando e acompanhando os chamados do início ao fim procurando sempre a melhor solução Manter atualizados os procedimentos técnicos Manter-se atualizado, lendo procedimentos operacionais, participando de reuniões, treinamentos, certificações e outros Manter atualizada a base de conhecimento: Acompanhar a revisão e atualização dos procedimentos operacionais (documentos), pesquisando novas soluções, analisando criticamente os processos e propondo melhorias Tratar as solicitações de serviço de forma rápida e eficiente, garantindo a satisfação dos clientes Interagir com outros colaboradores para resolução, tratativa e acompanhamento das solicitações pelo Cliente, incluindo equipes de servidores e redes
+Empresa .....:  RCV Soluções Tecnológicas LTDA</t>
+        </is>
+      </c>
+      <c r="H722" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro - RJ - 04/02/26 || Analista de Suporte Pleno || Realizar suporte técnico Nível 1 e Nível 2 ao usuário final, provendo soluções para incidentes e problemas em estações de trabalho Windows, Linux e MacOS e periféricos, como pacote Office e outros softwares Atender pronta e corretamente as solicitações dos clientes, registrando e acompanhando os chamados do início ao fim procurando sempre a melhor solução Manter atualizados os procedimentos técnicos Manter-se atualizado, lendo procedimentos operacionais, participando de reuniões, treinamentos, certificações e outros Manter atualizada a base de conhecimento: Acompanhar a revisão e atualização dos procedimentos operacionais (documentos), pesquisando novas soluções, analisando criticamente os processos e propondo melhorias Tratar as solicitações de serviço de forma rápida e eficiente, garantindo a satisfação dos clientes Interagir com outros colaboradores para resolução, tratativa e acompanhamento das solicitações pelo Cliente, incluindo equipes de servidores e redes || Empresa .....:  RCV Soluções Tecnológicas LTDA</t>
+        </is>
+      </c>
+      <c r="I722" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>04/02/2026</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t>82424</t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>Gerente de Programa (Agile e Waterfall)</t>
+        </is>
+      </c>
+      <c r="D723" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E723" t="inlineStr">
+        <is>
+          <t>Híbrido</t>
+        </is>
+      </c>
+      <c r="F723" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro - RJ - 04/02/26</t>
+        </is>
+      </c>
+      <c r="G723" t="inlineStr">
+        <is>
+          <t>Governança Estratégica Liderar o planejamento e evolução do programa Direcionar decisões do portfólio e do fórum de priorização Alinhar demandas com os objetivos estratégicos da empresa Trabalhar em sinergia com os Gerentes de Projetos das áreas envolvidas no Programa Atuar de maneira holística e consolidadora sobre as informações de projetos/programas Gestão de Interdependências Atuar como facilitador dos impedimentos entre projetos Apoiar o alinhamento entre executivos de negócios e TI Coordenar e comunicar a evolução do programa.  Gestão de Benefícios Garantir que projetos e features contribuam para o sucesso do programa Monitorar KPIs Atuar como líder estratégico para entrega de resultados de alta qualidade Comunicação Executiva Manter comunicação clara com stakeholders e patrocinadores Reportar status Acompanhar o Programa até sua entrega  Sólido Conhecimento de metodologia Agil e Preditiva. Azure Boards, Service Now e Ms Project  Botafogo - Hibrido / PJ
+Empresa .....:  GlobalTI</t>
+        </is>
+      </c>
+      <c r="H723" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro - RJ - 04/02/26 || Gerente de Programa (Agile e Waterfall) || Governança Estratégica Liderar o planejamento e evolução do programa Direcionar decisões do portfólio e do fórum de priorização Alinhar demandas com os objetivos estratégicos da empresa Trabalhar em sinergia com os Gerentes de Projetos das áreas envolvidas no Programa Atuar de maneira holística e consolidadora sobre as informações de projetos/programas Gestão de Interdependências Atuar como facilitador dos impedimentos entre projetos Apoiar o alinhamento entre executivos de negócios e TI Coordenar e comunicar a evolução do programa.  Gestão de Benefícios Garantir que projetos e features contribuam para o sucesso do programa Monitorar KPIs Atuar como líder estratégico para entrega de resultados de alta qualidade Comunicação Executiva Manter comunicação clara com stakeholders e patrocinadores Reportar status Acompanhar o Programa até sua entrega  Sólido Conhecimento de metodologia Agil e Preditiva. Azure Boards, Service Now e Ms Project  Botafogo - Hibrido / PJ || Empresa .....:  GlobalTI</t>
+        </is>
+      </c>
+      <c r="I723" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>04/02/2026</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t>82495</t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>Técnico em informática</t>
+        </is>
+      </c>
+      <c r="D724" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E724" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F724" t="inlineStr">
+        <is>
+          <t>São Bernardo do Campo - SP - 04/02/26</t>
+        </is>
+      </c>
+      <c r="G724" t="inlineStr">
+        <is>
+          <t>Técnico de Helpdesk N1 (Presencial – Alocado no Cliente)
+Horário: Segunda a sexta, 9h às 18h
+Local: Presencial – necessário residir no ABC
+Salário: R$ 2.500 + R$ 500 de ajuda de custo
+Buscamos um Técnico de Helpdesk N1 para atendimento inicial aos clientes, atuando
+presencialmente e remotamente na abertura e acompanhamento de chamados via GLPI, resolução de
+incidentes de primeiro nível e encaminhamento de casos ao N2 quando necessário.
+Responsabilidades:
+– Atendimento presencial e remoto;
+– Registro e acompanhamento de tickets no GLPI;
+– Suporte a Windows, Office 365, redes, hardware e software;
+– Instalação e configuração de computadores, impressoras e periféricos;
+– Manter comunicação clara e profissional.
+Conhecimentos necessários:
+Windows, Office 365, redes (IP, DNS), GLPI, atendimento remoto, Active Directory básico,
+manutenção de computadores, suporte a impressoras.
+Requisitos:
+Residir no ABC, ensino médio completo e experiência prévia em suporte técnico (diferencial).
+Empresa .....:  Confitec Tecnologia</t>
+        </is>
+      </c>
+      <c r="H724" t="inlineStr">
+        <is>
+          <t>São Bernardo do Campo - SP - 04/02/26 || Técnico em informática || Técnico de Helpdesk N1 (Presencial – Alocado no Cliente) || Horário: Segunda a sexta, 9h às 18h || Local: Presencial – necessário residir no ABC || Salário: R$ 2.500 + R$ 500 de ajuda de custo || Buscamos um Técnico de Helpdesk N1 para atendimento inicial aos clientes, atuando || presencialmente e remotamente na abertura e acompanhamento de chamados via GLPI, resolução de || incidentes de primeiro nível e encaminhamento de casos ao N2 quando necessário. || Responsabilidades: || – Atendimento presencial e remoto; || – Registro e acompanhamento de tickets no GLPI; || – Suporte a Windows, Office 365, redes, hardware e software; || – Instalação e configuração de computadores, impressoras e periféricos; || – Manter comunicação clara e profissional. || Conhecimentos necessários: || Windows, Office 365, redes (IP, DNS), GLPI, atendimento remoto, Active Directory básico, || manutenção de computadores, suporte a impressoras. || Requisitos: || Residir no ABC, ensino médio completo e experiência prévia em suporte técnico (diferencial). || Empresa .....:  Confitec Tecnologia</t>
+        </is>
+      </c>
+      <c r="I724" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>04/02/2026</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t>82287</t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>Analista Cloud - AWS</t>
+        </is>
+      </c>
+      <c r="D725" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E725" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F725" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 04/02/26</t>
+        </is>
+      </c>
+      <c r="G725" t="inlineStr">
+        <is>
+          <t>Buscamos um(a) Analista Cloud com sólida experiência em ambientes críticos e de alta disponibilidade, para atuar na sustentação, monitoramento e otimização de soluções em AWS. Esse(a) profissional será responsável por garantir estabilidade, segurança e performance das aplicações em nuvem, além de apoiar a evolução da arquitetura e das boas práticas de operação em ambientes produtivos. Administrar, monitorar e otimizar ambientes em AWS (EC2, S3, RDS, Lambda, ECS, CloudWatch, entre outros)  Implementar políticas de backup, recuperação e alta disponibilidade  Garantir resiliência, escalabilidade e segurança dos sistemas críticos  Automatizar processos de infraestrutura  Atuar em incidentes, problemas e mudanças, seguindo boas práticas de ITIL  Apoiar times de desenvolvimento e operações na melhoria contínua do ambiente  Gerenciar custos em AWS, propondo otimizações de recursos  Documentar procedimentos
+Empresa .....:  KYMO TECNOLOGIA E INOVAÇÃO EIRELI</t>
+        </is>
+      </c>
+      <c r="H725" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 04/02/26 || Analista Cloud - AWS || Buscamos um(a) Analista Cloud com sólida experiência em ambientes críticos e de alta disponibilidade, para atuar na sustentação, monitoramento e otimização de soluções em AWS. Esse(a) profissional será responsável por garantir estabilidade, segurança e performance das aplicações em nuvem, além de apoiar a evolução da arquitetura e das boas práticas de operação em ambientes produtivos. Administrar, monitorar e otimizar ambientes em AWS (EC2, S3, RDS, Lambda, ECS, CloudWatch, entre outros)  Implementar políticas de backup, recuperação e alta disponibilidade  Garantir resiliência, escalabilidade e segurança dos sistemas críticos  Automatizar processos de infraestrutura  Atuar em incidentes, problemas e mudanças, seguindo boas práticas de ITIL  Apoiar times de desenvolvimento e operações na melhoria contínua do ambiente  Gerenciar custos em AWS, propondo otimizações de recursos  Documentar procedimentos || Empresa .....:  KYMO TECNOLOGIA E INOVAÇÃO EIRELI</t>
+        </is>
+      </c>
+      <c r="I725" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>04/02/2026</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t>82358</t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>Analista de Business Intelligence</t>
+        </is>
+      </c>
+      <c r="D726" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E726" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F726" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 04/02/26</t>
+        </is>
+      </c>
+      <c r="G726" t="inlineStr">
+        <is>
+          <t>•	Levantar e entender necessidades de informação junto às áreas de negócio •	Extrair, tratar e consolidar dados de diferentes fontes (ERP, CRM, sistemas internos, etc.) •	Desenvolver, manter e aprimorar dashboards e relatórios gerenciais (ex: Power BI, Tableau) •	Garantir a qualidade, consistência e integridade dos dados •	Realizar análises exploratórias e diagnósticas para identificar tendências, padrões e oportunidades de melhoria •	Apoiar a definição de indicadores de desempenho (KPIs) e metas •	Automatizar processos de coleta e atualização de dados •	 Power BI (preferencial), Tableau...... QuickSight •	Raciocínio analítico e visão sistêmica •	Atenção a detalhes e qualidade das informações •	Boa comunicação e capacidade de traduzir dados em insights de negócio •	Proatividade e curiosidade para explorar dados e propor soluções •	Capacidade de trabalhar de forma colaborativa  Salário R$ 9.000,00 CLT PRESENCIAL + AMédica  AOdonto SVida VR e VT
+Empresa .....:  QUI VAGAS CONSULTORIA DE RH</t>
+        </is>
+      </c>
+      <c r="H726" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 04/02/26 || Analista de Business Intelligence || •	Levantar e entender necessidades de informação junto às áreas de negócio •	Extrair, tratar e consolidar dados de diferentes fontes (ERP, CRM, sistemas internos, etc.) •	Desenvolver, manter e aprimorar dashboards e relatórios gerenciais (ex: Power BI, Tableau) •	Garantir a qualidade, consistência e integridade dos dados •	Realizar análises exploratórias e diagnósticas para identificar tendências, padrões e oportunidades de melhoria •	Apoiar a definição de indicadores de desempenho (KPIs) e metas •	Automatizar processos de coleta e atualização de dados •	 Power BI (preferencial), Tableau...... QuickSight •	Raciocínio analítico e visão sistêmica •	Atenção a detalhes e qualidade das informações •	Boa comunicação e capacidade de traduzir dados em insights de negócio •	Proatividade e curiosidade para explorar dados e propor soluções •	Capacidade de trabalhar de forma colaborativa  Salário R$ 9.000,00 CLT PRESENCIAL + AMédica  AOdonto SVida VR e VT || Empresa .....:  QUI VAGAS CONSULTORIA DE RH</t>
+        </is>
+      </c>
+      <c r="I726" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>04/02/2026</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>82222</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>Analista de Infraestrura Sênior</t>
+        </is>
+      </c>
+      <c r="D727" t="inlineStr">
+        <is>
+          <t>Sênior</t>
+        </is>
+      </c>
+      <c r="E727" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F727" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 04/02/26</t>
+        </is>
+      </c>
+      <c r="G727" t="inlineStr">
+        <is>
+          <t>Analista de Infraestrura Sênior (Inglês Avançado)  Experiência em plataformas/operações em cloud (preferencialmente na plataforma OCI GEN2) Administração/gestão de ambiente Cloud Alocação de recursos Criação, configuração e gerenciamento de VMs Windows/Linux (VMs da OCI-Gen2 ou dentro de servidores bare metal) Procedimentos de snapshot/backup Configuração de rede na camada do IAAS Administração de Redes Windows Linux - Oracle Linux, Ubuntu, Debian Realizar troubleshooting de problemas relacionadas à rede e a infraestrutura Administração de proxy cache e reverso (Apache/Squid) Administração de Redes Windows Server Windows/Linux Gestão de Firewalls (IPtables) Virtualização por meio de KVM Criar e manter túneis VPN (Ipsec) Microsoft Active Directory Criar, Editar e Implementar GPOs Microsoft IIS Microsoft Windows TS Implantação, administração e manutenção de Microsofoft WSUS Aplicar atualizações e hoftotfix Implantação de Monitoramento de ambiente com Zabbix
+Empresa .....:  Entrust It</t>
+        </is>
+      </c>
+      <c r="H727" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 04/02/26 || Analista de Infraestrura Sênior || Analista de Infraestrura Sênior (Inglês Avançado)  Experiência em plataformas/operações em cloud (preferencialmente na plataforma OCI GEN2) Administração/gestão de ambiente Cloud Alocação de recursos Criação, configuração e gerenciamento de VMs Windows/Linux (VMs da OCI-Gen2 ou dentro de servidores bare metal) Procedimentos de snapshot/backup Configuração de rede na camada do IAAS Administração de Redes Windows Linux - Oracle Linux, Ubuntu, Debian Realizar troubleshooting de problemas relacionadas à rede e a infraestrutura Administração de proxy cache e reverso (Apache/Squid) Administração de Redes Windows Server Windows/Linux Gestão de Firewalls (IPtables) Virtualização por meio de KVM Criar e manter túneis VPN (Ipsec) Microsoft Active Directory Criar, Editar e Implementar GPOs Microsoft IIS Microsoft Windows TS Implantação, administração e manutenção de Microsofoft WSUS Aplicar atualizações e hoftotfix Implantação de Monitoramento de ambiente com Zabbix || Empresa .....:  Entrust It</t>
+        </is>
+      </c>
+      <c r="I727" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>04/02/2026</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>82409</t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>Analista de Infraestrutura Sênior</t>
+        </is>
+      </c>
+      <c r="D728" t="inlineStr">
+        <is>
+          <t>Sênior</t>
+        </is>
+      </c>
+      <c r="E728" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F728" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 04/02/26</t>
+        </is>
+      </c>
+      <c r="G728" t="inlineStr">
+        <is>
+          <t>Experiência Técnica: Foco em implementação de projetos. Experiência na área de tecnologia, preferencialmente na área bancária/financeira. Administração de Windows Server (desejável/diferencial ter Certificação). Administração de Linux Server (RedHat). Básico de Telecom (Switches, Roteadores, Vlan, Link de Dados) - Telecom (manutenção de terminais IPC e testes de gravações Verint). DFS. Citrix e Virtualização (Vmware / Oracle OLVM). Ferramentas de backup: Veeam. Ferramentas de e-mail e ferramentas de monitoramento como: SCOM, HPOpenView for Linux, Fluke NetFlow, Cacti e NNMi. SCCM. Administração de Storage / servidores Blades. Noções de Cloud.  DESEJÁVEL certificação ITIL V3.  Formação Acadêmica: Superior Completo.  Idioma: Inglês avançado para conversação. Disponibilidade para trabalhar eventualmente fora do horário comercial e final de semana.  Observações: Local de trabalho: Morumbi. Vaga Híbrida uma vez por semana presencial.
+Empresa .....:  Emphasys IT Services</t>
+        </is>
+      </c>
+      <c r="H728" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 04/02/26 || Analista de Infraestrutura Sênior || Experiência Técnica: Foco em implementação de projetos. Experiência na área de tecnologia, preferencialmente na área bancária/financeira. Administração de Windows Server (desejável/diferencial ter Certificação). Administração de Linux Server (RedHat). Básico de Telecom (Switches, Roteadores, Vlan, Link de Dados) - Telecom (manutenção de terminais IPC e testes de gravações Verint). DFS. Citrix e Virtualização (Vmware / Oracle OLVM). Ferramentas de backup: Veeam. Ferramentas de e-mail e ferramentas de monitoramento como: SCOM, HPOpenView for Linux, Fluke NetFlow, Cacti e NNMi. SCCM. Administração de Storage / servidores Blades. Noções de Cloud.  DESEJÁVEL certificação ITIL V3.  Formação Acadêmica: Superior Completo.  Idioma: Inglês avançado para conversação. Disponibilidade para trabalhar eventualmente fora do horário comercial e final de semana.  Observações: Local de trabalho: Morumbi. Vaga Híbrida uma vez por semana presencial. || Empresa .....:  Emphasys IT Services</t>
+        </is>
+      </c>
+      <c r="I728" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>04/02/2026</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t>82467</t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>Analista de Monitoramento</t>
+        </is>
+      </c>
+      <c r="D729" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E729" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F729" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 04/02/26</t>
+        </is>
+      </c>
+      <c r="G729" t="inlineStr">
+        <is>
+          <t>• Atender/resolver chamados clientes via telefone/e-mail/chat • Monitorar ambientes Ti através de ferramentas automáticas • Realizar análise/diagnóstico/testes p/resolução chamados e demandas • Formação Técnica/Superior completo ou em andamento p/cursos à área de TI • Inglês técnico para leitura/pesquisas em bases de conhecimento • Conhecimentos técnicos em: Windows Server, Linux, Oracle e SQLSERVER • Boa comunicação oral e escrita para trato por telefone e meios eletrônicos • Lidar bem com prazos, ter senso urgência e trabalhar sob pressão • Ser proativo, trabalhar em equipe  CONTRATACAO PJ - PRESENCIAL - ENVIAR PRETENSAO SALARIAL
+Empresa .....:  Traces Tecnologia</t>
+        </is>
+      </c>
+      <c r="H729" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 04/02/26 || Analista de Monitoramento || • Atender/resolver chamados clientes via telefone/e-mail/chat • Monitorar ambientes Ti através de ferramentas automáticas • Realizar análise/diagnóstico/testes p/resolução chamados e demandas • Formação Técnica/Superior completo ou em andamento p/cursos à área de TI • Inglês técnico para leitura/pesquisas em bases de conhecimento • Conhecimentos técnicos em: Windows Server, Linux, Oracle e SQLSERVER • Boa comunicação oral e escrita para trato por telefone e meios eletrônicos • Lidar bem com prazos, ter senso urgência e trabalhar sob pressão • Ser proativo, trabalhar em equipe  CONTRATACAO PJ - PRESENCIAL - ENVIAR PRETENSAO SALARIAL || Empresa .....:  Traces Tecnologia</t>
+        </is>
+      </c>
+      <c r="I729" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>04/02/2026</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>83186</t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>Analista de Negócios TI</t>
+        </is>
+      </c>
+      <c r="D730" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E730" t="inlineStr">
+        <is>
+          <t>Híbrido</t>
+        </is>
+      </c>
+      <c r="F730" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 04/02/26</t>
+        </is>
+      </c>
+      <c r="G730" t="inlineStr">
+        <is>
+          <t>Oportunidade em uma das maiores operadoras de saúde do Brasil  Buscamos profissional para atuar em projetos e sustentação, apoiando squads multidisciplinares, com forte interface entre negócio e tecnologia. A atuação envolve análise e priorização de demandas, suporte N1 e N2, testes, homologações e GMUDs, além de participação em projetos de evolução sistêmica e adequações regulatórias, utilizando Waterfall, Scrum e Kanban.  Modelo híbrido: presencial 2x por semana (Zona Sul de SP) Horário: 8h às 18h  PJ – 44h semanais Formação: superior em TI (completo ou cursando) Diferencial: experiência no segmento de saúde  Se você busca desafios, ambiente colaborativo e impacto nacional, essa vaga pode ser para você
+Empresa .....:  TalentGroup</t>
+        </is>
+      </c>
+      <c r="H730" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 04/02/26 || Analista de Negócios TI || Oportunidade em uma das maiores operadoras de saúde do Brasil  Buscamos profissional para atuar em projetos e sustentação, apoiando squads multidisciplinares, com forte interface entre negócio e tecnologia. A atuação envolve análise e priorização de demandas, suporte N1 e N2, testes, homologações e GMUDs, além de participação em projetos de evolução sistêmica e adequações regulatórias, utilizando Waterfall, Scrum e Kanban.  Modelo híbrido: presencial 2x por semana (Zona Sul de SP) Horário: 8h às 18h  PJ – 44h semanais Formação: superior em TI (completo ou cursando) Diferencial: experiência no segmento de saúde  Se você busca desafios, ambiente colaborativo e impacto nacional, essa vaga pode ser para você || Empresa .....:  TalentGroup</t>
+        </is>
+      </c>
+      <c r="I730" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>04/02/2026</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>82219</t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>Analista de Operações Datacenter</t>
+        </is>
+      </c>
+      <c r="D731" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E731" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F731" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 04/02/26</t>
+        </is>
+      </c>
+      <c r="G731" t="inlineStr">
+        <is>
+          <t>Analista de Operações Datacenter / Presencial - São Paulo  Responsável por executar atividades operacionais em datacenters, garantindo a instalação física de equipamentos, organização da infraestrutura, suporte a fornecedores e controle de inventário. Este profissional atuará em um ambiente dinâmico, com foco em precisão, segurança e conformidade com os padrões técnicos.  Horário de Trabalho: Segunda a sexta-feira, das 11h às 20h  Realizará deslocamentos frequentes entre os 4 datacenters da empresa, localizados em Santana de Parnaíba e São Paulo - Centro, conforme demanda das operações. Experiência prévia em ambientes de datacenter ou infraestrutura de TI. Conhecimento básico/intermediário em hardware de servidores, redes e cabeamento. Inglês intermediário (leitura de manuais, comunicação básica com fornecedores internacionais). Organização, atenção a detalhes e capacidade de seguir procedimentos técnicos.
+Empresa .....:  Mazzatech</t>
+        </is>
+      </c>
+      <c r="H731" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 04/02/26 || Analista de Operações Datacenter || Analista de Operações Datacenter / Presencial - São Paulo  Responsável por executar atividades operacionais em datacenters, garantindo a instalação física de equipamentos, organização da infraestrutura, suporte a fornecedores e controle de inventário. Este profissional atuará em um ambiente dinâmico, com foco em precisão, segurança e conformidade com os padrões técnicos.  Horário de Trabalho: Segunda a sexta-feira, das 11h às 20h  Realizará deslocamentos frequentes entre os 4 datacenters da empresa, localizados em Santana de Parnaíba e São Paulo - Centro, conforme demanda das operações. Experiência prévia em ambientes de datacenter ou infraestrutura de TI. Conhecimento básico/intermediário em hardware de servidores, redes e cabeamento. Inglês intermediário (leitura de manuais, comunicação básica com fornecedores internacionais). Organização, atenção a detalhes e capacidade de seguir procedimentos técnicos. || Empresa .....:  Mazzatech</t>
+        </is>
+      </c>
+      <c r="I731" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>04/02/2026</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>83557</t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>Analista de Processos – Pleno</t>
+        </is>
+      </c>
+      <c r="D732" t="inlineStr">
+        <is>
+          <t>Pleno</t>
+        </is>
+      </c>
+      <c r="E732" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F732" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 04/02/26</t>
+        </is>
+      </c>
+      <c r="G732" t="inlineStr">
+        <is>
+          <t>Requisitos Obrigatórios: •	Domínio do Pacote Office com Excel avançado e SQL. •	atuando sem supervisão constante e com foco em resultados •	Experiência em logística e melhoria de processos. •	Conhecimento em ferramentas de formulários (Forms) para criação de checklists •	Boa comunicação, organização e capacidade analítica e autogestão.  Métodos e Ferramentas Utilizadas: •	Fluxograma,Checklist, 5W2H e Diagrama de Ishikawa  Atividades a serem desenvolvidas: •	Realizar o mapeamento de processos, dentro e fora da empresa em São Paulo, incluindo parceiros. •	Documentar processos mapeados, seguindo rigorosamente os padrões definidos pelo cliente. •	Conduzir auditorias de processos e procedimentos, interno ou externo, incluindo visitas técnicas e acompanhamentos em campo, garantindo aderência aos padrões de qualidade estabelecido.  Modelo de Trabalho: Híbrido em São Paulo: 4 dias presenciais e 1 dia home office Possuir carro próprio
+Empresa .....:  SEMPRE IT SERVICOS DE TECNOLOGIA LTDA</t>
+        </is>
+      </c>
+      <c r="H732" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 04/02/26 || Analista de Processos – Pleno || Requisitos Obrigatórios: •	Domínio do Pacote Office com Excel avançado e SQL. •	atuando sem supervisão constante e com foco em resultados •	Experiência em logística e melhoria de processos. •	Conhecimento em ferramentas de formulários (Forms) para criação de checklists •	Boa comunicação, organização e capacidade analítica e autogestão.  Métodos e Ferramentas Utilizadas: •	Fluxograma,Checklist, 5W2H e Diagrama de Ishikawa  Atividades a serem desenvolvidas: •	Realizar o mapeamento de processos, dentro e fora da empresa em São Paulo, incluindo parceiros. •	Documentar processos mapeados, seguindo rigorosamente os padrões definidos pelo cliente. •	Conduzir auditorias de processos e procedimentos, interno ou externo, incluindo visitas técnicas e acompanhamentos em campo, garantindo aderência aos padrões de qualidade estabelecido.  Modelo de Trabalho: Híbrido em São Paulo: 4 dias presenciais e 1 dia home office Possuir carro próprio || Empresa .....:  SEMPRE IT SERVICOS DE TECNOLOGIA LTDA</t>
+        </is>
+      </c>
+      <c r="I732" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>04/02/2026</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>82223</t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>Analista de Sistema SR</t>
+        </is>
+      </c>
+      <c r="D733" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E733" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F733" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 04/02/26</t>
+        </is>
+      </c>
+      <c r="G733" t="inlineStr">
+        <is>
+          <t>Elaborar documentação planejada para garantir a clareza das especificações do sistema. Identificar oportunidades de otimização de processos e automação. Depurar pacotes e validar implementações antes da disponibilização para os clientes internos. Trabalhar de forma colaborativa com equipes multidisciplinares utilizando metodologias ágeis (Scrum, Kanban). Suporte técnico avançado para sistemas internos, solucionando incidentes e garantindo a continuidade dos serviços. Monitorar o desempenho das aplicações e implementar ações preventivas. Manter uma comunicação clara e eficaz com clientes internos, traduzindo necessidades de negócio para a equipe técnica. Desenvolver e ministrar treinamentos para usuários finais, garantindo o uso correto das soluções inovadoras. Criar manuais e materiais de apoio para facilitar a adoção de novas funcionalidades.  Sólida experiência com SQL Server, MySQL ou PostgreSQL. Vivência no setor de câmbio.
+Empresa .....:  Advanced Corretora de Câmbio</t>
+        </is>
+      </c>
+      <c r="H733" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 04/02/26 || Analista de Sistema SR || Elaborar documentação planejada para garantir a clareza das especificações do sistema. Identificar oportunidades de otimização de processos e automação. Depurar pacotes e validar implementações antes da disponibilização para os clientes internos. Trabalhar de forma colaborativa com equipes multidisciplinares utilizando metodologias ágeis (Scrum, Kanban). Suporte técnico avançado para sistemas internos, solucionando incidentes e garantindo a continuidade dos serviços. Monitorar o desempenho das aplicações e implementar ações preventivas. Manter uma comunicação clara e eficaz com clientes internos, traduzindo necessidades de negócio para a equipe técnica. Desenvolver e ministrar treinamentos para usuários finais, garantindo o uso correto das soluções inovadoras. Criar manuais e materiais de apoio para facilitar a adoção de novas funcionalidades.  Sólida experiência com SQL Server, MySQL ou PostgreSQL. Vivência no setor de câmbio. || Empresa .....:  Advanced Corretora de Câmbio</t>
+        </is>
+      </c>
+      <c r="I733" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>04/02/2026</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t>83574</t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>Analista de Sistemas Sênior  Java  Angular</t>
+        </is>
+      </c>
+      <c r="D734" t="inlineStr">
+        <is>
+          <t>Sênior</t>
+        </is>
+      </c>
+      <c r="E734" t="inlineStr">
+        <is>
+          <t>Híbrido</t>
+        </is>
+      </c>
+      <c r="F734" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 04/02/26</t>
+        </is>
+      </c>
+      <c r="G734" t="inlineStr">
+        <is>
+          <t>Buscamos Analista de Sistemas Sênior para atuar em um ambiente desafiador, com tecnologias modernas e espaço real para propor melhorias. Você fará parte de um time de TI que apoia áreas estratégicas do negócio.  Requisitos: Experiência sólida como Analista de Sistemas/Desenvolvedor(a) Sênior. Domínio de Java 8+ e Spring Boot 2+ em aplicações corporativas. Experiência prática com Angular 16+ em projetos relevantes. Conhecimento avançado em bancos de dados SQL e NoSQL. Vivência com uso de filas (mensageria) em integrações e sistemas distribuídos. Atuação em modelo de trabalho híbrido.  Diferenciais: Experiência aplicando Clean Architecture em projetos reais. Prática consistente de Clean Code e boas práticas de engenharia. Conhecimento de Design Patterns e sua aplicação no dia a dia. Vivência em ambientes de Governança de TI e boas práticas de qualidade. Perfil colaborativo, com foco em melhoria contínua.
+Empresa .....:  Topmind</t>
+        </is>
+      </c>
+      <c r="H734" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 04/02/26 || Analista de Sistemas Sênior  Java  Angular || Buscamos Analista de Sistemas Sênior para atuar em um ambiente desafiador, com tecnologias modernas e espaço real para propor melhorias. Você fará parte de um time de TI que apoia áreas estratégicas do negócio.  Requisitos: Experiência sólida como Analista de Sistemas/Desenvolvedor(a) Sênior. Domínio de Java 8+ e Spring Boot 2+ em aplicações corporativas. Experiência prática com Angular 16+ em projetos relevantes. Conhecimento avançado em bancos de dados SQL e NoSQL. Vivência com uso de filas (mensageria) em integrações e sistemas distribuídos. Atuação em modelo de trabalho híbrido.  Diferenciais: Experiência aplicando Clean Architecture em projetos reais. Prática consistente de Clean Code e boas práticas de engenharia. Conhecimento de Design Patterns e sua aplicação no dia a dia. Vivência em ambientes de Governança de TI e boas práticas de qualidade. Perfil colaborativo, com foco em melhoria contínua. || Empresa .....:  Topmind</t>
+        </is>
+      </c>
+      <c r="I734" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>04/02/2026</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>83569</t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>Analista de Suporte / Onboarding Técnico (N1)</t>
+        </is>
+      </c>
+      <c r="D735" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E735" t="inlineStr">
+        <is>
+          <t>Híbrido</t>
+        </is>
+      </c>
+      <c r="F735" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 04/02/26</t>
+        </is>
+      </c>
+      <c r="G735" t="inlineStr">
+        <is>
+          <t>Vaga: Analista de Suporte / Onboarding Técnico (N1) Paulista - SP  #127970 Híbrido (3x/semana) Contrato Prestador de Serviço  Temporário (4 meses) – cobertura licença-maternidade  Atividades principais: • Onboarding de clientes e acompanhamento da fase inicial • Atendimento N1 via Help Desk (tickets, triagem e SLA) • Suporte técnico em integrações (APIs REST, CSV e JSON) • Análise de erros operacionais e sistêmicos • Interface entre clientes e áreas internas • Suporte multicanal (WhatsApp, e-mail e Slack)  Requisitos: • Experiência em suporte técnico/operacional • Conhecimento em APIs REST (Postman) • Análise de arquivos CSV e JSON • Excel intermediário • Boa comunicação e perfil analítico  Diferencial: Inglês intermediário
+Empresa .....:  CBYK</t>
+        </is>
+      </c>
+      <c r="H735" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 04/02/26 || Analista de Suporte / Onboarding Técnico (N1) || Vaga: Analista de Suporte / Onboarding Técnico (N1) Paulista - SP  #127970 Híbrido (3x/semana) Contrato Prestador de Serviço  Temporário (4 meses) – cobertura licença-maternidade  Atividades principais: • Onboarding de clientes e acompanhamento da fase inicial • Atendimento N1 via Help Desk (tickets, triagem e SLA) • Suporte técnico em integrações (APIs REST, CSV e JSON) • Análise de erros operacionais e sistêmicos • Interface entre clientes e áreas internas • Suporte multicanal (WhatsApp, e-mail e Slack)  Requisitos: • Experiência em suporte técnico/operacional • Conhecimento em APIs REST (Postman) • Análise de arquivos CSV e JSON • Excel intermediário • Boa comunicação e perfil analítico  Diferencial: Inglês intermediário || Empresa .....:  CBYK</t>
+        </is>
+      </c>
+      <c r="I735" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>04/02/2026</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t>82839</t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>Analista de Suporte Tecnico Junior -Liberdade</t>
+        </is>
+      </c>
+      <c r="D736" t="inlineStr">
+        <is>
+          <t>Júnior</t>
+        </is>
+      </c>
+      <c r="E736" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F736" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 04/02/26</t>
+        </is>
+      </c>
+      <c r="G736" t="inlineStr">
+        <is>
+          <t>Analista de Suporte Junior - Noturno 12x36  Estamos buscando um profissional com experiência em suporte técnico voltado para voz e dados, incluindo configuração, implantação e manutenção de sistemas de telefonia e redes IP.  É essencial ter boa comunicação, habilidade para solucionar problemas e facilidade no relacionamento com clientes e equipe.  Diferenciais: • Certificações em Alcatel, Huawei, CCNA, Voice ou similares • Inglês desejável • CNH B será um diferencial  Perfil Ideal: • Comunicação clara • Raciocínio rápido • Organização e precisão • Abertura para aprender sempre  Remuneração 2.400,00+ Adicioal Noturno  VR de 33,00 ao Dia  Seguro de Vida  Previdência Privada  TotalPass  VT (Pago em Dinheiro)  Assistência Médica Bradesco ( pago 70  pela Empresa )  Assistência Odontológica Porto Seguro ( pago 50  pela Empresa )  Incentivos educacionais e parcerias com universidades  vaga Totalmente Presencial, Escala 12x36 -Noturno - Liberdade
+Empresa .....:  3CORPTECHNOLOGY</t>
+        </is>
+      </c>
+      <c r="H736" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 04/02/26 || Analista de Suporte Tecnico Junior -Liberdade || Analista de Suporte Junior - Noturno 12x36  Estamos buscando um profissional com experiência em suporte técnico voltado para voz e dados, incluindo configuração, implantação e manutenção de sistemas de telefonia e redes IP.  É essencial ter boa comunicação, habilidade para solucionar problemas e facilidade no relacionamento com clientes e equipe.  Diferenciais: • Certificações em Alcatel, Huawei, CCNA, Voice ou similares • Inglês desejável • CNH B será um diferencial  Perfil Ideal: • Comunicação clara • Raciocínio rápido • Organização e precisão • Abertura para aprender sempre  Remuneração 2.400,00+ Adicioal Noturno  VR de 33,00 ao Dia  Seguro de Vida  Previdência Privada  TotalPass  VT (Pago em Dinheiro)  Assistência Médica Bradesco ( pago 70  pela Empresa )  Assistência Odontológica Porto Seguro ( pago 50  pela Empresa )  Incentivos educacionais e parcerias com universidades  vaga Totalmente Presencial, Escala 12x36 -Noturno - Liberdade || Empresa .....:  3CORPTECHNOLOGY</t>
+        </is>
+      </c>
+      <c r="I736" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>04/02/2026</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t>82921</t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>Analista de TI</t>
+        </is>
+      </c>
+      <c r="D737" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E737" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F737" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 04/02/26</t>
+        </is>
+      </c>
+      <c r="G737" t="inlineStr">
+        <is>
+          <t>•	Atendimento a chamados, backups, instalação e manutenção de computadores, Windows, Linux, inventário de computadores, renovação de equipamentos, orçamentos, negociação com fornecedores, Fortigate, AD DC, DNS, Unify Ubiquiti, OCI, Oracle database, MDM, ibm, VPN. •   M365, Teams, Outlook, PowerBI, Banco de dados, Redes de computadores, Backup Veeam, Redes. •	Suporte em Infraestrutura. •	Avaliação de melhorias e performance de rede, segurança e inovações. •	Controle de contratos de infra, contas e pagamentos a fornecedores. •	Validação Backup semanal, inventário de parque de computadores e atualização semanal. •	Auditoria de acessos interno com revisão de redes, arquivos, dispositivos, auxiliando na segurança da infra. •	Participação de projetos globais de infra para atendimento de demandas da matriz.  Salário: R$ 3.450,00/mês. •	Seguro Saúde Bradesco Seguro Odonto Sul América, Seguro de Vida, VR 35,00 por dia, VT e PLR  Vaga presencial (próx a Paulista)
+Empresa .....:  QUI VAGAS CONSULTORIA DE RH</t>
+        </is>
+      </c>
+      <c r="H737" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 04/02/26 || Analista de TI || •	Atendimento a chamados, backups, instalação e manutenção de computadores, Windows, Linux, inventário de computadores, renovação de equipamentos, orçamentos, negociação com fornecedores, Fortigate, AD DC, DNS, Unify Ubiquiti, OCI, Oracle database, MDM, ibm, VPN. •   M365, Teams, Outlook, PowerBI, Banco de dados, Redes de computadores, Backup Veeam, Redes. •	Suporte em Infraestrutura. •	Avaliação de melhorias e performance de rede, segurança e inovações. •	Controle de contratos de infra, contas e pagamentos a fornecedores. •	Validação Backup semanal, inventário de parque de computadores e atualização semanal. •	Auditoria de acessos interno com revisão de redes, arquivos, dispositivos, auxiliando na segurança da infra. •	Participação de projetos globais de infra para atendimento de demandas da matriz.  Salário: R$ 3.450,00/mês. •	Seguro Saúde Bradesco Seguro Odonto Sul América, Seguro de Vida, VR 35,00 por dia, VT e PLR  Vaga presencial (próx a Paulista) || Empresa .....:  QUI VAGAS CONSULTORIA DE RH</t>
+        </is>
+      </c>
+      <c r="I737" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>04/02/2026</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t>82469</t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>ANALISTA SISTEMAS SUSTENTAÇÃO</t>
+        </is>
+      </c>
+      <c r="D738" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E738" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F738" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 04/02/26</t>
+        </is>
+      </c>
+      <c r="G738" t="inlineStr">
+        <is>
+          <t>ANALISTA SUSTENTAÇÃO DE SISTEMAS SÊNIOR PRESENCIAL SÃO PAULO  Experiência em sustentação/implantação de sistemas críticos no mercado financeiro. Domínio de integrações (APIs REST, mensageria), bancos de dados (Oracle/SQL Server/MySQL), queries/otimização e leitura de logs. Sistemas Operacionais Linux e Windows. Experiência com Infraestrutura, segurança da informação e redes. Experiência nas áreas de Governança/Compliance (evidências, auditoria) e gestão de fornecedores/SLAs.  Contratação PJ: 4 dias presenciais e 1 dia home office
+Empresa .....:  ARTIUM SOLUÇÕES</t>
+        </is>
+      </c>
+      <c r="H738" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 04/02/26 || ANALISTA SISTEMAS SUSTENTAÇÃO || ANALISTA SUSTENTAÇÃO DE SISTEMAS SÊNIOR PRESENCIAL SÃO PAULO  Experiência em sustentação/implantação de sistemas críticos no mercado financeiro. Domínio de integrações (APIs REST, mensageria), bancos de dados (Oracle/SQL Server/MySQL), queries/otimização e leitura de logs. Sistemas Operacionais Linux e Windows. Experiência com Infraestrutura, segurança da informação e redes. Experiência nas áreas de Governança/Compliance (evidências, auditoria) e gestão de fornecedores/SLAs.  Contratação PJ: 4 dias presenciais e 1 dia home office || Empresa .....:  ARTIUM SOLUÇÕES</t>
+        </is>
+      </c>
+      <c r="I738" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>04/02/2026</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t>82694</t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>Arquiteto de Integração</t>
+        </is>
+      </c>
+      <c r="D739" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E739" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F739" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 04/02/26</t>
+        </is>
+      </c>
+      <c r="G739" t="inlineStr">
+        <is>
+          <t>O Arquiteto de Integração é responsável por projetar, definir e supervisionar soluções de integração entre sistemas corporativos, produtivos e laboratoriais, garantindo que a troca de dados seja segura, rastreável, eficiente e aderente às diretrizes regulatórias e operacionais da indústria. Atua como referência técnica na arquitetura de integração, promovendo interoperabilidade, padronização e governança em todo o ecossistema tecnológico.  O QUE ESPERAMOS DE VOCÊ: Graduação Completa Engenharia da Computação, Ciência da Computação, Sistemas de Informação, Engenharia de Software ou áreas correlatas Conhecimento em Arquiteturas híbridas e integrações entre ambientes on-premise e cloud Padrões e tecnologias de integração (APIs REST/SOAP, mensageria, ESB, ETL, microsserviços) Boas práticas de arquitetura, segurança, governança e documentação.
+Empresa .....:  Biolab Sanus Farmacêutica</t>
+        </is>
+      </c>
+      <c r="H739" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 04/02/26 || Arquiteto de Integração || O Arquiteto de Integração é responsável por projetar, definir e supervisionar soluções de integração entre sistemas corporativos, produtivos e laboratoriais, garantindo que a troca de dados seja segura, rastreável, eficiente e aderente às diretrizes regulatórias e operacionais da indústria. Atua como referência técnica na arquitetura de integração, promovendo interoperabilidade, padronização e governança em todo o ecossistema tecnológico.  O QUE ESPERAMOS DE VOCÊ: Graduação Completa Engenharia da Computação, Ciência da Computação, Sistemas de Informação, Engenharia de Software ou áreas correlatas Conhecimento em Arquiteturas híbridas e integrações entre ambientes on-premise e cloud Padrões e tecnologias de integração (APIs REST/SOAP, mensageria, ESB, ETL, microsserviços) Boas práticas de arquitetura, segurança, governança e documentação. || Empresa .....:  Biolab Sanus Farmacêutica</t>
+        </is>
+      </c>
+      <c r="I739" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>04/02/2026</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t>83564</t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>Consultor(a) TOTVS Protheus Sênior</t>
+        </is>
+      </c>
+      <c r="D740" t="inlineStr">
+        <is>
+          <t>Sênior</t>
+        </is>
+      </c>
+      <c r="E740" t="inlineStr">
+        <is>
+          <t>Híbrido</t>
+        </is>
+      </c>
+      <c r="F740" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 04/02/26</t>
+        </is>
+      </c>
+      <c r="G740" t="inlineStr">
+        <is>
+          <t>Consultor(a)TOTVS Protheus Sênior  Modelo: Híbrido (2x presencial na semana) – São Paulo/SP - Morumbi Prazo de Projeto: Até 31/05/2026 (com chance de renovação) Regime de contrato: PJ  Principais requisitos: Experiência sólida em TOTVS Protheus (implantação, suporte ou evolução) Conhecimento em ADVPL Vivência com banco de dados (SQL Server ou Oracle) Atuação em módulos financeiros, contábeis e fiscais Integrações via API / Webservice Disponibilidade para viagens  Inglês avançado/fluente para conversação  Enviar o currículo atualizado em inglês e português.
+Empresa .....:  ITeam</t>
+        </is>
+      </c>
+      <c r="H740" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 04/02/26 || Consultor(a) TOTVS Protheus Sênior || Consultor(a)TOTVS Protheus Sênior  Modelo: Híbrido (2x presencial na semana) – São Paulo/SP - Morumbi Prazo de Projeto: Até 31/05/2026 (com chance de renovação) Regime de contrato: PJ  Principais requisitos: Experiência sólida em TOTVS Protheus (implantação, suporte ou evolução) Conhecimento em ADVPL Vivência com banco de dados (SQL Server ou Oracle) Atuação em módulos financeiros, contábeis e fiscais Integrações via API / Webservice Disponibilidade para viagens  Inglês avançado/fluente para conversação  Enviar o currículo atualizado em inglês e português. || Empresa .....:  ITeam</t>
+        </is>
+      </c>
+      <c r="I740" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>04/02/2026</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t>82357</t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>Coordenador de Operações de TI - BILÍNGUE INGLÊS</t>
+        </is>
+      </c>
+      <c r="D741" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E741" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F741" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 04/02/26</t>
+        </is>
+      </c>
+      <c r="G741" t="inlineStr">
+        <is>
+          <t>Atividades: •       Gestão de Operações e Serviços Acompanhar o funcionamento dos serviços de TI utilizados nas lojas (servidores, redes, PDVs, sistemas corporativos etc.). Avaliar e priorizar incidentes críticos, assegurando tratativas rápidas e eficazes. Garantir cumprimento de SLAs e OLAs definidos com clientes internos ou externos. Distribuir tarefas diárias entre analistas e técnicos conforme criticidade e competência técnica. Acompanhar performance individual e coletiva, dando feedback e direcionamento. Promover reuniões rápidas de alinhamento (daily meetings) e reuniões semanais de planejamento. Identificar gaps de capacitação e planejar treinamentos técnicos ou comportamentais.  •       Gestão de Incidentes, Problemas e Requisições Garantir que a equipe efetue registro, categorização e acompanhamento de tickets na ferramenta ITSM. Propor planos de melhoria para incidentes recorrentes.
+Empresa .....:  Engemon IT</t>
+        </is>
+      </c>
+      <c r="H741" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 04/02/26 || Coordenador de Operações de TI - BILÍNGUE INGLÊS || Atividades: •       Gestão de Operações e Serviços Acompanhar o funcionamento dos serviços de TI utilizados nas lojas (servidores, redes, PDVs, sistemas corporativos etc.). Avaliar e priorizar incidentes críticos, assegurando tratativas rápidas e eficazes. Garantir cumprimento de SLAs e OLAs definidos com clientes internos ou externos. Distribuir tarefas diárias entre analistas e técnicos conforme criticidade e competência técnica. Acompanhar performance individual e coletiva, dando feedback e direcionamento. Promover reuniões rápidas de alinhamento (daily meetings) e reuniões semanais de planejamento. Identificar gaps de capacitação e planejar treinamentos técnicos ou comportamentais.  •       Gestão de Incidentes, Problemas e Requisições Garantir que a equipe efetue registro, categorização e acompanhamento de tickets na ferramenta ITSM. Propor planos de melhoria para incidentes recorrentes. || Empresa .....:  Engemon IT</t>
+        </is>
+      </c>
+      <c r="I741" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>04/02/2026</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>82412</t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>Desenvolvedor .Net Pleno</t>
+        </is>
+      </c>
+      <c r="D742" t="inlineStr">
+        <is>
+          <t>Pleno</t>
+        </is>
+      </c>
+      <c r="E742" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F742" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 04/02/26</t>
+        </is>
+      </c>
+      <c r="G742" t="inlineStr">
+        <is>
+          <t>Experiência com desenvolvimento em .NET Core. Domínio de C# e arquitetura de microserviços. Experiência com SQL Server e modelagem de dados. Conhecimento em Microsoft Visual Studio e GitHub/ Github actions. Facilidade em propor soluções técnicas e não apenas executá-las.  Desenvolver e aprimorar serviços em .NET 8 e C#. Projetar e otimizar bancos de dados SQL Server e Azure SQL. Participar de revisões de código, testes unitários e integração contínua. Colaborar com equipes multifuncionais em metodologias ágeis. Documentar soluções e manter boas práticas de desenvolvimento.  Atuar no modelo presencial, tendo 1 dia remoto por semana. CLT(Proximo da Consolação)
+Empresa .....:  GlobalTI</t>
+        </is>
+      </c>
+      <c r="H742" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 04/02/26 || Desenvolvedor .Net Pleno || Experiência com desenvolvimento em .NET Core. Domínio de C# e arquitetura de microserviços. Experiência com SQL Server e modelagem de dados. Conhecimento em Microsoft Visual Studio e GitHub/ Github actions. Facilidade em propor soluções técnicas e não apenas executá-las.  Desenvolver e aprimorar serviços em .NET 8 e C#. Projetar e otimizar bancos de dados SQL Server e Azure SQL. Participar de revisões de código, testes unitários e integração contínua. Colaborar com equipes multifuncionais em metodologias ágeis. Documentar soluções e manter boas práticas de desenvolvimento.  Atuar no modelo presencial, tendo 1 dia remoto por semana. CLT(Proximo da Consolação) || Empresa .....:  GlobalTI</t>
+        </is>
+      </c>
+      <c r="I742" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>04/02/2026</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t>82610</t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>Desenvolvedor .NET Pleno</t>
+        </is>
+      </c>
+      <c r="D743" t="inlineStr">
+        <is>
+          <t>Pleno</t>
+        </is>
+      </c>
+      <c r="E743" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F743" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 04/02/26</t>
+        </is>
+      </c>
+      <c r="G743" t="inlineStr">
+        <is>
+          <t>.NET PLENO  Experiência com C# e .NET Framework/Core Atuação no desenvolvimento de APIs RESTful Experiência com bancos de dados relacionais e não relacionais (SQL Server, PostgreSQL, MongoDB) Experiência com mensageria PUB/SUB (RabbitMQ, entre outros) Uso de cache em aplicações (ex: Redis) Criação e otimização de queries complexas Conhecimentos sólidos em Docker e Kubernetes Experiência com ferramentas como OpenAPI (Swagger), Postman, Git, GitFlow e Jira Vivência em ambientes cloud (preferencialmente GCP) Experiência com observabilidade e monitoramento (ex: Datadog, Dynatrace) Conhecimento em microserviços (comunicação síncrona/assíncrona, Saga Pattern) Compreensão de arquiteturas de alta escala e performance.  Período de Alocação: 12 meses com possibilidade de renovação - PJ Modelo de Alocação: Remoto, com possíveis idas ao cliente pontuais - Zona Oeste/SP
+Empresa .....:  SOW Serviços</t>
+        </is>
+      </c>
+      <c r="H743" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 04/02/26 || Desenvolvedor .NET Pleno || .NET PLENO  Experiência com C# e .NET Framework/Core Atuação no desenvolvimento de APIs RESTful Experiência com bancos de dados relacionais e não relacionais (SQL Server, PostgreSQL, MongoDB) Experiência com mensageria PUB/SUB (RabbitMQ, entre outros) Uso de cache em aplicações (ex: Redis) Criação e otimização de queries complexas Conhecimentos sólidos em Docker e Kubernetes Experiência com ferramentas como OpenAPI (Swagger), Postman, Git, GitFlow e Jira Vivência em ambientes cloud (preferencialmente GCP) Experiência com observabilidade e monitoramento (ex: Datadog, Dynatrace) Conhecimento em microserviços (comunicação síncrona/assíncrona, Saga Pattern) Compreensão de arquiteturas de alta escala e performance.  Período de Alocação: 12 meses com possibilidade de renovação - PJ Modelo de Alocação: Remoto, com possíveis idas ao cliente pontuais - Zona Oeste/SP || Empresa .....:  SOW Serviços</t>
+        </is>
+      </c>
+      <c r="I743" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>04/02/2026</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t>82325</t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>Desenvolvedor .NET Sênior</t>
+        </is>
+      </c>
+      <c r="D744" t="inlineStr">
+        <is>
+          <t>Sênior</t>
+        </is>
+      </c>
+      <c r="E744" t="inlineStr">
+        <is>
+          <t>Híbrido</t>
+        </is>
+      </c>
+      <c r="F744" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 04/02/26</t>
+        </is>
+      </c>
+      <c r="G744" t="inlineStr">
+        <is>
+          <t>A Tech For está com oportunidade para Desenvolvedor (a) Sênior Full Stack .NET com forte atuação JavaScript,  em cliente do segmento bancário.  Modelo híbrido: 2 x semana presenciais situado na região oeste de SP, próximo ao Shopping Eldorado. PJ  Requisitos imprescindíveis: - À partir de 05 anos de experiência comprovada em desenvolvimento de software.  Proficiência em desenvolvimento com: - C# e .NET Framework/Core - MVC, HTML5, CSS3, JavaScript (ES6+) e TypeScript - Frameworks frontend como React ou Angular (diferencial) - SQL Server (Procedure, Function, Triggers, Views) - Web API - Domain-Driven Design (DDD) - Camada de persistência ORM (Dapper) - DevOps (Git/TFS - Azure DevOps). - Habilidades analíticas e conceituais, com capacidade de resolver problemas complexos. - Fortes habilidades didáticas, com capacidade de explicar conceitos técnicos de forma clara e acessível. - Objetividade, fluência verbal e escrita, e postura profissional.
+Empresa .....:  Tech For TI</t>
+        </is>
+      </c>
+      <c r="H744" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 04/02/26 || Desenvolvedor .NET Sênior || A Tech For está com oportunidade para Desenvolvedor (a) Sênior Full Stack .NET com forte atuação JavaScript,  em cliente do segmento bancário.  Modelo híbrido: 2 x semana presenciais situado na região oeste de SP, próximo ao Shopping Eldorado. PJ  Requisitos imprescindíveis: - À partir de 05 anos de experiência comprovada em desenvolvimento de software.  Proficiência em desenvolvimento com: - C# e .NET Framework/Core - MVC, HTML5, CSS3, JavaScript (ES6+) e TypeScript - Frameworks frontend como React ou Angular (diferencial) - SQL Server (Procedure, Function, Triggers, Views) - Web API - Domain-Driven Design (DDD) - Camada de persistência ORM (Dapper) - DevOps (Git/TFS - Azure DevOps). - Habilidades analíticas e conceituais, com capacidade de resolver problemas complexos. - Fortes habilidades didáticas, com capacidade de explicar conceitos técnicos de forma clara e acessível. - Objetividade, fluência verbal e escrita, e postura profissional. || Empresa .....:  Tech For TI</t>
+        </is>
+      </c>
+      <c r="I744" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>04/02/2026</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>82629</t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>Desenvolvedor Front End</t>
+        </is>
+      </c>
+      <c r="D745" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E745" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F745" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 04/02/26</t>
+        </is>
+      </c>
+      <c r="G745" t="inlineStr">
+        <is>
+          <t>Prazo: 3 meses. com chances de prorrogar Local: Remoto Contratação: PJ  Requisitos: Experiência em desenvolvimento Front End utilizando o framework Angular.
+Empresa .....:  Entrust IT</t>
+        </is>
+      </c>
+      <c r="H745" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 04/02/26 || Desenvolvedor Front End || Prazo: 3 meses. com chances de prorrogar Local: Remoto Contratação: PJ  Requisitos: Experiência em desenvolvimento Front End utilizando o framework Angular. || Empresa .....:  Entrust IT</t>
+        </is>
+      </c>
+      <c r="I745" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>04/02/2026</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t>83578</t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>Desenvolvedor Full Stack Python + React</t>
+        </is>
+      </c>
+      <c r="D746" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E746" t="inlineStr">
+        <is>
+          <t>Híbrido</t>
+        </is>
+      </c>
+      <c r="F746" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 04/02/26</t>
+        </is>
+      </c>
+      <c r="G746" t="inlineStr">
+        <is>
+          <t>Local: São Paulo/SP (Itaim Bibi) ou Curitiba/PR – Híbrido 3x/semana Horário: Comercial  Contrato: CLT  O que você vai fazer: Desenvolver aplicações full stack (Python/FastAPI + React/TypeScript) Trabalhar com bancos de dados relacionais (MySQL/PostgreSQL) Implantar apps em Docker e Kubernetes Integrar sistemas e APIs externas Aplicar DevSecOps e testes automatizados  Requisitos:  - 5+ anos de experiência em full stack  - Python + FastAPI / React + TypeScript  - Inglês avançado  - Docker/Kubernetes e bancos relacionais  Diferenciais: CI/CD, nuvem, DevSecOps, frameworks adicionais (Vue.js, Symfony)
+Empresa .....:  Ultracon</t>
+        </is>
+      </c>
+      <c r="H746" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 04/02/26 || Desenvolvedor Full Stack Python + React || Local: São Paulo/SP (Itaim Bibi) ou Curitiba/PR – Híbrido 3x/semana Horário: Comercial  Contrato: CLT  O que você vai fazer: Desenvolver aplicações full stack (Python/FastAPI + React/TypeScript) Trabalhar com bancos de dados relacionais (MySQL/PostgreSQL) Implantar apps em Docker e Kubernetes Integrar sistemas e APIs externas Aplicar DevSecOps e testes automatizados  Requisitos:  - 5+ anos de experiência em full stack  - Python + FastAPI / React + TypeScript  - Inglês avançado  - Docker/Kubernetes e bancos relacionais  Diferenciais: CI/CD, nuvem, DevSecOps, frameworks adicionais (Vue.js, Symfony) || Empresa .....:  Ultracon</t>
+        </is>
+      </c>
+      <c r="I746" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>04/02/2026</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>82466</t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>Desenvolvedor Full Stack Sênior</t>
+        </is>
+      </c>
+      <c r="D747" t="inlineStr">
+        <is>
+          <t>Sênior</t>
+        </is>
+      </c>
+      <c r="E747" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F747" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 04/02/26</t>
+        </is>
+      </c>
+      <c r="G747" t="inlineStr">
+        <is>
+          <t>Atue na sustentação e evolução de plataformas web, criando novas funcionalidades, revisando código e propondo melhorias contínuas.  Requisitos: Domínio em .NET Core (C#), React, JavaScript/TypeScript, MongoDB, SQL Server, CI/CD, Docker e Kubernetes. Certificação AWS é diferencial.
+Empresa .....:  NCM Sistemas e Consultoria Ltda</t>
+        </is>
+      </c>
+      <c r="H747" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 04/02/26 || Desenvolvedor Full Stack Sênior || Atue na sustentação e evolução de plataformas web, criando novas funcionalidades, revisando código e propondo melhorias contínuas.  Requisitos: Domínio em .NET Core (C#), React, JavaScript/TypeScript, MongoDB, SQL Server, CI/CD, Docker e Kubernetes. Certificação AWS é diferencial. || Empresa .....:  NCM Sistemas e Consultoria Ltda</t>
+        </is>
+      </c>
+      <c r="I747" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>04/02/2026</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>82635</t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>Desenvolvedor Fullstack (.Net Core + Angular)</t>
+        </is>
+      </c>
+      <c r="D748" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E748" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F748" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 04/02/26</t>
+        </is>
+      </c>
+      <c r="G748" t="inlineStr">
+        <is>
+          <t>• Back-end: • Experiência em desenvolvimento com .NET C#, versão (4,5, 6, 8) incluindo Framework e Core • Forte domínio de Redis, Oracle PL/SQL, com capacidade de modelar e otimizar grandes volumes de dados em sistemas complexos • Expertise na integração entre sistemas utilizando mensageria com IBM MQSeries, com conhecimento sobre padrões de design distribuído (como Pub/Sub).  • Front-end: • Proficiência em Angular, com habilidades para criar SPAs (Single-Page Applications) otimizadas. • Conhecimento de performance e boas práticas de UX/UI. • Ferramentas e Projetos: • Uso de ferramentas de gestão de projetos como Jira, CA Service Desk Manager (CA SDM) e Service Now futuramente, Confluence para organização e controle de tarefas.
+Empresa .....:  200DEV</t>
+        </is>
+      </c>
+      <c r="H748" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 04/02/26 || Desenvolvedor Fullstack (.Net Core + Angular) || • Back-end: • Experiência em desenvolvimento com .NET C#, versão (4,5, 6, 8) incluindo Framework e Core • Forte domínio de Redis, Oracle PL/SQL, com capacidade de modelar e otimizar grandes volumes de dados em sistemas complexos • Expertise na integração entre sistemas utilizando mensageria com IBM MQSeries, com conhecimento sobre padrões de design distribuído (como Pub/Sub).  • Front-end: • Proficiência em Angular, com habilidades para criar SPAs (Single-Page Applications) otimizadas. • Conhecimento de performance e boas práticas de UX/UI. • Ferramentas e Projetos: • Uso de ferramentas de gestão de projetos como Jira, CA Service Desk Manager (CA SDM) e Service Now futuramente, Confluence para organização e controle de tarefas. || Empresa .....:  200DEV</t>
+        </is>
+      </c>
+      <c r="I748" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>04/02/2026</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t>82311</t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>Desenvolvedor FullStack Sênior - .Java/Angular</t>
+        </is>
+      </c>
+      <c r="D749" t="inlineStr">
+        <is>
+          <t>Sênior</t>
+        </is>
+      </c>
+      <c r="E749" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F749" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 04/02/26</t>
+        </is>
+      </c>
+      <c r="G749" t="inlineStr">
+        <is>
+          <t>Principais Responsabilidades  Desenvolvimento e Arquitetura Implementar soluções utilizando Java 8+, Spring Boot e padrões modernos de arquitetura (Clean Architecture, Hexagonal). Projetar e desenvolver APIs RESTful com boas práticas de versionamento, segurança e escalabilidade. Criar e manter microserviços e contribuir para a migração de sistemas monolíticos para AWS.  Requisitos Técnicos (Hard Skills)  Java 8+ (streams, lambdas, API de datas). Angular 8+. Spring Boot (MVC, Data, Security). APIs RESTful com boas práticas. Bancos relacionais (PostgreSQL, desejável DB2). Git/GitHub, GitHub Actions, Maven, SonarQube, Nexus. Testes automatizados (JUnit, Mockito). Experiência com microserviços, arquitetura distribuída e cloud (AWS). Conhecimentos em segurança (criptografia, certificados digitais). Desejável: arquitetura orientada a eventos, ferramentas de transferência de arquivos (Connect Direct, XFB, CFT).
+Empresa .....:  RHTalentos</t>
+        </is>
+      </c>
+      <c r="H749" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 04/02/26 || Desenvolvedor FullStack Sênior - .Java/Angular || Principais Responsabilidades  Desenvolvimento e Arquitetura Implementar soluções utilizando Java 8+, Spring Boot e padrões modernos de arquitetura (Clean Architecture, Hexagonal). Projetar e desenvolver APIs RESTful com boas práticas de versionamento, segurança e escalabilidade. Criar e manter microserviços e contribuir para a migração de sistemas monolíticos para AWS.  Requisitos Técnicos (Hard Skills)  Java 8+ (streams, lambdas, API de datas). Angular 8+. Spring Boot (MVC, Data, Security). APIs RESTful com boas práticas. Bancos relacionais (PostgreSQL, desejável DB2). Git/GitHub, GitHub Actions, Maven, SonarQube, Nexus. Testes automatizados (JUnit, Mockito). Experiência com microserviços, arquitetura distribuída e cloud (AWS). Conhecimentos em segurança (criptografia, certificados digitais). Desejável: arquitetura orientada a eventos, ferramentas de transferência de arquivos (Connect Direct, XFB, CFT). || Empresa .....:  RHTalentos</t>
+        </is>
+      </c>
+      <c r="I749" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>04/02/2026</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t>82436</t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>Desenvolvedor Java</t>
+        </is>
+      </c>
+      <c r="D750" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E750" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F750" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 04/02/26</t>
+        </is>
+      </c>
+      <c r="G750" t="inlineStr">
+        <is>
+          <t>REQUISITOS E QUALIFICAÇÕES  Como requisitos necessários, precisamos que você tenha:  Graduação em Ciência da Computação, Engenharia de Software ou áreas afins. Experiência com desenvolvimento em JAVA e nos frameworks Spring MVC e Spring Boot Histórico do projeto de varejo/comércio eletrônico Experiência com desenvolvimento orientado a testes e frameworks de testes automatizados, como JUnit. Familiaridade com Git, pipelines de CI/CD e metodologias de desenvolvimento Ágil Inglês Intermediário.  Será um diferencial se você tiver: Experiência com projeto de E-commerce desenvolvidos em plataforma Hybris (SAP Commerce Cloud) Experiência com plataformas de nuvem (AWS, Azure ou SAP Cloud Platform). Espanhol básico
+Empresa .....:  Ewave do Brasil</t>
+        </is>
+      </c>
+      <c r="H750" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 04/02/26 || Desenvolvedor Java || REQUISITOS E QUALIFICAÇÕES  Como requisitos necessários, precisamos que você tenha:  Graduação em Ciência da Computação, Engenharia de Software ou áreas afins. Experiência com desenvolvimento em JAVA e nos frameworks Spring MVC e Spring Boot Histórico do projeto de varejo/comércio eletrônico Experiência com desenvolvimento orientado a testes e frameworks de testes automatizados, como JUnit. Familiaridade com Git, pipelines de CI/CD e metodologias de desenvolvimento Ágil Inglês Intermediário.  Será um diferencial se você tiver: Experiência com projeto de E-commerce desenvolvidos em plataforma Hybris (SAP Commerce Cloud) Experiência com plataformas de nuvem (AWS, Azure ou SAP Cloud Platform). Espanhol básico || Empresa .....:  Ewave do Brasil</t>
+        </is>
+      </c>
+      <c r="I750" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>04/02/2026</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t>82772</t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>DESENVOLVEDOR JAVA JÚNIOR  - HÍBRIDO SÃO PAULO/SP</t>
+        </is>
+      </c>
+      <c r="D751" t="inlineStr">
+        <is>
+          <t>Júnior</t>
+        </is>
+      </c>
+      <c r="E751" t="inlineStr">
+        <is>
+          <t>Híbrido</t>
+        </is>
+      </c>
+      <c r="F751" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 04/02/26</t>
+        </is>
+      </c>
+      <c r="G751" t="inlineStr">
+        <is>
+          <t>ATUAÇÃO HÍBRIDA 3X POR SEMANA NO BAIRRO DO MORUMBI, ZONA SUL DE SÃO PAULO/SP Contratação CLT+ Benefícios  Objetivo do Cargo: Profissional Junior com base sólida em programação e forte adaptabilidade tecnológica. Possuir experiência inicial com Java, mas mantém postura flexível, aberta e orientada ao aprendizado, permitindo atuar com tranquilidade também em Python, C# e outras linguagens quando necessário. Demonstra curiosidade, boa comunicação e capacidade de colaboração, além de equilíbrio emocional em cenários de pressão.  Requisitos: •	Fundamentos de Programação: lógica bem estruturada, conhecimento de algoritmos, estruturas de dados e noções de arquitetura de software. •	Linguagens Principais: •	Java (nível júnior) •	Python (bom domínio para automações e scripts) •	C# (familiaridade com desenvolvimento desktop e serviços) •	Multiplataforma: •	Desenvolvimento web (HTML, CSS, JavaScript, APIs REST) •	Aplicações desktop (JavaFX, .NET WPF/WinForms)
+Empresa .....:  KLB Group</t>
+        </is>
+      </c>
+      <c r="H751" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 04/02/26 || DESENVOLVEDOR JAVA JÚNIOR  - HÍBRIDO SÃO PAULO/SP || ATUAÇÃO HÍBRIDA 3X POR SEMANA NO BAIRRO DO MORUMBI, ZONA SUL DE SÃO PAULO/SP Contratação CLT+ Benefícios  Objetivo do Cargo: Profissional Junior com base sólida em programação e forte adaptabilidade tecnológica. Possuir experiência inicial com Java, mas mantém postura flexível, aberta e orientada ao aprendizado, permitindo atuar com tranquilidade também em Python, C# e outras linguagens quando necessário. Demonstra curiosidade, boa comunicação e capacidade de colaboração, além de equilíbrio emocional em cenários de pressão.  Requisitos: •	Fundamentos de Programação: lógica bem estruturada, conhecimento de algoritmos, estruturas de dados e noções de arquitetura de software. •	Linguagens Principais: •	Java (nível júnior) •	Python (bom domínio para automações e scripts) •	C# (familiaridade com desenvolvimento desktop e serviços) •	Multiplataforma: •	Desenvolvimento web (HTML, CSS, JavaScript, APIs REST) •	Aplicações desktop (JavaFX, .NET WPF/WinForms) || Empresa .....:  KLB Group</t>
+        </is>
+      </c>
+      <c r="I751" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>04/02/2026</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t>83566</t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>DESENVOLVEDOR JUNIOR I / URGENTE</t>
+        </is>
+      </c>
+      <c r="D752" t="inlineStr">
+        <is>
+          <t>Júnior</t>
+        </is>
+      </c>
+      <c r="E752" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F752" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 04/02/26</t>
+        </is>
+      </c>
+      <c r="G752" t="inlineStr">
+        <is>
+          <t>Atuar no desenvolvimento e manutenção de aplicações utilizando C# .NET (Web Forms). Criar e ajustar consultas e procedimentos em SQL Server. Implementar funcionalidades no front-end utilizando JavaScript e jQuery. Realizar correções de bugs, melhorias e novas implementações no sistema. Trabalhar em conjunto com outros desenvolvedores para evoluir aplicações internas.  Requisitos Técnicos: Conhecimentos básicos em C# .NET com foco em Web Forms e MVC. Experiência com SQL (consultas, inserts, updates e joins). Experiência em JavaScript e jQuery. Capacidade de compreender código legado e aplicar boas práticas.  IA será um diferencial.
+Empresa .....:  VIGNA ADVOGADOS ASSOCIADOS</t>
+        </is>
+      </c>
+      <c r="H752" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 04/02/26 || DESENVOLVEDOR JUNIOR I / URGENTE || Atuar no desenvolvimento e manutenção de aplicações utilizando C# .NET (Web Forms). Criar e ajustar consultas e procedimentos em SQL Server. Implementar funcionalidades no front-end utilizando JavaScript e jQuery. Realizar correções de bugs, melhorias e novas implementações no sistema. Trabalhar em conjunto com outros desenvolvedores para evoluir aplicações internas.  Requisitos Técnicos: Conhecimentos básicos em C# .NET com foco em Web Forms e MVC. Experiência com SQL (consultas, inserts, updates e joins). Experiência em JavaScript e jQuery. Capacidade de compreender código legado e aplicar boas práticas.  IA será um diferencial. || Empresa .....:  VIGNA ADVOGADOS ASSOCIADOS</t>
+        </is>
+      </c>
+      <c r="I752" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>04/02/2026</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t>83568</t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>DESENVOLVEDOR REACT / REACT NATIVE SÊNIOR - INGLÊS</t>
+        </is>
+      </c>
+      <c r="D753" t="inlineStr">
+        <is>
+          <t>Sênior</t>
+        </is>
+      </c>
+      <c r="E753" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F753" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 04/02/26</t>
+        </is>
+      </c>
+      <c r="G753" t="inlineStr">
+        <is>
+          <t>Atuação Totalmente remota Contratação PJ  Requisitos Mandatórios: •	INGLÊS AVANÇADO (MANDATÓRIO, INTERAÇÃO COM TIME GLOBAL) •	Imprescindível Experiência com React e React Native essenciais •	Experiência com Node Js •	Conhecimento nativo (iOS ou Android) diferencial •	Conhecimento de ciclo de vida •	Componentes •	Hooks •	Gerenciamento de estado •	Navegação •	Banco de Dados SQL •	APIs •	Arquitetura de boas práticas  Diferencial: - Ter atuado em um aplicativo móvel complexo - Conhecer TypeScript - Conhecer Expo, CI e CD também são diferenciais.  Atribuições: - Desenvolver e manter aplicativos móveis, alocações web e backend, utilizando React Native, React e node.js - Colaborar com times multidisciplinares, realizando a integração de novos recursos e soluções. - Participar de revisões de código e testes para garantir a entrega de soluções eficientes e escaláveis.
+Empresa .....:  KLB Group</t>
+        </is>
+      </c>
+      <c r="H753" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 04/02/26 || DESENVOLVEDOR REACT / REACT NATIVE SÊNIOR - INGLÊS || Atuação Totalmente remota Contratação PJ  Requisitos Mandatórios: •	INGLÊS AVANÇADO (MANDATÓRIO, INTERAÇÃO COM TIME GLOBAL) •	Imprescindível Experiência com React e React Native essenciais •	Experiência com Node Js •	Conhecimento nativo (iOS ou Android) diferencial •	Conhecimento de ciclo de vida •	Componentes •	Hooks •	Gerenciamento de estado •	Navegação •	Banco de Dados SQL •	APIs •	Arquitetura de boas práticas  Diferencial: - Ter atuado em um aplicativo móvel complexo - Conhecer TypeScript - Conhecer Expo, CI e CD também são diferenciais.  Atribuições: - Desenvolver e manter aplicativos móveis, alocações web e backend, utilizando React Native, React e node.js - Colaborar com times multidisciplinares, realizando a integração de novos recursos e soluções. - Participar de revisões de código e testes para garantir a entrega de soluções eficientes e escaláveis. || Empresa .....:  KLB Group</t>
+        </is>
+      </c>
+      <c r="I753" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>04/02/2026</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t>82233</t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>Desenvolvimento Fullstack Sênior</t>
+        </is>
+      </c>
+      <c r="D754" t="inlineStr">
+        <is>
+          <t>Sênior</t>
+        </is>
+      </c>
+      <c r="E754" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F754" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 04/02/26</t>
+        </is>
+      </c>
+      <c r="G754" t="inlineStr">
+        <is>
+          <t>Alto conhecimento em ASP Classico .NET Framework (Asp .NET , C# , MVC),  iReport (Jaspter) Delphi 5 Familiaridade com Git e fluxo de CI/CD (preferencialmente no Azure DevOps) Conhecimento em Docker
+Empresa .....:  WTime</t>
+        </is>
+      </c>
+      <c r="H754" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 04/02/26 || Desenvolvimento Fullstack Sênior || Alto conhecimento em ASP Classico .NET Framework (Asp .NET , C# , MVC),  iReport (Jaspter) Delphi 5 Familiaridade com Git e fluxo de CI/CD (preferencialmente no Azure DevOps) Conhecimento em Docker || Empresa .....:  WTime</t>
+        </is>
+      </c>
+      <c r="I754" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>04/02/2026</t>
+        </is>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t>83562</t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>Engenheiro DevOps Pleno</t>
+        </is>
+      </c>
+      <c r="D755" t="inlineStr">
+        <is>
+          <t>Pleno</t>
+        </is>
+      </c>
+      <c r="E755" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F755" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 04/02/26</t>
+        </is>
+      </c>
+      <c r="G755" t="inlineStr">
+        <is>
+          <t>Engenheiro DevOps Pleno Forma de atendimento: São Paulo – Zona Sul/Oeste Modelo de trabalho: Híbrido (2 presenciais, 3 remotos) Duração do contrato: 12 meses  Requisitos: Inglês: Avançado ou Fluente OpenShift - Intermediate Jenkins - Intermediate UNIX Shell - Intermediate Git -  Basic Ansible - Intermediate Kibana - Basic Windows- Intermediate JIRA - Intermediate Gradle -  Basic Dynatrace -  Basic AWS (Amazon Web Services) -  Basic
+Empresa .....:  WA FENIX IT SERVICES  SOLUTIONS</t>
+        </is>
+      </c>
+      <c r="H755" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 04/02/26 || Engenheiro DevOps Pleno || Engenheiro DevOps Pleno Forma de atendimento: São Paulo – Zona Sul/Oeste Modelo de trabalho: Híbrido (2 presenciais, 3 remotos) Duração do contrato: 12 meses  Requisitos: Inglês: Avançado ou Fluente OpenShift - Intermediate Jenkins - Intermediate UNIX Shell - Intermediate Git -  Basic Ansible - Intermediate Kibana - Basic Windows- Intermediate JIRA - Intermediate Gradle -  Basic Dynatrace -  Basic AWS (Amazon Web Services) -  Basic || Empresa .....:  WA FENIX IT SERVICES  SOLUTIONS</t>
+        </is>
+      </c>
+      <c r="I755" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>04/02/2026</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t>83563</t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>Especialista DBA SQL</t>
+        </is>
+      </c>
+      <c r="D756" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E756" t="inlineStr">
+        <is>
+          <t>Híbrido</t>
+        </is>
+      </c>
+      <c r="F756" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 04/02/26</t>
+        </is>
+      </c>
+      <c r="G756" t="inlineStr">
+        <is>
+          <t>Especialista DBA SQL  Modelo: Híbrido (3x presencial na semana) – São Paulo/SP - Morumbi Prazo de Projeto: 2 meses Regime de contrato: PJ  Principais requisitos: DBA SQL Server avançado Forte atuação em tuning e performance (queries, índices, particionamento) Experiência com configuração e otimização de ambiente SQL Server Conhecimento em SQL / T-SQL / PowerShell Experiência com criptografia de dados Vivência com SSIS e SSRS  Necessário: Inglês avançado para conversação  Enviar o currículo em português e inglês.
+Empresa .....:  ITeam</t>
+        </is>
+      </c>
+      <c r="H756" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 04/02/26 || Especialista DBA SQL || Especialista DBA SQL  Modelo: Híbrido (3x presencial na semana) – São Paulo/SP - Morumbi Prazo de Projeto: 2 meses Regime de contrato: PJ  Principais requisitos: DBA SQL Server avançado Forte atuação em tuning e performance (queries, índices, particionamento) Experiência com configuração e otimização de ambiente SQL Server Conhecimento em SQL / T-SQL / PowerShell Experiência com criptografia de dados Vivência com SSIS e SSRS  Necessário: Inglês avançado para conversação  Enviar o currículo em português e inglês. || Empresa .....:  ITeam</t>
+        </is>
+      </c>
+      <c r="I756" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>04/02/2026</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t>83561</t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>Especialista Desenvolvedor Java Sênior (híbrido)</t>
+        </is>
+      </c>
+      <c r="D757" t="inlineStr">
+        <is>
+          <t>Sênior</t>
+        </is>
+      </c>
+      <c r="E757" t="inlineStr">
+        <is>
+          <t>Híbrido</t>
+        </is>
+      </c>
+      <c r="F757" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 04/02/26</t>
+        </is>
+      </c>
+      <c r="G757" t="inlineStr">
+        <is>
+          <t>Função: Especialista Desenvolvedor Java Sênior Nivel: Sênior Local: Híbrido  Idioma: Proficiência em inglês, escrito e falado, necessária para comunicação eficaz em um ambiente internacional (mínimo nível B2)  Período: 12 meses ( possibilidade de prorrogação)  Requisitos obrigatórios: •	Experiência prática em desenvolvimento Java em tempo real, com histórico comprovado na entrega de soluções robustas e de alto desempenho •	Experiência sólida com GitHub e JaCoCo (Java Code Coverage).  Experiência altamente desejável: •	Experiência comprovada na implementação de soluções utilizando o produto Caplin •	Experiência sólida com o protocolo FIX, incluindo desenho e implementação de integrações baseadas em FIX.  Competências desejáveis: •	Experiência prática com Node.js, especialmente em contextos financeiros
+Empresa .....:  WA Fênix IT Service  Solutions</t>
+        </is>
+      </c>
+      <c r="H757" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 04/02/26 || Especialista Desenvolvedor Java Sênior (híbrido) || Função: Especialista Desenvolvedor Java Sênior Nivel: Sênior Local: Híbrido  Idioma: Proficiência em inglês, escrito e falado, necessária para comunicação eficaz em um ambiente internacional (mínimo nível B2)  Período: 12 meses ( possibilidade de prorrogação)  Requisitos obrigatórios: •	Experiência prática em desenvolvimento Java em tempo real, com histórico comprovado na entrega de soluções robustas e de alto desempenho •	Experiência sólida com GitHub e JaCoCo (Java Code Coverage).  Experiência altamente desejável: •	Experiência comprovada na implementação de soluções utilizando o produto Caplin •	Experiência sólida com o protocolo FIX, incluindo desenho e implementação de integrações baseadas em FIX.  Competências desejáveis: •	Experiência prática com Node.js, especialmente em contextos financeiros || Empresa .....:  WA Fênix IT Service  Solutions</t>
+        </is>
+      </c>
+      <c r="I757" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>04/02/2026</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t>82961</t>
+        </is>
+      </c>
+      <c r="C758" t="inlineStr">
+        <is>
+          <t>Gerente de Projeto de TI</t>
+        </is>
+      </c>
+      <c r="D758" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E758" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F758" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 04/02/26</t>
+        </is>
+      </c>
+      <c r="G758" t="inlineStr">
+        <is>
+          <t>Requisitos: Graduação obrigatória em áreas de Exatas: TI, Engenharia da Computação, Ciência da Computação, Física, Química, Matemática, Estatística, Análise de Sistemas ou correlatas  Conhecimentos técnicos: PMBOK (ênfase em WBS) Modelagem Relacional e Não Relacional (SQL / NoSQL) Métricas de Qualidade de Software e testes automatizados  Responsabilidades Planejar, executar e controlar projetos de TI (metodologia PMI) Gerenciar problemas, promovendo colaboração e comunicação eficaz Coleta de requisitos, gestão de escopo, WBS e cronogramas Interface entre TI e áreas de negócio / stakeholders Priorizar demandas junto à diretoria Gestão de portfólio de projetos (sistemas, infraestrutura e fornecedores) Reportes executivos semanais (status, riscos e recomendações) Garantir entregas, ajustando escopo, prazos e recursos Alinhamento de times internos e parceiros externos Condução de reuniões mensais de performance Atuação em Governança e Compliance
+Empresa .....:  Ivo Services</t>
+        </is>
+      </c>
+      <c r="H758" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 04/02/26 || Gerente de Projeto de TI || Requisitos: Graduação obrigatória em áreas de Exatas: TI, Engenharia da Computação, Ciência da Computação, Física, Química, Matemática, Estatística, Análise de Sistemas ou correlatas  Conhecimentos técnicos: PMBOK (ênfase em WBS) Modelagem Relacional e Não Relacional (SQL / NoSQL) Métricas de Qualidade de Software e testes automatizados  Responsabilidades Planejar, executar e controlar projetos de TI (metodologia PMI) Gerenciar problemas, promovendo colaboração e comunicação eficaz Coleta de requisitos, gestão de escopo, WBS e cronogramas Interface entre TI e áreas de negócio / stakeholders Priorizar demandas junto à diretoria Gestão de portfólio de projetos (sistemas, infraestrutura e fornecedores) Reportes executivos semanais (status, riscos e recomendações) Garantir entregas, ajustando escopo, prazos e recursos Alinhamento de times internos e parceiros externos Condução de reuniões mensais de performance Atuação em Governança e Compliance || Empresa .....:  Ivo Services</t>
+        </is>
+      </c>
+      <c r="I758" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>04/02/2026</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t>83570</t>
+        </is>
+      </c>
+      <c r="C759" t="inlineStr">
+        <is>
+          <t>Gerente de Projeto de TI</t>
+        </is>
+      </c>
+      <c r="D759" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E759" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F759" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 04/02/26</t>
+        </is>
+      </c>
+      <c r="G759" t="inlineStr">
+        <is>
+          <t>Vaga: Especialista em Gestão de Projetos de TI Atuação híbrida (2 dias home office e 3 presenciais – Zona Leste e Zona Sul/SP), modelo cooperado, com informar pretensão salarial.  Responsável por planejar, executar e controlar projetos de TI com base na metodologia PMI, atuando na coleta de requisitos, gestão de escopo, WBS, cronograma, orçamento e riscos. Fará a interface entre TI e áreas de negócio, apoiando a diretoria na priorização de demandas e garantindo o alinhamento estratégico dos projetos.  Atuará na gestão do portfólio de projetos, acompanhamento de parceiros externos, governança e compliance, além da elaboração de reportes executivos semanais com indicadores, riscos e ajustes necessários para garantir a entrega dos projetos.  Requisitos: graduação em TI ou áreas de exatas, domínio de PMBOK/WBS, conhecimentos em SQL e NoSQL, métricas de qualidade de software, boa comunicação, organização, foco em resultados e inglês intermediário.
+Empresa .....:  IVO SERVICES TECH RECRUIT</t>
+        </is>
+      </c>
+      <c r="H759" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 04/02/26 || Gerente de Projeto de TI || Vaga: Especialista em Gestão de Projetos de TI Atuação híbrida (2 dias home office e 3 presenciais – Zona Leste e Zona Sul/SP), modelo cooperado, com informar pretensão salarial.  Responsável por planejar, executar e controlar projetos de TI com base na metodologia PMI, atuando na coleta de requisitos, gestão de escopo, WBS, cronograma, orçamento e riscos. Fará a interface entre TI e áreas de negócio, apoiando a diretoria na priorização de demandas e garantindo o alinhamento estratégico dos projetos.  Atuará na gestão do portfólio de projetos, acompanhamento de parceiros externos, governança e compliance, além da elaboração de reportes executivos semanais com indicadores, riscos e ajustes necessários para garantir a entrega dos projetos.  Requisitos: graduação em TI ou áreas de exatas, domínio de PMBOK/WBS, conhecimentos em SQL e NoSQL, métricas de qualidade de software, boa comunicação, organização, foco em resultados e inglês intermediário. || Empresa .....:  IVO SERVICES TECH RECRUIT</t>
+        </is>
+      </c>
+      <c r="I759" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>04/02/2026</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t>82246</t>
+        </is>
+      </c>
+      <c r="C760" t="inlineStr">
+        <is>
+          <t>PM / PO Especialista - Híbrido SP</t>
+        </is>
+      </c>
+      <c r="D760" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E760" t="inlineStr">
+        <is>
+          <t>Híbrido</t>
+        </is>
+      </c>
+      <c r="F760" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 04/02/26</t>
+        </is>
+      </c>
+      <c r="G760" t="inlineStr">
+        <is>
+          <t>Estamos em busca de um(a) Product Owner. Para atuar em uma das maiores empresas varejista farmacêutica do Brasil.  Profissional será responsável por liderar estratégias de produto e inovação, com foco em identificar oportunidades de crescimento, estruturar hipóteses de negócio e traduzir insights em soluções de alto impacto. Atuará na coordenação de múltiplos squads, garantindo alinhamento entre as áreas de produto, design e tecnologia, além de gerenciar indicadores (OKRs, KPIs) e assegurar entregas com eficiência e coerência estratégica. Deverá promover uma liderança colaborativa e orientada por dados, facilitando processos de discovery, prototipagem e validação de ideias, sempre equilibrando valor ao usuário e viabilidade técnica. O papel também exige forte capacidade de comunicação e influência, elaborando apresentações executivas, relatórios e narrativas estratégicas para o C-Level. Experiência com IA generativa, Team Topologies, DevOps, dual-track agile.
+Empresa .....:  3CON Consultoria e Sistemas S/A</t>
+        </is>
+      </c>
+      <c r="H760" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 04/02/26 || PM / PO Especialista - Híbrido SP || Estamos em busca de um(a) Product Owner. Para atuar em uma das maiores empresas varejista farmacêutica do Brasil.  Profissional será responsável por liderar estratégias de produto e inovação, com foco em identificar oportunidades de crescimento, estruturar hipóteses de negócio e traduzir insights em soluções de alto impacto. Atuará na coordenação de múltiplos squads, garantindo alinhamento entre as áreas de produto, design e tecnologia, além de gerenciar indicadores (OKRs, KPIs) e assegurar entregas com eficiência e coerência estratégica. Deverá promover uma liderança colaborativa e orientada por dados, facilitando processos de discovery, prototipagem e validação de ideias, sempre equilibrando valor ao usuário e viabilidade técnica. O papel também exige forte capacidade de comunicação e influência, elaborando apresentações executivas, relatórios e narrativas estratégicas para o C-Level. Experiência com IA generativa, Team Topologies, DevOps, dual-track agile. || Empresa .....:  3CON Consultoria e Sistemas S/A</t>
+        </is>
+      </c>
+      <c r="I760" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>04/02/2026</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t>82414</t>
+        </is>
+      </c>
+      <c r="C761" t="inlineStr">
+        <is>
+          <t>PMO - Seguros</t>
+        </is>
+      </c>
+      <c r="D761" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E761" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F761" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 04/02/26</t>
+        </is>
+      </c>
+      <c r="G761" t="inlineStr">
+        <is>
+          <t>Experiência em PMO ou gestão de projetos no setor segurador. Conhecimento em ferramentas de gestão: MS Project, Jira, Confluence, Power BI. Familiaridade com normas regulatórias do setor de seguros (ex.: SUSEP, Solvência II).  Atuaando no planejamento, monitoramento e otimização de projetos, colaborando com equipes multidisciplinares e stakeholders de alto nível.  Responsabilidades principais: Atuar como ponto central para governança de projetos, garantindo alinhamento com as diretrizes corporativas e regulatórias do setor de seguros. Desenvolver e manter metodologias, templates e indicadores de performance (KPIs) para gestão de projetos. Coordenar reuniões de status, reportando progresso, riscos e planos de mitigação para stakeholders internos e externos. Garantir comunicação clara e eficaz em inglês e espanhol com equipes globais, fornecedores e parceiros. Apoiar a integração de sistemas e processos relacionados a seguros, compliance e gestão de riscos.  Presencial/PJ
+Empresa .....:  GlobalTI</t>
+        </is>
+      </c>
+      <c r="H761" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 04/02/26 || PMO - Seguros || Experiência em PMO ou gestão de projetos no setor segurador. Conhecimento em ferramentas de gestão: MS Project, Jira, Confluence, Power BI. Familiaridade com normas regulatórias do setor de seguros (ex.: SUSEP, Solvência II).  Atuaando no planejamento, monitoramento e otimização de projetos, colaborando com equipes multidisciplinares e stakeholders de alto nível.  Responsabilidades principais: Atuar como ponto central para governança de projetos, garantindo alinhamento com as diretrizes corporativas e regulatórias do setor de seguros. Desenvolver e manter metodologias, templates e indicadores de performance (KPIs) para gestão de projetos. Coordenar reuniões de status, reportando progresso, riscos e planos de mitigação para stakeholders internos e externos. Garantir comunicação clara e eficaz em inglês e espanhol com equipes globais, fornecedores e parceiros. Apoiar a integração de sistemas e processos relacionados a seguros, compliance e gestão de riscos.  Presencial/PJ || Empresa .....:  GlobalTI</t>
+        </is>
+      </c>
+      <c r="I761" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>04/02/2026</t>
+        </is>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t>83560</t>
+        </is>
+      </c>
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>PROGRAMADOR</t>
+        </is>
+      </c>
+      <c r="D762" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E762" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F762" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 04/02/26</t>
+        </is>
+      </c>
+      <c r="G762" t="inlineStr">
+        <is>
+          <t>Atuar no desenvolvimento e manutenção de sistemas, analisando as especificações funcionais e técnicas do produto para compreender as necessidades de desenvolvimento, esclarecer dúvidas e alinhar o escopo junto ao Analista de Sistemas. Desmembrar funcionalidades em etapas, estimar prazos, registrar tarefas no sistema SSA e elaborar código, banco de dados, tabelas, scripts e demais componentes necessários. Realizar testes unitários para garantir qualidade, consistência e integridade das funcionalidades, registrar comentários no código e no TFS, gerar versões do projeto, publicar, liberar para testes e realizar ajustes conforme especificações. Utilizar linguagens e tecnologias como ASP Clássico (VB), C#/.NET Core, ASP.NET MVC, Razor, WebForms, JavaScript, HTML5, CSS3, jQuery, SOAP, REST, Web APIs, Bootstrap, Entity Framework, Dapper e SQL Server.  Enviar cv com pretensão salarial CLT E PJ.
+Empresa .....:  CH MASTER DATA</t>
+        </is>
+      </c>
+      <c r="H762" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 04/02/26 || PROGRAMADOR || Atuar no desenvolvimento e manutenção de sistemas, analisando as especificações funcionais e técnicas do produto para compreender as necessidades de desenvolvimento, esclarecer dúvidas e alinhar o escopo junto ao Analista de Sistemas. Desmembrar funcionalidades em etapas, estimar prazos, registrar tarefas no sistema SSA e elaborar código, banco de dados, tabelas, scripts e demais componentes necessários. Realizar testes unitários para garantir qualidade, consistência e integridade das funcionalidades, registrar comentários no código e no TFS, gerar versões do projeto, publicar, liberar para testes e realizar ajustes conforme especificações. Utilizar linguagens e tecnologias como ASP Clássico (VB), C#/.NET Core, ASP.NET MVC, Razor, WebForms, JavaScript, HTML5, CSS3, jQuery, SOAP, REST, Web APIs, Bootstrap, Entity Framework, Dapper e SQL Server.  Enviar cv com pretensão salarial CLT E PJ. || Empresa .....:  CH MASTER DATA</t>
+        </is>
+      </c>
+      <c r="I762" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>04/02/2026</t>
+        </is>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t>83559</t>
+        </is>
+      </c>
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>PROGRAMADOR ASP.CLASSICO</t>
+        </is>
+      </c>
+      <c r="D763" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E763" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F763" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 04/02/26</t>
+        </is>
+      </c>
+      <c r="G763" t="inlineStr">
+        <is>
+          <t>Atuar no desenvolvimento e manutenção de sistemas, analisando as especificações funcionais e técnicas do produto para compreender as necessidades de desenvolvimento, esclarecer dúvidas e alinhar o escopo junto ao Analista de Sistemas. Desmembrar funcionalidades em etapas, estimar prazos, registrar tarefas no sistema SSA e elaborar código, banco de dados, tabelas, scripts e demais componentes necessários. Realizar testes unitários para garantir qualidade, consistência e integridade das funcionalidades, registrar comentários no código e no TFS, gerar versões do projeto, publicar, liberar para testes e realizar ajustes conforme especificações. Utilizar linguagens e tecnologias como ASP Clássico (VB), C#/.NET Core, ASP.NET MVC, Razor, WebForms, JavaScript, HTML5, CSS3, jQuery, SOAP, REST, Web APIs, Bootstrap, Entity Framework, Dapper e SQL Server.  Enviar cv com pretensão salarial CLT E PJ.
+Empresa .....:  CH MASTER DATA</t>
+        </is>
+      </c>
+      <c r="H763" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 04/02/26 || PROGRAMADOR ASP.CLASSICO || Atuar no desenvolvimento e manutenção de sistemas, analisando as especificações funcionais e técnicas do produto para compreender as necessidades de desenvolvimento, esclarecer dúvidas e alinhar o escopo junto ao Analista de Sistemas. Desmembrar funcionalidades em etapas, estimar prazos, registrar tarefas no sistema SSA e elaborar código, banco de dados, tabelas, scripts e demais componentes necessários. Realizar testes unitários para garantir qualidade, consistência e integridade das funcionalidades, registrar comentários no código e no TFS, gerar versões do projeto, publicar, liberar para testes e realizar ajustes conforme especificações. Utilizar linguagens e tecnologias como ASP Clássico (VB), C#/.NET Core, ASP.NET MVC, Razor, WebForms, JavaScript, HTML5, CSS3, jQuery, SOAP, REST, Web APIs, Bootstrap, Entity Framework, Dapper e SQL Server.  Enviar cv com pretensão salarial CLT E PJ. || Empresa .....:  CH MASTER DATA</t>
+        </is>
+      </c>
+      <c r="I763" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>04/02/2026</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t>83575</t>
+        </is>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>SAP FICO - VERTEX</t>
+        </is>
+      </c>
+      <c r="D764" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E764" t="inlineStr">
+        <is>
+          <t>Híbrido</t>
+        </is>
+      </c>
+      <c r="F764" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 04/02/26</t>
+        </is>
+      </c>
+      <c r="G764" t="inlineStr">
+        <is>
+          <t>Oportunidade para atuar com foco em integração de soluções fiscais e configuração de módulos financeiros em ambiente SAP.  Principais Responsabilidades: Integração Vertex: Configurar e suportar o Vertex (Tax Product Category, Tax Assist Rules) no S/4HANA ou ECC para cálculos de Sales  Use Tax e VAT.  Configuração FICO: Atuar em nível avançado nos sub-módulos GL, AP, AR, Asset Accounting e CCA/CO-PA.  Gestão de Requisitos Fiscais: Traduzir necessidades de negócio em especificações técnicas, garantindo conformidade com regulamentações globais e locais.  Liderança Funcional: Comandar o design, testes (SIT/UAT) e troubleshoot de APIs e Web Services entre SAP e Vertex.  Colaboração: Alinhamento com os times de SD (O2C) e MM (P2P) para determinação de impostos.  Requisitos: Inglês Avançado (imprescindível para conversação).  Modelo de trabalho Híbrido em São Paulo (SP).
+Empresa .....:  Randstad Brasil Recursos Humanos LTDA</t>
+        </is>
+      </c>
+      <c r="H764" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 04/02/26 || SAP FICO - VERTEX || Oportunidade para atuar com foco em integração de soluções fiscais e configuração de módulos financeiros em ambiente SAP.  Principais Responsabilidades: Integração Vertex: Configurar e suportar o Vertex (Tax Product Category, Tax Assist Rules) no S/4HANA ou ECC para cálculos de Sales  Use Tax e VAT.  Configuração FICO: Atuar em nível avançado nos sub-módulos GL, AP, AR, Asset Accounting e CCA/CO-PA.  Gestão de Requisitos Fiscais: Traduzir necessidades de negócio em especificações técnicas, garantindo conformidade com regulamentações globais e locais.  Liderança Funcional: Comandar o design, testes (SIT/UAT) e troubleshoot de APIs e Web Services entre SAP e Vertex.  Colaboração: Alinhamento com os times de SD (O2C) e MM (P2P) para determinação de impostos.  Requisitos: Inglês Avançado (imprescindível para conversação).  Modelo de trabalho Híbrido em São Paulo (SP). || Empresa .....:  Randstad Brasil Recursos Humanos LTDA</t>
+        </is>
+      </c>
+      <c r="I764" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>04/02/2026</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t>82859</t>
+        </is>
+      </c>
+      <c r="C765" t="inlineStr">
+        <is>
+          <t>Supervisor de Operações de TI</t>
+        </is>
+      </c>
+      <c r="D765" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E765" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F765" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 04/02/26</t>
+        </is>
+      </c>
+      <c r="G765" t="inlineStr">
+        <is>
+          <t>Gestão de Equipes: Liderar, treinar e coordenar Técnicos de Suporte Jr. l, ll, e lll. Conhecimento em gestão de quadro de funcionários, dimensionamento por demanda. Conhecimento em gestão de escala de trabalho de colaboradores. Infraestrutura: Supervisionar servidores, redes (LAN/WAN), bancos de dados, storage, backup e segurança (firewall, antivírus). Suporte Técnico: Gerenciar a equipe de suporte (help desk), garantindo a resolução rápida de problemas (preventiva e corretiva). Conhecimento em gestão de tickets e dimensionamento de chamados e SLA. Segurança da Informação: Fazer cumprir políticas de segurança e monitorar o controle de acesso e dados. Relacionamento com o Negócio: Identificar necessidades e propor soluções tecnológicas alinhadas aos objetivos da empresa.  Formação: Graduação em Ciência da Computação, Sistemas de Informação ou áreas correlatas. Metodologias: Conhecimento em ITIL e COBIT é um diferencial.
+Empresa .....:  randstad Brasil</t>
+        </is>
+      </c>
+      <c r="H765" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 04/02/26 || Supervisor de Operações de TI || Gestão de Equipes: Liderar, treinar e coordenar Técnicos de Suporte Jr. l, ll, e lll. Conhecimento em gestão de quadro de funcionários, dimensionamento por demanda. Conhecimento em gestão de escala de trabalho de colaboradores. Infraestrutura: Supervisionar servidores, redes (LAN/WAN), bancos de dados, storage, backup e segurança (firewall, antivírus). Suporte Técnico: Gerenciar a equipe de suporte (help desk), garantindo a resolução rápida de problemas (preventiva e corretiva). Conhecimento em gestão de tickets e dimensionamento de chamados e SLA. Segurança da Informação: Fazer cumprir políticas de segurança e monitorar o controle de acesso e dados. Relacionamento com o Negócio: Identificar necessidades e propor soluções tecnológicas alinhadas aos objetivos da empresa.  Formação: Graduação em Ciência da Computação, Sistemas de Informação ou áreas correlatas. Metodologias: Conhecimento em ITIL e COBIT é um diferencial. || Empresa .....:  randstad Brasil</t>
+        </is>
+      </c>
+      <c r="I765" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>04/02/2026</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t>82430</t>
+        </is>
+      </c>
+      <c r="C766" t="inlineStr">
+        <is>
+          <t>Supervisor de Service Desk - DrJoe Technology</t>
+        </is>
+      </c>
+      <c r="D766" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E766" t="inlineStr">
+        <is>
+          <t>Híbrido</t>
+        </is>
+      </c>
+      <c r="F766" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 04/02/26</t>
+        </is>
+      </c>
+      <c r="G766" t="inlineStr">
+        <is>
+          <t>- Gestão de equipe: Liderar o time de Service Desk (Níveis 1 e 2) com foco em desenvolvimento e resultados - Monitoramento de SLA: Acompanhar indicadores de performance e garantir cumprimento dos acordos com clientes - Melhoria contínua: Garantir aderência aos procedimentos operacionais e propor melhorias nos processos - Suporte técnico ativo: Apoiar o time no atendimento de Nível 1 e 2 quando necessário - Controle de qualidade: Realizar análises de qualidade e gerar relatórios de performance - Relacionamento consultivo: Manter proximidade com clientes, atuando como braço direito nas demandas de TI  Perfil Ideal: - Formação: Curso técnico completo em TI (ou equivalente). Certificações ITIL, HDI ou similares, experiência em gestão de Service Desk e como você pode contribuiu serão diferenciais - Experiência: 2-3 anos em suporte técnico ou coordenação de Service Desk  Salário: R$ 3.000,00 / CLT / Plano Médico /  VR e VT /   Híbrido  Pleno (3-5 anos de experiência)
+Empresa .....:  DrJoe</t>
+        </is>
+      </c>
+      <c r="H766" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 04/02/26 || Supervisor de Service Desk - DrJoe Technology || - Gestão de equipe: Liderar o time de Service Desk (Níveis 1 e 2) com foco em desenvolvimento e resultados - Monitoramento de SLA: Acompanhar indicadores de performance e garantir cumprimento dos acordos com clientes - Melhoria contínua: Garantir aderência aos procedimentos operacionais e propor melhorias nos processos - Suporte técnico ativo: Apoiar o time no atendimento de Nível 1 e 2 quando necessário - Controle de qualidade: Realizar análises de qualidade e gerar relatórios de performance - Relacionamento consultivo: Manter proximidade com clientes, atuando como braço direito nas demandas de TI  Perfil Ideal: - Formação: Curso técnico completo em TI (ou equivalente). Certificações ITIL, HDI ou similares, experiência em gestão de Service Desk e como você pode contribuiu serão diferenciais - Experiência: 2-3 anos em suporte técnico ou coordenação de Service Desk  Salário: R$ 3.000,00 / CLT / Plano Médico /  VR e VT /   Híbrido  Pleno (3-5 anos de experiência) || Empresa .....:  DrJoe</t>
+        </is>
+      </c>
+      <c r="I766" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>04/02/2026</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t>83551</t>
+        </is>
+      </c>
+      <c r="C767" t="inlineStr">
+        <is>
+          <t>Analista de Gestão de Ativos</t>
+        </is>
+      </c>
+      <c r="D767" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E767" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F767" t="inlineStr">
+        <is>
+          <t>Barueri - SP - 03/02/26</t>
+        </is>
+      </c>
+      <c r="G767" t="inlineStr">
+        <is>
+          <t>Responsável pela gestão, controle e governança dos ativos de TI, assegurando a rastreabilidade, disponibilidade e uso adequado de equipamentos e recursos tecnológicos. Atuar de forma integrada com o time de TI, suprimentos e áreas de negócio, realizando o controle de estoque, ciclo de vida dos ativos e planejamento de necessidades, garantindo eficiência operacional, redução de custos e conformidade com políticas internas de forma Corporativa para todas as Unidades.
+Empresa .....:  Mk Tech</t>
+        </is>
+      </c>
+      <c r="H767" t="inlineStr">
+        <is>
+          <t>Barueri - SP - 03/02/26 || Analista de Gestão de Ativos || Responsável pela gestão, controle e governança dos ativos de TI, assegurando a rastreabilidade, disponibilidade e uso adequado de equipamentos e recursos tecnológicos. Atuar de forma integrada com o time de TI, suprimentos e áreas de negócio, realizando o controle de estoque, ciclo de vida dos ativos e planejamento de necessidades, garantindo eficiência operacional, redução de custos e conformidade com políticas internas de forma Corporativa para todas as Unidades. || Empresa .....:  Mk Tech</t>
+        </is>
+      </c>
+      <c r="I767" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>04/02/2026</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t>82613</t>
+        </is>
+      </c>
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>Arquiteto de Soluções  Oracle</t>
+        </is>
+      </c>
+      <c r="D768" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E768" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F768" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 03/02/26</t>
+        </is>
+      </c>
+      <c r="G768" t="inlineStr">
+        <is>
+          <t>Somos a Randstad, líder global em soluções de Recursos Humanos. Unimos tecnologia e paixão por pessoas para conectar talentos às melhores oportunidades no mundo todo.  Com mais de 65 anos de experiência, presença em 39 países e uma equipe de 40.000 profissionais, ajudamos milhões de pessoas a conquistar novos desafios e centenas de milhares de empresas a encontrar os talentos ideais.  Agora, temos uma oportunidade imperdível para um de nossos clientes e buscamos profissionais com o seguinte perfil: Arquiteto Oracle  O Arquiteto de Soluções Oracle liderará a estratégia, o design e a implementação de arquiteturas complexas baseadas em tecnologias Oracle, sendo responsável por garantir que as soluções de banco de dados, middleware e aplicações sejam escaláveis, seguras e alinhadas com as necessidades de negócio.  Tem interesse em saber mais? Envia seu curriculo
+Empresa .....:  Randstad</t>
+        </is>
+      </c>
+      <c r="H768" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 03/02/26 || Arquiteto de Soluções  Oracle || Somos a Randstad, líder global em soluções de Recursos Humanos. Unimos tecnologia e paixão por pessoas para conectar talentos às melhores oportunidades no mundo todo.  Com mais de 65 anos de experiência, presença em 39 países e uma equipe de 40.000 profissionais, ajudamos milhões de pessoas a conquistar novos desafios e centenas de milhares de empresas a encontrar os talentos ideais.  Agora, temos uma oportunidade imperdível para um de nossos clientes e buscamos profissionais com o seguinte perfil: Arquiteto Oracle  O Arquiteto de Soluções Oracle liderará a estratégia, o design e a implementação de arquiteturas complexas baseadas em tecnologias Oracle, sendo responsável por garantir que as soluções de banco de dados, middleware e aplicações sejam escaláveis, seguras e alinhadas com as necessidades de negócio.  Tem interesse em saber mais? Envia seu curriculo || Empresa .....:  Randstad</t>
+        </is>
+      </c>
+      <c r="I768" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>04/02/2026</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t>82661</t>
+        </is>
+      </c>
+      <c r="C769" t="inlineStr">
+        <is>
+          <t>Desenvolvedor Python com IA</t>
+        </is>
+      </c>
+      <c r="D769" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E769" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F769" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 03/02/26</t>
+        </is>
+      </c>
+      <c r="G769" t="inlineStr">
+        <is>
+          <t>Desenvolvimento de soluções avançadas de machine learning, incluindo modelos de processamento de linguagem natural (NLP) e modelos baseados em Inteligência Artificial Generativa (LLM, GPT, LLaMA etc).  Desenvolvimento de modelos utilizando APIs de IA Generativa, como OpenAI, Ollama, entre outras. Desenvolvimento de software em Python Criação de documentação detalhada dos projeto  Experiência com Machine Learning, com ênfase em Deep Learning e NLP/NLU. Familiaridade com APIs de IA Generativa, especialmente Azure OpenAI (GPT), Ollama. Experiência em Arquitetura de Retrieval Augmented Generation (RAG).  Conhecimento técnico abrangente de Machine Learning e Deep Learning, especialmente relacionado a LLMs. Experiência com o framework LangChain. Habilidade em programação Python e análise de dados.  Experiência com frameworks de aprendizado profundo como TensorFlow, PyTorch ou Scikit-learn. Experiência no deploy de modelos em produção.
+Empresa .....:  K2 Partnering</t>
+        </is>
+      </c>
+      <c r="H769" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 03/02/26 || Desenvolvedor Python com IA || Desenvolvimento de soluções avançadas de machine learning, incluindo modelos de processamento de linguagem natural (NLP) e modelos baseados em Inteligência Artificial Generativa (LLM, GPT, LLaMA etc).  Desenvolvimento de modelos utilizando APIs de IA Generativa, como OpenAI, Ollama, entre outras. Desenvolvimento de software em Python Criação de documentação detalhada dos projeto  Experiência com Machine Learning, com ênfase em Deep Learning e NLP/NLU. Familiaridade com APIs de IA Generativa, especialmente Azure OpenAI (GPT), Ollama. Experiência em Arquitetura de Retrieval Augmented Generation (RAG).  Conhecimento técnico abrangente de Machine Learning e Deep Learning, especialmente relacionado a LLMs. Experiência com o framework LangChain. Habilidade em programação Python e análise de dados.  Experiência com frameworks de aprendizado profundo como TensorFlow, PyTorch ou Scikit-learn. Experiência no deploy de modelos em produção. || Empresa .....:  K2 Partnering</t>
+        </is>
+      </c>
+      <c r="I769" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>04/02/2026</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t>83549</t>
+        </is>
+      </c>
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>Analista de Suporte Jr</t>
+        </is>
+      </c>
+      <c r="D770" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E770" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F770" t="inlineStr">
+        <is>
+          <t>Santo André - SP - 03/02/26</t>
+        </is>
+      </c>
+      <c r="G770" t="inlineStr">
+        <is>
+          <t>ATIVIDADES Atendimento a tickets de Suporte a Computadores e Usuários, ser o elo entre os usuários e o time de terceiro Nível para a resolução dos problemas, monitoramento de aplicações, manutenção preventiva em desktop e laptops, formatação de computadores, instalação de aplicativos/impressoras e atualizado da documentação.  FORMAÇÃO Estar cursando ou concluída a Graduação nas áreas de Tecnologia Curso de Montagem e Manutenção de Computadores (será um diferencial).  EXPERIÊNCIA 6 Meses no Mínimo  BENEFÍCIOS Salário: R$2.410,00 (mês) Vale Transporte, Vale Alimentação e Refeição, TotalPass (Gympass), Starbem (Plataforma de acesso a psicólogos e nutricionistas), Avus (descontos em consultas presenciais, exames e farmácias), Plano de Saúde e odontológico, Seguro de Vida, além de Treinamentos em cursos oficiais da Microsoft.  Local: Santo André – SP. Formato de trabalho: Presencial. Horário: Segunda à sexta-feira, das 09h00 às 18h00.
+Empresa .....:  TC do Brasil</t>
+        </is>
+      </c>
+      <c r="H770" t="inlineStr">
+        <is>
+          <t>Santo André - SP - 03/02/26 || Analista de Suporte Jr || ATIVIDADES Atendimento a tickets de Suporte a Computadores e Usuários, ser o elo entre os usuários e o time de terceiro Nível para a resolução dos problemas, monitoramento de aplicações, manutenção preventiva em desktop e laptops, formatação de computadores, instalação de aplicativos/impressoras e atualizado da documentação.  FORMAÇÃO Estar cursando ou concluída a Graduação nas áreas de Tecnologia Curso de Montagem e Manutenção de Computadores (será um diferencial).  EXPERIÊNCIA 6 Meses no Mínimo  BENEFÍCIOS Salário: R$2.410,00 (mês) Vale Transporte, Vale Alimentação e Refeição, TotalPass (Gympass), Starbem (Plataforma de acesso a psicólogos e nutricionistas), Avus (descontos em consultas presenciais, exames e farmácias), Plano de Saúde e odontológico, Seguro de Vida, além de Treinamentos em cursos oficiais da Microsoft.  Local: Santo André – SP. Formato de trabalho: Presencial. Horário: Segunda à sexta-feira, das 09h00 às 18h00. || Empresa .....:  TC do Brasil</t>
+        </is>
+      </c>
+      <c r="I770" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>04/02/2026</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t>82317</t>
+        </is>
+      </c>
+      <c r="C771" t="inlineStr">
+        <is>
+          <t>Analista de Infraenstrutura Senior</t>
+        </is>
+      </c>
+      <c r="D771" t="inlineStr">
+        <is>
+          <t>Sênior</t>
+        </is>
+      </c>
+      <c r="E771" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F771" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 03/02/26</t>
+        </is>
+      </c>
+      <c r="G771" t="inlineStr">
+        <is>
+          <t>Experiência em instalação, administração e manutenção de servidores nos sistemas operacionais Windows e Linux (RedHat/SuSE/Ubuntu – diferentes distribuições e versões) Experiência em administração de Windows Server: PowerShell Scripting, Active Directory, DNS, DHCP, Print Server, Terminal Server, IIS, File Server, Certificados Digitais, Load Balancers, GPO (Group Policy)  Experiência em administração de servidores Linux: BASH Scripting, LVM, SSH, SFTP, HTTP, HTTPS, NTP, SMTP, DNS, Clusters (Pace Maker / RHCL / SUSE Cluster), configuração de Multipath Experiência com storages DELL/EMC e switches SAN HPE/Brocade (será um diferencial)  Capacidade de identificar problemas, analisar causas e aplicar resolução Documentar configurações e implementações realizadas no dia a dia, relacionadas à administração de sistemas operacionais e mudanças implementadas  Conhecimento na elaboração de relatórios de capacidade dos ambientes Atendimento a chamados Inglês para conversação.
+Empresa .....:  Ewave do Brasil</t>
+        </is>
+      </c>
+      <c r="H771" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 03/02/26 || Analista de Infraenstrutura Senior || Experiência em instalação, administração e manutenção de servidores nos sistemas operacionais Windows e Linux (RedHat/SuSE/Ubuntu – diferentes distribuições e versões) Experiência em administração de Windows Server: PowerShell Scripting, Active Directory, DNS, DHCP, Print Server, Terminal Server, IIS, File Server, Certificados Digitais, Load Balancers, GPO (Group Policy)  Experiência em administração de servidores Linux: BASH Scripting, LVM, SSH, SFTP, HTTP, HTTPS, NTP, SMTP, DNS, Clusters (Pace Maker / RHCL / SUSE Cluster), configuração de Multipath Experiência com storages DELL/EMC e switches SAN HPE/Brocade (será um diferencial)  Capacidade de identificar problemas, analisar causas e aplicar resolução Documentar configurações e implementações realizadas no dia a dia, relacionadas à administração de sistemas operacionais e mudanças implementadas  Conhecimento na elaboração de relatórios de capacidade dos ambientes Atendimento a chamados Inglês para conversação. || Empresa .....:  Ewave do Brasil</t>
+        </is>
+      </c>
+      <c r="I771" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>04/02/2026</t>
+        </is>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t>83541</t>
+        </is>
+      </c>
+      <c r="C772" t="inlineStr">
+        <is>
+          <t>Analista de TI  (Infraestrutura e Sistemas)</t>
+        </is>
+      </c>
+      <c r="D772" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E772" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F772" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 03/02/26</t>
+        </is>
+      </c>
+      <c r="G772" t="inlineStr">
+        <is>
+          <t>Analista de Infraestrutura e Suporte  Sobre a Vaga: Buscamos um profissional dinâmico para gerir nossa infra e atuar como elo estratégico entre usuários e consultoria ERP. Ideal para quem deseja se especializar em TOTVS Protheus.  Responsabilidades: Gestão de Windows Server, AD, Azure e Microsoft 365. Segurança: Configuração de Firewall, regras de acesso e VPN. Interface Protheus: Suporte N1, diagnóstico de problemas e direcionamento técnico para consultoria externa. Suporte N2/N3 (Hardware/Software) e documentação técnica. Requisitos: Experiência mínima de 2 anos em servidores Windows e infraestrutura. Prática em Firewall e Redes (TCP/IP, DNS, DHCP). Perfil analítico e formação superior em TI. Disponibilidade para atuação Totalmente presencial em SP (Mooca).  Diferenciais: Interesse real em aprender MSSQL, linguagem ADVPL e rotinas Protheus. Proatividade e disciplina com processos.  Benefícios: VR/VA, VT, Assistência Médica/Odonto e Seguro de Vida.
+Empresa .....:  DVA COMERCIO</t>
+        </is>
+      </c>
+      <c r="H772" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 03/02/26 || Analista de TI  (Infraestrutura e Sistemas) || Analista de Infraestrutura e Suporte  Sobre a Vaga: Buscamos um profissional dinâmico para gerir nossa infra e atuar como elo estratégico entre usuários e consultoria ERP. Ideal para quem deseja se especializar em TOTVS Protheus.  Responsabilidades: Gestão de Windows Server, AD, Azure e Microsoft 365. Segurança: Configuração de Firewall, regras de acesso e VPN. Interface Protheus: Suporte N1, diagnóstico de problemas e direcionamento técnico para consultoria externa. Suporte N2/N3 (Hardware/Software) e documentação técnica. Requisitos: Experiência mínima de 2 anos em servidores Windows e infraestrutura. Prática em Firewall e Redes (TCP/IP, DNS, DHCP). Perfil analítico e formação superior em TI. Disponibilidade para atuação Totalmente presencial em SP (Mooca).  Diferenciais: Interesse real em aprender MSSQL, linguagem ADVPL e rotinas Protheus. Proatividade e disciplina com processos.  Benefícios: VR/VA, VT, Assistência Médica/Odonto e Seguro de Vida. || Empresa .....:  DVA COMERCIO</t>
+        </is>
+      </c>
+      <c r="I772" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>04/02/2026</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t>82559</t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr">
+        <is>
+          <t>Desenvolvedor Fullstack</t>
+        </is>
+      </c>
+      <c r="D773" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E773" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F773" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 03/02/26</t>
+        </is>
+      </c>
+      <c r="G773" t="inlineStr">
+        <is>
+          <t>Prazo: 3 meses, com chance de prorrogação Local: Remoto Contratação: PJ  Conhecimentos nas Linguagens e Frameworks: C#, Typescript, .NetCore, Angular8+ e React Experiência com desenvolvimento de Microsserviços, CQRS e Kafka Conhecimentos em Banco de Dados relacionais e não relacionais (SQL Server/MongoDB) Conhecimentos em metodologias ágeis (Scrum) Conhecimentos em padrões de arquitetura e práticas como: Clean Code, DDD (Domain-Drive Design), Princípios SOLID, Design Patterns, ORM (Entity Framework/Dapper), Mensageria(Kafka/RabbitMQ), CQRS e Microsserviços Conhecimentos em Docker/Containers e Kubernetes  Será considerado um diferencial: Conhecimento em ambientes Cloud (AWS, GCP, Azure, Oracle,...) Conhecimento em desenvolvimento seguro Conhecimento em AKS, EKS, K8S, Rancher
+Empresa .....:  Entrust IT</t>
+        </is>
+      </c>
+      <c r="H773" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 03/02/26 || Desenvolvedor Fullstack || Prazo: 3 meses, com chance de prorrogação Local: Remoto Contratação: PJ  Conhecimentos nas Linguagens e Frameworks: C#, Typescript, .NetCore, Angular8+ e React Experiência com desenvolvimento de Microsserviços, CQRS e Kafka Conhecimentos em Banco de Dados relacionais e não relacionais (SQL Server/MongoDB) Conhecimentos em metodologias ágeis (Scrum) Conhecimentos em padrões de arquitetura e práticas como: Clean Code, DDD (Domain-Drive Design), Princípios SOLID, Design Patterns, ORM (Entity Framework/Dapper), Mensageria(Kafka/RabbitMQ), CQRS e Microsserviços Conhecimentos em Docker/Containers e Kubernetes  Será considerado um diferencial: Conhecimento em ambientes Cloud (AWS, GCP, Azure, Oracle,...) Conhecimento em desenvolvimento seguro Conhecimento em AKS, EKS, K8S, Rancher || Empresa .....:  Entrust IT</t>
+        </is>
+      </c>
+      <c r="I773" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>04/02/2026</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t>82686</t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr">
+        <is>
+          <t>Engenheiro de Dados</t>
+        </is>
+      </c>
+      <c r="D774" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E774" t="inlineStr">
+        <is>
+          <t>Presencial/Outros</t>
+        </is>
+      </c>
+      <c r="F774" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 03/02/26</t>
+        </is>
+      </c>
+      <c r="G774" t="inlineStr">
+        <is>
+          <t>Principais Atividades: Desenvolver e manter pipelines de dados usando Airflow Otimizar consultas e estruturas no BigQuery Implementar e documentar melhorias na arquitetura de dados existente Garantir qualidade, consistência e rastreabilidade das informações Integrar dados de diferentes origens (APIs, bancos de dados, planilhas, etc.) Apoiar iniciativas de melhorias na arquitetura e padronização de dados.  Pré-Requisitos: Ensino superior completo em Engenharia da Computação, Ciência da Computação, Sistemas de Informação, Matemática, Estatística ou áreas correlatas Experiência sólida em Python para desenvolvimento de pipelines e automações Conhecimento em Airflow Domínio de SQL e BigQuery Experiência com modelagem de dados (camadas raw, bronze, silver, gold) Conhecimento em boas práticas de desenvolvimento e versionamento (Git) Noções de monitoramento de pipelines e performance de queries no GCP
+Empresa .....:  Grupo H2</t>
+        </is>
+      </c>
+      <c r="H774" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 03/02/26 || Engenheiro de Dados || Principais Atividades: Desenvolver e manter pipelines de dados usando Airflow Otimizar consultas e estruturas no BigQuery Implementar e documentar melhorias na arquitetura de dados existente Garantir qualidade, consistência e rastreabilidade das informações Integrar dados de diferentes origens (APIs, bancos de dados, planilhas, etc.) Apoiar iniciativas de melhorias na arquitetura e padronização de dados.  Pré-Requisitos: Ensino superior completo em Engenharia da Computação, Ciência da Computação, Sistemas de Informação, Matemática, Estatística ou áreas correlatas Experiência sólida em Python para desenvolvimento de pipelines e automações Conhecimento em Airflow Domínio de SQL e BigQuery Experiência com modelagem de dados (camadas raw, bronze, silver, gold) Conhecimento em boas práticas de desenvolvimento e versionamento (Git) Noções de monitoramento de pipelines e performance de queries no GCP || Empresa .....:  Grupo H2</t>
+        </is>
+      </c>
+      <c r="I774" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>04/02/2026</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t>83543</t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>SAP VIM</t>
+        </is>
+      </c>
+      <c r="D775" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="E775" t="inlineStr">
+        <is>
+          <t>Híbrido</t>
+        </is>
+      </c>
+      <c r="F775" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 03/02/26</t>
+        </is>
+      </c>
+      <c r="G775" t="inlineStr">
+        <is>
+          <t>O profissional será responsável por liderar o design, configuração e implementação de módulos OpenText SAP VIM (incluindo ICC, Enterprise Scan e OCR). O objetivo principal é otimizar o ciclo de Contas a Pagar e automação de faturas.  Principais Responsabilidades: Configurar SAP VIM e integrar com SAP ECC/S4HANA (FI/MM). Desenvolver especificações funcionais para customizações, interfaces e relatórios. Gerenciar fluxos de aprovação, exceções e suporte ponta a ponta (PO e Non-PO). Realizar testes (unitários, integrados e UAT) e ministrar treinamentos.  Requisitos Essenciais: Experiência sólida com SAP VIM/OpenText e tecnologias OCR. Domínio dos processos de SAP FI (AP) e SAP MM.  Inglês Avançado/Fluente.  Diferenciais: Conhecimento em S/4HANA, Fiori, Ariba e certificações OpenText.  Perfil: Mindset voltado à resolução de problemas, proatividade e habilidade em times multiculturais.  Híbrido em SP CLT
+Empresa .....:  Randstad Brasil Recursos Humanos LTDA</t>
+        </is>
+      </c>
+      <c r="H775" t="inlineStr">
+        <is>
+          <t>São Paulo - SP - 03/02/26 || SAP VIM || O profissional será responsável por liderar o design, configuração e implementação de módulos OpenText SAP VIM (incluindo ICC, Enterprise Scan e OCR). O objetivo principal é otimizar o ciclo de Contas a Pagar e automação de faturas.  Principais Responsabilidades: Configurar SAP VIM e integrar com SAP ECC/S4HANA (FI/MM). Desenvolver especificações funcionais para customizações, interfaces e relatórios. Gerenciar fluxos de aprovação, exceções e suporte ponta a ponta (PO e Non-PO). Realizar testes (unitários, integrados e UAT) e ministrar treinamentos.  Requisitos Essenciais: Experiência sólida com SAP VIM/OpenText e tecnologias OCR. Domínio dos processos de SAP FI (AP) e SAP MM.  Inglês Avançado/Fluente.  Diferenciais: Conhecimento em S/4HANA, Fiori, Ariba e certificações OpenText.  Perfil: Mindset voltado à resolução de problemas, proatividade e habilidade em times multiculturais.  Híbrido em SP CLT || Empresa .....:  Randstad Brasil Recursos Humanos LTDA</t>
+        </is>
+      </c>
+      <c r="I775" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>04/02/2026</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t>83538</t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>Analista Desenvolvedor Pl-Sql Sênior</t>
+        </is>
+      </c>
+      <c r="D776" t="inlineStr">
+        <is>
+          <t>Sênior</t>
+        </is>
+      </c>
+      <c r="E776" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="F776" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 02/02/26</t>
+        </is>
+      </c>
+      <c r="G776" t="inlineStr">
+        <is>
+          <t>Buscamos um(a) desenvolvedor(a) experiente para atuar em soluções estratégicas com PL/SQL, em uma das maiores operadoras de saúde do Brasil, em um ambiente desafiador e de alta complexidade.  Atuação com Oracle, PL/SQL, procedures, functions, triggers e packages, além de análise de performance e suporte às áreas de negócio. Desenvolvimento de rotinas de ETL, integrações e processamento de grandes volumes de dados. Criação e manutenção de jobs e schedulers no Oracle.  Contratação PJ – 44h semanais  contrato indeterminado Superior completo ou cursando (TI)  Imprescindível experiência com operadoras de Saúde ou sistemas na área da Saúde.
+Empresa .....:  TalentGroup</t>
+        </is>
+      </c>
+      <c r="H776" t="inlineStr">
+        <is>
+          <t>Home Office - HO - 02/02/26 || Analista Desenvolvedor Pl-Sql Sênior || Buscamos um(a) desenvolvedor(a) experiente para atuar em soluções estratégicas com PL/SQL, em uma das maiores operadoras de saúde do Brasil, em um ambiente desafiador e de alta complexidade.  Atuação com Oracle, PL/SQL, procedures, functions, triggers e packages, além de análise de performance e suporte às áreas de negócio. Desenvolvimento de rotinas de ETL, integrações e processamento de grandes volumes de dados. Criação e manutenção de jobs e schedulers no Oracle.  Contratação PJ – 44h semanais  contrato indeterminado Superior completo ou cursando (TI)  Imprescindível experiência com operadoras de Saúde ou sistemas na área da Saúde. || Empresa .....:  TalentGroup</t>
+        </is>
+      </c>
+      <c r="I776" t="n">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>